<commit_message>
Added tmc memory for filter
</commit_message>
<xml_diff>
--- a/Firmware/memory_map.xlsx
+++ b/Firmware/memory_map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ST\OpenFFBoard\Firmware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D360BDE6-347F-42FD-92E7-DF81C4ABC881}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06A5C4BF-F00F-4A83-8D1C-194AF4026273}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12750" yWindow="4575" windowWidth="28800" windowHeight="15435" xr2:uid="{4859EFD2-ECA4-5640-B170-200D9DB85F48}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{4859EFD2-ECA4-5640-B170-200D9DB85F48}"/>
   </bookViews>
   <sheets>
     <sheet name="Memory setup" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="369">
   <si>
     <t>// Ports</t>
   </si>
@@ -1603,6 +1603,24 @@
   </si>
   <si>
     <t>ADR_FLASH_VERSION</t>
+  </si>
+  <si>
+    <t>ADR_TMC1_TRQ_FILT</t>
+  </si>
+  <si>
+    <t>0x32C</t>
+  </si>
+  <si>
+    <t>ADR_TMC2_TRQ_FILT</t>
+  </si>
+  <si>
+    <t>0x36C</t>
+  </si>
+  <si>
+    <t>0x3AC</t>
+  </si>
+  <si>
+    <t>ADR_TMC3_TRQ_FILT</t>
   </si>
 </sst>
 </file>
@@ -2113,10 +2131,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C5323F2-8FDE-7443-A989-42E1FE5B01C7}">
-  <dimension ref="A1:G168"/>
+  <dimension ref="A1:G171"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView topLeftCell="A137" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A172" sqref="A172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -3094,33 +3112,33 @@
       </c>
     </row>
     <row r="77" spans="1:6">
-      <c r="A77" s="1" t="s">
+      <c r="B77" s="9" t="s">
+        <v>363</v>
+      </c>
+      <c r="C77" s="11" t="s">
+        <v>364</v>
+      </c>
+      <c r="E77" s="23">
+        <v>1</v>
+      </c>
+      <c r="F77" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6">
+      <c r="A78" s="1" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6">
-      <c r="B78" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="C78" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="D78" s="12" t="s">
-        <v>243</v>
-      </c>
-      <c r="E78" s="15">
-        <v>1</v>
-      </c>
-      <c r="F78" s="15">
-        <v>1</v>
       </c>
     </row>
     <row r="79" spans="1:6">
       <c r="B79" s="9" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C79" s="11" t="s">
-        <v>130</v>
+        <v>128</v>
+      </c>
+      <c r="D79" s="12" t="s">
+        <v>243</v>
       </c>
       <c r="E79" s="15">
         <v>1</v>
@@ -3131,10 +3149,10 @@
     </row>
     <row r="80" spans="1:6">
       <c r="B80" s="9" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C80" s="11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E80" s="15">
         <v>1</v>
@@ -3145,13 +3163,10 @@
     </row>
     <row r="81" spans="1:6">
       <c r="B81" s="9" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C81" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="D81" s="12" t="s">
-        <v>244</v>
+        <v>132</v>
       </c>
       <c r="E81" s="15">
         <v>1</v>
@@ -3162,13 +3177,13 @@
     </row>
     <row r="82" spans="1:6">
       <c r="B82" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C82" s="11" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D82" s="12" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E82" s="15">
         <v>1</v>
@@ -3179,13 +3194,13 @@
     </row>
     <row r="83" spans="1:6">
       <c r="B83" s="9" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C83" s="11" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D83" s="12" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E83" s="15">
         <v>1</v>
@@ -3196,13 +3211,13 @@
     </row>
     <row r="84" spans="1:6">
       <c r="B84" s="9" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C84" s="11" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D84" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E84" s="15">
         <v>1</v>
@@ -3213,13 +3228,13 @@
     </row>
     <row r="85" spans="1:6">
       <c r="B85" s="9" t="s">
-        <v>310</v>
+        <v>139</v>
       </c>
       <c r="C85" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="D85" s="24" t="s">
-        <v>309</v>
+        <v>140</v>
+      </c>
+      <c r="D85" s="12" t="s">
+        <v>247</v>
       </c>
       <c r="E85" s="15">
         <v>1</v>
@@ -3230,49 +3245,52 @@
     </row>
     <row r="86" spans="1:6">
       <c r="B86" s="9" t="s">
+        <v>310</v>
+      </c>
+      <c r="C86" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="D86" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="E86" s="15">
+        <v>1</v>
+      </c>
+      <c r="F86" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6">
+      <c r="B87" s="9" t="s">
         <v>306</v>
       </c>
-      <c r="C86" s="11" t="s">
+      <c r="C87" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="D86" s="12" t="s">
+      <c r="D87" s="12" t="s">
         <v>305</v>
       </c>
-      <c r="E86" s="15">
-        <v>1</v>
-      </c>
-      <c r="F86" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6">
-      <c r="A87" s="1" t="s">
+      <c r="E87" s="15">
+        <v>1</v>
+      </c>
+      <c r="F87" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6">
+      <c r="A88" s="1" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6">
-      <c r="B88" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="C88" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="D88" s="12" t="s">
-        <v>249</v>
-      </c>
-      <c r="E88" s="15">
-        <v>1</v>
-      </c>
-      <c r="F88" s="15">
-        <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:6">
       <c r="B89" s="9" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C89" s="11" t="s">
-        <v>146</v>
+        <v>144</v>
+      </c>
+      <c r="D89" s="12" t="s">
+        <v>249</v>
       </c>
       <c r="E89" s="15">
         <v>1</v>
@@ -3283,13 +3301,10 @@
     </row>
     <row r="90" spans="1:6">
       <c r="B90" s="9" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C90" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="D90" s="12" t="s">
-        <v>250</v>
+        <v>146</v>
       </c>
       <c r="E90" s="15">
         <v>1</v>
@@ -3300,21 +3315,27 @@
     </row>
     <row r="91" spans="1:6">
       <c r="B91" s="9" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C91" s="11" t="s">
-        <v>150</v>
+        <v>148</v>
+      </c>
+      <c r="D91" s="12" t="s">
+        <v>250</v>
       </c>
       <c r="E91" s="15">
+        <v>1</v>
+      </c>
+      <c r="F91" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="92" spans="1:6">
       <c r="B92" s="9" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C92" s="11" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E92" s="15">
         <v>1</v>
@@ -3322,10 +3343,10 @@
     </row>
     <row r="93" spans="1:6">
       <c r="B93" s="9" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C93" s="11" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E93" s="15">
         <v>1</v>
@@ -3333,24 +3354,21 @@
     </row>
     <row r="94" spans="1:6">
       <c r="B94" s="9" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C94" s="11" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E94" s="15">
-        <v>1</v>
-      </c>
-      <c r="F94" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="95" spans="1:6">
       <c r="B95" s="9" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C95" s="11" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E95" s="15">
         <v>1</v>
@@ -3361,10 +3379,10 @@
     </row>
     <row r="96" spans="1:6">
       <c r="B96" s="9" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C96" s="11" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E96" s="15">
         <v>1</v>
@@ -3375,10 +3393,10 @@
     </row>
     <row r="97" spans="1:6">
       <c r="B97" s="9" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C97" s="11" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E97" s="15">
         <v>1</v>
@@ -3389,10 +3407,10 @@
     </row>
     <row r="98" spans="1:6">
       <c r="B98" s="9" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C98" s="11" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E98" s="15">
         <v>1</v>
@@ -3403,31 +3421,37 @@
     </row>
     <row r="99" spans="1:6">
       <c r="B99" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="C99" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="E99" s="15">
+        <v>1</v>
+      </c>
+      <c r="F99" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6">
+      <c r="B100" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="C99" s="11" t="s">
+      <c r="C100" s="11" t="s">
         <v>166</v>
       </c>
-      <c r="E99" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6">
-      <c r="A100" s="1" t="s">
-        <v>13</v>
+      <c r="E100" s="15">
+        <v>1</v>
       </c>
     </row>
     <row r="101" spans="1:6">
       <c r="B101" s="9" t="s">
-        <v>167</v>
+        <v>365</v>
       </c>
       <c r="C101" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="D101" s="12" t="s">
-        <v>243</v>
-      </c>
-      <c r="E101" s="15">
+        <v>366</v>
+      </c>
+      <c r="E101" s="23">
         <v>1</v>
       </c>
       <c r="F101" s="15">
@@ -3435,25 +3459,19 @@
       </c>
     </row>
     <row r="102" spans="1:6">
-      <c r="B102" s="9" t="s">
-        <v>169</v>
-      </c>
-      <c r="C102" s="11" t="s">
-        <v>170</v>
-      </c>
-      <c r="E102" s="15">
-        <v>1</v>
-      </c>
-      <c r="F102" s="15">
-        <v>1</v>
+      <c r="A102" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="103" spans="1:6">
       <c r="B103" s="9" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C103" s="11" t="s">
-        <v>172</v>
+        <v>168</v>
+      </c>
+      <c r="D103" s="12" t="s">
+        <v>243</v>
       </c>
       <c r="E103" s="15">
         <v>1</v>
@@ -3464,13 +3482,10 @@
     </row>
     <row r="104" spans="1:6">
       <c r="B104" s="9" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C104" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="D104" s="12" t="s">
-        <v>244</v>
+        <v>170</v>
       </c>
       <c r="E104" s="15">
         <v>1</v>
@@ -3481,13 +3496,10 @@
     </row>
     <row r="105" spans="1:6">
       <c r="B105" s="9" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C105" s="11" t="s">
-        <v>176</v>
-      </c>
-      <c r="D105" s="12" t="s">
-        <v>245</v>
+        <v>172</v>
       </c>
       <c r="E105" s="15">
         <v>1</v>
@@ -3498,13 +3510,13 @@
     </row>
     <row r="106" spans="1:6">
       <c r="B106" s="9" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C106" s="11" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="D106" s="12" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="E106" s="15">
         <v>1</v>
@@ -3515,13 +3527,13 @@
     </row>
     <row r="107" spans="1:6">
       <c r="B107" s="9" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C107" s="11" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D107" s="12" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E107" s="15">
         <v>1</v>
@@ -3532,13 +3544,13 @@
     </row>
     <row r="108" spans="1:6">
       <c r="B108" s="9" t="s">
-        <v>311</v>
+        <v>177</v>
       </c>
       <c r="C108" s="11" t="s">
-        <v>181</v>
-      </c>
-      <c r="D108" s="24" t="s">
-        <v>309</v>
+        <v>178</v>
+      </c>
+      <c r="D108" s="12" t="s">
+        <v>246</v>
       </c>
       <c r="E108" s="15">
         <v>1</v>
@@ -3549,13 +3561,13 @@
     </row>
     <row r="109" spans="1:6">
       <c r="B109" s="9" t="s">
-        <v>307</v>
+        <v>179</v>
       </c>
       <c r="C109" s="11" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D109" s="12" t="s">
-        <v>305</v>
+        <v>247</v>
       </c>
       <c r="E109" s="15">
         <v>1</v>
@@ -3565,19 +3577,31 @@
       </c>
     </row>
     <row r="110" spans="1:6">
-      <c r="A110" s="1" t="s">
-        <v>14</v>
+      <c r="B110" s="9" t="s">
+        <v>311</v>
+      </c>
+      <c r="C110" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="D110" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="E110" s="15">
+        <v>1</v>
+      </c>
+      <c r="F110" s="15">
+        <v>1</v>
       </c>
     </row>
     <row r="111" spans="1:6">
       <c r="B111" s="9" t="s">
-        <v>183</v>
+        <v>307</v>
       </c>
       <c r="C111" s="11" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D111" s="12" t="s">
-        <v>249</v>
+        <v>305</v>
       </c>
       <c r="E111" s="15">
         <v>1</v>
@@ -3587,28 +3611,19 @@
       </c>
     </row>
     <row r="112" spans="1:6">
-      <c r="B112" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="C112" s="11" t="s">
-        <v>186</v>
-      </c>
-      <c r="E112" s="15">
-        <v>1</v>
-      </c>
-      <c r="F112" s="15">
-        <v>1</v>
+      <c r="A112" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="113" spans="1:6">
       <c r="B113" s="9" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C113" s="11" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="D113" s="12" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E113" s="15">
         <v>1</v>
@@ -3619,32 +3634,41 @@
     </row>
     <row r="114" spans="1:6">
       <c r="B114" s="9" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C114" s="11" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="E114" s="15">
+        <v>1</v>
+      </c>
+      <c r="F114" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="115" spans="1:6">
       <c r="B115" s="9" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C115" s="11" t="s">
-        <v>192</v>
+        <v>188</v>
+      </c>
+      <c r="D115" s="12" t="s">
+        <v>250</v>
       </c>
       <c r="E115" s="15">
+        <v>1</v>
+      </c>
+      <c r="F115" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="116" spans="1:6">
       <c r="B116" s="9" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C116" s="11" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="E116" s="15">
         <v>1</v>
@@ -3652,38 +3676,32 @@
     </row>
     <row r="117" spans="1:6">
       <c r="B117" s="9" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C117" s="11" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E117" s="15">
-        <v>1</v>
-      </c>
-      <c r="F117" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="118" spans="1:6">
       <c r="B118" s="9" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C118" s="11" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="E118" s="15">
-        <v>1</v>
-      </c>
-      <c r="F118" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="119" spans="1:6">
       <c r="B119" s="9" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C119" s="11" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="E119" s="15">
         <v>1</v>
@@ -3694,10 +3712,10 @@
     </row>
     <row r="120" spans="1:6">
       <c r="B120" s="9" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C120" s="11" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="E120" s="15">
         <v>1</v>
@@ -3708,10 +3726,10 @@
     </row>
     <row r="121" spans="1:6">
       <c r="B121" s="9" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C121" s="11" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="E121" s="15">
         <v>1</v>
@@ -3722,45 +3740,51 @@
     </row>
     <row r="122" spans="1:6">
       <c r="B122" s="9" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C122" s="11" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="E122" s="15">
         <v>1</v>
       </c>
+      <c r="F122" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="123" spans="1:6">
-      <c r="A123" s="1" t="s">
-        <v>15</v>
+      <c r="B123" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="C123" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="E123" s="15">
+        <v>1</v>
+      </c>
+      <c r="F123" s="15">
+        <v>1</v>
       </c>
     </row>
     <row r="124" spans="1:6">
       <c r="B124" s="9" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C124" s="11" t="s">
-        <v>208</v>
-      </c>
-      <c r="D124" s="12" t="s">
-        <v>251</v>
+        <v>206</v>
       </c>
       <c r="E124" s="15">
-        <v>1</v>
-      </c>
-      <c r="F124" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="125" spans="1:6">
       <c r="B125" s="9" t="s">
-        <v>209</v>
+        <v>368</v>
       </c>
       <c r="C125" s="11" t="s">
-        <v>210</v>
-      </c>
-      <c r="E125" s="15">
+        <v>367</v>
+      </c>
+      <c r="E125" s="23">
         <v>1</v>
       </c>
       <c r="F125" s="15">
@@ -3768,33 +3792,33 @@
       </c>
     </row>
     <row r="126" spans="1:6">
-      <c r="B126" s="9" t="s">
-        <v>211</v>
-      </c>
-      <c r="C126" s="11" t="s">
-        <v>212</v>
-      </c>
-      <c r="E126" s="15">
-        <v>1</v>
-      </c>
-      <c r="F126" s="15">
-        <v>1</v>
+      <c r="A126" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="127" spans="1:6">
-      <c r="A127" t="s">
-        <v>278</v>
+      <c r="B127" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="C127" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="D127" s="12" t="s">
+        <v>251</v>
+      </c>
+      <c r="E127" s="15">
+        <v>1</v>
+      </c>
+      <c r="F127" s="15">
+        <v>1</v>
       </c>
     </row>
     <row r="128" spans="1:6">
       <c r="B128" s="9" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C128" s="11" t="s">
-        <v>214</v>
-      </c>
-      <c r="D128" s="12" t="s">
-        <v>252</v>
+        <v>210</v>
       </c>
       <c r="E128" s="15">
         <v>1</v>
@@ -3805,13 +3829,10 @@
     </row>
     <row r="129" spans="1:6">
       <c r="B129" s="9" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C129" s="11" t="s">
-        <v>216</v>
-      </c>
-      <c r="D129" s="12" t="s">
-        <v>253</v>
+        <v>212</v>
       </c>
       <c r="E129" s="15">
         <v>1</v>
@@ -3821,31 +3842,19 @@
       </c>
     </row>
     <row r="130" spans="1:6">
-      <c r="B130" s="9" t="s">
-        <v>217</v>
-      </c>
-      <c r="C130" s="11" t="s">
-        <v>218</v>
-      </c>
-      <c r="D130" s="12" t="s">
-        <v>254</v>
-      </c>
-      <c r="E130" s="15">
-        <v>1</v>
-      </c>
-      <c r="F130" s="15">
-        <v>1</v>
+      <c r="A130" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="131" spans="1:6">
       <c r="B131" s="9" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="C131" s="11" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="D131" s="12" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="E131" s="15">
         <v>1</v>
@@ -3856,10 +3865,10 @@
     </row>
     <row r="132" spans="1:6">
       <c r="B132" s="9" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="C132" s="11" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="D132" s="12" t="s">
         <v>253</v>
@@ -3873,10 +3882,10 @@
     </row>
     <row r="133" spans="1:6">
       <c r="B133" s="9" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="C133" s="11" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="D133" s="12" t="s">
         <v>254</v>
@@ -3890,10 +3899,10 @@
     </row>
     <row r="134" spans="1:6">
       <c r="B134" s="9" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="C134" s="11" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="D134" s="12" t="s">
         <v>255</v>
@@ -3907,10 +3916,10 @@
     </row>
     <row r="135" spans="1:6">
       <c r="B135" s="9" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="C135" s="11" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="D135" s="12" t="s">
         <v>253</v>
@@ -3924,10 +3933,10 @@
     </row>
     <row r="136" spans="1:6">
       <c r="B136" s="9" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="C136" s="11" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="D136" s="12" t="s">
         <v>254</v>
@@ -3940,16 +3949,31 @@
       </c>
     </row>
     <row r="137" spans="1:6">
-      <c r="A137" s="1" t="s">
-        <v>16</v>
+      <c r="B137" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="C137" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="D137" s="12" t="s">
+        <v>255</v>
+      </c>
+      <c r="E137" s="15">
+        <v>1</v>
+      </c>
+      <c r="F137" s="15">
+        <v>1</v>
       </c>
     </row>
     <row r="138" spans="1:6">
       <c r="B138" s="9" t="s">
-        <v>300</v>
+        <v>227</v>
       </c>
       <c r="C138" s="11" t="s">
-        <v>301</v>
+        <v>228</v>
+      </c>
+      <c r="D138" s="12" t="s">
+        <v>253</v>
       </c>
       <c r="E138" s="15">
         <v>1</v>
@@ -3959,14 +3983,16 @@
       </c>
     </row>
     <row r="139" spans="1:6">
-      <c r="A139" s="20"/>
       <c r="B139" s="9" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C139" s="11" t="s">
-        <v>232</v>
-      </c>
-      <c r="E139" s="23">
+        <v>230</v>
+      </c>
+      <c r="D139" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="E139" s="15">
         <v>1</v>
       </c>
       <c r="F139" s="15">
@@ -3974,107 +4000,97 @@
       </c>
     </row>
     <row r="140" spans="1:6">
-      <c r="A140" s="20" t="s">
-        <v>295</v>
+      <c r="A140" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="141" spans="1:6">
       <c r="B141" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="C141" s="11" t="s">
+        <v>301</v>
+      </c>
+      <c r="E141" s="15">
+        <v>1</v>
+      </c>
+      <c r="F141" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6">
+      <c r="A142" s="20"/>
+      <c r="B142" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="C142" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="E142" s="23">
+        <v>1</v>
+      </c>
+      <c r="F142" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6">
+      <c r="A143" s="20" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6">
+      <c r="B144" s="9" t="s">
         <v>296</v>
       </c>
-      <c r="C141" s="11" t="s">
+      <c r="C144" s="11" t="s">
         <v>298</v>
       </c>
-      <c r="E141" s="23">
-        <v>1</v>
-      </c>
-      <c r="F141" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="142" spans="1:6">
-      <c r="B142" s="9" t="s">
+      <c r="E144" s="23">
+        <v>1</v>
+      </c>
+      <c r="F144" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6">
+      <c r="B145" s="9" t="s">
         <v>297</v>
       </c>
-      <c r="C142" s="11" t="s">
+      <c r="C145" s="11" t="s">
         <v>299</v>
       </c>
-      <c r="E142" s="23">
-        <v>1</v>
-      </c>
-      <c r="F142" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="143" spans="1:6">
-      <c r="A143" t="s">
+      <c r="E145" s="23">
+        <v>1</v>
+      </c>
+      <c r="F145" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6">
+      <c r="A146" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="144" spans="1:6">
-      <c r="B144" s="25" t="s">
+    <row r="147" spans="1:6">
+      <c r="B147" s="25" t="s">
         <v>313</v>
       </c>
-      <c r="C144" s="26" t="s">
+      <c r="C147" s="26" t="s">
         <v>314</v>
       </c>
-      <c r="E144" s="23">
-        <v>1</v>
-      </c>
-      <c r="F144" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="145" spans="1:6">
-      <c r="B145" s="25" t="s">
+      <c r="E147" s="23">
+        <v>1</v>
+      </c>
+      <c r="F147" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6">
+      <c r="B148" s="25" t="s">
         <v>330</v>
       </c>
-      <c r="C145" s="26" t="s">
+      <c r="C148" s="26" t="s">
         <v>315</v>
-      </c>
-      <c r="E145" s="23">
-        <v>1</v>
-      </c>
-      <c r="F145" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="146" spans="1:6">
-      <c r="B146" s="25" t="s">
-        <v>331</v>
-      </c>
-      <c r="C146" s="26" t="s">
-        <v>316</v>
-      </c>
-      <c r="E146" s="23">
-        <v>1</v>
-      </c>
-      <c r="F146" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="147" spans="1:6">
-      <c r="A147" s="21"/>
-      <c r="B147" s="25" t="s">
-        <v>333</v>
-      </c>
-      <c r="C147" s="26" t="s">
-        <v>317</v>
-      </c>
-      <c r="E147" s="23">
-        <v>1</v>
-      </c>
-      <c r="F147" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="148" spans="1:6">
-      <c r="A148" s="21"/>
-      <c r="B148" s="25" t="s">
-        <v>332</v>
-      </c>
-      <c r="C148" s="26" t="s">
-        <v>318</v>
       </c>
       <c r="E148" s="23">
         <v>1</v>
@@ -4085,10 +4101,10 @@
     </row>
     <row r="149" spans="1:6">
       <c r="B149" s="25" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="C149" s="26" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="E149" s="23">
         <v>1</v>
@@ -4098,11 +4114,12 @@
       </c>
     </row>
     <row r="150" spans="1:6">
+      <c r="A150" s="21"/>
       <c r="B150" s="25" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C150" s="26" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E150" s="23">
         <v>1</v>
@@ -4112,11 +4129,12 @@
       </c>
     </row>
     <row r="151" spans="1:6">
+      <c r="A151" s="21"/>
       <c r="B151" s="25" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="C151" s="26" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="E151" s="23">
         <v>1</v>
@@ -4127,10 +4145,10 @@
     </row>
     <row r="152" spans="1:6">
       <c r="B152" s="25" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="C152" s="26" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="E152" s="23">
         <v>1</v>
@@ -4141,10 +4159,10 @@
     </row>
     <row r="153" spans="1:6">
       <c r="B153" s="25" t="s">
-        <v>344</v>
+        <v>335</v>
       </c>
       <c r="C153" s="26" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="E153" s="23">
         <v>1</v>
@@ -4155,10 +4173,10 @@
     </row>
     <row r="154" spans="1:6">
       <c r="B154" s="25" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C154" s="26" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="E154" s="23">
         <v>1</v>
@@ -4169,10 +4187,10 @@
     </row>
     <row r="155" spans="1:6">
       <c r="B155" s="25" t="s">
-        <v>338</v>
+        <v>343</v>
       </c>
       <c r="C155" s="26" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="E155" s="23">
         <v>1</v>
@@ -4183,10 +4201,10 @@
     </row>
     <row r="156" spans="1:6">
       <c r="B156" s="25" t="s">
-        <v>339</v>
+        <v>344</v>
       </c>
       <c r="C156" s="26" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="E156" s="23">
         <v>1</v>
@@ -4197,10 +4215,10 @@
     </row>
     <row r="157" spans="1:6">
       <c r="B157" s="25" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="C157" s="26" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="E157" s="23">
         <v>1</v>
@@ -4211,10 +4229,10 @@
     </row>
     <row r="158" spans="1:6">
       <c r="B158" s="25" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C158" s="26" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="E158" s="23">
         <v>1</v>
@@ -4225,10 +4243,10 @@
     </row>
     <row r="159" spans="1:6">
       <c r="B159" s="25" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="C159" s="26" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="E159" s="23">
         <v>1</v>
@@ -4239,10 +4257,10 @@
     </row>
     <row r="160" spans="1:6">
       <c r="B160" s="25" t="s">
-        <v>353</v>
-      </c>
-      <c r="C160" s="27" t="s">
-        <v>345</v>
+        <v>340</v>
+      </c>
+      <c r="C160" s="26" t="s">
+        <v>327</v>
       </c>
       <c r="E160" s="23">
         <v>1</v>
@@ -4253,10 +4271,10 @@
     </row>
     <row r="161" spans="1:6">
       <c r="B161" s="25" t="s">
-        <v>354</v>
-      </c>
-      <c r="C161" s="27" t="s">
-        <v>346</v>
+        <v>341</v>
+      </c>
+      <c r="C161" s="26" t="s">
+        <v>328</v>
       </c>
       <c r="E161" s="23">
         <v>1</v>
@@ -4267,10 +4285,10 @@
     </row>
     <row r="162" spans="1:6">
       <c r="B162" s="25" t="s">
-        <v>355</v>
-      </c>
-      <c r="C162" s="27" t="s">
-        <v>347</v>
+        <v>342</v>
+      </c>
+      <c r="C162" s="26" t="s">
+        <v>329</v>
       </c>
       <c r="E162" s="23">
         <v>1</v>
@@ -4281,10 +4299,10 @@
     </row>
     <row r="163" spans="1:6">
       <c r="B163" s="25" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="C163" s="27" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="E163" s="23">
         <v>1</v>
@@ -4295,10 +4313,10 @@
     </row>
     <row r="164" spans="1:6">
       <c r="B164" s="25" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="C164" s="27" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="E164" s="23">
         <v>1</v>
@@ -4309,10 +4327,10 @@
     </row>
     <row r="165" spans="1:6">
       <c r="B165" s="25" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="C165" s="27" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="E165" s="23">
         <v>1</v>
@@ -4323,10 +4341,10 @@
     </row>
     <row r="166" spans="1:6">
       <c r="B166" s="25" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="C166" s="27" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="E166" s="23">
         <v>1</v>
@@ -4337,20 +4355,62 @@
     </row>
     <row r="167" spans="1:6">
       <c r="B167" s="25" t="s">
+        <v>357</v>
+      </c>
+      <c r="C167" s="27" t="s">
+        <v>349</v>
+      </c>
+      <c r="E167" s="23">
+        <v>1</v>
+      </c>
+      <c r="F167" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6">
+      <c r="B168" s="25" t="s">
+        <v>358</v>
+      </c>
+      <c r="C168" s="27" t="s">
+        <v>350</v>
+      </c>
+      <c r="E168" s="23">
+        <v>1</v>
+      </c>
+      <c r="F168" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6">
+      <c r="B169" s="25" t="s">
+        <v>359</v>
+      </c>
+      <c r="C169" s="27" t="s">
+        <v>351</v>
+      </c>
+      <c r="E169" s="23">
+        <v>1</v>
+      </c>
+      <c r="F169" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6">
+      <c r="B170" s="25" t="s">
         <v>360</v>
       </c>
-      <c r="C167" s="27" t="s">
+      <c r="C170" s="27" t="s">
         <v>352</v>
       </c>
-      <c r="E167" s="23">
-        <v>1</v>
-      </c>
-      <c r="F167" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="168" spans="1:6">
-      <c r="A168" t="s">
+      <c r="E170" s="23">
+        <v>1</v>
+      </c>
+      <c r="F170" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6">
+      <c r="A171" t="s">
         <v>290</v>
       </c>
     </row>
@@ -4364,8 +4424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A28F574A-1A18-F84B-837D-BB0502A7BBD8}">
   <dimension ref="A1:C336"/>
   <sheetViews>
-    <sheetView topLeftCell="A189" workbookViewId="0">
-      <selection activeCell="A204" sqref="A204"/>
+    <sheetView tabSelected="1" topLeftCell="A184" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37:A226"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -4436,7 +4496,7 @@
     <row r="15" spans="1:2">
       <c r="A15" s="2" t="str">
         <f>_xlfn.CONCAT("#define NB_OF_VAR ",FIXED(SUM('Memory setup'!E:E),0))</f>
-        <v>#define NB_OF_VAR 141</v>
+        <v>#define NB_OF_VAR 144</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -4452,7 +4512,7 @@
     <row r="19" spans="1:1">
       <c r="A19" s="2" t="str">
         <f>_xlfn.CONCAT("#define NB_EXPORTABLE_ADR ",FIXED(SUM('Memory setup'!F:F),0))</f>
-        <v>#define NB_EXPORTABLE_ADR 126</v>
+        <v>#define NB_EXPORTABLE_ADR 129</v>
       </c>
     </row>
     <row r="20" spans="1:1">
@@ -4958,571 +5018,571 @@
     <row r="112" spans="1:1">
       <c r="A112" t="str">
         <f>IF('Memory setup'!A77&lt;&gt;"",IF('Memory setup'!A77="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A77),IF('Memory setup'!E77=1,_xlfn.CONCAT("#define ",'Memory setup'!B77," ",'Memory setup'!C77," ",'Memory setup'!D77),""))</f>
-        <v>// AXIS2</v>
+        <v xml:space="preserve">#define ADR_TMC1_TRQ_FILT 0x32C </v>
       </c>
     </row>
     <row r="113" spans="1:1">
       <c r="A113" t="str">
         <f>IF('Memory setup'!A78&lt;&gt;"",IF('Memory setup'!A78="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A78),IF('Memory setup'!E78=1,_xlfn.CONCAT("#define ",'Memory setup'!B78," ",'Memory setup'!C78," ",'Memory setup'!D78),""))</f>
-        <v>#define ADR_AXIS2_CONFIG 0x341 // 0-2 ENC, 3-5 DRV</v>
+        <v>// AXIS2</v>
       </c>
     </row>
     <row r="114" spans="1:1">
       <c r="A114" t="str">
         <f>IF('Memory setup'!A79&lt;&gt;"",IF('Memory setup'!A79="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A79),IF('Memory setup'!E79=1,_xlfn.CONCAT("#define ",'Memory setup'!B79," ",'Memory setup'!C79," ",'Memory setup'!D79),""))</f>
-        <v xml:space="preserve">#define ADR_AXIS2_POWER 0x342 </v>
+        <v>#define ADR_AXIS2_CONFIG 0x341 // 0-2 ENC, 3-5 DRV</v>
       </c>
     </row>
     <row r="115" spans="1:1">
       <c r="A115" t="str">
         <f>IF('Memory setup'!A80&lt;&gt;"",IF('Memory setup'!A80="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A80),IF('Memory setup'!E80=1,_xlfn.CONCAT("#define ",'Memory setup'!B80," ",'Memory setup'!C80," ",'Memory setup'!D80),""))</f>
-        <v xml:space="preserve">#define ADR_AXIS2_DEGREES 0x343 </v>
+        <v xml:space="preserve">#define ADR_AXIS2_POWER 0x342 </v>
       </c>
     </row>
     <row r="116" spans="1:1">
       <c r="A116" t="str">
         <f>IF('Memory setup'!A81&lt;&gt;"",IF('Memory setup'!A81="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A81),IF('Memory setup'!E81=1,_xlfn.CONCAT("#define ",'Memory setup'!B81," ",'Memory setup'!C81," ",'Memory setup'!D81),""))</f>
-        <v>#define ADR_AXIS2_MAX_SPEED 0x344 // Store the max speed</v>
+        <v xml:space="preserve">#define ADR_AXIS2_DEGREES 0x343 </v>
       </c>
     </row>
     <row r="117" spans="1:1">
       <c r="A117" t="str">
         <f>IF('Memory setup'!A82&lt;&gt;"",IF('Memory setup'!A82="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A82),IF('Memory setup'!E82=1,_xlfn.CONCAT("#define ",'Memory setup'!B82," ",'Memory setup'!C82," ",'Memory setup'!D82),""))</f>
-        <v>#define ADR_AXIS2_MAX_ACCEL 0x345 // Store the max accel</v>
+        <v>#define ADR_AXIS2_MAX_SPEED 0x344 // Store the max speed</v>
       </c>
     </row>
     <row r="118" spans="1:1">
       <c r="A118" t="str">
         <f>IF('Memory setup'!A83&lt;&gt;"",IF('Memory setup'!A83="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A83),IF('Memory setup'!E83=1,_xlfn.CONCAT("#define ",'Memory setup'!B83," ",'Memory setup'!C83," ",'Memory setup'!D83),""))</f>
-        <v>#define ADR_AXIS2_ENDSTOP 0x347 // 0-7 endstop margin, 8-15 endstop stiffness</v>
+        <v>#define ADR_AXIS2_MAX_ACCEL 0x345 // Store the max accel</v>
       </c>
     </row>
     <row r="119" spans="1:1">
       <c r="A119" t="str">
         <f>IF('Memory setup'!A84&lt;&gt;"",IF('Memory setup'!A84="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A84),IF('Memory setup'!E84=1,_xlfn.CONCAT("#define ",'Memory setup'!B84," ",'Memory setup'!C84," ",'Memory setup'!D84),""))</f>
-        <v>#define ADR_AXIS2_EFFECTS1 0x348 // 0-7 idlespring, 8-15 damper</v>
+        <v>#define ADR_AXIS2_ENDSTOP 0x347 // 0-7 endstop margin, 8-15 endstop stiffness</v>
       </c>
     </row>
     <row r="120" spans="1:1">
       <c r="A120" t="str">
         <f>IF('Memory setup'!A85&lt;&gt;"",IF('Memory setup'!A85="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A85),IF('Memory setup'!E85=1,_xlfn.CONCAT("#define ",'Memory setup'!B85," ",'Memory setup'!C85," ",'Memory setup'!D85),""))</f>
-        <v>#define ADR_AXIS2_SPEEDACCEL_FILTER 0x349 // Speed/Accel filter Lowpass profile</v>
+        <v>#define ADR_AXIS2_EFFECTS1 0x348 // 0-7 idlespring, 8-15 damper</v>
       </c>
     </row>
     <row r="121" spans="1:1">
       <c r="A121" t="str">
         <f>IF('Memory setup'!A86&lt;&gt;"",IF('Memory setup'!A86="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A86),IF('Memory setup'!E86=1,_xlfn.CONCAT("#define ",'Memory setup'!B86," ",'Memory setup'!C86," ",'Memory setup'!D86),""))</f>
-        <v>#define ADR_AXIS2_ENC_RATIO 0x34A // Store the encoder ratio for an axis</v>
+        <v>#define ADR_AXIS2_SPEEDACCEL_FILTER 0x349 // Speed/Accel filter Lowpass profile</v>
       </c>
     </row>
     <row r="122" spans="1:1">
       <c r="A122" t="str">
         <f>IF('Memory setup'!A87&lt;&gt;"",IF('Memory setup'!A87="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A87),IF('Memory setup'!E87=1,_xlfn.CONCAT("#define ",'Memory setup'!B87," ",'Memory setup'!C87," ",'Memory setup'!D87),""))</f>
-        <v>// TMC2</v>
+        <v>#define ADR_AXIS2_ENC_RATIO 0x34A // Store the encoder ratio for an axis</v>
       </c>
     </row>
     <row r="123" spans="1:1">
       <c r="A123" t="str">
         <f>IF('Memory setup'!A88&lt;&gt;"",IF('Memory setup'!A88="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A88),IF('Memory setup'!E88=1,_xlfn.CONCAT("#define ",'Memory setup'!B88," ",'Memory setup'!C88," ",'Memory setup'!D88),""))</f>
-        <v>#define ADR_TMC2_MOTCONF 0x360 // 0-2: MotType 3-5: PhiE source 6-15: Poles</v>
+        <v>// TMC2</v>
       </c>
     </row>
     <row r="124" spans="1:1">
       <c r="A124" t="str">
         <f>IF('Memory setup'!A89&lt;&gt;"",IF('Memory setup'!A89="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A89),IF('Memory setup'!E89=1,_xlfn.CONCAT("#define ",'Memory setup'!B89," ",'Memory setup'!C89," ",'Memory setup'!D89),""))</f>
-        <v xml:space="preserve">#define ADR_TMC2_CPR 0x361 </v>
+        <v>#define ADR_TMC2_MOTCONF 0x360 // 0-2: MotType 3-5: PhiE source 6-15: Poles</v>
       </c>
     </row>
     <row r="125" spans="1:1">
       <c r="A125" t="str">
         <f>IF('Memory setup'!A90&lt;&gt;"",IF('Memory setup'!A90="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A90),IF('Memory setup'!E90=1,_xlfn.CONCAT("#define ",'Memory setup'!B90," ",'Memory setup'!C90," ",'Memory setup'!D90),""))</f>
-        <v>#define ADR_TMC2_ENCA 0x362 // Misc</v>
+        <v xml:space="preserve">#define ADR_TMC2_CPR 0x361 </v>
       </c>
     </row>
     <row r="126" spans="1:1">
       <c r="A126" t="str">
         <f>IF('Memory setup'!A91&lt;&gt;"",IF('Memory setup'!A91="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A91),IF('Memory setup'!E91=1,_xlfn.CONCAT("#define ",'Memory setup'!B91," ",'Memory setup'!C91," ",'Memory setup'!D91),""))</f>
-        <v xml:space="preserve">#define ADR_TMC2_ADC_I0_OFS 0x363 </v>
+        <v>#define ADR_TMC2_ENCA 0x362 // Misc</v>
       </c>
     </row>
     <row r="127" spans="1:1">
       <c r="A127" t="str">
         <f>IF('Memory setup'!A92&lt;&gt;"",IF('Memory setup'!A92="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A92),IF('Memory setup'!E92=1,_xlfn.CONCAT("#define ",'Memory setup'!B92," ",'Memory setup'!C92," ",'Memory setup'!D92),""))</f>
-        <v xml:space="preserve">#define ADR_TMC2_ADC_I1_OFS 0x364 </v>
+        <v xml:space="preserve">#define ADR_TMC2_ADC_I0_OFS 0x363 </v>
       </c>
     </row>
     <row r="128" spans="1:1">
       <c r="A128" t="str">
         <f>IF('Memory setup'!A93&lt;&gt;"",IF('Memory setup'!A93="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A93),IF('Memory setup'!E93=1,_xlfn.CONCAT("#define ",'Memory setup'!B93," ",'Memory setup'!C93," ",'Memory setup'!D93),""))</f>
-        <v xml:space="preserve">#define ADR_TMC2_ENC_OFFSET 0x365 </v>
+        <v xml:space="preserve">#define ADR_TMC2_ADC_I1_OFS 0x364 </v>
       </c>
     </row>
     <row r="129" spans="1:1">
       <c r="A129" t="str">
         <f>IF('Memory setup'!A94&lt;&gt;"",IF('Memory setup'!A94="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A94),IF('Memory setup'!E94=1,_xlfn.CONCAT("#define ",'Memory setup'!B94," ",'Memory setup'!C94," ",'Memory setup'!D94),""))</f>
-        <v xml:space="preserve">#define ADR_TMC2_OFFSETFLUX 0x366 </v>
+        <v xml:space="preserve">#define ADR_TMC2_ENC_OFFSET 0x365 </v>
       </c>
     </row>
     <row r="130" spans="1:1">
       <c r="A130" t="str">
         <f>IF('Memory setup'!A95&lt;&gt;"",IF('Memory setup'!A95="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A95),IF('Memory setup'!E95=1,_xlfn.CONCAT("#define ",'Memory setup'!B95," ",'Memory setup'!C95," ",'Memory setup'!D95),""))</f>
-        <v xml:space="preserve">#define ADR_TMC2_TORQUE_P 0x367 </v>
+        <v xml:space="preserve">#define ADR_TMC2_OFFSETFLUX 0x366 </v>
       </c>
     </row>
     <row r="131" spans="1:1">
       <c r="A131" t="str">
         <f>IF('Memory setup'!A96&lt;&gt;"",IF('Memory setup'!A96="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A96),IF('Memory setup'!E96=1,_xlfn.CONCAT("#define ",'Memory setup'!B96," ",'Memory setup'!C96," ",'Memory setup'!D96),""))</f>
-        <v xml:space="preserve">#define ADR_TMC2_TORQUE_I 0x368 </v>
+        <v xml:space="preserve">#define ADR_TMC2_TORQUE_P 0x367 </v>
       </c>
     </row>
     <row r="132" spans="1:1">
       <c r="A132" t="str">
         <f>IF('Memory setup'!A97&lt;&gt;"",IF('Memory setup'!A97="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A97),IF('Memory setup'!E97=1,_xlfn.CONCAT("#define ",'Memory setup'!B97," ",'Memory setup'!C97," ",'Memory setup'!D97),""))</f>
-        <v xml:space="preserve">#define ADR_TMC2_FLUX_P 0x369 </v>
+        <v xml:space="preserve">#define ADR_TMC2_TORQUE_I 0x368 </v>
       </c>
     </row>
     <row r="133" spans="1:1">
       <c r="A133" t="str">
         <f>IF('Memory setup'!A98&lt;&gt;"",IF('Memory setup'!A98="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A98),IF('Memory setup'!E98=1,_xlfn.CONCAT("#define ",'Memory setup'!B98," ",'Memory setup'!C98," ",'Memory setup'!D98),""))</f>
-        <v xml:space="preserve">#define ADR_TMC2_FLUX_I 0x36A </v>
+        <v xml:space="preserve">#define ADR_TMC2_FLUX_P 0x369 </v>
       </c>
     </row>
     <row r="134" spans="1:1">
       <c r="A134" t="str">
         <f>IF('Memory setup'!A99&lt;&gt;"",IF('Memory setup'!A99="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A99),IF('Memory setup'!E99=1,_xlfn.CONCAT("#define ",'Memory setup'!B99," ",'Memory setup'!C99," ",'Memory setup'!D99),""))</f>
-        <v xml:space="preserve">#define ADR_TMC2_PHIE_OFS 0x36B </v>
+        <v xml:space="preserve">#define ADR_TMC2_FLUX_I 0x36A </v>
       </c>
     </row>
     <row r="135" spans="1:1">
       <c r="A135" t="str">
         <f>IF('Memory setup'!A100&lt;&gt;"",IF('Memory setup'!A100="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A100),IF('Memory setup'!E100=1,_xlfn.CONCAT("#define ",'Memory setup'!B100," ",'Memory setup'!C100," ",'Memory setup'!D100),""))</f>
-        <v>// AXIS3</v>
+        <v xml:space="preserve">#define ADR_TMC2_PHIE_OFS 0x36B </v>
       </c>
     </row>
     <row r="136" spans="1:1">
       <c r="A136" t="str">
         <f>IF('Memory setup'!A101&lt;&gt;"",IF('Memory setup'!A101="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A101),IF('Memory setup'!E101=1,_xlfn.CONCAT("#define ",'Memory setup'!B101," ",'Memory setup'!C101," ",'Memory setup'!D101),""))</f>
-        <v>#define ADR_AXIS3_CONFIG 0x381 // 0-2 ENC, 3-5 DRV</v>
+        <v xml:space="preserve">#define ADR_TMC2_TRQ_FILT 0x36C </v>
       </c>
     </row>
     <row r="137" spans="1:1">
       <c r="A137" t="str">
         <f>IF('Memory setup'!A102&lt;&gt;"",IF('Memory setup'!A102="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A102),IF('Memory setup'!E102=1,_xlfn.CONCAT("#define ",'Memory setup'!B102," ",'Memory setup'!C102," ",'Memory setup'!D102),""))</f>
-        <v xml:space="preserve">#define ADR_AXIS3_POWER 0x382 </v>
+        <v>// AXIS3</v>
       </c>
     </row>
     <row r="138" spans="1:1">
       <c r="A138" t="str">
         <f>IF('Memory setup'!A103&lt;&gt;"",IF('Memory setup'!A103="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A103),IF('Memory setup'!E103=1,_xlfn.CONCAT("#define ",'Memory setup'!B103," ",'Memory setup'!C103," ",'Memory setup'!D103),""))</f>
-        <v xml:space="preserve">#define ADR_AXIS3_DEGREES 0x383 </v>
+        <v>#define ADR_AXIS3_CONFIG 0x381 // 0-2 ENC, 3-5 DRV</v>
       </c>
     </row>
     <row r="139" spans="1:1">
       <c r="A139" t="str">
         <f>IF('Memory setup'!A104&lt;&gt;"",IF('Memory setup'!A104="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A104),IF('Memory setup'!E104=1,_xlfn.CONCAT("#define ",'Memory setup'!B104," ",'Memory setup'!C104," ",'Memory setup'!D104),""))</f>
-        <v>#define ADR_AXIS3_MAX_SPEED 0x384 // Store the max speed</v>
+        <v xml:space="preserve">#define ADR_AXIS3_POWER 0x382 </v>
       </c>
     </row>
     <row r="140" spans="1:1">
       <c r="A140" t="str">
         <f>IF('Memory setup'!A105&lt;&gt;"",IF('Memory setup'!A105="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A105),IF('Memory setup'!E105=1,_xlfn.CONCAT("#define ",'Memory setup'!B105," ",'Memory setup'!C105," ",'Memory setup'!D105),""))</f>
-        <v>#define ADR_AXIS3_MAX_ACCEL 0x385 // Store the max accel</v>
+        <v xml:space="preserve">#define ADR_AXIS3_DEGREES 0x383 </v>
       </c>
     </row>
     <row r="141" spans="1:1">
       <c r="A141" t="str">
         <f>IF('Memory setup'!A106&lt;&gt;"",IF('Memory setup'!A106="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A106),IF('Memory setup'!E106=1,_xlfn.CONCAT("#define ",'Memory setup'!B106," ",'Memory setup'!C106," ",'Memory setup'!D106),""))</f>
-        <v>#define ADR_AXIS3_ENDSTOP 0x387 // 0-7 endstop margin, 8-15 endstop stiffness</v>
+        <v>#define ADR_AXIS3_MAX_SPEED 0x384 // Store the max speed</v>
       </c>
     </row>
     <row r="142" spans="1:1">
       <c r="A142" t="str">
         <f>IF('Memory setup'!A107&lt;&gt;"",IF('Memory setup'!A107="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A107),IF('Memory setup'!E107=1,_xlfn.CONCAT("#define ",'Memory setup'!B107," ",'Memory setup'!C107," ",'Memory setup'!D107),""))</f>
-        <v>#define ADR_AXIS3_EFFECTS1 0x388 // 0-7 idlespring, 8-15 damper</v>
+        <v>#define ADR_AXIS3_MAX_ACCEL 0x385 // Store the max accel</v>
       </c>
     </row>
     <row r="143" spans="1:1">
       <c r="A143" t="str">
         <f>IF('Memory setup'!A108&lt;&gt;"",IF('Memory setup'!A108="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A108),IF('Memory setup'!E108=1,_xlfn.CONCAT("#define ",'Memory setup'!B108," ",'Memory setup'!C108," ",'Memory setup'!D108),""))</f>
-        <v>#define ADR_AXIS3_SPEEDACCEL_FILTER 0x389 // Speed/Accel filter Lowpass profile</v>
+        <v>#define ADR_AXIS3_ENDSTOP 0x387 // 0-7 endstop margin, 8-15 endstop stiffness</v>
       </c>
     </row>
     <row r="144" spans="1:1">
       <c r="A144" t="str">
         <f>IF('Memory setup'!A109&lt;&gt;"",IF('Memory setup'!A109="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A109),IF('Memory setup'!E109=1,_xlfn.CONCAT("#define ",'Memory setup'!B109," ",'Memory setup'!C109," ",'Memory setup'!D109),""))</f>
-        <v>#define ADR_AXIS3_ENC_RATIO 0x38A // Store the encoder ratio for an axis</v>
+        <v>#define ADR_AXIS3_EFFECTS1 0x388 // 0-7 idlespring, 8-15 damper</v>
       </c>
     </row>
     <row r="145" spans="1:1">
       <c r="A145" t="str">
         <f>IF('Memory setup'!A110&lt;&gt;"",IF('Memory setup'!A110="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A110),IF('Memory setup'!E110=1,_xlfn.CONCAT("#define ",'Memory setup'!B110," ",'Memory setup'!C110," ",'Memory setup'!D110),""))</f>
-        <v>// TMC3</v>
+        <v>#define ADR_AXIS3_SPEEDACCEL_FILTER 0x389 // Speed/Accel filter Lowpass profile</v>
       </c>
     </row>
     <row r="146" spans="1:1">
       <c r="A146" t="str">
         <f>IF('Memory setup'!A111&lt;&gt;"",IF('Memory setup'!A111="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A111),IF('Memory setup'!E111=1,_xlfn.CONCAT("#define ",'Memory setup'!B111," ",'Memory setup'!C111," ",'Memory setup'!D111),""))</f>
-        <v>#define ADR_TMC3_MOTCONF 0x3A0 // 0-2: MotType 3-5: PhiE source 6-15: Poles</v>
+        <v>#define ADR_AXIS3_ENC_RATIO 0x38A // Store the encoder ratio for an axis</v>
       </c>
     </row>
     <row r="147" spans="1:1">
       <c r="A147" t="str">
         <f>IF('Memory setup'!A112&lt;&gt;"",IF('Memory setup'!A112="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A112),IF('Memory setup'!E112=1,_xlfn.CONCAT("#define ",'Memory setup'!B112," ",'Memory setup'!C112," ",'Memory setup'!D112),""))</f>
-        <v xml:space="preserve">#define ADR_TMC3_CPR 0x3A1 </v>
+        <v>// TMC3</v>
       </c>
     </row>
     <row r="148" spans="1:1">
       <c r="A148" t="str">
         <f>IF('Memory setup'!A113&lt;&gt;"",IF('Memory setup'!A113="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A113),IF('Memory setup'!E113=1,_xlfn.CONCAT("#define ",'Memory setup'!B113," ",'Memory setup'!C113," ",'Memory setup'!D113),""))</f>
-        <v>#define ADR_TMC3_ENCA 0x3A2 // Misc</v>
+        <v>#define ADR_TMC3_MOTCONF 0x3A0 // 0-2: MotType 3-5: PhiE source 6-15: Poles</v>
       </c>
     </row>
     <row r="149" spans="1:1">
       <c r="A149" t="str">
         <f>IF('Memory setup'!A114&lt;&gt;"",IF('Memory setup'!A114="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A114),IF('Memory setup'!E114=1,_xlfn.CONCAT("#define ",'Memory setup'!B114," ",'Memory setup'!C114," ",'Memory setup'!D114),""))</f>
-        <v xml:space="preserve">#define ADR_TMC3_ADC_I0_OFS 0x3A3 </v>
+        <v xml:space="preserve">#define ADR_TMC3_CPR 0x3A1 </v>
       </c>
     </row>
     <row r="150" spans="1:1">
       <c r="A150" t="str">
         <f>IF('Memory setup'!A115&lt;&gt;"",IF('Memory setup'!A115="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A115),IF('Memory setup'!E115=1,_xlfn.CONCAT("#define ",'Memory setup'!B115," ",'Memory setup'!C115," ",'Memory setup'!D115),""))</f>
-        <v xml:space="preserve">#define ADR_TMC3_ADC_I1_OFS 0x3A4 </v>
+        <v>#define ADR_TMC3_ENCA 0x3A2 // Misc</v>
       </c>
     </row>
     <row r="151" spans="1:1">
       <c r="A151" t="str">
         <f>IF('Memory setup'!A116&lt;&gt;"",IF('Memory setup'!A116="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A116),IF('Memory setup'!E116=1,_xlfn.CONCAT("#define ",'Memory setup'!B116," ",'Memory setup'!C116," ",'Memory setup'!D116),""))</f>
-        <v xml:space="preserve">#define ADR_TMC3_ENC_OFFSET 0x3A5 </v>
+        <v xml:space="preserve">#define ADR_TMC3_ADC_I0_OFS 0x3A3 </v>
       </c>
     </row>
     <row r="152" spans="1:1">
       <c r="A152" t="str">
         <f>IF('Memory setup'!A117&lt;&gt;"",IF('Memory setup'!A117="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A117),IF('Memory setup'!E117=1,_xlfn.CONCAT("#define ",'Memory setup'!B117," ",'Memory setup'!C117," ",'Memory setup'!D117),""))</f>
-        <v xml:space="preserve">#define ADR_TMC3_OFFSETFLUX 0x3A6 </v>
+        <v xml:space="preserve">#define ADR_TMC3_ADC_I1_OFS 0x3A4 </v>
       </c>
     </row>
     <row r="153" spans="1:1">
       <c r="A153" t="str">
         <f>IF('Memory setup'!A118&lt;&gt;"",IF('Memory setup'!A118="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A118),IF('Memory setup'!E118=1,_xlfn.CONCAT("#define ",'Memory setup'!B118," ",'Memory setup'!C118," ",'Memory setup'!D118),""))</f>
-        <v xml:space="preserve">#define ADR_TMC3_TORQUE_P 0x3A7 </v>
+        <v xml:space="preserve">#define ADR_TMC3_ENC_OFFSET 0x3A5 </v>
       </c>
     </row>
     <row r="154" spans="1:1">
       <c r="A154" t="str">
         <f>IF('Memory setup'!A119&lt;&gt;"",IF('Memory setup'!A119="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A119),IF('Memory setup'!E119=1,_xlfn.CONCAT("#define ",'Memory setup'!B119," ",'Memory setup'!C119," ",'Memory setup'!D119),""))</f>
-        <v xml:space="preserve">#define ADR_TMC3_TORQUE_I 0x3A8 </v>
+        <v xml:space="preserve">#define ADR_TMC3_OFFSETFLUX 0x3A6 </v>
       </c>
     </row>
     <row r="155" spans="1:1">
       <c r="A155" t="str">
         <f>IF('Memory setup'!A120&lt;&gt;"",IF('Memory setup'!A120="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A120),IF('Memory setup'!E120=1,_xlfn.CONCAT("#define ",'Memory setup'!B120," ",'Memory setup'!C120," ",'Memory setup'!D120),""))</f>
-        <v xml:space="preserve">#define ADR_TMC3_FLUX_P 0x3A9 </v>
+        <v xml:space="preserve">#define ADR_TMC3_TORQUE_P 0x3A7 </v>
       </c>
     </row>
     <row r="156" spans="1:1">
       <c r="A156" t="str">
         <f>IF('Memory setup'!A121&lt;&gt;"",IF('Memory setup'!A121="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A121),IF('Memory setup'!E121=1,_xlfn.CONCAT("#define ",'Memory setup'!B121," ",'Memory setup'!C121," ",'Memory setup'!D121),""))</f>
-        <v xml:space="preserve">#define ADR_TMC3_FLUX_I 0x3AA </v>
+        <v xml:space="preserve">#define ADR_TMC3_TORQUE_I 0x3A8 </v>
       </c>
     </row>
     <row r="157" spans="1:1">
       <c r="A157" t="str">
         <f>IF('Memory setup'!A122&lt;&gt;"",IF('Memory setup'!A122="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A122),IF('Memory setup'!E122=1,_xlfn.CONCAT("#define ",'Memory setup'!B122," ",'Memory setup'!C122," ",'Memory setup'!D122),""))</f>
-        <v xml:space="preserve">#define ADR_TMC3_PHIE_OFS 0x3AB </v>
+        <v xml:space="preserve">#define ADR_TMC3_FLUX_P 0x3A9 </v>
       </c>
     </row>
     <row r="158" spans="1:1">
       <c r="A158" t="str">
         <f>IF('Memory setup'!A123&lt;&gt;"",IF('Memory setup'!A123="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A123),IF('Memory setup'!E123=1,_xlfn.CONCAT("#define ",'Memory setup'!B123," ",'Memory setup'!C123," ",'Memory setup'!D123),""))</f>
-        <v>// Odrive</v>
+        <v xml:space="preserve">#define ADR_TMC3_FLUX_I 0x3AA </v>
       </c>
     </row>
     <row r="159" spans="1:1">
       <c r="A159" t="str">
         <f>IF('Memory setup'!A124&lt;&gt;"",IF('Memory setup'!A124="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A124),IF('Memory setup'!E124=1,_xlfn.CONCAT("#define ",'Memory setup'!B124," ",'Memory setup'!C124," ",'Memory setup'!D124),""))</f>
-        <v>#define ADR_ODRIVE_CANID 0x3D0 //0-6 ID M0, 7-12 ID M1, 13-15 can speed</v>
+        <v xml:space="preserve">#define ADR_TMC3_PHIE_OFS 0x3AB </v>
       </c>
     </row>
     <row r="160" spans="1:1">
       <c r="A160" t="str">
         <f>IF('Memory setup'!A125&lt;&gt;"",IF('Memory setup'!A125="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A125),IF('Memory setup'!E125=1,_xlfn.CONCAT("#define ",'Memory setup'!B125," ",'Memory setup'!C125," ",'Memory setup'!D125),""))</f>
-        <v xml:space="preserve">#define ADR_ODRIVE_SETTING1_M0 0x3D1 </v>
+        <v xml:space="preserve">#define ADR_TMC3_TRQ_FILT 0x3AC </v>
       </c>
     </row>
     <row r="161" spans="1:1">
       <c r="A161" t="str">
         <f>IF('Memory setup'!A126&lt;&gt;"",IF('Memory setup'!A126="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A126),IF('Memory setup'!E126=1,_xlfn.CONCAT("#define ",'Memory setup'!B126," ",'Memory setup'!C126," ",'Memory setup'!D126),""))</f>
-        <v xml:space="preserve">#define ADR_ODRIVE_SETTING1_M1 0x3D2 </v>
+        <v>// Odrive</v>
       </c>
     </row>
     <row r="162" spans="1:1">
       <c r="A162" t="str">
         <f>IF('Memory setup'!A127&lt;&gt;"",IF('Memory setup'!A127="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A127),IF('Memory setup'!E127=1,_xlfn.CONCAT("#define ",'Memory setup'!B127," ",'Memory setup'!C127," ",'Memory setup'!D127),""))</f>
-        <v>// VESC Section</v>
+        <v>#define ADR_ODRIVE_CANID 0x3D0 //0-6 ID M0, 7-12 ID M1, 13-15 can speed</v>
       </c>
     </row>
     <row r="163" spans="1:1">
       <c r="A163" t="str">
         <f>IF('Memory setup'!A128&lt;&gt;"",IF('Memory setup'!A128="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A128),IF('Memory setup'!E128=1,_xlfn.CONCAT("#define ",'Memory setup'!B128," ",'Memory setup'!C128," ",'Memory setup'!D128),""))</f>
-        <v>#define ADR_VESC1_CANID 0x3E0 //0-7 AxisCanID, 8-16 VescCanId</v>
+        <v xml:space="preserve">#define ADR_ODRIVE_SETTING1_M0 0x3D1 </v>
       </c>
     </row>
     <row r="164" spans="1:1">
       <c r="A164" t="str">
         <f>IF('Memory setup'!A129&lt;&gt;"",IF('Memory setup'!A129="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A129),IF('Memory setup'!E129=1,_xlfn.CONCAT("#define ",'Memory setup'!B129," ",'Memory setup'!C129," ",'Memory setup'!D129),""))</f>
-        <v>#define ADR_VESC1_DATA 0x3E1 //0-2 can speed, 3 useVescEncoder</v>
+        <v xml:space="preserve">#define ADR_ODRIVE_SETTING1_M1 0x3D2 </v>
       </c>
     </row>
     <row r="165" spans="1:1">
       <c r="A165" t="str">
         <f>IF('Memory setup'!A130&lt;&gt;"",IF('Memory setup'!A130="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A130),IF('Memory setup'!E130=1,_xlfn.CONCAT("#define ",'Memory setup'!B130," ",'Memory setup'!C130," ",'Memory setup'!D130),""))</f>
-        <v>#define ADR_VESC1_OFFSET 0x3E2 //16b offset</v>
+        <v>// VESC Section</v>
       </c>
     </row>
     <row r="166" spans="1:1">
       <c r="A166" t="str">
         <f>IF('Memory setup'!A131&lt;&gt;"",IF('Memory setup'!A131="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A131),IF('Memory setup'!E131=1,_xlfn.CONCAT("#define ",'Memory setup'!B131," ",'Memory setup'!C131," ",'Memory setup'!D131),""))</f>
-        <v>#define ADR_VESC2_CANID 0x3E3 //0-8 AxisCanID, 8-16 VescCanId</v>
+        <v>#define ADR_VESC1_CANID 0x3E0 //0-7 AxisCanID, 8-16 VescCanId</v>
       </c>
     </row>
     <row r="167" spans="1:1">
       <c r="A167" t="str">
         <f>IF('Memory setup'!A132&lt;&gt;"",IF('Memory setup'!A132="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A132),IF('Memory setup'!E132=1,_xlfn.CONCAT("#define ",'Memory setup'!B132," ",'Memory setup'!C132," ",'Memory setup'!D132),""))</f>
-        <v>#define ADR_VESC2_DATA 0x3E4 //0-2 can speed, 3 useVescEncoder</v>
+        <v>#define ADR_VESC1_DATA 0x3E1 //0-2 can speed, 3 useVescEncoder</v>
       </c>
     </row>
     <row r="168" spans="1:1">
       <c r="A168" t="str">
         <f>IF('Memory setup'!A133&lt;&gt;"",IF('Memory setup'!A133="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A133),IF('Memory setup'!E133=1,_xlfn.CONCAT("#define ",'Memory setup'!B133," ",'Memory setup'!C133," ",'Memory setup'!D133),""))</f>
-        <v>#define ADR_VESC2_OFFSET 0x3E5 //16b offset</v>
+        <v>#define ADR_VESC1_OFFSET 0x3E2 //16b offset</v>
       </c>
     </row>
     <row r="169" spans="1:1">
       <c r="A169" t="str">
         <f>IF('Memory setup'!A134&lt;&gt;"",IF('Memory setup'!A134="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A134),IF('Memory setup'!E134=1,_xlfn.CONCAT("#define ",'Memory setup'!B134," ",'Memory setup'!C134," ",'Memory setup'!D134),""))</f>
-        <v>#define ADR_VESC3_CANID 0x3E6 //0-8 AxisCanID, 8-16 VescCanId</v>
+        <v>#define ADR_VESC2_CANID 0x3E3 //0-8 AxisCanID, 8-16 VescCanId</v>
       </c>
     </row>
     <row r="170" spans="1:1">
       <c r="A170" t="str">
         <f>IF('Memory setup'!A135&lt;&gt;"",IF('Memory setup'!A135="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A135),IF('Memory setup'!E135=1,_xlfn.CONCAT("#define ",'Memory setup'!B135," ",'Memory setup'!C135," ",'Memory setup'!D135),""))</f>
-        <v>#define ADR_VESC3_DATA 0x3E7 //0-2 can speed, 3 useVescEncoder</v>
+        <v>#define ADR_VESC2_DATA 0x3E4 //0-2 can speed, 3 useVescEncoder</v>
       </c>
     </row>
     <row r="171" spans="1:1">
       <c r="A171" t="str">
         <f>IF('Memory setup'!A136&lt;&gt;"",IF('Memory setup'!A136="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A136),IF('Memory setup'!E136=1,_xlfn.CONCAT("#define ",'Memory setup'!B136," ",'Memory setup'!C136," ",'Memory setup'!D136),""))</f>
-        <v>#define ADR_VESC3_OFFSET 0x3E8 //16b offset</v>
+        <v>#define ADR_VESC2_OFFSET 0x3E5 //16b offset</v>
       </c>
     </row>
     <row r="172" spans="1:1">
       <c r="A172" t="str">
         <f>IF('Memory setup'!A137&lt;&gt;"",IF('Memory setup'!A137="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A137),IF('Memory setup'!E137=1,_xlfn.CONCAT("#define ",'Memory setup'!B137," ",'Memory setup'!C137," ",'Memory setup'!D137),""))</f>
-        <v>//MT Encoder</v>
+        <v>#define ADR_VESC3_CANID 0x3E6 //0-8 AxisCanID, 8-16 VescCanId</v>
       </c>
     </row>
     <row r="173" spans="1:1">
       <c r="A173" t="str">
         <f>IF('Memory setup'!A138&lt;&gt;"",IF('Memory setup'!A138="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A138),IF('Memory setup'!E138=1,_xlfn.CONCAT("#define ",'Memory setup'!B138," ",'Memory setup'!C138," ",'Memory setup'!D138),""))</f>
-        <v xml:space="preserve">#define ADR_MTENC_OFS 0x400 </v>
+        <v>#define ADR_VESC3_DATA 0x3E7 //0-2 can speed, 3 useVescEncoder</v>
       </c>
     </row>
     <row r="174" spans="1:1">
       <c r="A174" t="str">
         <f>IF('Memory setup'!A139&lt;&gt;"",IF('Memory setup'!A139="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A139),IF('Memory setup'!E139=1,_xlfn.CONCAT("#define ",'Memory setup'!B139," ",'Memory setup'!C139," ",'Memory setup'!D139),""))</f>
-        <v xml:space="preserve">#define ADR_MTENC_CONF1 0x401 </v>
+        <v>#define ADR_VESC3_OFFSET 0x3E8 //16b offset</v>
       </c>
     </row>
     <row r="175" spans="1:1">
       <c r="A175" t="str">
         <f>IF('Memory setup'!A140&lt;&gt;"",IF('Memory setup'!A140="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A140),IF('Memory setup'!E140=1,_xlfn.CONCAT("#define ",'Memory setup'!B140," ",'Memory setup'!C140," ",'Memory setup'!D140),""))</f>
-        <v>// Biss-C</v>
+        <v>//MT Encoder</v>
       </c>
     </row>
     <row r="176" spans="1:1">
       <c r="A176" t="str">
         <f>IF('Memory setup'!A141&lt;&gt;"",IF('Memory setup'!A141="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A141),IF('Memory setup'!E141=1,_xlfn.CONCAT("#define ",'Memory setup'!B141," ",'Memory setup'!C141," ",'Memory setup'!D141),""))</f>
-        <v xml:space="preserve">#define ADR_BISSENC_CONF1 0x410 </v>
+        <v xml:space="preserve">#define ADR_MTENC_OFS 0x400 </v>
       </c>
     </row>
     <row r="177" spans="1:1">
       <c r="A177" t="str">
         <f>IF('Memory setup'!A142&lt;&gt;"",IF('Memory setup'!A142="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A142),IF('Memory setup'!E142=1,_xlfn.CONCAT("#define ",'Memory setup'!B142," ",'Memory setup'!C142," ",'Memory setup'!D142),""))</f>
-        <v xml:space="preserve">#define ADR_BISSENC_OFS 0x411 </v>
+        <v xml:space="preserve">#define ADR_MTENC_CONF1 0x401 </v>
       </c>
     </row>
     <row r="178" spans="1:1">
       <c r="A178" t="str">
         <f>IF('Memory setup'!A143&lt;&gt;"",IF('Memory setup'!A143="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A143),IF('Memory setup'!E143=1,_xlfn.CONCAT("#define ",'Memory setup'!B143," ",'Memory setup'!C143," ",'Memory setup'!D143),""))</f>
-        <v>// Analog min/max calibrations</v>
+        <v>// Biss-C</v>
       </c>
     </row>
     <row r="179" spans="1:1">
       <c r="A179" t="str">
         <f>IF('Memory setup'!A144&lt;&gt;"",IF('Memory setup'!A144="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A144),IF('Memory setup'!E144=1,_xlfn.CONCAT("#define ",'Memory setup'!B144," ",'Memory setup'!C144," ",'Memory setup'!D144),""))</f>
-        <v xml:space="preserve">#define ADR_LOCALANALOG_MIN_0 0x500 </v>
+        <v xml:space="preserve">#define ADR_BISSENC_CONF1 0x410 </v>
       </c>
     </row>
     <row r="180" spans="1:1">
       <c r="A180" t="str">
         <f>IF('Memory setup'!A145&lt;&gt;"",IF('Memory setup'!A145="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A145),IF('Memory setup'!E145=1,_xlfn.CONCAT("#define ",'Memory setup'!B145," ",'Memory setup'!C145," ",'Memory setup'!D145),""))</f>
-        <v xml:space="preserve">#define ADR_LOCALANALOG_MAX_0 0x501 </v>
+        <v xml:space="preserve">#define ADR_BISSENC_OFS 0x411 </v>
       </c>
     </row>
     <row r="181" spans="1:1">
       <c r="A181" t="str">
         <f>IF('Memory setup'!A146&lt;&gt;"",IF('Memory setup'!A146="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A146),IF('Memory setup'!E146=1,_xlfn.CONCAT("#define ",'Memory setup'!B146," ",'Memory setup'!C146," ",'Memory setup'!D146),""))</f>
-        <v xml:space="preserve">#define ADR_LOCALANALOG_MIN_1 0x502 </v>
+        <v>// Analog min/max calibrations</v>
       </c>
     </row>
     <row r="182" spans="1:1">
       <c r="A182" t="str">
         <f>IF('Memory setup'!A147&lt;&gt;"",IF('Memory setup'!A147="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A147),IF('Memory setup'!E147=1,_xlfn.CONCAT("#define ",'Memory setup'!B147," ",'Memory setup'!C147," ",'Memory setup'!D147),""))</f>
-        <v xml:space="preserve">#define ADR_LOCALANALOG_MAX_1 0x503 </v>
+        <v xml:space="preserve">#define ADR_LOCALANALOG_MIN_0 0x500 </v>
       </c>
     </row>
     <row r="183" spans="1:1">
       <c r="A183" t="str">
         <f>IF('Memory setup'!A148&lt;&gt;"",IF('Memory setup'!A148="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A148),IF('Memory setup'!E148=1,_xlfn.CONCAT("#define ",'Memory setup'!B148," ",'Memory setup'!C148," ",'Memory setup'!D148),""))</f>
-        <v xml:space="preserve">#define ADR_LOCALANALOG_MIN_2 0x504 </v>
+        <v xml:space="preserve">#define ADR_LOCALANALOG_MAX_0 0x501 </v>
       </c>
     </row>
     <row r="184" spans="1:1">
       <c r="A184" t="str">
         <f>IF('Memory setup'!A149&lt;&gt;"",IF('Memory setup'!A149="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A149),IF('Memory setup'!E149=1,_xlfn.CONCAT("#define ",'Memory setup'!B149," ",'Memory setup'!C149," ",'Memory setup'!D149),""))</f>
-        <v xml:space="preserve">#define ADR_LOCALANALOG_MAX_2 0x505 </v>
+        <v xml:space="preserve">#define ADR_LOCALANALOG_MIN_1 0x502 </v>
       </c>
     </row>
     <row r="185" spans="1:1">
       <c r="A185" t="str">
         <f>IF('Memory setup'!A150&lt;&gt;"",IF('Memory setup'!A150="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A150),IF('Memory setup'!E150=1,_xlfn.CONCAT("#define ",'Memory setup'!B150," ",'Memory setup'!C150," ",'Memory setup'!D150),""))</f>
-        <v xml:space="preserve">#define ADR_LOCALANALOG_MIN_3 0x506 </v>
+        <v xml:space="preserve">#define ADR_LOCALANALOG_MAX_1 0x503 </v>
       </c>
     </row>
     <row r="186" spans="1:1">
       <c r="A186" t="str">
         <f>IF('Memory setup'!A151&lt;&gt;"",IF('Memory setup'!A151="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A151),IF('Memory setup'!E151=1,_xlfn.CONCAT("#define ",'Memory setup'!B151," ",'Memory setup'!C151," ",'Memory setup'!D151),""))</f>
-        <v xml:space="preserve">#define ADR_LOCALANALOG_MAX_3 0x507 </v>
+        <v xml:space="preserve">#define ADR_LOCALANALOG_MIN_2 0x504 </v>
       </c>
     </row>
     <row r="187" spans="1:1">
       <c r="A187" t="str">
         <f>IF('Memory setup'!A152&lt;&gt;"",IF('Memory setup'!A152="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A152),IF('Memory setup'!E152=1,_xlfn.CONCAT("#define ",'Memory setup'!B152," ",'Memory setup'!C152," ",'Memory setup'!D152),""))</f>
-        <v xml:space="preserve">#define ADR_LOCALANALOG_MIN_4 0x508 </v>
+        <v xml:space="preserve">#define ADR_LOCALANALOG_MAX_2 0x505 </v>
       </c>
     </row>
     <row r="188" spans="1:1">
       <c r="A188" t="str">
         <f>IF('Memory setup'!A153&lt;&gt;"",IF('Memory setup'!A153="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A153),IF('Memory setup'!E153=1,_xlfn.CONCAT("#define ",'Memory setup'!B153," ",'Memory setup'!C153," ",'Memory setup'!D153),""))</f>
-        <v xml:space="preserve">#define ADR_LOCALANALOG_MAX_4 0x509 </v>
+        <v xml:space="preserve">#define ADR_LOCALANALOG_MIN_3 0x506 </v>
       </c>
     </row>
     <row r="189" spans="1:1">
       <c r="A189" t="str">
         <f>IF('Memory setup'!A154&lt;&gt;"",IF('Memory setup'!A154="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A154),IF('Memory setup'!E154=1,_xlfn.CONCAT("#define ",'Memory setup'!B154," ",'Memory setup'!C154," ",'Memory setup'!D154),""))</f>
-        <v xml:space="preserve">#define ADR_LOCALANALOG_MIN_5 0x50A </v>
+        <v xml:space="preserve">#define ADR_LOCALANALOG_MAX_3 0x507 </v>
       </c>
     </row>
     <row r="190" spans="1:1">
       <c r="A190" t="str">
         <f>IF('Memory setup'!A155&lt;&gt;"",IF('Memory setup'!A155="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A155),IF('Memory setup'!E155=1,_xlfn.CONCAT("#define ",'Memory setup'!B155," ",'Memory setup'!C155," ",'Memory setup'!D155),""))</f>
-        <v xml:space="preserve">#define ADR_LOCALANALOG_MAX_5 0x50B </v>
+        <v xml:space="preserve">#define ADR_LOCALANALOG_MIN_4 0x508 </v>
       </c>
     </row>
     <row r="191" spans="1:1">
       <c r="A191" t="str">
         <f>IF('Memory setup'!A156&lt;&gt;"",IF('Memory setup'!A156="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A156),IF('Memory setup'!E156=1,_xlfn.CONCAT("#define ",'Memory setup'!B156," ",'Memory setup'!C156," ",'Memory setup'!D156),""))</f>
-        <v xml:space="preserve">#define ADR_LOCALANALOG_MIN_6 0x50C </v>
+        <v xml:space="preserve">#define ADR_LOCALANALOG_MAX_4 0x509 </v>
       </c>
     </row>
     <row r="192" spans="1:1">
       <c r="A192" t="str">
         <f>IF('Memory setup'!A157&lt;&gt;"",IF('Memory setup'!A157="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A157),IF('Memory setup'!E157=1,_xlfn.CONCAT("#define ",'Memory setup'!B157," ",'Memory setup'!C157," ",'Memory setup'!D157),""))</f>
-        <v xml:space="preserve">#define ADR_LOCALANALOG_MAX_6 0x50D </v>
+        <v xml:space="preserve">#define ADR_LOCALANALOG_MIN_5 0x50A </v>
       </c>
     </row>
     <row r="193" spans="1:1">
       <c r="A193" t="str">
         <f>IF('Memory setup'!A158&lt;&gt;"",IF('Memory setup'!A158="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A158),IF('Memory setup'!E158=1,_xlfn.CONCAT("#define ",'Memory setup'!B158," ",'Memory setup'!C158," ",'Memory setup'!D158),""))</f>
-        <v xml:space="preserve">#define ADR_LOCALANALOG_MIN_7 0x50E </v>
+        <v xml:space="preserve">#define ADR_LOCALANALOG_MAX_5 0x50B </v>
       </c>
     </row>
     <row r="194" spans="1:1">
       <c r="A194" t="str">
         <f>IF('Memory setup'!A159&lt;&gt;"",IF('Memory setup'!A159="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A159),IF('Memory setup'!E159=1,_xlfn.CONCAT("#define ",'Memory setup'!B159," ",'Memory setup'!C159," ",'Memory setup'!D159),""))</f>
-        <v xml:space="preserve">#define ADR_LOCALANALOG_MAX_7 0x50F </v>
+        <v xml:space="preserve">#define ADR_LOCALANALOG_MIN_6 0x50C </v>
       </c>
     </row>
     <row r="195" spans="1:1">
       <c r="A195" t="str">
         <f>IF('Memory setup'!A160&lt;&gt;"",IF('Memory setup'!A160="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A160),IF('Memory setup'!E160=1,_xlfn.CONCAT("#define ",'Memory setup'!B160," ",'Memory setup'!C160," ",'Memory setup'!D160),""))</f>
-        <v xml:space="preserve">#define ADR_ADS111X_MIN_0 0x510 </v>
+        <v xml:space="preserve">#define ADR_LOCALANALOG_MAX_6 0x50D </v>
       </c>
     </row>
     <row r="196" spans="1:1">
       <c r="A196" t="str">
         <f>IF('Memory setup'!A161&lt;&gt;"",IF('Memory setup'!A161="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A161),IF('Memory setup'!E161=1,_xlfn.CONCAT("#define ",'Memory setup'!B161," ",'Memory setup'!C161," ",'Memory setup'!D161),""))</f>
-        <v xml:space="preserve">#define ADR_ADS111X_MAX_0 0x511 </v>
+        <v xml:space="preserve">#define ADR_LOCALANALOG_MIN_7 0x50E </v>
       </c>
     </row>
     <row r="197" spans="1:1">
       <c r="A197" t="str">
         <f>IF('Memory setup'!A162&lt;&gt;"",IF('Memory setup'!A162="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A162),IF('Memory setup'!E162=1,_xlfn.CONCAT("#define ",'Memory setup'!B162," ",'Memory setup'!C162," ",'Memory setup'!D162),""))</f>
-        <v xml:space="preserve">#define ADR_ADS111X_MIN_1 0x512 </v>
+        <v xml:space="preserve">#define ADR_LOCALANALOG_MAX_7 0x50F </v>
       </c>
     </row>
     <row r="198" spans="1:1">
       <c r="A198" t="str">
         <f>IF('Memory setup'!A163&lt;&gt;"",IF('Memory setup'!A163="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A163),IF('Memory setup'!E163=1,_xlfn.CONCAT("#define ",'Memory setup'!B163," ",'Memory setup'!C163," ",'Memory setup'!D163),""))</f>
-        <v xml:space="preserve">#define ADR_ADS111X_MAX_1 0x513 </v>
+        <v xml:space="preserve">#define ADR_ADS111X_MIN_0 0x510 </v>
       </c>
     </row>
     <row r="199" spans="1:1">
       <c r="A199" t="str">
         <f>IF('Memory setup'!A164&lt;&gt;"",IF('Memory setup'!A164="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A164),IF('Memory setup'!E164=1,_xlfn.CONCAT("#define ",'Memory setup'!B164," ",'Memory setup'!C164," ",'Memory setup'!D164),""))</f>
-        <v xml:space="preserve">#define ADR_ADS111X_MIN_2 0x514 </v>
+        <v xml:space="preserve">#define ADR_ADS111X_MAX_0 0x511 </v>
       </c>
     </row>
     <row r="200" spans="1:1">
       <c r="A200" t="str">
         <f>IF('Memory setup'!A165&lt;&gt;"",IF('Memory setup'!A165="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A165),IF('Memory setup'!E165=1,_xlfn.CONCAT("#define ",'Memory setup'!B165," ",'Memory setup'!C165," ",'Memory setup'!D165),""))</f>
-        <v xml:space="preserve">#define ADR_ADS111X_MAX_2 0x515 </v>
+        <v xml:space="preserve">#define ADR_ADS111X_MIN_1 0x512 </v>
       </c>
     </row>
     <row r="201" spans="1:1">
       <c r="A201" t="str">
         <f>IF('Memory setup'!A166&lt;&gt;"",IF('Memory setup'!A166="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A166),IF('Memory setup'!E166=1,_xlfn.CONCAT("#define ",'Memory setup'!B166," ",'Memory setup'!C166," ",'Memory setup'!D166),""))</f>
-        <v xml:space="preserve">#define ADR_ADS111X_MIN_3 0x516 </v>
+        <v xml:space="preserve">#define ADR_ADS111X_MAX_1 0x513 </v>
       </c>
     </row>
     <row r="202" spans="1:1">
       <c r="A202" t="str">
         <f>IF('Memory setup'!A167&lt;&gt;"",IF('Memory setup'!A167="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A167),IF('Memory setup'!E167=1,_xlfn.CONCAT("#define ",'Memory setup'!B167," ",'Memory setup'!C167," ",'Memory setup'!D167),""))</f>
-        <v xml:space="preserve">#define ADR_ADS111X_MAX_3 0x517 </v>
+        <v xml:space="preserve">#define ADR_ADS111X_MIN_2 0x514 </v>
       </c>
     </row>
     <row r="203" spans="1:1">
       <c r="A203" t="str">
         <f>IF('Memory setup'!A168&lt;&gt;"",IF('Memory setup'!A168="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A168),IF('Memory setup'!E168=1,_xlfn.CONCAT("#define ",'Memory setup'!B168," ",'Memory setup'!C168," ",'Memory setup'!D168),""))</f>
-        <v>#endif /* EEPROM_ADDRESSES_H_ */</v>
+        <v xml:space="preserve">#define ADR_ADS111X_MAX_2 0x515 </v>
       </c>
     </row>
     <row r="204" spans="1:1">
       <c r="A204" t="str">
         <f>IF('Memory setup'!A169&lt;&gt;"",IF('Memory setup'!A169="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A169),IF('Memory setup'!E169=1,_xlfn.CONCAT("#define ",'Memory setup'!B169," ",'Memory setup'!C169," ",'Memory setup'!D169),""))</f>
-        <v/>
+        <v xml:space="preserve">#define ADR_ADS111X_MIN_3 0x516 </v>
       </c>
     </row>
     <row r="205" spans="1:1">
       <c r="A205" t="str">
         <f>IF('Memory setup'!A170&lt;&gt;"",IF('Memory setup'!A170="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A170),IF('Memory setup'!E170=1,_xlfn.CONCAT("#define ",'Memory setup'!B170," ",'Memory setup'!C170," ",'Memory setup'!D170),""))</f>
-        <v/>
+        <v xml:space="preserve">#define ADR_ADS111X_MAX_3 0x517 </v>
       </c>
     </row>
     <row r="206" spans="1:1">
       <c r="A206" t="str">
         <f>IF('Memory setup'!A171&lt;&gt;"",IF('Memory setup'!A171="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A171),IF('Memory setup'!E171=1,_xlfn.CONCAT("#define ",'Memory setup'!B171," ",'Memory setup'!C171," ",'Memory setup'!D171),""))</f>
-        <v/>
+        <v>#endif /* EEPROM_ADDRESSES_H_ */</v>
       </c>
     </row>
     <row r="207" spans="1:1">
@@ -5611,37 +5671,37 @@
     </row>
     <row r="221" spans="1:1">
       <c r="A221" t="str">
-        <f>IF('Memory setup'!A177&lt;&gt;"",IF('Memory setup'!A177="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A177),IF('Memory setup'!E177=1,_xlfn.CONCAT("#define ",'Memory setup'!B177," ",'Memory setup'!C177," ",'Memory setup'!D177),""))</f>
+        <f>IF('Memory setup'!A186&lt;&gt;"",IF('Memory setup'!A186="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A186),IF('Memory setup'!E186=1,_xlfn.CONCAT("#define ",'Memory setup'!B186," ",'Memory setup'!C186," ",'Memory setup'!D186),""))</f>
         <v/>
       </c>
     </row>
     <row r="222" spans="1:1">
       <c r="A222" t="str">
-        <f>IF('Memory setup'!A178&lt;&gt;"",IF('Memory setup'!A178="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A178),IF('Memory setup'!E178=1,_xlfn.CONCAT("#define ",'Memory setup'!B178," ",'Memory setup'!C178," ",'Memory setup'!D178),""))</f>
+        <f>IF('Memory setup'!A187&lt;&gt;"",IF('Memory setup'!A187="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A187),IF('Memory setup'!E187=1,_xlfn.CONCAT("#define ",'Memory setup'!B187," ",'Memory setup'!C187," ",'Memory setup'!D187),""))</f>
         <v/>
       </c>
     </row>
     <row r="223" spans="1:1">
       <c r="A223" t="str">
-        <f>IF('Memory setup'!A179&lt;&gt;"",IF('Memory setup'!A179="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A179),IF('Memory setup'!E179=1,_xlfn.CONCAT("#define ",'Memory setup'!B179," ",'Memory setup'!C179," ",'Memory setup'!D179),""))</f>
+        <f>IF('Memory setup'!A188&lt;&gt;"",IF('Memory setup'!A188="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A188),IF('Memory setup'!E188=1,_xlfn.CONCAT("#define ",'Memory setup'!B188," ",'Memory setup'!C188," ",'Memory setup'!D188),""))</f>
         <v/>
       </c>
     </row>
     <row r="224" spans="1:1">
       <c r="A224" t="str">
-        <f>IF('Memory setup'!A180&lt;&gt;"",IF('Memory setup'!A180="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A180),IF('Memory setup'!E180=1,_xlfn.CONCAT("#define ",'Memory setup'!B180," ",'Memory setup'!C180," ",'Memory setup'!D180),""))</f>
+        <f>IF('Memory setup'!A189&lt;&gt;"",IF('Memory setup'!A189="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A189),IF('Memory setup'!E189=1,_xlfn.CONCAT("#define ",'Memory setup'!B189," ",'Memory setup'!C189," ",'Memory setup'!D189),""))</f>
         <v/>
       </c>
     </row>
     <row r="225" spans="1:1">
       <c r="A225" t="str">
-        <f>IF('Memory setup'!A181&lt;&gt;"",IF('Memory setup'!A181="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A181),IF('Memory setup'!E181=1,_xlfn.CONCAT("#define ",'Memory setup'!B181," ",'Memory setup'!C181," ",'Memory setup'!D181),""))</f>
+        <f>IF('Memory setup'!A190&lt;&gt;"",IF('Memory setup'!A190="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A190),IF('Memory setup'!E190=1,_xlfn.CONCAT("#define ",'Memory setup'!B190," ",'Memory setup'!C190," ",'Memory setup'!D190),""))</f>
         <v/>
       </c>
     </row>
     <row r="226" spans="1:1">
       <c r="A226" t="str">
-        <f>IF('Memory setup'!A187&lt;&gt;"",IF('Memory setup'!A187="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A187),IF('Memory setup'!E187=1,_xlfn.CONCAT("#define ",'Memory setup'!B187," ",'Memory setup'!C187," ",'Memory setup'!D187),""))</f>
+        <f>IF('Memory setup'!A191&lt;&gt;"",IF('Memory setup'!A191="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A191),IF('Memory setup'!E191=1,_xlfn.CONCAT("#define ",'Memory setup'!B191," ",'Memory setup'!C191," ",'Memory setup'!D191),""))</f>
         <v/>
       </c>
     </row>
@@ -6313,8 +6373,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A15747F3-05ED-504F-B11C-F6CFE07DDC85}">
   <dimension ref="A1:C193"/>
   <sheetViews>
-    <sheetView topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="I186" sqref="I186"/>
+    <sheetView topLeftCell="A163" workbookViewId="0">
+      <selection activeCell="A187" sqref="A187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -7455,29 +7515,29 @@
     <row r="94" spans="1:3">
       <c r="A94" t="str">
         <f>IF('Memory setup'!A77&lt;&gt;"",IF('Memory setup'!A77&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A77,"};"),"")</f>
-        <v>// AXIS2</v>
+        <v/>
       </c>
       <c r="B94" t="str">
         <f>IF('Memory setup'!E77=1,'Memory setup'!B77,IF('Memory setup'!B77&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B77),""))</f>
-        <v/>
+        <v>ADR_TMC1_TRQ_FILT</v>
       </c>
       <c r="C94" t="str">
         <f>IF(AND(B94&lt;&gt;"",'Memory setup'!A78&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v/>
+        <v>,</v>
       </c>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" t="str">
         <f>IF('Memory setup'!A78&lt;&gt;"",IF('Memory setup'!A78&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A78,"};"),"")</f>
-        <v/>
+        <v>// AXIS2</v>
       </c>
       <c r="B95" t="str">
         <f>IF('Memory setup'!E78=1,'Memory setup'!B78,IF('Memory setup'!B78&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B78),""))</f>
-        <v>ADR_AXIS2_CONFIG</v>
+        <v/>
       </c>
       <c r="C95" t="str">
         <f>IF(AND(B95&lt;&gt;"",'Memory setup'!A79&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v>,</v>
+        <v/>
       </c>
     </row>
     <row r="96" spans="1:3">
@@ -7487,7 +7547,7 @@
       </c>
       <c r="B96" t="str">
         <f>IF('Memory setup'!E79=1,'Memory setup'!B79,IF('Memory setup'!B79&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B79),""))</f>
-        <v>ADR_AXIS2_POWER</v>
+        <v>ADR_AXIS2_CONFIG</v>
       </c>
       <c r="C96" t="str">
         <f>IF(AND(B96&lt;&gt;"",'Memory setup'!A80&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -7501,7 +7561,7 @@
       </c>
       <c r="B97" t="str">
         <f>IF('Memory setup'!E80=1,'Memory setup'!B80,IF('Memory setup'!B80&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B80),""))</f>
-        <v>ADR_AXIS2_DEGREES</v>
+        <v>ADR_AXIS2_POWER</v>
       </c>
       <c r="C97" t="str">
         <f>IF(AND(B97&lt;&gt;"",'Memory setup'!A81&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -7515,7 +7575,7 @@
       </c>
       <c r="B98" t="str">
         <f>IF('Memory setup'!E81=1,'Memory setup'!B81,IF('Memory setup'!B81&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B81),""))</f>
-        <v>ADR_AXIS2_MAX_SPEED</v>
+        <v>ADR_AXIS2_DEGREES</v>
       </c>
       <c r="C98" t="str">
         <f>IF(AND(B98&lt;&gt;"",'Memory setup'!A82&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -7529,7 +7589,7 @@
       </c>
       <c r="B99" t="str">
         <f>IF('Memory setup'!E82=1,'Memory setup'!B82,IF('Memory setup'!B82&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B82),""))</f>
-        <v>ADR_AXIS2_MAX_ACCEL</v>
+        <v>ADR_AXIS2_MAX_SPEED</v>
       </c>
       <c r="C99" t="str">
         <f>IF(AND(B99&lt;&gt;"",'Memory setup'!A83&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -7543,7 +7603,7 @@
       </c>
       <c r="B100" t="str">
         <f>IF('Memory setup'!E83=1,'Memory setup'!B83,IF('Memory setup'!B83&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B83),""))</f>
-        <v>ADR_AXIS2_ENDSTOP</v>
+        <v>ADR_AXIS2_MAX_ACCEL</v>
       </c>
       <c r="C100" t="str">
         <f>IF(AND(B100&lt;&gt;"",'Memory setup'!A84&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -7557,7 +7617,7 @@
       </c>
       <c r="B101" t="str">
         <f>IF('Memory setup'!E84=1,'Memory setup'!B84,IF('Memory setup'!B84&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B84),""))</f>
-        <v>ADR_AXIS2_EFFECTS1</v>
+        <v>ADR_AXIS2_ENDSTOP</v>
       </c>
       <c r="C101" t="str">
         <f>IF(AND(B101&lt;&gt;"",'Memory setup'!A85&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -7571,7 +7631,7 @@
       </c>
       <c r="B102" t="str">
         <f>IF('Memory setup'!E85=1,'Memory setup'!B85,IF('Memory setup'!B85&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B85),""))</f>
-        <v>ADR_AXIS2_SPEEDACCEL_FILTER</v>
+        <v>ADR_AXIS2_EFFECTS1</v>
       </c>
       <c r="C102" t="str">
         <f>IF(AND(B102&lt;&gt;"",'Memory setup'!A86&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -7585,7 +7645,7 @@
       </c>
       <c r="B103" t="str">
         <f>IF('Memory setup'!E86=1,'Memory setup'!B86,IF('Memory setup'!B86&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B86),""))</f>
-        <v>ADR_AXIS2_ENC_RATIO</v>
+        <v>ADR_AXIS2_SPEEDACCEL_FILTER</v>
       </c>
       <c r="C103" t="str">
         <f>IF(AND(B103&lt;&gt;"",'Memory setup'!A87&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -7595,29 +7655,29 @@
     <row r="104" spans="1:3">
       <c r="A104" t="str">
         <f>IF('Memory setup'!A87&lt;&gt;"",IF('Memory setup'!A87&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A87,"};"),"")</f>
-        <v>// TMC2</v>
+        <v/>
       </c>
       <c r="B104" t="str">
         <f>IF('Memory setup'!E87=1,'Memory setup'!B87,IF('Memory setup'!B87&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B87),""))</f>
-        <v/>
+        <v>ADR_AXIS2_ENC_RATIO</v>
       </c>
       <c r="C104" t="str">
         <f>IF(AND(B104&lt;&gt;"",'Memory setup'!A88&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v/>
+        <v>,</v>
       </c>
     </row>
     <row r="105" spans="1:3">
       <c r="A105" t="str">
         <f>IF('Memory setup'!A88&lt;&gt;"",IF('Memory setup'!A88&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A88,"};"),"")</f>
-        <v/>
+        <v>// TMC2</v>
       </c>
       <c r="B105" t="str">
         <f>IF('Memory setup'!E88=1,'Memory setup'!B88,IF('Memory setup'!B88&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B88),""))</f>
-        <v>ADR_TMC2_MOTCONF</v>
+        <v/>
       </c>
       <c r="C105" t="str">
         <f>IF(AND(B105&lt;&gt;"",'Memory setup'!A89&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v>,</v>
+        <v/>
       </c>
     </row>
     <row r="106" spans="1:3">
@@ -7627,7 +7687,7 @@
       </c>
       <c r="B106" t="str">
         <f>IF('Memory setup'!E89=1,'Memory setup'!B89,IF('Memory setup'!B89&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B89),""))</f>
-        <v>ADR_TMC2_CPR</v>
+        <v>ADR_TMC2_MOTCONF</v>
       </c>
       <c r="C106" t="str">
         <f>IF(AND(B106&lt;&gt;"",'Memory setup'!A90&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -7641,7 +7701,7 @@
       </c>
       <c r="B107" t="str">
         <f>IF('Memory setup'!E90=1,'Memory setup'!B90,IF('Memory setup'!B90&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B90),""))</f>
-        <v>ADR_TMC2_ENCA</v>
+        <v>ADR_TMC2_CPR</v>
       </c>
       <c r="C107" t="str">
         <f>IF(AND(B107&lt;&gt;"",'Memory setup'!A91&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -7655,7 +7715,7 @@
       </c>
       <c r="B108" t="str">
         <f>IF('Memory setup'!E91=1,'Memory setup'!B91,IF('Memory setup'!B91&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B91),""))</f>
-        <v>ADR_TMC2_ADC_I0_OFS</v>
+        <v>ADR_TMC2_ENCA</v>
       </c>
       <c r="C108" t="str">
         <f>IF(AND(B108&lt;&gt;"",'Memory setup'!A92&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -7669,7 +7729,7 @@
       </c>
       <c r="B109" t="str">
         <f>IF('Memory setup'!E92=1,'Memory setup'!B92,IF('Memory setup'!B92&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B92),""))</f>
-        <v>ADR_TMC2_ADC_I1_OFS</v>
+        <v>ADR_TMC2_ADC_I0_OFS</v>
       </c>
       <c r="C109" t="str">
         <f>IF(AND(B109&lt;&gt;"",'Memory setup'!A93&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -7683,7 +7743,7 @@
       </c>
       <c r="B110" t="str">
         <f>IF('Memory setup'!E93=1,'Memory setup'!B93,IF('Memory setup'!B93&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B93),""))</f>
-        <v>ADR_TMC2_ENC_OFFSET</v>
+        <v>ADR_TMC2_ADC_I1_OFS</v>
       </c>
       <c r="C110" t="str">
         <f>IF(AND(B110&lt;&gt;"",'Memory setup'!A94&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -7697,7 +7757,7 @@
       </c>
       <c r="B111" t="str">
         <f>IF('Memory setup'!E94=1,'Memory setup'!B94,IF('Memory setup'!B94&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B94),""))</f>
-        <v>ADR_TMC2_OFFSETFLUX</v>
+        <v>ADR_TMC2_ENC_OFFSET</v>
       </c>
       <c r="C111" t="str">
         <f>IF(AND(B111&lt;&gt;"",'Memory setup'!A95&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -7711,7 +7771,7 @@
       </c>
       <c r="B112" t="str">
         <f>IF('Memory setup'!E95=1,'Memory setup'!B95,IF('Memory setup'!B95&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B95),""))</f>
-        <v>ADR_TMC2_TORQUE_P</v>
+        <v>ADR_TMC2_OFFSETFLUX</v>
       </c>
       <c r="C112" t="str">
         <f>IF(AND(B112&lt;&gt;"",'Memory setup'!A96&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -7725,7 +7785,7 @@
       </c>
       <c r="B113" t="str">
         <f>IF('Memory setup'!E96=1,'Memory setup'!B96,IF('Memory setup'!B96&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B96),""))</f>
-        <v>ADR_TMC2_TORQUE_I</v>
+        <v>ADR_TMC2_TORQUE_P</v>
       </c>
       <c r="C113" t="str">
         <f>IF(AND(B113&lt;&gt;"",'Memory setup'!A97&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -7739,7 +7799,7 @@
       </c>
       <c r="B114" t="str">
         <f>IF('Memory setup'!E97=1,'Memory setup'!B97,IF('Memory setup'!B97&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B97),""))</f>
-        <v>ADR_TMC2_FLUX_P</v>
+        <v>ADR_TMC2_TORQUE_I</v>
       </c>
       <c r="C114" t="str">
         <f>IF(AND(B114&lt;&gt;"",'Memory setup'!A98&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -7753,7 +7813,7 @@
       </c>
       <c r="B115" t="str">
         <f>IF('Memory setup'!E98=1,'Memory setup'!B98,IF('Memory setup'!B98&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B98),""))</f>
-        <v>ADR_TMC2_FLUX_I</v>
+        <v>ADR_TMC2_FLUX_P</v>
       </c>
       <c r="C115" t="str">
         <f>IF(AND(B115&lt;&gt;"",'Memory setup'!A99&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -7767,7 +7827,7 @@
       </c>
       <c r="B116" t="str">
         <f>IF('Memory setup'!E99=1,'Memory setup'!B99,IF('Memory setup'!B99&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B99),""))</f>
-        <v>ADR_TMC2_PHIE_OFS</v>
+        <v>ADR_TMC2_FLUX_I</v>
       </c>
       <c r="C116" t="str">
         <f>IF(AND(B116&lt;&gt;"",'Memory setup'!A100&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -7777,15 +7837,15 @@
     <row r="117" spans="1:3">
       <c r="A117" t="str">
         <f>IF('Memory setup'!A100&lt;&gt;"",IF('Memory setup'!A100&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A100,"};"),"")</f>
-        <v>// AXIS3</v>
+        <v/>
       </c>
       <c r="B117" t="str">
         <f>IF('Memory setup'!E100=1,'Memory setup'!B100,IF('Memory setup'!B100&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B100),""))</f>
-        <v/>
+        <v>ADR_TMC2_PHIE_OFS</v>
       </c>
       <c r="C117" t="str">
         <f>IF(AND(B117&lt;&gt;"",'Memory setup'!A101&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v/>
+        <v>,</v>
       </c>
     </row>
     <row r="118" spans="1:3">
@@ -7795,7 +7855,7 @@
       </c>
       <c r="B118" t="str">
         <f>IF('Memory setup'!E101=1,'Memory setup'!B101,IF('Memory setup'!B101&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B101),""))</f>
-        <v>ADR_AXIS3_CONFIG</v>
+        <v>ADR_TMC2_TRQ_FILT</v>
       </c>
       <c r="C118" t="str">
         <f>IF(AND(B118&lt;&gt;"",'Memory setup'!A102&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -7805,15 +7865,15 @@
     <row r="119" spans="1:3">
       <c r="A119" t="str">
         <f>IF('Memory setup'!A102&lt;&gt;"",IF('Memory setup'!A102&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A102,"};"),"")</f>
-        <v/>
+        <v>// AXIS3</v>
       </c>
       <c r="B119" t="str">
         <f>IF('Memory setup'!E102=1,'Memory setup'!B102,IF('Memory setup'!B102&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B102),""))</f>
-        <v>ADR_AXIS3_POWER</v>
+        <v/>
       </c>
       <c r="C119" t="str">
         <f>IF(AND(B119&lt;&gt;"",'Memory setup'!A103&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v>,</v>
+        <v/>
       </c>
     </row>
     <row r="120" spans="1:3">
@@ -7823,7 +7883,7 @@
       </c>
       <c r="B120" t="str">
         <f>IF('Memory setup'!E103=1,'Memory setup'!B103,IF('Memory setup'!B103&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B103),""))</f>
-        <v>ADR_AXIS3_DEGREES</v>
+        <v>ADR_AXIS3_CONFIG</v>
       </c>
       <c r="C120" t="str">
         <f>IF(AND(B120&lt;&gt;"",'Memory setup'!A104&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -7837,7 +7897,7 @@
       </c>
       <c r="B121" t="str">
         <f>IF('Memory setup'!E104=1,'Memory setup'!B104,IF('Memory setup'!B104&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B104),""))</f>
-        <v>ADR_AXIS3_MAX_SPEED</v>
+        <v>ADR_AXIS3_POWER</v>
       </c>
       <c r="C121" t="str">
         <f>IF(AND(B121&lt;&gt;"",'Memory setup'!A105&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -7851,7 +7911,7 @@
       </c>
       <c r="B122" t="str">
         <f>IF('Memory setup'!E105=1,'Memory setup'!B105,IF('Memory setup'!B105&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B105),""))</f>
-        <v>ADR_AXIS3_MAX_ACCEL</v>
+        <v>ADR_AXIS3_DEGREES</v>
       </c>
       <c r="C122" t="str">
         <f>IF(AND(B122&lt;&gt;"",'Memory setup'!A106&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -7865,7 +7925,7 @@
       </c>
       <c r="B123" t="str">
         <f>IF('Memory setup'!E106=1,'Memory setup'!B106,IF('Memory setup'!B106&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B106),""))</f>
-        <v>ADR_AXIS3_ENDSTOP</v>
+        <v>ADR_AXIS3_MAX_SPEED</v>
       </c>
       <c r="C123" t="str">
         <f>IF(AND(B123&lt;&gt;"",'Memory setup'!A107&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -7879,7 +7939,7 @@
       </c>
       <c r="B124" t="str">
         <f>IF('Memory setup'!E107=1,'Memory setup'!B107,IF('Memory setup'!B107&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B107),""))</f>
-        <v>ADR_AXIS3_EFFECTS1</v>
+        <v>ADR_AXIS3_MAX_ACCEL</v>
       </c>
       <c r="C124" t="str">
         <f>IF(AND(B124&lt;&gt;"",'Memory setup'!A108&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -7893,7 +7953,7 @@
       </c>
       <c r="B125" t="str">
         <f>IF('Memory setup'!E108=1,'Memory setup'!B108,IF('Memory setup'!B108&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B108),""))</f>
-        <v>ADR_AXIS3_SPEEDACCEL_FILTER</v>
+        <v>ADR_AXIS3_ENDSTOP</v>
       </c>
       <c r="C125" t="str">
         <f>IF(AND(B125&lt;&gt;"",'Memory setup'!A109&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -7907,7 +7967,7 @@
       </c>
       <c r="B126" t="str">
         <f>IF('Memory setup'!E109=1,'Memory setup'!B109,IF('Memory setup'!B109&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B109),""))</f>
-        <v>ADR_AXIS3_ENC_RATIO</v>
+        <v>ADR_AXIS3_EFFECTS1</v>
       </c>
       <c r="C126" t="str">
         <f>IF(AND(B126&lt;&gt;"",'Memory setup'!A110&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -7917,15 +7977,15 @@
     <row r="127" spans="1:3">
       <c r="A127" t="str">
         <f>IF('Memory setup'!A110&lt;&gt;"",IF('Memory setup'!A110&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A110,"};"),"")</f>
-        <v>// TMC3</v>
+        <v/>
       </c>
       <c r="B127" t="str">
         <f>IF('Memory setup'!E110=1,'Memory setup'!B110,IF('Memory setup'!B110&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B110),""))</f>
-        <v/>
+        <v>ADR_AXIS3_SPEEDACCEL_FILTER</v>
       </c>
       <c r="C127" t="str">
         <f>IF(AND(B127&lt;&gt;"",'Memory setup'!A111&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v/>
+        <v>,</v>
       </c>
     </row>
     <row r="128" spans="1:3">
@@ -7935,7 +7995,7 @@
       </c>
       <c r="B128" t="str">
         <f>IF('Memory setup'!E111=1,'Memory setup'!B111,IF('Memory setup'!B111&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B111),""))</f>
-        <v>ADR_TMC3_MOTCONF</v>
+        <v>ADR_AXIS3_ENC_RATIO</v>
       </c>
       <c r="C128" t="str">
         <f>IF(AND(B128&lt;&gt;"",'Memory setup'!A112&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -7945,15 +8005,15 @@
     <row r="129" spans="1:3">
       <c r="A129" t="str">
         <f>IF('Memory setup'!A112&lt;&gt;"",IF('Memory setup'!A112&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A112,"};"),"")</f>
-        <v/>
+        <v>// TMC3</v>
       </c>
       <c r="B129" t="str">
         <f>IF('Memory setup'!E112=1,'Memory setup'!B112,IF('Memory setup'!B112&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B112),""))</f>
-        <v>ADR_TMC3_CPR</v>
+        <v/>
       </c>
       <c r="C129" t="str">
         <f>IF(AND(B129&lt;&gt;"",'Memory setup'!A113&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v>,</v>
+        <v/>
       </c>
     </row>
     <row r="130" spans="1:3">
@@ -7963,7 +8023,7 @@
       </c>
       <c r="B130" t="str">
         <f>IF('Memory setup'!E113=1,'Memory setup'!B113,IF('Memory setup'!B113&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B113),""))</f>
-        <v>ADR_TMC3_ENCA</v>
+        <v>ADR_TMC3_MOTCONF</v>
       </c>
       <c r="C130" t="str">
         <f>IF(AND(B130&lt;&gt;"",'Memory setup'!A114&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -7977,7 +8037,7 @@
       </c>
       <c r="B131" t="str">
         <f>IF('Memory setup'!E114=1,'Memory setup'!B114,IF('Memory setup'!B114&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B114),""))</f>
-        <v>ADR_TMC3_ADC_I0_OFS</v>
+        <v>ADR_TMC3_CPR</v>
       </c>
       <c r="C131" t="str">
         <f>IF(AND(B131&lt;&gt;"",'Memory setup'!A115&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -7991,7 +8051,7 @@
       </c>
       <c r="B132" t="str">
         <f>IF('Memory setup'!E115=1,'Memory setup'!B115,IF('Memory setup'!B115&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B115),""))</f>
-        <v>ADR_TMC3_ADC_I1_OFS</v>
+        <v>ADR_TMC3_ENCA</v>
       </c>
       <c r="C132" t="str">
         <f>IF(AND(B132&lt;&gt;"",'Memory setup'!A116&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8005,7 +8065,7 @@
       </c>
       <c r="B133" t="str">
         <f>IF('Memory setup'!E116=1,'Memory setup'!B116,IF('Memory setup'!B116&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B116),""))</f>
-        <v>ADR_TMC3_ENC_OFFSET</v>
+        <v>ADR_TMC3_ADC_I0_OFS</v>
       </c>
       <c r="C133" t="str">
         <f>IF(AND(B133&lt;&gt;"",'Memory setup'!A117&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8019,7 +8079,7 @@
       </c>
       <c r="B134" t="str">
         <f>IF('Memory setup'!E117=1,'Memory setup'!B117,IF('Memory setup'!B117&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B117),""))</f>
-        <v>ADR_TMC3_OFFSETFLUX</v>
+        <v>ADR_TMC3_ADC_I1_OFS</v>
       </c>
       <c r="C134" t="str">
         <f>IF(AND(B134&lt;&gt;"",'Memory setup'!A118&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8033,7 +8093,7 @@
       </c>
       <c r="B135" t="str">
         <f>IF('Memory setup'!E118=1,'Memory setup'!B118,IF('Memory setup'!B118&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B118),""))</f>
-        <v>ADR_TMC3_TORQUE_P</v>
+        <v>ADR_TMC3_ENC_OFFSET</v>
       </c>
       <c r="C135" t="str">
         <f>IF(AND(B135&lt;&gt;"",'Memory setup'!A119&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8047,7 +8107,7 @@
       </c>
       <c r="B136" t="str">
         <f>IF('Memory setup'!E119=1,'Memory setup'!B119,IF('Memory setup'!B119&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B119),""))</f>
-        <v>ADR_TMC3_TORQUE_I</v>
+        <v>ADR_TMC3_OFFSETFLUX</v>
       </c>
       <c r="C136" t="str">
         <f>IF(AND(B136&lt;&gt;"",'Memory setup'!A120&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8061,7 +8121,7 @@
       </c>
       <c r="B137" t="str">
         <f>IF('Memory setup'!E120=1,'Memory setup'!B120,IF('Memory setup'!B120&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B120),""))</f>
-        <v>ADR_TMC3_FLUX_P</v>
+        <v>ADR_TMC3_TORQUE_P</v>
       </c>
       <c r="C137" t="str">
         <f>IF(AND(B137&lt;&gt;"",'Memory setup'!A121&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8075,7 +8135,7 @@
       </c>
       <c r="B138" t="str">
         <f>IF('Memory setup'!E121=1,'Memory setup'!B121,IF('Memory setup'!B121&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B121),""))</f>
-        <v>ADR_TMC3_FLUX_I</v>
+        <v>ADR_TMC3_TORQUE_I</v>
       </c>
       <c r="C138" t="str">
         <f>IF(AND(B138&lt;&gt;"",'Memory setup'!A122&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8089,7 +8149,7 @@
       </c>
       <c r="B139" t="str">
         <f>IF('Memory setup'!E122=1,'Memory setup'!B122,IF('Memory setup'!B122&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B122),""))</f>
-        <v>ADR_TMC3_PHIE_OFS</v>
+        <v>ADR_TMC3_FLUX_P</v>
       </c>
       <c r="C139" t="str">
         <f>IF(AND(B139&lt;&gt;"",'Memory setup'!A123&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8099,15 +8159,15 @@
     <row r="140" spans="1:3">
       <c r="A140" t="str">
         <f>IF('Memory setup'!A123&lt;&gt;"",IF('Memory setup'!A123&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A123,"};"),"")</f>
-        <v>// Odrive</v>
+        <v/>
       </c>
       <c r="B140" t="str">
         <f>IF('Memory setup'!E123=1,'Memory setup'!B123,IF('Memory setup'!B123&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B123),""))</f>
-        <v/>
+        <v>ADR_TMC3_FLUX_I</v>
       </c>
       <c r="C140" t="str">
         <f>IF(AND(B140&lt;&gt;"",'Memory setup'!A124&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v/>
+        <v>,</v>
       </c>
     </row>
     <row r="141" spans="1:3">
@@ -8117,7 +8177,7 @@
       </c>
       <c r="B141" t="str">
         <f>IF('Memory setup'!E124=1,'Memory setup'!B124,IF('Memory setup'!B124&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B124),""))</f>
-        <v>ADR_ODRIVE_CANID</v>
+        <v>ADR_TMC3_PHIE_OFS</v>
       </c>
       <c r="C141" t="str">
         <f>IF(AND(B141&lt;&gt;"",'Memory setup'!A125&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8131,7 +8191,7 @@
       </c>
       <c r="B142" t="str">
         <f>IF('Memory setup'!E125=1,'Memory setup'!B125,IF('Memory setup'!B125&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B125),""))</f>
-        <v>ADR_ODRIVE_SETTING1_M0</v>
+        <v>ADR_TMC3_TRQ_FILT</v>
       </c>
       <c r="C142" t="str">
         <f>IF(AND(B142&lt;&gt;"",'Memory setup'!A126&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8141,29 +8201,29 @@
     <row r="143" spans="1:3">
       <c r="A143" t="str">
         <f>IF('Memory setup'!A126&lt;&gt;"",IF('Memory setup'!A126&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A126,"};"),"")</f>
-        <v/>
+        <v>// Odrive</v>
       </c>
       <c r="B143" t="str">
         <f>IF('Memory setup'!E126=1,'Memory setup'!B126,IF('Memory setup'!B126&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B126),""))</f>
-        <v>ADR_ODRIVE_SETTING1_M1</v>
+        <v/>
       </c>
       <c r="C143" t="str">
         <f>IF(AND(B143&lt;&gt;"",'Memory setup'!A127&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v>,</v>
+        <v/>
       </c>
     </row>
     <row r="144" spans="1:3">
       <c r="A144" t="str">
         <f>IF('Memory setup'!A127&lt;&gt;"",IF('Memory setup'!A127&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A127,"};"),"")</f>
-        <v>// VESC Section</v>
+        <v/>
       </c>
       <c r="B144" t="str">
         <f>IF('Memory setup'!E127=1,'Memory setup'!B127,IF('Memory setup'!B127&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B127),""))</f>
-        <v/>
+        <v>ADR_ODRIVE_CANID</v>
       </c>
       <c r="C144" t="str">
         <f>IF(AND(B144&lt;&gt;"",'Memory setup'!A128&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v/>
+        <v>,</v>
       </c>
     </row>
     <row r="145" spans="1:3">
@@ -8173,7 +8233,7 @@
       </c>
       <c r="B145" t="str">
         <f>IF('Memory setup'!E128=1,'Memory setup'!B128,IF('Memory setup'!B128&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B128),""))</f>
-        <v>ADR_VESC1_CANID</v>
+        <v>ADR_ODRIVE_SETTING1_M0</v>
       </c>
       <c r="C145" t="str">
         <f>IF(AND(B145&lt;&gt;"",'Memory setup'!A129&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8187,7 +8247,7 @@
       </c>
       <c r="B146" t="str">
         <f>IF('Memory setup'!E129=1,'Memory setup'!B129,IF('Memory setup'!B129&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B129),""))</f>
-        <v>ADR_VESC1_DATA</v>
+        <v>ADR_ODRIVE_SETTING1_M1</v>
       </c>
       <c r="C146" t="str">
         <f>IF(AND(B146&lt;&gt;"",'Memory setup'!A130&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8197,15 +8257,15 @@
     <row r="147" spans="1:3">
       <c r="A147" t="str">
         <f>IF('Memory setup'!A130&lt;&gt;"",IF('Memory setup'!A130&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A130,"};"),"")</f>
-        <v/>
+        <v>// VESC Section</v>
       </c>
       <c r="B147" t="str">
         <f>IF('Memory setup'!E130=1,'Memory setup'!B130,IF('Memory setup'!B130&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B130),""))</f>
-        <v>ADR_VESC1_OFFSET</v>
+        <v/>
       </c>
       <c r="C147" t="str">
         <f>IF(AND(B147&lt;&gt;"",'Memory setup'!A131&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v>,</v>
+        <v/>
       </c>
     </row>
     <row r="148" spans="1:3">
@@ -8215,7 +8275,7 @@
       </c>
       <c r="B148" t="str">
         <f>IF('Memory setup'!E131=1,'Memory setup'!B131,IF('Memory setup'!B131&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B131),""))</f>
-        <v>ADR_VESC2_CANID</v>
+        <v>ADR_VESC1_CANID</v>
       </c>
       <c r="C148" t="str">
         <f>IF(AND(B148&lt;&gt;"",'Memory setup'!A132&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8229,7 +8289,7 @@
       </c>
       <c r="B149" t="str">
         <f>IF('Memory setup'!E132=1,'Memory setup'!B132,IF('Memory setup'!B132&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B132),""))</f>
-        <v>ADR_VESC2_DATA</v>
+        <v>ADR_VESC1_DATA</v>
       </c>
       <c r="C149" t="str">
         <f>IF(AND(B149&lt;&gt;"",'Memory setup'!A133&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8243,7 +8303,7 @@
       </c>
       <c r="B150" t="str">
         <f>IF('Memory setup'!E133=1,'Memory setup'!B133,IF('Memory setup'!B133&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B133),""))</f>
-        <v>ADR_VESC2_OFFSET</v>
+        <v>ADR_VESC1_OFFSET</v>
       </c>
       <c r="C150" t="str">
         <f>IF(AND(B150&lt;&gt;"",'Memory setup'!A134&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8257,7 +8317,7 @@
       </c>
       <c r="B151" t="str">
         <f>IF('Memory setup'!E134=1,'Memory setup'!B134,IF('Memory setup'!B134&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B134),""))</f>
-        <v>ADR_VESC3_CANID</v>
+        <v>ADR_VESC2_CANID</v>
       </c>
       <c r="C151" t="str">
         <f>IF(AND(B151&lt;&gt;"",'Memory setup'!A135&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8271,7 +8331,7 @@
       </c>
       <c r="B152" t="str">
         <f>IF('Memory setup'!E135=1,'Memory setup'!B135,IF('Memory setup'!B135&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B135),""))</f>
-        <v>ADR_VESC3_DATA</v>
+        <v>ADR_VESC2_DATA</v>
       </c>
       <c r="C152" t="str">
         <f>IF(AND(B152&lt;&gt;"",'Memory setup'!A136&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8285,7 +8345,7 @@
       </c>
       <c r="B153" t="str">
         <f>IF('Memory setup'!E136=1,'Memory setup'!B136,IF('Memory setup'!B136&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B136),""))</f>
-        <v>ADR_VESC3_OFFSET</v>
+        <v>ADR_VESC2_OFFSET</v>
       </c>
       <c r="C153" t="str">
         <f>IF(AND(B153&lt;&gt;"",'Memory setup'!A137&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8295,15 +8355,15 @@
     <row r="154" spans="1:3">
       <c r="A154" t="str">
         <f>IF('Memory setup'!A137&lt;&gt;"",IF('Memory setup'!A137&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A137,"};"),"")</f>
-        <v>//MT Encoder</v>
+        <v/>
       </c>
       <c r="B154" t="str">
         <f>IF('Memory setup'!E137=1,'Memory setup'!B137,IF('Memory setup'!B137&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B137),""))</f>
-        <v/>
+        <v>ADR_VESC3_CANID</v>
       </c>
       <c r="C154" t="str">
         <f>IF(AND(B154&lt;&gt;"",'Memory setup'!A138&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v/>
+        <v>,</v>
       </c>
     </row>
     <row r="155" spans="1:3">
@@ -8313,7 +8373,7 @@
       </c>
       <c r="B155" t="str">
         <f>IF('Memory setup'!E138=1,'Memory setup'!B138,IF('Memory setup'!B138&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B138),""))</f>
-        <v>ADR_MTENC_OFS</v>
+        <v>ADR_VESC3_DATA</v>
       </c>
       <c r="C155" t="str">
         <f>IF(AND(B155&lt;&gt;"",'Memory setup'!A139&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8327,7 +8387,7 @@
       </c>
       <c r="B156" t="str">
         <f>IF('Memory setup'!E139=1,'Memory setup'!B139,IF('Memory setup'!B139&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B139),""))</f>
-        <v>ADR_MTENC_CONF1</v>
+        <v>ADR_VESC3_OFFSET</v>
       </c>
       <c r="C156" t="str">
         <f>IF(AND(B156&lt;&gt;"",'Memory setup'!A140&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8337,7 +8397,7 @@
     <row r="157" spans="1:3">
       <c r="A157" t="str">
         <f>IF('Memory setup'!A140&lt;&gt;"",IF('Memory setup'!A140&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A140,"};"),"")</f>
-        <v>// Biss-C</v>
+        <v>//MT Encoder</v>
       </c>
       <c r="B157" t="str">
         <f>IF('Memory setup'!E140=1,'Memory setup'!B140,IF('Memory setup'!B140&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B140),""))</f>
@@ -8355,7 +8415,7 @@
       </c>
       <c r="B158" t="str">
         <f>IF('Memory setup'!E141=1,'Memory setup'!B141,IF('Memory setup'!B141&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B141),""))</f>
-        <v>ADR_BISSENC_CONF1</v>
+        <v>ADR_MTENC_OFS</v>
       </c>
       <c r="C158" t="str">
         <f>IF(AND(B158&lt;&gt;"",'Memory setup'!A142&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8369,7 +8429,7 @@
       </c>
       <c r="B159" t="str">
         <f>IF('Memory setup'!E142=1,'Memory setup'!B142,IF('Memory setup'!B142&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B142),""))</f>
-        <v>ADR_BISSENC_OFS</v>
+        <v>ADR_MTENC_CONF1</v>
       </c>
       <c r="C159" t="str">
         <f>IF(AND(B159&lt;&gt;"",'Memory setup'!A143&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8379,7 +8439,7 @@
     <row r="160" spans="1:3">
       <c r="A160" t="str">
         <f>IF('Memory setup'!A143&lt;&gt;"",IF('Memory setup'!A143&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A143,"};"),"")</f>
-        <v>// Analog min/max calibrations</v>
+        <v>// Biss-C</v>
       </c>
       <c r="B160" t="str">
         <f>IF('Memory setup'!E143=1,'Memory setup'!B143,IF('Memory setup'!B143&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B143),""))</f>
@@ -8397,7 +8457,7 @@
       </c>
       <c r="B161" t="str">
         <f>IF('Memory setup'!E144=1,'Memory setup'!B144,IF('Memory setup'!B144&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B144),""))</f>
-        <v>ADR_LOCALANALOG_MIN_0</v>
+        <v>ADR_BISSENC_CONF1</v>
       </c>
       <c r="C161" t="str">
         <f>IF(AND(B161&lt;&gt;"",'Memory setup'!A145&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8411,7 +8471,7 @@
       </c>
       <c r="B162" t="str">
         <f>IF('Memory setup'!E145=1,'Memory setup'!B145,IF('Memory setup'!B145&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B145),""))</f>
-        <v>ADR_LOCALANALOG_MAX_0</v>
+        <v>ADR_BISSENC_OFS</v>
       </c>
       <c r="C162" t="str">
         <f>IF(AND(B162&lt;&gt;"",'Memory setup'!A146&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8421,15 +8481,15 @@
     <row r="163" spans="1:3">
       <c r="A163" t="str">
         <f>IF('Memory setup'!A146&lt;&gt;"",IF('Memory setup'!A146&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A146,"};"),"")</f>
-        <v/>
+        <v>// Analog min/max calibrations</v>
       </c>
       <c r="B163" t="str">
         <f>IF('Memory setup'!E146=1,'Memory setup'!B146,IF('Memory setup'!B146&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B146),""))</f>
-        <v>ADR_LOCALANALOG_MIN_1</v>
+        <v/>
       </c>
       <c r="C163" t="str">
         <f>IF(AND(B163&lt;&gt;"",'Memory setup'!A147&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v>,</v>
+        <v/>
       </c>
     </row>
     <row r="164" spans="1:3">
@@ -8439,7 +8499,7 @@
       </c>
       <c r="B164" t="str">
         <f>IF('Memory setup'!E147=1,'Memory setup'!B147,IF('Memory setup'!B147&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B147),""))</f>
-        <v>ADR_LOCALANALOG_MAX_1</v>
+        <v>ADR_LOCALANALOG_MIN_0</v>
       </c>
       <c r="C164" t="str">
         <f>IF(AND(B164&lt;&gt;"",'Memory setup'!A148&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8453,7 +8513,7 @@
       </c>
       <c r="B165" t="str">
         <f>IF('Memory setup'!E148=1,'Memory setup'!B148,IF('Memory setup'!B148&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B148),""))</f>
-        <v>ADR_LOCALANALOG_MIN_2</v>
+        <v>ADR_LOCALANALOG_MAX_0</v>
       </c>
       <c r="C165" t="str">
         <f>IF(AND(B165&lt;&gt;"",'Memory setup'!A149&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8467,7 +8527,7 @@
       </c>
       <c r="B166" t="str">
         <f>IF('Memory setup'!E149=1,'Memory setup'!B149,IF('Memory setup'!B149&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B149),""))</f>
-        <v>ADR_LOCALANALOG_MAX_2</v>
+        <v>ADR_LOCALANALOG_MIN_1</v>
       </c>
       <c r="C166" t="str">
         <f>IF(AND(B166&lt;&gt;"",'Memory setup'!A150&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8481,7 +8541,7 @@
       </c>
       <c r="B167" t="str">
         <f>IF('Memory setup'!E150=1,'Memory setup'!B150,IF('Memory setup'!B150&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B150),""))</f>
-        <v>ADR_LOCALANALOG_MIN_3</v>
+        <v>ADR_LOCALANALOG_MAX_1</v>
       </c>
       <c r="C167" t="str">
         <f>IF(AND(B167&lt;&gt;"",'Memory setup'!A151&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8495,7 +8555,7 @@
       </c>
       <c r="B168" t="str">
         <f>IF('Memory setup'!E151=1,'Memory setup'!B151,IF('Memory setup'!B151&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B151),""))</f>
-        <v>ADR_LOCALANALOG_MAX_3</v>
+        <v>ADR_LOCALANALOG_MIN_2</v>
       </c>
       <c r="C168" t="str">
         <f>IF(AND(B168&lt;&gt;"",'Memory setup'!A152&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8509,7 +8569,7 @@
       </c>
       <c r="B169" t="str">
         <f>IF('Memory setup'!E152=1,'Memory setup'!B152,IF('Memory setup'!B152&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B152),""))</f>
-        <v>ADR_LOCALANALOG_MIN_4</v>
+        <v>ADR_LOCALANALOG_MAX_2</v>
       </c>
       <c r="C169" t="str">
         <f>IF(AND(B169&lt;&gt;"",'Memory setup'!A153&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8523,7 +8583,7 @@
       </c>
       <c r="B170" t="str">
         <f>IF('Memory setup'!E153=1,'Memory setup'!B153,IF('Memory setup'!B153&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B153),""))</f>
-        <v>ADR_LOCALANALOG_MAX_4</v>
+        <v>ADR_LOCALANALOG_MIN_3</v>
       </c>
       <c r="C170" t="str">
         <f>IF(AND(B170&lt;&gt;"",'Memory setup'!A154&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8537,7 +8597,7 @@
       </c>
       <c r="B171" t="str">
         <f>IF('Memory setup'!E154=1,'Memory setup'!B154,IF('Memory setup'!B154&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B154),""))</f>
-        <v>ADR_LOCALANALOG_MIN_5</v>
+        <v>ADR_LOCALANALOG_MAX_3</v>
       </c>
       <c r="C171" t="str">
         <f>IF(AND(B171&lt;&gt;"",'Memory setup'!A155&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8551,7 +8611,7 @@
       </c>
       <c r="B172" t="str">
         <f>IF('Memory setup'!E155=1,'Memory setup'!B155,IF('Memory setup'!B155&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B155),""))</f>
-        <v>ADR_LOCALANALOG_MAX_5</v>
+        <v>ADR_LOCALANALOG_MIN_4</v>
       </c>
       <c r="C172" t="str">
         <f>IF(AND(B172&lt;&gt;"",'Memory setup'!A156&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8565,7 +8625,7 @@
       </c>
       <c r="B173" t="str">
         <f>IF('Memory setup'!E156=1,'Memory setup'!B156,IF('Memory setup'!B156&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B156),""))</f>
-        <v>ADR_LOCALANALOG_MIN_6</v>
+        <v>ADR_LOCALANALOG_MAX_4</v>
       </c>
       <c r="C173" t="str">
         <f>IF(AND(B173&lt;&gt;"",'Memory setup'!A157&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8579,7 +8639,7 @@
       </c>
       <c r="B174" t="str">
         <f>IF('Memory setup'!E157=1,'Memory setup'!B157,IF('Memory setup'!B157&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B157),""))</f>
-        <v>ADR_LOCALANALOG_MAX_6</v>
+        <v>ADR_LOCALANALOG_MIN_5</v>
       </c>
       <c r="C174" t="str">
         <f>IF(AND(B174&lt;&gt;"",'Memory setup'!A158&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8593,7 +8653,7 @@
       </c>
       <c r="B175" t="str">
         <f>IF('Memory setup'!E158=1,'Memory setup'!B158,IF('Memory setup'!B158&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B158),""))</f>
-        <v>ADR_LOCALANALOG_MIN_7</v>
+        <v>ADR_LOCALANALOG_MAX_5</v>
       </c>
       <c r="C175" t="str">
         <f>IF(AND(B175&lt;&gt;"",'Memory setup'!A159&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8607,7 +8667,7 @@
       </c>
       <c r="B176" t="str">
         <f>IF('Memory setup'!E159=1,'Memory setup'!B159,IF('Memory setup'!B159&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B159),""))</f>
-        <v>ADR_LOCALANALOG_MAX_7</v>
+        <v>ADR_LOCALANALOG_MIN_6</v>
       </c>
       <c r="C176" t="str">
         <f>IF(AND(B176&lt;&gt;"",'Memory setup'!A160&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8621,7 +8681,7 @@
       </c>
       <c r="B177" t="str">
         <f>IF('Memory setup'!E160=1,'Memory setup'!B160,IF('Memory setup'!B160&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B160),""))</f>
-        <v>ADR_ADS111X_MIN_0</v>
+        <v>ADR_LOCALANALOG_MAX_6</v>
       </c>
       <c r="C177" t="str">
         <f>IF(AND(B177&lt;&gt;"",'Memory setup'!A161&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8635,7 +8695,7 @@
       </c>
       <c r="B178" t="str">
         <f>IF('Memory setup'!E161=1,'Memory setup'!B161,IF('Memory setup'!B161&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B161),""))</f>
-        <v>ADR_ADS111X_MAX_0</v>
+        <v>ADR_LOCALANALOG_MIN_7</v>
       </c>
       <c r="C178" t="str">
         <f>IF(AND(B178&lt;&gt;"",'Memory setup'!A162&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8649,7 +8709,7 @@
       </c>
       <c r="B179" t="str">
         <f>IF('Memory setup'!E162=1,'Memory setup'!B162,IF('Memory setup'!B162&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B162),""))</f>
-        <v>ADR_ADS111X_MIN_1</v>
+        <v>ADR_LOCALANALOG_MAX_7</v>
       </c>
       <c r="C179" t="str">
         <f>IF(AND(B179&lt;&gt;"",'Memory setup'!A163&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8663,7 +8723,7 @@
       </c>
       <c r="B180" t="str">
         <f>IF('Memory setup'!E163=1,'Memory setup'!B163,IF('Memory setup'!B163&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B163),""))</f>
-        <v>ADR_ADS111X_MAX_1</v>
+        <v>ADR_ADS111X_MIN_0</v>
       </c>
       <c r="C180" t="str">
         <f>IF(AND(B180&lt;&gt;"",'Memory setup'!A164&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8677,7 +8737,7 @@
       </c>
       <c r="B181" t="str">
         <f>IF('Memory setup'!E164=1,'Memory setup'!B164,IF('Memory setup'!B164&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B164),""))</f>
-        <v>ADR_ADS111X_MIN_2</v>
+        <v>ADR_ADS111X_MAX_0</v>
       </c>
       <c r="C181" t="str">
         <f>IF(AND(B181&lt;&gt;"",'Memory setup'!A165&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8691,7 +8751,7 @@
       </c>
       <c r="B182" t="str">
         <f>IF('Memory setup'!E165=1,'Memory setup'!B165,IF('Memory setup'!B165&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B165),""))</f>
-        <v>ADR_ADS111X_MAX_2</v>
+        <v>ADR_ADS111X_MIN_1</v>
       </c>
       <c r="C182" t="str">
         <f>IF(AND(B182&lt;&gt;"",'Memory setup'!A166&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8705,7 +8765,7 @@
       </c>
       <c r="B183" t="str">
         <f>IF('Memory setup'!E166=1,'Memory setup'!B166,IF('Memory setup'!B166&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B166),""))</f>
-        <v>ADR_ADS111X_MIN_3</v>
+        <v>ADR_ADS111X_MAX_1</v>
       </c>
       <c r="C183" t="str">
         <f>IF(AND(B183&lt;&gt;"",'Memory setup'!A167&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8719,25 +8779,25 @@
       </c>
       <c r="B184" t="str">
         <f>IF('Memory setup'!E167=1,'Memory setup'!B167,IF('Memory setup'!B167&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B167),""))</f>
-        <v>ADR_ADS111X_MAX_3</v>
+        <v>ADR_ADS111X_MIN_2</v>
       </c>
       <c r="C184" t="str">
         <f>IF(AND(B184&lt;&gt;"",'Memory setup'!A168&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v/>
+        <v>,</v>
       </c>
     </row>
     <row r="185" spans="1:3">
       <c r="A185" t="str">
         <f>IF('Memory setup'!A168&lt;&gt;"",IF('Memory setup'!A168&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A168,"};"),"")</f>
-        <v>};</v>
+        <v/>
       </c>
       <c r="B185" t="str">
         <f>IF('Memory setup'!E168=1,'Memory setup'!B168,IF('Memory setup'!B168&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B168),""))</f>
-        <v/>
+        <v>ADR_ADS111X_MAX_2</v>
       </c>
       <c r="C185" t="str">
         <f>IF(AND(B185&lt;&gt;"",'Memory setup'!A169&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v/>
+        <v>,</v>
       </c>
     </row>
     <row r="186" spans="1:3">
@@ -8747,11 +8807,11 @@
       </c>
       <c r="B186" t="str">
         <f>IF('Memory setup'!E169=1,'Memory setup'!B169,IF('Memory setup'!B169&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B169),""))</f>
-        <v/>
+        <v>ADR_ADS111X_MIN_3</v>
       </c>
       <c r="C186" t="str">
         <f>IF(AND(B186&lt;&gt;"",'Memory setup'!A170&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v/>
+        <v>,</v>
       </c>
     </row>
     <row r="187" spans="1:3">
@@ -8761,7 +8821,7 @@
       </c>
       <c r="B187" t="str">
         <f>IF('Memory setup'!E170=1,'Memory setup'!B170,IF('Memory setup'!B170&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B170),""))</f>
-        <v/>
+        <v>ADR_ADS111X_MAX_3</v>
       </c>
       <c r="C187" t="str">
         <f>IF(AND(B187&lt;&gt;"",'Memory setup'!A171&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8771,7 +8831,7 @@
     <row r="188" spans="1:3">
       <c r="A188" t="str">
         <f>IF('Memory setup'!A171&lt;&gt;"",IF('Memory setup'!A171&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A171,"};"),"")</f>
-        <v/>
+        <v>};</v>
       </c>
       <c r="B188" t="str">
         <f>IF('Memory setup'!E171=1,'Memory setup'!B171,IF('Memory setup'!B171&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B171),""))</f>
@@ -8850,10 +8910,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCCA2C71-4C90-094A-BE8E-41D3DABF8E95}">
-  <dimension ref="A1:C187"/>
+  <dimension ref="A1:C191"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="A171" sqref="A1:XFD171"/>
+    <sheetView topLeftCell="A143" workbookViewId="0">
+      <selection activeCell="A175" sqref="A175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -9940,29 +10000,29 @@
     <row r="81" spans="1:3">
       <c r="A81" t="str">
         <f>IF('Memory setup'!A77&lt;&gt;"",IF('Memory setup'!A77&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A77,"};"),"")</f>
-        <v>// AXIS2</v>
+        <v/>
       </c>
       <c r="B81" t="str">
         <f>IF('Memory setup'!F77=1,'Memory setup'!B77,IF('Memory setup'!B77&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B77),""))</f>
-        <v/>
+        <v>ADR_TMC1_TRQ_FILT</v>
       </c>
       <c r="C81" t="str">
         <f>IF(AND(B81&lt;&gt;"",'Memory setup'!A78&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v/>
+        <v>,</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" t="str">
         <f>IF('Memory setup'!A78&lt;&gt;"",IF('Memory setup'!A78&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A78,"};"),"")</f>
-        <v/>
+        <v>// AXIS2</v>
       </c>
       <c r="B82" t="str">
         <f>IF('Memory setup'!F78=1,'Memory setup'!B78,IF('Memory setup'!B78&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B78),""))</f>
-        <v>ADR_AXIS2_CONFIG</v>
+        <v/>
       </c>
       <c r="C82" t="str">
         <f>IF(AND(B82&lt;&gt;"",'Memory setup'!A79&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v>,</v>
+        <v/>
       </c>
     </row>
     <row r="83" spans="1:3">
@@ -9972,7 +10032,7 @@
       </c>
       <c r="B83" t="str">
         <f>IF('Memory setup'!F79=1,'Memory setup'!B79,IF('Memory setup'!B79&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B79),""))</f>
-        <v>ADR_AXIS2_POWER</v>
+        <v>ADR_AXIS2_CONFIG</v>
       </c>
       <c r="C83" t="str">
         <f>IF(AND(B83&lt;&gt;"",'Memory setup'!A80&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -9986,7 +10046,7 @@
       </c>
       <c r="B84" t="str">
         <f>IF('Memory setup'!F80=1,'Memory setup'!B80,IF('Memory setup'!B80&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B80),""))</f>
-        <v>ADR_AXIS2_DEGREES</v>
+        <v>ADR_AXIS2_POWER</v>
       </c>
       <c r="C84" t="str">
         <f>IF(AND(B84&lt;&gt;"",'Memory setup'!A81&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10000,7 +10060,7 @@
       </c>
       <c r="B85" t="str">
         <f>IF('Memory setup'!F81=1,'Memory setup'!B81,IF('Memory setup'!B81&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B81),""))</f>
-        <v>ADR_AXIS2_MAX_SPEED</v>
+        <v>ADR_AXIS2_DEGREES</v>
       </c>
       <c r="C85" t="str">
         <f>IF(AND(B85&lt;&gt;"",'Memory setup'!A82&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10014,7 +10074,7 @@
       </c>
       <c r="B86" t="str">
         <f>IF('Memory setup'!F82=1,'Memory setup'!B82,IF('Memory setup'!B82&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B82),""))</f>
-        <v>ADR_AXIS2_MAX_ACCEL</v>
+        <v>ADR_AXIS2_MAX_SPEED</v>
       </c>
       <c r="C86" t="str">
         <f>IF(AND(B86&lt;&gt;"",'Memory setup'!A83&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10028,7 +10088,7 @@
       </c>
       <c r="B87" t="str">
         <f>IF('Memory setup'!F83=1,'Memory setup'!B83,IF('Memory setup'!B83&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B83),""))</f>
-        <v>ADR_AXIS2_ENDSTOP</v>
+        <v>ADR_AXIS2_MAX_ACCEL</v>
       </c>
       <c r="C87" t="str">
         <f>IF(AND(B87&lt;&gt;"",'Memory setup'!A84&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10042,7 +10102,7 @@
       </c>
       <c r="B88" t="str">
         <f>IF('Memory setup'!F84=1,'Memory setup'!B84,IF('Memory setup'!B84&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B84),""))</f>
-        <v>ADR_AXIS2_EFFECTS1</v>
+        <v>ADR_AXIS2_ENDSTOP</v>
       </c>
       <c r="C88" t="str">
         <f>IF(AND(B88&lt;&gt;"",'Memory setup'!A85&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10056,7 +10116,7 @@
       </c>
       <c r="B89" t="str">
         <f>IF('Memory setup'!F85=1,'Memory setup'!B85,IF('Memory setup'!B85&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B85),""))</f>
-        <v>ADR_AXIS2_SPEEDACCEL_FILTER</v>
+        <v>ADR_AXIS2_EFFECTS1</v>
       </c>
       <c r="C89" t="str">
         <f>IF(AND(B89&lt;&gt;"",'Memory setup'!A86&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10070,7 +10130,7 @@
       </c>
       <c r="B90" t="str">
         <f>IF('Memory setup'!F86=1,'Memory setup'!B86,IF('Memory setup'!B86&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B86),""))</f>
-        <v>ADR_AXIS2_ENC_RATIO</v>
+        <v>ADR_AXIS2_SPEEDACCEL_FILTER</v>
       </c>
       <c r="C90" t="str">
         <f>IF(AND(B90&lt;&gt;"",'Memory setup'!A87&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10080,29 +10140,29 @@
     <row r="91" spans="1:3">
       <c r="A91" t="str">
         <f>IF('Memory setup'!A87&lt;&gt;"",IF('Memory setup'!A87&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A87,"};"),"")</f>
-        <v>// TMC2</v>
+        <v/>
       </c>
       <c r="B91" t="str">
         <f>IF('Memory setup'!F87=1,'Memory setup'!B87,IF('Memory setup'!B87&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B87),""))</f>
-        <v/>
+        <v>ADR_AXIS2_ENC_RATIO</v>
       </c>
       <c r="C91" t="str">
         <f>IF(AND(B91&lt;&gt;"",'Memory setup'!A88&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v/>
+        <v>,</v>
       </c>
     </row>
     <row r="92" spans="1:3">
       <c r="A92" t="str">
         <f>IF('Memory setup'!A88&lt;&gt;"",IF('Memory setup'!A88&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A88,"};"),"")</f>
-        <v/>
+        <v>// TMC2</v>
       </c>
       <c r="B92" t="str">
         <f>IF('Memory setup'!F88=1,'Memory setup'!B88,IF('Memory setup'!B88&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B88),""))</f>
-        <v>ADR_TMC2_MOTCONF</v>
+        <v/>
       </c>
       <c r="C92" t="str">
         <f>IF(AND(B92&lt;&gt;"",'Memory setup'!A89&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v>,</v>
+        <v/>
       </c>
     </row>
     <row r="93" spans="1:3">
@@ -10112,7 +10172,7 @@
       </c>
       <c r="B93" t="str">
         <f>IF('Memory setup'!F89=1,'Memory setup'!B89,IF('Memory setup'!B89&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B89),""))</f>
-        <v>ADR_TMC2_CPR</v>
+        <v>ADR_TMC2_MOTCONF</v>
       </c>
       <c r="C93" t="str">
         <f>IF(AND(B93&lt;&gt;"",'Memory setup'!A90&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10126,7 +10186,7 @@
       </c>
       <c r="B94" t="str">
         <f>IF('Memory setup'!F90=1,'Memory setup'!B90,IF('Memory setup'!B90&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B90),""))</f>
-        <v>ADR_TMC2_ENCA</v>
+        <v>ADR_TMC2_CPR</v>
       </c>
       <c r="C94" t="str">
         <f>IF(AND(B94&lt;&gt;"",'Memory setup'!A91&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10140,7 +10200,7 @@
       </c>
       <c r="B95" t="str">
         <f>IF('Memory setup'!F91=1,'Memory setup'!B91,IF('Memory setup'!B91&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B91),""))</f>
-        <v>//ADR_TMC2_ADC_I0_OFS</v>
+        <v>ADR_TMC2_ENCA</v>
       </c>
       <c r="C95" t="str">
         <f>IF(AND(B95&lt;&gt;"",'Memory setup'!A92&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10154,7 +10214,7 @@
       </c>
       <c r="B96" t="str">
         <f>IF('Memory setup'!F92=1,'Memory setup'!B92,IF('Memory setup'!B92&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B92),""))</f>
-        <v>//ADR_TMC2_ADC_I1_OFS</v>
+        <v>//ADR_TMC2_ADC_I0_OFS</v>
       </c>
       <c r="C96" t="str">
         <f>IF(AND(B96&lt;&gt;"",'Memory setup'!A93&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10168,7 +10228,7 @@
       </c>
       <c r="B97" t="str">
         <f>IF('Memory setup'!F93=1,'Memory setup'!B93,IF('Memory setup'!B93&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B93),""))</f>
-        <v>//ADR_TMC2_ENC_OFFSET</v>
+        <v>//ADR_TMC2_ADC_I1_OFS</v>
       </c>
       <c r="C97" t="str">
         <f>IF(AND(B97&lt;&gt;"",'Memory setup'!A94&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10182,7 +10242,7 @@
       </c>
       <c r="B98" t="str">
         <f>IF('Memory setup'!F94=1,'Memory setup'!B94,IF('Memory setup'!B94&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B94),""))</f>
-        <v>ADR_TMC2_OFFSETFLUX</v>
+        <v>//ADR_TMC2_ENC_OFFSET</v>
       </c>
       <c r="C98" t="str">
         <f>IF(AND(B98&lt;&gt;"",'Memory setup'!A95&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10196,7 +10256,7 @@
       </c>
       <c r="B99" t="str">
         <f>IF('Memory setup'!F95=1,'Memory setup'!B95,IF('Memory setup'!B95&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B95),""))</f>
-        <v>ADR_TMC2_TORQUE_P</v>
+        <v>ADR_TMC2_OFFSETFLUX</v>
       </c>
       <c r="C99" t="str">
         <f>IF(AND(B99&lt;&gt;"",'Memory setup'!A96&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10210,7 +10270,7 @@
       </c>
       <c r="B100" t="str">
         <f>IF('Memory setup'!F96=1,'Memory setup'!B96,IF('Memory setup'!B96&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B96),""))</f>
-        <v>ADR_TMC2_TORQUE_I</v>
+        <v>ADR_TMC2_TORQUE_P</v>
       </c>
       <c r="C100" t="str">
         <f>IF(AND(B100&lt;&gt;"",'Memory setup'!A97&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10224,7 +10284,7 @@
       </c>
       <c r="B101" t="str">
         <f>IF('Memory setup'!F97=1,'Memory setup'!B97,IF('Memory setup'!B97&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B97),""))</f>
-        <v>ADR_TMC2_FLUX_P</v>
+        <v>ADR_TMC2_TORQUE_I</v>
       </c>
       <c r="C101" t="str">
         <f>IF(AND(B101&lt;&gt;"",'Memory setup'!A98&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10238,7 +10298,7 @@
       </c>
       <c r="B102" t="str">
         <f>IF('Memory setup'!F98=1,'Memory setup'!B98,IF('Memory setup'!B98&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B98),""))</f>
-        <v>ADR_TMC2_FLUX_I</v>
+        <v>ADR_TMC2_FLUX_P</v>
       </c>
       <c r="C102" t="str">
         <f>IF(AND(B102&lt;&gt;"",'Memory setup'!A99&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10252,7 +10312,7 @@
       </c>
       <c r="B103" t="str">
         <f>IF('Memory setup'!F99=1,'Memory setup'!B99,IF('Memory setup'!B99&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B99),""))</f>
-        <v>//ADR_TMC2_PHIE_OFS</v>
+        <v>ADR_TMC2_FLUX_I</v>
       </c>
       <c r="C103" t="str">
         <f>IF(AND(B103&lt;&gt;"",'Memory setup'!A100&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10262,15 +10322,15 @@
     <row r="104" spans="1:3">
       <c r="A104" t="str">
         <f>IF('Memory setup'!A100&lt;&gt;"",IF('Memory setup'!A100&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A100,"};"),"")</f>
-        <v>// AXIS3</v>
+        <v/>
       </c>
       <c r="B104" t="str">
         <f>IF('Memory setup'!F100=1,'Memory setup'!B100,IF('Memory setup'!B100&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B100),""))</f>
-        <v/>
+        <v>//ADR_TMC2_PHIE_OFS</v>
       </c>
       <c r="C104" t="str">
         <f>IF(AND(B104&lt;&gt;"",'Memory setup'!A101&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v/>
+        <v>,</v>
       </c>
     </row>
     <row r="105" spans="1:3">
@@ -10280,7 +10340,7 @@
       </c>
       <c r="B105" t="str">
         <f>IF('Memory setup'!F101=1,'Memory setup'!B101,IF('Memory setup'!B101&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B101),""))</f>
-        <v>ADR_AXIS3_CONFIG</v>
+        <v>ADR_TMC2_TRQ_FILT</v>
       </c>
       <c r="C105" t="str">
         <f>IF(AND(B105&lt;&gt;"",'Memory setup'!A102&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10290,15 +10350,15 @@
     <row r="106" spans="1:3">
       <c r="A106" t="str">
         <f>IF('Memory setup'!A102&lt;&gt;"",IF('Memory setup'!A102&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A102,"};"),"")</f>
-        <v/>
+        <v>// AXIS3</v>
       </c>
       <c r="B106" t="str">
         <f>IF('Memory setup'!F102=1,'Memory setup'!B102,IF('Memory setup'!B102&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B102),""))</f>
-        <v>ADR_AXIS3_POWER</v>
+        <v/>
       </c>
       <c r="C106" t="str">
         <f>IF(AND(B106&lt;&gt;"",'Memory setup'!A103&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v>,</v>
+        <v/>
       </c>
     </row>
     <row r="107" spans="1:3">
@@ -10308,7 +10368,7 @@
       </c>
       <c r="B107" t="str">
         <f>IF('Memory setup'!F103=1,'Memory setup'!B103,IF('Memory setup'!B103&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B103),""))</f>
-        <v>ADR_AXIS3_DEGREES</v>
+        <v>ADR_AXIS3_CONFIG</v>
       </c>
       <c r="C107" t="str">
         <f>IF(AND(B107&lt;&gt;"",'Memory setup'!A104&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10322,7 +10382,7 @@
       </c>
       <c r="B108" t="str">
         <f>IF('Memory setup'!F104=1,'Memory setup'!B104,IF('Memory setup'!B104&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B104),""))</f>
-        <v>ADR_AXIS3_MAX_SPEED</v>
+        <v>ADR_AXIS3_POWER</v>
       </c>
       <c r="C108" t="str">
         <f>IF(AND(B108&lt;&gt;"",'Memory setup'!A105&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10336,7 +10396,7 @@
       </c>
       <c r="B109" t="str">
         <f>IF('Memory setup'!F105=1,'Memory setup'!B105,IF('Memory setup'!B105&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B105),""))</f>
-        <v>ADR_AXIS3_MAX_ACCEL</v>
+        <v>ADR_AXIS3_DEGREES</v>
       </c>
       <c r="C109" t="str">
         <f>IF(AND(B109&lt;&gt;"",'Memory setup'!A106&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10350,7 +10410,7 @@
       </c>
       <c r="B110" t="str">
         <f>IF('Memory setup'!F106=1,'Memory setup'!B106,IF('Memory setup'!B106&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B106),""))</f>
-        <v>ADR_AXIS3_ENDSTOP</v>
+        <v>ADR_AXIS3_MAX_SPEED</v>
       </c>
       <c r="C110" t="str">
         <f>IF(AND(B110&lt;&gt;"",'Memory setup'!A107&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10364,7 +10424,7 @@
       </c>
       <c r="B111" t="str">
         <f>IF('Memory setup'!F107=1,'Memory setup'!B107,IF('Memory setup'!B107&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B107),""))</f>
-        <v>ADR_AXIS3_EFFECTS1</v>
+        <v>ADR_AXIS3_MAX_ACCEL</v>
       </c>
       <c r="C111" t="str">
         <f>IF(AND(B111&lt;&gt;"",'Memory setup'!A108&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10378,7 +10438,7 @@
       </c>
       <c r="B112" t="str">
         <f>IF('Memory setup'!F108=1,'Memory setup'!B108,IF('Memory setup'!B108&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B108),""))</f>
-        <v>ADR_AXIS3_SPEEDACCEL_FILTER</v>
+        <v>ADR_AXIS3_ENDSTOP</v>
       </c>
       <c r="C112" t="str">
         <f>IF(AND(B112&lt;&gt;"",'Memory setup'!A109&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10392,7 +10452,7 @@
       </c>
       <c r="B113" t="str">
         <f>IF('Memory setup'!F109=1,'Memory setup'!B109,IF('Memory setup'!B109&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B109),""))</f>
-        <v>ADR_AXIS3_ENC_RATIO</v>
+        <v>ADR_AXIS3_EFFECTS1</v>
       </c>
       <c r="C113" t="str">
         <f>IF(AND(B113&lt;&gt;"",'Memory setup'!A110&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10402,15 +10462,15 @@
     <row r="114" spans="1:3">
       <c r="A114" t="str">
         <f>IF('Memory setup'!A110&lt;&gt;"",IF('Memory setup'!A110&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A110,"};"),"")</f>
-        <v>// TMC3</v>
+        <v/>
       </c>
       <c r="B114" t="str">
         <f>IF('Memory setup'!F110=1,'Memory setup'!B110,IF('Memory setup'!B110&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B110),""))</f>
-        <v/>
+        <v>ADR_AXIS3_SPEEDACCEL_FILTER</v>
       </c>
       <c r="C114" t="str">
         <f>IF(AND(B114&lt;&gt;"",'Memory setup'!A111&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v/>
+        <v>,</v>
       </c>
     </row>
     <row r="115" spans="1:3">
@@ -10420,7 +10480,7 @@
       </c>
       <c r="B115" t="str">
         <f>IF('Memory setup'!F111=1,'Memory setup'!B111,IF('Memory setup'!B111&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B111),""))</f>
-        <v>ADR_TMC3_MOTCONF</v>
+        <v>ADR_AXIS3_ENC_RATIO</v>
       </c>
       <c r="C115" t="str">
         <f>IF(AND(B115&lt;&gt;"",'Memory setup'!A112&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10430,15 +10490,15 @@
     <row r="116" spans="1:3">
       <c r="A116" t="str">
         <f>IF('Memory setup'!A112&lt;&gt;"",IF('Memory setup'!A112&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A112,"};"),"")</f>
-        <v/>
+        <v>// TMC3</v>
       </c>
       <c r="B116" t="str">
         <f>IF('Memory setup'!F112=1,'Memory setup'!B112,IF('Memory setup'!B112&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B112),""))</f>
-        <v>ADR_TMC3_CPR</v>
+        <v/>
       </c>
       <c r="C116" t="str">
         <f>IF(AND(B116&lt;&gt;"",'Memory setup'!A113&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v>,</v>
+        <v/>
       </c>
     </row>
     <row r="117" spans="1:3">
@@ -10448,7 +10508,7 @@
       </c>
       <c r="B117" t="str">
         <f>IF('Memory setup'!F113=1,'Memory setup'!B113,IF('Memory setup'!B113&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B113),""))</f>
-        <v>ADR_TMC3_ENCA</v>
+        <v>ADR_TMC3_MOTCONF</v>
       </c>
       <c r="C117" t="str">
         <f>IF(AND(B117&lt;&gt;"",'Memory setup'!A114&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10462,7 +10522,7 @@
       </c>
       <c r="B118" t="str">
         <f>IF('Memory setup'!F114=1,'Memory setup'!B114,IF('Memory setup'!B114&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B114),""))</f>
-        <v>//ADR_TMC3_ADC_I0_OFS</v>
+        <v>ADR_TMC3_CPR</v>
       </c>
       <c r="C118" t="str">
         <f>IF(AND(B118&lt;&gt;"",'Memory setup'!A115&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10476,7 +10536,7 @@
       </c>
       <c r="B119" t="str">
         <f>IF('Memory setup'!F115=1,'Memory setup'!B115,IF('Memory setup'!B115&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B115),""))</f>
-        <v>//ADR_TMC3_ADC_I1_OFS</v>
+        <v>ADR_TMC3_ENCA</v>
       </c>
       <c r="C119" t="str">
         <f>IF(AND(B119&lt;&gt;"",'Memory setup'!A116&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10490,7 +10550,7 @@
       </c>
       <c r="B120" t="str">
         <f>IF('Memory setup'!F116=1,'Memory setup'!B116,IF('Memory setup'!B116&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B116),""))</f>
-        <v>//ADR_TMC3_ENC_OFFSET</v>
+        <v>//ADR_TMC3_ADC_I0_OFS</v>
       </c>
       <c r="C120" t="str">
         <f>IF(AND(B120&lt;&gt;"",'Memory setup'!A117&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10504,7 +10564,7 @@
       </c>
       <c r="B121" t="str">
         <f>IF('Memory setup'!F117=1,'Memory setup'!B117,IF('Memory setup'!B117&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B117),""))</f>
-        <v>ADR_TMC3_OFFSETFLUX</v>
+        <v>//ADR_TMC3_ADC_I1_OFS</v>
       </c>
       <c r="C121" t="str">
         <f>IF(AND(B121&lt;&gt;"",'Memory setup'!A118&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10518,7 +10578,7 @@
       </c>
       <c r="B122" t="str">
         <f>IF('Memory setup'!F118=1,'Memory setup'!B118,IF('Memory setup'!B118&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B118),""))</f>
-        <v>ADR_TMC3_TORQUE_P</v>
+        <v>//ADR_TMC3_ENC_OFFSET</v>
       </c>
       <c r="C122" t="str">
         <f>IF(AND(B122&lt;&gt;"",'Memory setup'!A119&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10532,7 +10592,7 @@
       </c>
       <c r="B123" t="str">
         <f>IF('Memory setup'!F119=1,'Memory setup'!B119,IF('Memory setup'!B119&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B119),""))</f>
-        <v>ADR_TMC3_TORQUE_I</v>
+        <v>ADR_TMC3_OFFSETFLUX</v>
       </c>
       <c r="C123" t="str">
         <f>IF(AND(B123&lt;&gt;"",'Memory setup'!A120&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10546,7 +10606,7 @@
       </c>
       <c r="B124" t="str">
         <f>IF('Memory setup'!F120=1,'Memory setup'!B120,IF('Memory setup'!B120&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B120),""))</f>
-        <v>ADR_TMC3_FLUX_P</v>
+        <v>ADR_TMC3_TORQUE_P</v>
       </c>
       <c r="C124" t="str">
         <f>IF(AND(B124&lt;&gt;"",'Memory setup'!A121&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10560,7 +10620,7 @@
       </c>
       <c r="B125" t="str">
         <f>IF('Memory setup'!F121=1,'Memory setup'!B121,IF('Memory setup'!B121&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B121),""))</f>
-        <v>ADR_TMC3_FLUX_I</v>
+        <v>ADR_TMC3_TORQUE_I</v>
       </c>
       <c r="C125" t="str">
         <f>IF(AND(B125&lt;&gt;"",'Memory setup'!A122&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10574,7 +10634,7 @@
       </c>
       <c r="B126" t="str">
         <f>IF('Memory setup'!F122=1,'Memory setup'!B122,IF('Memory setup'!B122&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B122),""))</f>
-        <v>//ADR_TMC3_PHIE_OFS</v>
+        <v>ADR_TMC3_FLUX_P</v>
       </c>
       <c r="C126" t="str">
         <f>IF(AND(B126&lt;&gt;"",'Memory setup'!A123&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10584,15 +10644,15 @@
     <row r="127" spans="1:3">
       <c r="A127" t="str">
         <f>IF('Memory setup'!A123&lt;&gt;"",IF('Memory setup'!A123&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A123,"};"),"")</f>
-        <v>// Odrive</v>
+        <v/>
       </c>
       <c r="B127" t="str">
         <f>IF('Memory setup'!F123=1,'Memory setup'!B123,IF('Memory setup'!B123&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B123),""))</f>
-        <v/>
+        <v>ADR_TMC3_FLUX_I</v>
       </c>
       <c r="C127" t="str">
         <f>IF(AND(B127&lt;&gt;"",'Memory setup'!A124&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v/>
+        <v>,</v>
       </c>
     </row>
     <row r="128" spans="1:3">
@@ -10602,7 +10662,7 @@
       </c>
       <c r="B128" t="str">
         <f>IF('Memory setup'!F124=1,'Memory setup'!B124,IF('Memory setup'!B124&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B124),""))</f>
-        <v>ADR_ODRIVE_CANID</v>
+        <v>//ADR_TMC3_PHIE_OFS</v>
       </c>
       <c r="C128" t="str">
         <f>IF(AND(B128&lt;&gt;"",'Memory setup'!A125&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10616,7 +10676,7 @@
       </c>
       <c r="B129" t="str">
         <f>IF('Memory setup'!F125=1,'Memory setup'!B125,IF('Memory setup'!B125&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B125),""))</f>
-        <v>ADR_ODRIVE_SETTING1_M0</v>
+        <v>ADR_TMC3_TRQ_FILT</v>
       </c>
       <c r="C129" t="str">
         <f>IF(AND(B129&lt;&gt;"",'Memory setup'!A126&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10626,29 +10686,29 @@
     <row r="130" spans="1:3">
       <c r="A130" t="str">
         <f>IF('Memory setup'!A126&lt;&gt;"",IF('Memory setup'!A126&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A126,"};"),"")</f>
-        <v/>
+        <v>// Odrive</v>
       </c>
       <c r="B130" t="str">
         <f>IF('Memory setup'!F126=1,'Memory setup'!B126,IF('Memory setup'!B126&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B126),""))</f>
-        <v>ADR_ODRIVE_SETTING1_M1</v>
+        <v/>
       </c>
       <c r="C130" t="str">
         <f>IF(AND(B130&lt;&gt;"",'Memory setup'!A127&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v>,</v>
+        <v/>
       </c>
     </row>
     <row r="131" spans="1:3">
       <c r="A131" t="str">
         <f>IF('Memory setup'!A127&lt;&gt;"",IF('Memory setup'!A127&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A127,"};"),"")</f>
-        <v>// VESC Section</v>
+        <v/>
       </c>
       <c r="B131" t="str">
         <f>IF('Memory setup'!F127=1,'Memory setup'!B127,IF('Memory setup'!B127&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B127),""))</f>
-        <v/>
+        <v>ADR_ODRIVE_CANID</v>
       </c>
       <c r="C131" t="str">
         <f>IF(AND(B131&lt;&gt;"",'Memory setup'!A128&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v/>
+        <v>,</v>
       </c>
     </row>
     <row r="132" spans="1:3">
@@ -10658,7 +10718,7 @@
       </c>
       <c r="B132" t="str">
         <f>IF('Memory setup'!F128=1,'Memory setup'!B128,IF('Memory setup'!B128&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B128),""))</f>
-        <v>ADR_VESC1_CANID</v>
+        <v>ADR_ODRIVE_SETTING1_M0</v>
       </c>
       <c r="C132" t="str">
         <f>IF(AND(B132&lt;&gt;"",'Memory setup'!A129&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10672,7 +10732,7 @@
       </c>
       <c r="B133" t="str">
         <f>IF('Memory setup'!F129=1,'Memory setup'!B129,IF('Memory setup'!B129&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B129),""))</f>
-        <v>ADR_VESC1_DATA</v>
+        <v>ADR_ODRIVE_SETTING1_M1</v>
       </c>
       <c r="C133" t="str">
         <f>IF(AND(B133&lt;&gt;"",'Memory setup'!A130&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10682,15 +10742,15 @@
     <row r="134" spans="1:3">
       <c r="A134" t="str">
         <f>IF('Memory setup'!A130&lt;&gt;"",IF('Memory setup'!A130&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A130,"};"),"")</f>
-        <v/>
+        <v>// VESC Section</v>
       </c>
       <c r="B134" t="str">
         <f>IF('Memory setup'!F130=1,'Memory setup'!B130,IF('Memory setup'!B130&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B130),""))</f>
-        <v>ADR_VESC1_OFFSET</v>
+        <v/>
       </c>
       <c r="C134" t="str">
         <f>IF(AND(B134&lt;&gt;"",'Memory setup'!A131&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v>,</v>
+        <v/>
       </c>
     </row>
     <row r="135" spans="1:3">
@@ -10700,7 +10760,7 @@
       </c>
       <c r="B135" t="str">
         <f>IF('Memory setup'!F131=1,'Memory setup'!B131,IF('Memory setup'!B131&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B131),""))</f>
-        <v>ADR_VESC2_CANID</v>
+        <v>ADR_VESC1_CANID</v>
       </c>
       <c r="C135" t="str">
         <f>IF(AND(B135&lt;&gt;"",'Memory setup'!A132&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10714,7 +10774,7 @@
       </c>
       <c r="B136" t="str">
         <f>IF('Memory setup'!F132=1,'Memory setup'!B132,IF('Memory setup'!B132&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B132),""))</f>
-        <v>ADR_VESC2_DATA</v>
+        <v>ADR_VESC1_DATA</v>
       </c>
       <c r="C136" t="str">
         <f>IF(AND(B136&lt;&gt;"",'Memory setup'!A133&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10728,7 +10788,7 @@
       </c>
       <c r="B137" t="str">
         <f>IF('Memory setup'!F133=1,'Memory setup'!B133,IF('Memory setup'!B133&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B133),""))</f>
-        <v>ADR_VESC2_OFFSET</v>
+        <v>ADR_VESC1_OFFSET</v>
       </c>
       <c r="C137" t="str">
         <f>IF(AND(B137&lt;&gt;"",'Memory setup'!A134&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10742,7 +10802,7 @@
       </c>
       <c r="B138" t="str">
         <f>IF('Memory setup'!F134=1,'Memory setup'!B134,IF('Memory setup'!B134&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B134),""))</f>
-        <v>ADR_VESC3_CANID</v>
+        <v>ADR_VESC2_CANID</v>
       </c>
       <c r="C138" t="str">
         <f>IF(AND(B138&lt;&gt;"",'Memory setup'!A135&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10756,7 +10816,7 @@
       </c>
       <c r="B139" t="str">
         <f>IF('Memory setup'!F135=1,'Memory setup'!B135,IF('Memory setup'!B135&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B135),""))</f>
-        <v>ADR_VESC3_DATA</v>
+        <v>ADR_VESC2_DATA</v>
       </c>
       <c r="C139" t="str">
         <f>IF(AND(B139&lt;&gt;"",'Memory setup'!A136&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10770,7 +10830,7 @@
       </c>
       <c r="B140" t="str">
         <f>IF('Memory setup'!F136=1,'Memory setup'!B136,IF('Memory setup'!B136&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B136),""))</f>
-        <v>ADR_VESC3_OFFSET</v>
+        <v>ADR_VESC2_OFFSET</v>
       </c>
       <c r="C140" t="str">
         <f>IF(AND(B140&lt;&gt;"",'Memory setup'!A137&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10780,15 +10840,15 @@
     <row r="141" spans="1:3">
       <c r="A141" t="str">
         <f>IF('Memory setup'!A137&lt;&gt;"",IF('Memory setup'!A137&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A137,"};"),"")</f>
-        <v>//MT Encoder</v>
+        <v/>
       </c>
       <c r="B141" t="str">
         <f>IF('Memory setup'!F137=1,'Memory setup'!B137,IF('Memory setup'!B137&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B137),""))</f>
-        <v/>
+        <v>ADR_VESC3_CANID</v>
       </c>
       <c r="C141" t="str">
         <f>IF(AND(B141&lt;&gt;"",'Memory setup'!A138&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v/>
+        <v>,</v>
       </c>
     </row>
     <row r="142" spans="1:3">
@@ -10798,7 +10858,7 @@
       </c>
       <c r="B142" t="str">
         <f>IF('Memory setup'!F138=1,'Memory setup'!B138,IF('Memory setup'!B138&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B138),""))</f>
-        <v>ADR_MTENC_OFS</v>
+        <v>ADR_VESC3_DATA</v>
       </c>
       <c r="C142" t="str">
         <f>IF(AND(B142&lt;&gt;"",'Memory setup'!A139&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10812,7 +10872,7 @@
       </c>
       <c r="B143" t="str">
         <f>IF('Memory setup'!F139=1,'Memory setup'!B139,IF('Memory setup'!B139&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B139),""))</f>
-        <v>ADR_MTENC_CONF1</v>
+        <v>ADR_VESC3_OFFSET</v>
       </c>
       <c r="C143" t="str">
         <f>IF(AND(B143&lt;&gt;"",'Memory setup'!A140&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10822,7 +10882,7 @@
     <row r="144" spans="1:3">
       <c r="A144" t="str">
         <f>IF('Memory setup'!A140&lt;&gt;"",IF('Memory setup'!A140&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A140,"};"),"")</f>
-        <v>// Biss-C</v>
+        <v>//MT Encoder</v>
       </c>
       <c r="B144" t="str">
         <f>IF('Memory setup'!F140=1,'Memory setup'!B140,IF('Memory setup'!B140&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B140),""))</f>
@@ -10840,7 +10900,7 @@
       </c>
       <c r="B145" t="str">
         <f>IF('Memory setup'!F141=1,'Memory setup'!B141,IF('Memory setup'!B141&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B141),""))</f>
-        <v>ADR_BISSENC_CONF1</v>
+        <v>ADR_MTENC_OFS</v>
       </c>
       <c r="C145" t="str">
         <f>IF(AND(B145&lt;&gt;"",'Memory setup'!A142&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10854,7 +10914,7 @@
       </c>
       <c r="B146" t="str">
         <f>IF('Memory setup'!F142=1,'Memory setup'!B142,IF('Memory setup'!B142&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B142),""))</f>
-        <v>ADR_BISSENC_OFS</v>
+        <v>ADR_MTENC_CONF1</v>
       </c>
       <c r="C146" t="str">
         <f>IF(AND(B146&lt;&gt;"",'Memory setup'!A143&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10864,7 +10924,7 @@
     <row r="147" spans="1:3">
       <c r="A147" t="str">
         <f>IF('Memory setup'!A143&lt;&gt;"",IF('Memory setup'!A143&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A143,"};"),"")</f>
-        <v>// Analog min/max calibrations</v>
+        <v>// Biss-C</v>
       </c>
       <c r="B147" t="str">
         <f>IF('Memory setup'!F143=1,'Memory setup'!B143,IF('Memory setup'!B143&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B143),""))</f>
@@ -10882,7 +10942,7 @@
       </c>
       <c r="B148" t="str">
         <f>IF('Memory setup'!F144=1,'Memory setup'!B144,IF('Memory setup'!B144&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B144),""))</f>
-        <v>ADR_LOCALANALOG_MIN_0</v>
+        <v>ADR_BISSENC_CONF1</v>
       </c>
       <c r="C148" t="str">
         <f>IF(AND(B148&lt;&gt;"",'Memory setup'!A145&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10896,7 +10956,7 @@
       </c>
       <c r="B149" t="str">
         <f>IF('Memory setup'!F145=1,'Memory setup'!B145,IF('Memory setup'!B145&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B145),""))</f>
-        <v>ADR_LOCALANALOG_MAX_0</v>
+        <v>ADR_BISSENC_OFS</v>
       </c>
       <c r="C149" t="str">
         <f>IF(AND(B149&lt;&gt;"",'Memory setup'!A146&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10906,15 +10966,15 @@
     <row r="150" spans="1:3">
       <c r="A150" t="str">
         <f>IF('Memory setup'!A146&lt;&gt;"",IF('Memory setup'!A146&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A146,"};"),"")</f>
-        <v/>
+        <v>// Analog min/max calibrations</v>
       </c>
       <c r="B150" t="str">
         <f>IF('Memory setup'!F146=1,'Memory setup'!B146,IF('Memory setup'!B146&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B146),""))</f>
-        <v>ADR_LOCALANALOG_MIN_1</v>
+        <v/>
       </c>
       <c r="C150" t="str">
         <f>IF(AND(B150&lt;&gt;"",'Memory setup'!A147&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v>,</v>
+        <v/>
       </c>
     </row>
     <row r="151" spans="1:3">
@@ -10924,7 +10984,7 @@
       </c>
       <c r="B151" t="str">
         <f>IF('Memory setup'!F147=1,'Memory setup'!B147,IF('Memory setup'!B147&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B147),""))</f>
-        <v>ADR_LOCALANALOG_MAX_1</v>
+        <v>ADR_LOCALANALOG_MIN_0</v>
       </c>
       <c r="C151" t="str">
         <f>IF(AND(B151&lt;&gt;"",'Memory setup'!A148&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10938,7 +10998,7 @@
       </c>
       <c r="B152" t="str">
         <f>IF('Memory setup'!F148=1,'Memory setup'!B148,IF('Memory setup'!B148&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B148),""))</f>
-        <v>ADR_LOCALANALOG_MIN_2</v>
+        <v>ADR_LOCALANALOG_MAX_0</v>
       </c>
       <c r="C152" t="str">
         <f>IF(AND(B152&lt;&gt;"",'Memory setup'!A149&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10952,7 +11012,7 @@
       </c>
       <c r="B153" t="str">
         <f>IF('Memory setup'!F149=1,'Memory setup'!B149,IF('Memory setup'!B149&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B149),""))</f>
-        <v>ADR_LOCALANALOG_MAX_2</v>
+        <v>ADR_LOCALANALOG_MIN_1</v>
       </c>
       <c r="C153" t="str">
         <f>IF(AND(B153&lt;&gt;"",'Memory setup'!A150&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10966,7 +11026,7 @@
       </c>
       <c r="B154" t="str">
         <f>IF('Memory setup'!F150=1,'Memory setup'!B150,IF('Memory setup'!B150&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B150),""))</f>
-        <v>ADR_LOCALANALOG_MIN_3</v>
+        <v>ADR_LOCALANALOG_MAX_1</v>
       </c>
       <c r="C154" t="str">
         <f>IF(AND(B154&lt;&gt;"",'Memory setup'!A151&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10980,7 +11040,7 @@
       </c>
       <c r="B155" t="str">
         <f>IF('Memory setup'!F151=1,'Memory setup'!B151,IF('Memory setup'!B151&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B151),""))</f>
-        <v>ADR_LOCALANALOG_MAX_3</v>
+        <v>ADR_LOCALANALOG_MIN_2</v>
       </c>
       <c r="C155" t="str">
         <f>IF(AND(B155&lt;&gt;"",'Memory setup'!A152&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10994,7 +11054,7 @@
       </c>
       <c r="B156" t="str">
         <f>IF('Memory setup'!F152=1,'Memory setup'!B152,IF('Memory setup'!B152&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B152),""))</f>
-        <v>ADR_LOCALANALOG_MIN_4</v>
+        <v>ADR_LOCALANALOG_MAX_2</v>
       </c>
       <c r="C156" t="str">
         <f>IF(AND(B156&lt;&gt;"",'Memory setup'!A153&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -11008,7 +11068,7 @@
       </c>
       <c r="B157" t="str">
         <f>IF('Memory setup'!F153=1,'Memory setup'!B153,IF('Memory setup'!B153&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B153),""))</f>
-        <v>ADR_LOCALANALOG_MAX_4</v>
+        <v>ADR_LOCALANALOG_MIN_3</v>
       </c>
       <c r="C157" t="str">
         <f>IF(AND(B157&lt;&gt;"",'Memory setup'!A154&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -11022,7 +11082,7 @@
       </c>
       <c r="B158" t="str">
         <f>IF('Memory setup'!F154=1,'Memory setup'!B154,IF('Memory setup'!B154&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B154),""))</f>
-        <v>ADR_LOCALANALOG_MIN_5</v>
+        <v>ADR_LOCALANALOG_MAX_3</v>
       </c>
       <c r="C158" t="str">
         <f>IF(AND(B158&lt;&gt;"",'Memory setup'!A155&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -11036,7 +11096,7 @@
       </c>
       <c r="B159" t="str">
         <f>IF('Memory setup'!F155=1,'Memory setup'!B155,IF('Memory setup'!B155&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B155),""))</f>
-        <v>ADR_LOCALANALOG_MAX_5</v>
+        <v>ADR_LOCALANALOG_MIN_4</v>
       </c>
       <c r="C159" t="str">
         <f>IF(AND(B159&lt;&gt;"",'Memory setup'!A156&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -11050,7 +11110,7 @@
       </c>
       <c r="B160" t="str">
         <f>IF('Memory setup'!F156=1,'Memory setup'!B156,IF('Memory setup'!B156&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B156),""))</f>
-        <v>ADR_LOCALANALOG_MIN_6</v>
+        <v>ADR_LOCALANALOG_MAX_4</v>
       </c>
       <c r="C160" t="str">
         <f>IF(AND(B160&lt;&gt;"",'Memory setup'!A157&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -11064,7 +11124,7 @@
       </c>
       <c r="B161" t="str">
         <f>IF('Memory setup'!F157=1,'Memory setup'!B157,IF('Memory setup'!B157&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B157),""))</f>
-        <v>ADR_LOCALANALOG_MAX_6</v>
+        <v>ADR_LOCALANALOG_MIN_5</v>
       </c>
       <c r="C161" t="str">
         <f>IF(AND(B161&lt;&gt;"",'Memory setup'!A158&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -11078,7 +11138,7 @@
       </c>
       <c r="B162" t="str">
         <f>IF('Memory setup'!F158=1,'Memory setup'!B158,IF('Memory setup'!B158&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B158),""))</f>
-        <v>ADR_LOCALANALOG_MIN_7</v>
+        <v>ADR_LOCALANALOG_MAX_5</v>
       </c>
       <c r="C162" t="str">
         <f>IF(AND(B162&lt;&gt;"",'Memory setup'!A159&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -11092,7 +11152,7 @@
       </c>
       <c r="B163" t="str">
         <f>IF('Memory setup'!F159=1,'Memory setup'!B159,IF('Memory setup'!B159&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B159),""))</f>
-        <v>ADR_LOCALANALOG_MAX_7</v>
+        <v>ADR_LOCALANALOG_MIN_6</v>
       </c>
       <c r="C163" t="str">
         <f>IF(AND(B163&lt;&gt;"",'Memory setup'!A160&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -11106,7 +11166,7 @@
       </c>
       <c r="B164" t="str">
         <f>IF('Memory setup'!F160=1,'Memory setup'!B160,IF('Memory setup'!B160&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B160),""))</f>
-        <v>ADR_ADS111X_MIN_0</v>
+        <v>ADR_LOCALANALOG_MAX_6</v>
       </c>
       <c r="C164" t="str">
         <f>IF(AND(B164&lt;&gt;"",'Memory setup'!A161&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -11120,7 +11180,7 @@
       </c>
       <c r="B165" t="str">
         <f>IF('Memory setup'!F161=1,'Memory setup'!B161,IF('Memory setup'!B161&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B161),""))</f>
-        <v>ADR_ADS111X_MAX_0</v>
+        <v>ADR_LOCALANALOG_MIN_7</v>
       </c>
       <c r="C165" t="str">
         <f>IF(AND(B165&lt;&gt;"",'Memory setup'!A162&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -11134,7 +11194,7 @@
       </c>
       <c r="B166" t="str">
         <f>IF('Memory setup'!F162=1,'Memory setup'!B162,IF('Memory setup'!B162&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B162),""))</f>
-        <v>ADR_ADS111X_MIN_1</v>
+        <v>ADR_LOCALANALOG_MAX_7</v>
       </c>
       <c r="C166" t="str">
         <f>IF(AND(B166&lt;&gt;"",'Memory setup'!A163&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -11148,7 +11208,7 @@
       </c>
       <c r="B167" t="str">
         <f>IF('Memory setup'!F163=1,'Memory setup'!B163,IF('Memory setup'!B163&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B163),""))</f>
-        <v>ADR_ADS111X_MAX_1</v>
+        <v>ADR_ADS111X_MIN_0</v>
       </c>
       <c r="C167" t="str">
         <f>IF(AND(B167&lt;&gt;"",'Memory setup'!A164&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -11162,7 +11222,7 @@
       </c>
       <c r="B168" t="str">
         <f>IF('Memory setup'!F164=1,'Memory setup'!B164,IF('Memory setup'!B164&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B164),""))</f>
-        <v>ADR_ADS111X_MIN_2</v>
+        <v>ADR_ADS111X_MAX_0</v>
       </c>
       <c r="C168" t="str">
         <f>IF(AND(B168&lt;&gt;"",'Memory setup'!A165&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -11176,7 +11236,7 @@
       </c>
       <c r="B169" t="str">
         <f>IF('Memory setup'!F165=1,'Memory setup'!B165,IF('Memory setup'!B165&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B165),""))</f>
-        <v>ADR_ADS111X_MAX_2</v>
+        <v>ADR_ADS111X_MIN_1</v>
       </c>
       <c r="C169" t="str">
         <f>IF(AND(B169&lt;&gt;"",'Memory setup'!A166&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -11190,7 +11250,7 @@
       </c>
       <c r="B170" t="str">
         <f>IF('Memory setup'!F166=1,'Memory setup'!B166,IF('Memory setup'!B166&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B166),""))</f>
-        <v>ADR_ADS111X_MIN_3</v>
+        <v>ADR_ADS111X_MAX_1</v>
       </c>
       <c r="C170" t="str">
         <f>IF(AND(B170&lt;&gt;"",'Memory setup'!A167&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -11204,25 +11264,25 @@
       </c>
       <c r="B171" t="str">
         <f>IF('Memory setup'!F167=1,'Memory setup'!B167,IF('Memory setup'!B167&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B167),""))</f>
-        <v>ADR_ADS111X_MAX_3</v>
+        <v>ADR_ADS111X_MIN_2</v>
       </c>
       <c r="C171" t="str">
         <f>IF(AND(B171&lt;&gt;"",'Memory setup'!A168&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v/>
+        <v>,</v>
       </c>
     </row>
     <row r="172" spans="1:3">
       <c r="A172" t="str">
         <f>IF('Memory setup'!A168&lt;&gt;"",IF('Memory setup'!A168&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A168,"};"),"")</f>
-        <v>};</v>
+        <v/>
       </c>
       <c r="B172" t="str">
         <f>IF('Memory setup'!F168=1,'Memory setup'!B168,IF('Memory setup'!B168&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B168),""))</f>
-        <v/>
+        <v>ADR_ADS111X_MAX_2</v>
       </c>
       <c r="C172" t="str">
         <f>IF(AND(B172&lt;&gt;"",'Memory setup'!A169&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v/>
+        <v>,</v>
       </c>
     </row>
     <row r="173" spans="1:3">
@@ -11232,11 +11292,11 @@
       </c>
       <c r="B173" t="str">
         <f>IF('Memory setup'!F169=1,'Memory setup'!B169,IF('Memory setup'!B169&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B169),""))</f>
-        <v/>
+        <v>ADR_ADS111X_MIN_3</v>
       </c>
       <c r="C173" t="str">
         <f>IF(AND(B173&lt;&gt;"",'Memory setup'!A170&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v/>
+        <v>,</v>
       </c>
     </row>
     <row r="174" spans="1:3">
@@ -11246,7 +11306,7 @@
       </c>
       <c r="B174" t="str">
         <f>IF('Memory setup'!F170=1,'Memory setup'!B170,IF('Memory setup'!B170&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B170),""))</f>
-        <v/>
+        <v>ADR_ADS111X_MAX_3</v>
       </c>
       <c r="C174" t="str">
         <f>IF(AND(B174&lt;&gt;"",'Memory setup'!A171&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -11256,7 +11316,7 @@
     <row r="175" spans="1:3">
       <c r="A175" t="str">
         <f>IF('Memory setup'!A171&lt;&gt;"",IF('Memory setup'!A171&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A171,"};"),"")</f>
-        <v/>
+        <v>};</v>
       </c>
       <c r="B175" t="str">
         <f>IF('Memory setup'!F171=1,'Memory setup'!B171,IF('Memory setup'!B171&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B171),""))</f>
@@ -11367,71 +11427,127 @@
     </row>
     <row r="183" spans="1:3">
       <c r="A183" t="str">
-        <f>IF('Memory setup'!A175&lt;&gt;"",IF('Memory setup'!A175&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A175,"};"),"")</f>
+        <f>IF('Memory setup'!A179&lt;&gt;"",IF('Memory setup'!A179&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A179,"};"),"")</f>
         <v/>
       </c>
       <c r="B183" t="str">
-        <f>IF('Memory setup'!F175=1,'Memory setup'!B175,IF('Memory setup'!B175&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B175),""))</f>
+        <f>IF('Memory setup'!F179=1,'Memory setup'!B179,IF('Memory setup'!B179&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B179),""))</f>
         <v/>
       </c>
       <c r="C183" t="str">
-        <f>IF(AND(B183&lt;&gt;"",'Memory setup'!A176&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
+        <f>IF(AND(B183&lt;&gt;"",'Memory setup'!A180&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
         <v/>
       </c>
     </row>
     <row r="184" spans="1:3">
       <c r="A184" t="str">
-        <f>IF('Memory setup'!A176&lt;&gt;"",IF('Memory setup'!A176&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A176,"};"),"")</f>
+        <f>IF('Memory setup'!A180&lt;&gt;"",IF('Memory setup'!A180&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A180,"};"),"")</f>
         <v/>
       </c>
       <c r="B184" t="str">
-        <f>IF('Memory setup'!F176=1,'Memory setup'!B176,IF('Memory setup'!B176&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B176),""))</f>
+        <f>IF('Memory setup'!F180=1,'Memory setup'!B180,IF('Memory setup'!B180&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B180),""))</f>
         <v/>
       </c>
       <c r="C184" t="str">
-        <f>IF(AND(B184&lt;&gt;"",'Memory setup'!A177&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
+        <f>IF(AND(B184&lt;&gt;"",'Memory setup'!A181&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
         <v/>
       </c>
     </row>
     <row r="185" spans="1:3">
       <c r="A185" t="str">
-        <f>IF('Memory setup'!A177&lt;&gt;"",IF('Memory setup'!A177&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A177,"};"),"")</f>
+        <f>IF('Memory setup'!A181&lt;&gt;"",IF('Memory setup'!A181&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A181,"};"),"")</f>
         <v/>
       </c>
       <c r="B185" t="str">
-        <f>IF('Memory setup'!F177=1,'Memory setup'!B177,IF('Memory setup'!B177&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B177),""))</f>
+        <f>IF('Memory setup'!F181=1,'Memory setup'!B181,IF('Memory setup'!B181&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B181),""))</f>
         <v/>
       </c>
       <c r="C185" t="str">
-        <f>IF(AND(B185&lt;&gt;"",'Memory setup'!A178&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
+        <f>IF(AND(B185&lt;&gt;"",'Memory setup'!A182&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
         <v/>
       </c>
     </row>
     <row r="186" spans="1:3">
       <c r="A186" t="str">
-        <f>IF('Memory setup'!A178&lt;&gt;"",IF('Memory setup'!A178&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A178,"};"),"")</f>
+        <f>IF('Memory setup'!A182&lt;&gt;"",IF('Memory setup'!A182&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A182,"};"),"")</f>
         <v/>
       </c>
       <c r="B186" t="str">
-        <f>IF('Memory setup'!F178=1,'Memory setup'!B178,IF('Memory setup'!B178&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B178),""))</f>
+        <f>IF('Memory setup'!F182=1,'Memory setup'!B182,IF('Memory setup'!B182&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B182),""))</f>
         <v/>
       </c>
       <c r="C186" t="str">
-        <f>IF(AND(B186&lt;&gt;"",'Memory setup'!A179&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
+        <f>IF(AND(B186&lt;&gt;"",'Memory setup'!A183&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
         <v/>
       </c>
     </row>
     <row r="187" spans="1:3">
       <c r="A187" t="str">
-        <f>IF('Memory setup'!A179&lt;&gt;"",IF('Memory setup'!A179&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A179,"};"),"")</f>
+        <f>IF('Memory setup'!A183&lt;&gt;"",IF('Memory setup'!A183&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A183,"};"),"")</f>
         <v/>
       </c>
       <c r="B187" t="str">
-        <f>IF('Memory setup'!F179=1,'Memory setup'!B179,IF('Memory setup'!B179&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B179),""))</f>
+        <f>IF('Memory setup'!F183=1,'Memory setup'!B183,IF('Memory setup'!B183&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B183),""))</f>
         <v/>
       </c>
       <c r="C187" t="str">
-        <f>IF(AND(B187&lt;&gt;"",'Memory setup'!A180&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
+        <f>IF(AND(B187&lt;&gt;"",'Memory setup'!A184&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="188" spans="1:3">
+      <c r="A188" t="str">
+        <f>IF('Memory setup'!A184&lt;&gt;"",IF('Memory setup'!A184&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A184,"};"),"")</f>
+        <v/>
+      </c>
+      <c r="B188" t="str">
+        <f>IF('Memory setup'!F184=1,'Memory setup'!B184,IF('Memory setup'!B184&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B184),""))</f>
+        <v/>
+      </c>
+      <c r="C188" t="str">
+        <f>IF(AND(B188&lt;&gt;"",'Memory setup'!A185&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="189" spans="1:3">
+      <c r="A189" t="str">
+        <f>IF('Memory setup'!A185&lt;&gt;"",IF('Memory setup'!A185&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A185,"};"),"")</f>
+        <v/>
+      </c>
+      <c r="B189" t="str">
+        <f>IF('Memory setup'!F185=1,'Memory setup'!B185,IF('Memory setup'!B185&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B185),""))</f>
+        <v/>
+      </c>
+      <c r="C189" t="str">
+        <f>IF(AND(B189&lt;&gt;"",'Memory setup'!A186&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="190" spans="1:3">
+      <c r="A190" t="str">
+        <f>IF('Memory setup'!A186&lt;&gt;"",IF('Memory setup'!A186&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A186,"};"),"")</f>
+        <v/>
+      </c>
+      <c r="B190" t="str">
+        <f>IF('Memory setup'!F186=1,'Memory setup'!B186,IF('Memory setup'!B186&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B186),""))</f>
+        <v/>
+      </c>
+      <c r="C190" t="str">
+        <f>IF(AND(B190&lt;&gt;"",'Memory setup'!A187&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="191" spans="1:3">
+      <c r="A191" t="str">
+        <f>IF('Memory setup'!A187&lt;&gt;"",IF('Memory setup'!A187&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A187,"};"),"")</f>
+        <v/>
+      </c>
+      <c r="B191" t="str">
+        <f>IF('Memory setup'!F187=1,'Memory setup'!B187,IF('Memory setup'!B187&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B187),""))</f>
+        <v/>
+      </c>
+      <c r="C191" t="str">
+        <f>IF(AND(B191&lt;&gt;"",'Memory setup'!A188&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
TMC4671 Internal Biquad for torque (#80)
* Created TMC4671Biquad class

* Added TMC filter commands

* Added tmc memory for filter

* Configurator update
</commit_message>
<xml_diff>
--- a/Firmware/memory_map.xlsx
+++ b/Firmware/memory_map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ST\OpenFFBoard\Firmware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D360BDE6-347F-42FD-92E7-DF81C4ABC881}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06A5C4BF-F00F-4A83-8D1C-194AF4026273}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12750" yWindow="4575" windowWidth="28800" windowHeight="15435" xr2:uid="{4859EFD2-ECA4-5640-B170-200D9DB85F48}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{4859EFD2-ECA4-5640-B170-200D9DB85F48}"/>
   </bookViews>
   <sheets>
     <sheet name="Memory setup" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="369">
   <si>
     <t>// Ports</t>
   </si>
@@ -1603,6 +1603,24 @@
   </si>
   <si>
     <t>ADR_FLASH_VERSION</t>
+  </si>
+  <si>
+    <t>ADR_TMC1_TRQ_FILT</t>
+  </si>
+  <si>
+    <t>0x32C</t>
+  </si>
+  <si>
+    <t>ADR_TMC2_TRQ_FILT</t>
+  </si>
+  <si>
+    <t>0x36C</t>
+  </si>
+  <si>
+    <t>0x3AC</t>
+  </si>
+  <si>
+    <t>ADR_TMC3_TRQ_FILT</t>
   </si>
 </sst>
 </file>
@@ -2113,10 +2131,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C5323F2-8FDE-7443-A989-42E1FE5B01C7}">
-  <dimension ref="A1:G168"/>
+  <dimension ref="A1:G171"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView topLeftCell="A137" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A172" sqref="A172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -3094,33 +3112,33 @@
       </c>
     </row>
     <row r="77" spans="1:6">
-      <c r="A77" s="1" t="s">
+      <c r="B77" s="9" t="s">
+        <v>363</v>
+      </c>
+      <c r="C77" s="11" t="s">
+        <v>364</v>
+      </c>
+      <c r="E77" s="23">
+        <v>1</v>
+      </c>
+      <c r="F77" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6">
+      <c r="A78" s="1" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6">
-      <c r="B78" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="C78" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="D78" s="12" t="s">
-        <v>243</v>
-      </c>
-      <c r="E78" s="15">
-        <v>1</v>
-      </c>
-      <c r="F78" s="15">
-        <v>1</v>
       </c>
     </row>
     <row r="79" spans="1:6">
       <c r="B79" s="9" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C79" s="11" t="s">
-        <v>130</v>
+        <v>128</v>
+      </c>
+      <c r="D79" s="12" t="s">
+        <v>243</v>
       </c>
       <c r="E79" s="15">
         <v>1</v>
@@ -3131,10 +3149,10 @@
     </row>
     <row r="80" spans="1:6">
       <c r="B80" s="9" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C80" s="11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E80" s="15">
         <v>1</v>
@@ -3145,13 +3163,10 @@
     </row>
     <row r="81" spans="1:6">
       <c r="B81" s="9" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C81" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="D81" s="12" t="s">
-        <v>244</v>
+        <v>132</v>
       </c>
       <c r="E81" s="15">
         <v>1</v>
@@ -3162,13 +3177,13 @@
     </row>
     <row r="82" spans="1:6">
       <c r="B82" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C82" s="11" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D82" s="12" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E82" s="15">
         <v>1</v>
@@ -3179,13 +3194,13 @@
     </row>
     <row r="83" spans="1:6">
       <c r="B83" s="9" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C83" s="11" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D83" s="12" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E83" s="15">
         <v>1</v>
@@ -3196,13 +3211,13 @@
     </row>
     <row r="84" spans="1:6">
       <c r="B84" s="9" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C84" s="11" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D84" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E84" s="15">
         <v>1</v>
@@ -3213,13 +3228,13 @@
     </row>
     <row r="85" spans="1:6">
       <c r="B85" s="9" t="s">
-        <v>310</v>
+        <v>139</v>
       </c>
       <c r="C85" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="D85" s="24" t="s">
-        <v>309</v>
+        <v>140</v>
+      </c>
+      <c r="D85" s="12" t="s">
+        <v>247</v>
       </c>
       <c r="E85" s="15">
         <v>1</v>
@@ -3230,49 +3245,52 @@
     </row>
     <row r="86" spans="1:6">
       <c r="B86" s="9" t="s">
+        <v>310</v>
+      </c>
+      <c r="C86" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="D86" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="E86" s="15">
+        <v>1</v>
+      </c>
+      <c r="F86" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6">
+      <c r="B87" s="9" t="s">
         <v>306</v>
       </c>
-      <c r="C86" s="11" t="s">
+      <c r="C87" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="D86" s="12" t="s">
+      <c r="D87" s="12" t="s">
         <v>305</v>
       </c>
-      <c r="E86" s="15">
-        <v>1</v>
-      </c>
-      <c r="F86" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6">
-      <c r="A87" s="1" t="s">
+      <c r="E87" s="15">
+        <v>1</v>
+      </c>
+      <c r="F87" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6">
+      <c r="A88" s="1" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6">
-      <c r="B88" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="C88" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="D88" s="12" t="s">
-        <v>249</v>
-      </c>
-      <c r="E88" s="15">
-        <v>1</v>
-      </c>
-      <c r="F88" s="15">
-        <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:6">
       <c r="B89" s="9" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C89" s="11" t="s">
-        <v>146</v>
+        <v>144</v>
+      </c>
+      <c r="D89" s="12" t="s">
+        <v>249</v>
       </c>
       <c r="E89" s="15">
         <v>1</v>
@@ -3283,13 +3301,10 @@
     </row>
     <row r="90" spans="1:6">
       <c r="B90" s="9" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C90" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="D90" s="12" t="s">
-        <v>250</v>
+        <v>146</v>
       </c>
       <c r="E90" s="15">
         <v>1</v>
@@ -3300,21 +3315,27 @@
     </row>
     <row r="91" spans="1:6">
       <c r="B91" s="9" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C91" s="11" t="s">
-        <v>150</v>
+        <v>148</v>
+      </c>
+      <c r="D91" s="12" t="s">
+        <v>250</v>
       </c>
       <c r="E91" s="15">
+        <v>1</v>
+      </c>
+      <c r="F91" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="92" spans="1:6">
       <c r="B92" s="9" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C92" s="11" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E92" s="15">
         <v>1</v>
@@ -3322,10 +3343,10 @@
     </row>
     <row r="93" spans="1:6">
       <c r="B93" s="9" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C93" s="11" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E93" s="15">
         <v>1</v>
@@ -3333,24 +3354,21 @@
     </row>
     <row r="94" spans="1:6">
       <c r="B94" s="9" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C94" s="11" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E94" s="15">
-        <v>1</v>
-      </c>
-      <c r="F94" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="95" spans="1:6">
       <c r="B95" s="9" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C95" s="11" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E95" s="15">
         <v>1</v>
@@ -3361,10 +3379,10 @@
     </row>
     <row r="96" spans="1:6">
       <c r="B96" s="9" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C96" s="11" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E96" s="15">
         <v>1</v>
@@ -3375,10 +3393,10 @@
     </row>
     <row r="97" spans="1:6">
       <c r="B97" s="9" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C97" s="11" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E97" s="15">
         <v>1</v>
@@ -3389,10 +3407,10 @@
     </row>
     <row r="98" spans="1:6">
       <c r="B98" s="9" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C98" s="11" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E98" s="15">
         <v>1</v>
@@ -3403,31 +3421,37 @@
     </row>
     <row r="99" spans="1:6">
       <c r="B99" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="C99" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="E99" s="15">
+        <v>1</v>
+      </c>
+      <c r="F99" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6">
+      <c r="B100" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="C99" s="11" t="s">
+      <c r="C100" s="11" t="s">
         <v>166</v>
       </c>
-      <c r="E99" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6">
-      <c r="A100" s="1" t="s">
-        <v>13</v>
+      <c r="E100" s="15">
+        <v>1</v>
       </c>
     </row>
     <row r="101" spans="1:6">
       <c r="B101" s="9" t="s">
-        <v>167</v>
+        <v>365</v>
       </c>
       <c r="C101" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="D101" s="12" t="s">
-        <v>243</v>
-      </c>
-      <c r="E101" s="15">
+        <v>366</v>
+      </c>
+      <c r="E101" s="23">
         <v>1</v>
       </c>
       <c r="F101" s="15">
@@ -3435,25 +3459,19 @@
       </c>
     </row>
     <row r="102" spans="1:6">
-      <c r="B102" s="9" t="s">
-        <v>169</v>
-      </c>
-      <c r="C102" s="11" t="s">
-        <v>170</v>
-      </c>
-      <c r="E102" s="15">
-        <v>1</v>
-      </c>
-      <c r="F102" s="15">
-        <v>1</v>
+      <c r="A102" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="103" spans="1:6">
       <c r="B103" s="9" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C103" s="11" t="s">
-        <v>172</v>
+        <v>168</v>
+      </c>
+      <c r="D103" s="12" t="s">
+        <v>243</v>
       </c>
       <c r="E103" s="15">
         <v>1</v>
@@ -3464,13 +3482,10 @@
     </row>
     <row r="104" spans="1:6">
       <c r="B104" s="9" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C104" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="D104" s="12" t="s">
-        <v>244</v>
+        <v>170</v>
       </c>
       <c r="E104" s="15">
         <v>1</v>
@@ -3481,13 +3496,10 @@
     </row>
     <row r="105" spans="1:6">
       <c r="B105" s="9" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C105" s="11" t="s">
-        <v>176</v>
-      </c>
-      <c r="D105" s="12" t="s">
-        <v>245</v>
+        <v>172</v>
       </c>
       <c r="E105" s="15">
         <v>1</v>
@@ -3498,13 +3510,13 @@
     </row>
     <row r="106" spans="1:6">
       <c r="B106" s="9" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C106" s="11" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="D106" s="12" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="E106" s="15">
         <v>1</v>
@@ -3515,13 +3527,13 @@
     </row>
     <row r="107" spans="1:6">
       <c r="B107" s="9" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C107" s="11" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D107" s="12" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E107" s="15">
         <v>1</v>
@@ -3532,13 +3544,13 @@
     </row>
     <row r="108" spans="1:6">
       <c r="B108" s="9" t="s">
-        <v>311</v>
+        <v>177</v>
       </c>
       <c r="C108" s="11" t="s">
-        <v>181</v>
-      </c>
-      <c r="D108" s="24" t="s">
-        <v>309</v>
+        <v>178</v>
+      </c>
+      <c r="D108" s="12" t="s">
+        <v>246</v>
       </c>
       <c r="E108" s="15">
         <v>1</v>
@@ -3549,13 +3561,13 @@
     </row>
     <row r="109" spans="1:6">
       <c r="B109" s="9" t="s">
-        <v>307</v>
+        <v>179</v>
       </c>
       <c r="C109" s="11" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D109" s="12" t="s">
-        <v>305</v>
+        <v>247</v>
       </c>
       <c r="E109" s="15">
         <v>1</v>
@@ -3565,19 +3577,31 @@
       </c>
     </row>
     <row r="110" spans="1:6">
-      <c r="A110" s="1" t="s">
-        <v>14</v>
+      <c r="B110" s="9" t="s">
+        <v>311</v>
+      </c>
+      <c r="C110" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="D110" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="E110" s="15">
+        <v>1</v>
+      </c>
+      <c r="F110" s="15">
+        <v>1</v>
       </c>
     </row>
     <row r="111" spans="1:6">
       <c r="B111" s="9" t="s">
-        <v>183</v>
+        <v>307</v>
       </c>
       <c r="C111" s="11" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D111" s="12" t="s">
-        <v>249</v>
+        <v>305</v>
       </c>
       <c r="E111" s="15">
         <v>1</v>
@@ -3587,28 +3611,19 @@
       </c>
     </row>
     <row r="112" spans="1:6">
-      <c r="B112" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="C112" s="11" t="s">
-        <v>186</v>
-      </c>
-      <c r="E112" s="15">
-        <v>1</v>
-      </c>
-      <c r="F112" s="15">
-        <v>1</v>
+      <c r="A112" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="113" spans="1:6">
       <c r="B113" s="9" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C113" s="11" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="D113" s="12" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E113" s="15">
         <v>1</v>
@@ -3619,32 +3634,41 @@
     </row>
     <row r="114" spans="1:6">
       <c r="B114" s="9" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C114" s="11" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="E114" s="15">
+        <v>1</v>
+      </c>
+      <c r="F114" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="115" spans="1:6">
       <c r="B115" s="9" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C115" s="11" t="s">
-        <v>192</v>
+        <v>188</v>
+      </c>
+      <c r="D115" s="12" t="s">
+        <v>250</v>
       </c>
       <c r="E115" s="15">
+        <v>1</v>
+      </c>
+      <c r="F115" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="116" spans="1:6">
       <c r="B116" s="9" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C116" s="11" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="E116" s="15">
         <v>1</v>
@@ -3652,38 +3676,32 @@
     </row>
     <row r="117" spans="1:6">
       <c r="B117" s="9" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C117" s="11" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E117" s="15">
-        <v>1</v>
-      </c>
-      <c r="F117" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="118" spans="1:6">
       <c r="B118" s="9" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C118" s="11" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="E118" s="15">
-        <v>1</v>
-      </c>
-      <c r="F118" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="119" spans="1:6">
       <c r="B119" s="9" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C119" s="11" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="E119" s="15">
         <v>1</v>
@@ -3694,10 +3712,10 @@
     </row>
     <row r="120" spans="1:6">
       <c r="B120" s="9" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C120" s="11" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="E120" s="15">
         <v>1</v>
@@ -3708,10 +3726,10 @@
     </row>
     <row r="121" spans="1:6">
       <c r="B121" s="9" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C121" s="11" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="E121" s="15">
         <v>1</v>
@@ -3722,45 +3740,51 @@
     </row>
     <row r="122" spans="1:6">
       <c r="B122" s="9" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C122" s="11" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="E122" s="15">
         <v>1</v>
       </c>
+      <c r="F122" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="123" spans="1:6">
-      <c r="A123" s="1" t="s">
-        <v>15</v>
+      <c r="B123" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="C123" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="E123" s="15">
+        <v>1</v>
+      </c>
+      <c r="F123" s="15">
+        <v>1</v>
       </c>
     </row>
     <row r="124" spans="1:6">
       <c r="B124" s="9" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C124" s="11" t="s">
-        <v>208</v>
-      </c>
-      <c r="D124" s="12" t="s">
-        <v>251</v>
+        <v>206</v>
       </c>
       <c r="E124" s="15">
-        <v>1</v>
-      </c>
-      <c r="F124" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="125" spans="1:6">
       <c r="B125" s="9" t="s">
-        <v>209</v>
+        <v>368</v>
       </c>
       <c r="C125" s="11" t="s">
-        <v>210</v>
-      </c>
-      <c r="E125" s="15">
+        <v>367</v>
+      </c>
+      <c r="E125" s="23">
         <v>1</v>
       </c>
       <c r="F125" s="15">
@@ -3768,33 +3792,33 @@
       </c>
     </row>
     <row r="126" spans="1:6">
-      <c r="B126" s="9" t="s">
-        <v>211</v>
-      </c>
-      <c r="C126" s="11" t="s">
-        <v>212</v>
-      </c>
-      <c r="E126" s="15">
-        <v>1</v>
-      </c>
-      <c r="F126" s="15">
-        <v>1</v>
+      <c r="A126" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="127" spans="1:6">
-      <c r="A127" t="s">
-        <v>278</v>
+      <c r="B127" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="C127" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="D127" s="12" t="s">
+        <v>251</v>
+      </c>
+      <c r="E127" s="15">
+        <v>1</v>
+      </c>
+      <c r="F127" s="15">
+        <v>1</v>
       </c>
     </row>
     <row r="128" spans="1:6">
       <c r="B128" s="9" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C128" s="11" t="s">
-        <v>214</v>
-      </c>
-      <c r="D128" s="12" t="s">
-        <v>252</v>
+        <v>210</v>
       </c>
       <c r="E128" s="15">
         <v>1</v>
@@ -3805,13 +3829,10 @@
     </row>
     <row r="129" spans="1:6">
       <c r="B129" s="9" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C129" s="11" t="s">
-        <v>216</v>
-      </c>
-      <c r="D129" s="12" t="s">
-        <v>253</v>
+        <v>212</v>
       </c>
       <c r="E129" s="15">
         <v>1</v>
@@ -3821,31 +3842,19 @@
       </c>
     </row>
     <row r="130" spans="1:6">
-      <c r="B130" s="9" t="s">
-        <v>217</v>
-      </c>
-      <c r="C130" s="11" t="s">
-        <v>218</v>
-      </c>
-      <c r="D130" s="12" t="s">
-        <v>254</v>
-      </c>
-      <c r="E130" s="15">
-        <v>1</v>
-      </c>
-      <c r="F130" s="15">
-        <v>1</v>
+      <c r="A130" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="131" spans="1:6">
       <c r="B131" s="9" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="C131" s="11" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="D131" s="12" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="E131" s="15">
         <v>1</v>
@@ -3856,10 +3865,10 @@
     </row>
     <row r="132" spans="1:6">
       <c r="B132" s="9" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="C132" s="11" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="D132" s="12" t="s">
         <v>253</v>
@@ -3873,10 +3882,10 @@
     </row>
     <row r="133" spans="1:6">
       <c r="B133" s="9" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="C133" s="11" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="D133" s="12" t="s">
         <v>254</v>
@@ -3890,10 +3899,10 @@
     </row>
     <row r="134" spans="1:6">
       <c r="B134" s="9" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="C134" s="11" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="D134" s="12" t="s">
         <v>255</v>
@@ -3907,10 +3916,10 @@
     </row>
     <row r="135" spans="1:6">
       <c r="B135" s="9" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="C135" s="11" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="D135" s="12" t="s">
         <v>253</v>
@@ -3924,10 +3933,10 @@
     </row>
     <row r="136" spans="1:6">
       <c r="B136" s="9" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="C136" s="11" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="D136" s="12" t="s">
         <v>254</v>
@@ -3940,16 +3949,31 @@
       </c>
     </row>
     <row r="137" spans="1:6">
-      <c r="A137" s="1" t="s">
-        <v>16</v>
+      <c r="B137" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="C137" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="D137" s="12" t="s">
+        <v>255</v>
+      </c>
+      <c r="E137" s="15">
+        <v>1</v>
+      </c>
+      <c r="F137" s="15">
+        <v>1</v>
       </c>
     </row>
     <row r="138" spans="1:6">
       <c r="B138" s="9" t="s">
-        <v>300</v>
+        <v>227</v>
       </c>
       <c r="C138" s="11" t="s">
-        <v>301</v>
+        <v>228</v>
+      </c>
+      <c r="D138" s="12" t="s">
+        <v>253</v>
       </c>
       <c r="E138" s="15">
         <v>1</v>
@@ -3959,14 +3983,16 @@
       </c>
     </row>
     <row r="139" spans="1:6">
-      <c r="A139" s="20"/>
       <c r="B139" s="9" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C139" s="11" t="s">
-        <v>232</v>
-      </c>
-      <c r="E139" s="23">
+        <v>230</v>
+      </c>
+      <c r="D139" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="E139" s="15">
         <v>1</v>
       </c>
       <c r="F139" s="15">
@@ -3974,107 +4000,97 @@
       </c>
     </row>
     <row r="140" spans="1:6">
-      <c r="A140" s="20" t="s">
-        <v>295</v>
+      <c r="A140" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="141" spans="1:6">
       <c r="B141" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="C141" s="11" t="s">
+        <v>301</v>
+      </c>
+      <c r="E141" s="15">
+        <v>1</v>
+      </c>
+      <c r="F141" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6">
+      <c r="A142" s="20"/>
+      <c r="B142" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="C142" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="E142" s="23">
+        <v>1</v>
+      </c>
+      <c r="F142" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6">
+      <c r="A143" s="20" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6">
+      <c r="B144" s="9" t="s">
         <v>296</v>
       </c>
-      <c r="C141" s="11" t="s">
+      <c r="C144" s="11" t="s">
         <v>298</v>
       </c>
-      <c r="E141" s="23">
-        <v>1</v>
-      </c>
-      <c r="F141" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="142" spans="1:6">
-      <c r="B142" s="9" t="s">
+      <c r="E144" s="23">
+        <v>1</v>
+      </c>
+      <c r="F144" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6">
+      <c r="B145" s="9" t="s">
         <v>297</v>
       </c>
-      <c r="C142" s="11" t="s">
+      <c r="C145" s="11" t="s">
         <v>299</v>
       </c>
-      <c r="E142" s="23">
-        <v>1</v>
-      </c>
-      <c r="F142" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="143" spans="1:6">
-      <c r="A143" t="s">
+      <c r="E145" s="23">
+        <v>1</v>
+      </c>
+      <c r="F145" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6">
+      <c r="A146" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="144" spans="1:6">
-      <c r="B144" s="25" t="s">
+    <row r="147" spans="1:6">
+      <c r="B147" s="25" t="s">
         <v>313</v>
       </c>
-      <c r="C144" s="26" t="s">
+      <c r="C147" s="26" t="s">
         <v>314</v>
       </c>
-      <c r="E144" s="23">
-        <v>1</v>
-      </c>
-      <c r="F144" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="145" spans="1:6">
-      <c r="B145" s="25" t="s">
+      <c r="E147" s="23">
+        <v>1</v>
+      </c>
+      <c r="F147" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6">
+      <c r="B148" s="25" t="s">
         <v>330</v>
       </c>
-      <c r="C145" s="26" t="s">
+      <c r="C148" s="26" t="s">
         <v>315</v>
-      </c>
-      <c r="E145" s="23">
-        <v>1</v>
-      </c>
-      <c r="F145" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="146" spans="1:6">
-      <c r="B146" s="25" t="s">
-        <v>331</v>
-      </c>
-      <c r="C146" s="26" t="s">
-        <v>316</v>
-      </c>
-      <c r="E146" s="23">
-        <v>1</v>
-      </c>
-      <c r="F146" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="147" spans="1:6">
-      <c r="A147" s="21"/>
-      <c r="B147" s="25" t="s">
-        <v>333</v>
-      </c>
-      <c r="C147" s="26" t="s">
-        <v>317</v>
-      </c>
-      <c r="E147" s="23">
-        <v>1</v>
-      </c>
-      <c r="F147" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="148" spans="1:6">
-      <c r="A148" s="21"/>
-      <c r="B148" s="25" t="s">
-        <v>332</v>
-      </c>
-      <c r="C148" s="26" t="s">
-        <v>318</v>
       </c>
       <c r="E148" s="23">
         <v>1</v>
@@ -4085,10 +4101,10 @@
     </row>
     <row r="149" spans="1:6">
       <c r="B149" s="25" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="C149" s="26" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="E149" s="23">
         <v>1</v>
@@ -4098,11 +4114,12 @@
       </c>
     </row>
     <row r="150" spans="1:6">
+      <c r="A150" s="21"/>
       <c r="B150" s="25" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C150" s="26" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E150" s="23">
         <v>1</v>
@@ -4112,11 +4129,12 @@
       </c>
     </row>
     <row r="151" spans="1:6">
+      <c r="A151" s="21"/>
       <c r="B151" s="25" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="C151" s="26" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="E151" s="23">
         <v>1</v>
@@ -4127,10 +4145,10 @@
     </row>
     <row r="152" spans="1:6">
       <c r="B152" s="25" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="C152" s="26" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="E152" s="23">
         <v>1</v>
@@ -4141,10 +4159,10 @@
     </row>
     <row r="153" spans="1:6">
       <c r="B153" s="25" t="s">
-        <v>344</v>
+        <v>335</v>
       </c>
       <c r="C153" s="26" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="E153" s="23">
         <v>1</v>
@@ -4155,10 +4173,10 @@
     </row>
     <row r="154" spans="1:6">
       <c r="B154" s="25" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C154" s="26" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="E154" s="23">
         <v>1</v>
@@ -4169,10 +4187,10 @@
     </row>
     <row r="155" spans="1:6">
       <c r="B155" s="25" t="s">
-        <v>338</v>
+        <v>343</v>
       </c>
       <c r="C155" s="26" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="E155" s="23">
         <v>1</v>
@@ -4183,10 +4201,10 @@
     </row>
     <row r="156" spans="1:6">
       <c r="B156" s="25" t="s">
-        <v>339</v>
+        <v>344</v>
       </c>
       <c r="C156" s="26" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="E156" s="23">
         <v>1</v>
@@ -4197,10 +4215,10 @@
     </row>
     <row r="157" spans="1:6">
       <c r="B157" s="25" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="C157" s="26" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="E157" s="23">
         <v>1</v>
@@ -4211,10 +4229,10 @@
     </row>
     <row r="158" spans="1:6">
       <c r="B158" s="25" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C158" s="26" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="E158" s="23">
         <v>1</v>
@@ -4225,10 +4243,10 @@
     </row>
     <row r="159" spans="1:6">
       <c r="B159" s="25" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="C159" s="26" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="E159" s="23">
         <v>1</v>
@@ -4239,10 +4257,10 @@
     </row>
     <row r="160" spans="1:6">
       <c r="B160" s="25" t="s">
-        <v>353</v>
-      </c>
-      <c r="C160" s="27" t="s">
-        <v>345</v>
+        <v>340</v>
+      </c>
+      <c r="C160" s="26" t="s">
+        <v>327</v>
       </c>
       <c r="E160" s="23">
         <v>1</v>
@@ -4253,10 +4271,10 @@
     </row>
     <row r="161" spans="1:6">
       <c r="B161" s="25" t="s">
-        <v>354</v>
-      </c>
-      <c r="C161" s="27" t="s">
-        <v>346</v>
+        <v>341</v>
+      </c>
+      <c r="C161" s="26" t="s">
+        <v>328</v>
       </c>
       <c r="E161" s="23">
         <v>1</v>
@@ -4267,10 +4285,10 @@
     </row>
     <row r="162" spans="1:6">
       <c r="B162" s="25" t="s">
-        <v>355</v>
-      </c>
-      <c r="C162" s="27" t="s">
-        <v>347</v>
+        <v>342</v>
+      </c>
+      <c r="C162" s="26" t="s">
+        <v>329</v>
       </c>
       <c r="E162" s="23">
         <v>1</v>
@@ -4281,10 +4299,10 @@
     </row>
     <row r="163" spans="1:6">
       <c r="B163" s="25" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="C163" s="27" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="E163" s="23">
         <v>1</v>
@@ -4295,10 +4313,10 @@
     </row>
     <row r="164" spans="1:6">
       <c r="B164" s="25" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="C164" s="27" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="E164" s="23">
         <v>1</v>
@@ -4309,10 +4327,10 @@
     </row>
     <row r="165" spans="1:6">
       <c r="B165" s="25" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="C165" s="27" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="E165" s="23">
         <v>1</v>
@@ -4323,10 +4341,10 @@
     </row>
     <row r="166" spans="1:6">
       <c r="B166" s="25" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="C166" s="27" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="E166" s="23">
         <v>1</v>
@@ -4337,20 +4355,62 @@
     </row>
     <row r="167" spans="1:6">
       <c r="B167" s="25" t="s">
+        <v>357</v>
+      </c>
+      <c r="C167" s="27" t="s">
+        <v>349</v>
+      </c>
+      <c r="E167" s="23">
+        <v>1</v>
+      </c>
+      <c r="F167" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6">
+      <c r="B168" s="25" t="s">
+        <v>358</v>
+      </c>
+      <c r="C168" s="27" t="s">
+        <v>350</v>
+      </c>
+      <c r="E168" s="23">
+        <v>1</v>
+      </c>
+      <c r="F168" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6">
+      <c r="B169" s="25" t="s">
+        <v>359</v>
+      </c>
+      <c r="C169" s="27" t="s">
+        <v>351</v>
+      </c>
+      <c r="E169" s="23">
+        <v>1</v>
+      </c>
+      <c r="F169" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6">
+      <c r="B170" s="25" t="s">
         <v>360</v>
       </c>
-      <c r="C167" s="27" t="s">
+      <c r="C170" s="27" t="s">
         <v>352</v>
       </c>
-      <c r="E167" s="23">
-        <v>1</v>
-      </c>
-      <c r="F167" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="168" spans="1:6">
-      <c r="A168" t="s">
+      <c r="E170" s="23">
+        <v>1</v>
+      </c>
+      <c r="F170" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6">
+      <c r="A171" t="s">
         <v>290</v>
       </c>
     </row>
@@ -4364,8 +4424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A28F574A-1A18-F84B-837D-BB0502A7BBD8}">
   <dimension ref="A1:C336"/>
   <sheetViews>
-    <sheetView topLeftCell="A189" workbookViewId="0">
-      <selection activeCell="A204" sqref="A204"/>
+    <sheetView tabSelected="1" topLeftCell="A184" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37:A226"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -4436,7 +4496,7 @@
     <row r="15" spans="1:2">
       <c r="A15" s="2" t="str">
         <f>_xlfn.CONCAT("#define NB_OF_VAR ",FIXED(SUM('Memory setup'!E:E),0))</f>
-        <v>#define NB_OF_VAR 141</v>
+        <v>#define NB_OF_VAR 144</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -4452,7 +4512,7 @@
     <row r="19" spans="1:1">
       <c r="A19" s="2" t="str">
         <f>_xlfn.CONCAT("#define NB_EXPORTABLE_ADR ",FIXED(SUM('Memory setup'!F:F),0))</f>
-        <v>#define NB_EXPORTABLE_ADR 126</v>
+        <v>#define NB_EXPORTABLE_ADR 129</v>
       </c>
     </row>
     <row r="20" spans="1:1">
@@ -4958,571 +5018,571 @@
     <row r="112" spans="1:1">
       <c r="A112" t="str">
         <f>IF('Memory setup'!A77&lt;&gt;"",IF('Memory setup'!A77="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A77),IF('Memory setup'!E77=1,_xlfn.CONCAT("#define ",'Memory setup'!B77," ",'Memory setup'!C77," ",'Memory setup'!D77),""))</f>
-        <v>// AXIS2</v>
+        <v xml:space="preserve">#define ADR_TMC1_TRQ_FILT 0x32C </v>
       </c>
     </row>
     <row r="113" spans="1:1">
       <c r="A113" t="str">
         <f>IF('Memory setup'!A78&lt;&gt;"",IF('Memory setup'!A78="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A78),IF('Memory setup'!E78=1,_xlfn.CONCAT("#define ",'Memory setup'!B78," ",'Memory setup'!C78," ",'Memory setup'!D78),""))</f>
-        <v>#define ADR_AXIS2_CONFIG 0x341 // 0-2 ENC, 3-5 DRV</v>
+        <v>// AXIS2</v>
       </c>
     </row>
     <row r="114" spans="1:1">
       <c r="A114" t="str">
         <f>IF('Memory setup'!A79&lt;&gt;"",IF('Memory setup'!A79="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A79),IF('Memory setup'!E79=1,_xlfn.CONCAT("#define ",'Memory setup'!B79," ",'Memory setup'!C79," ",'Memory setup'!D79),""))</f>
-        <v xml:space="preserve">#define ADR_AXIS2_POWER 0x342 </v>
+        <v>#define ADR_AXIS2_CONFIG 0x341 // 0-2 ENC, 3-5 DRV</v>
       </c>
     </row>
     <row r="115" spans="1:1">
       <c r="A115" t="str">
         <f>IF('Memory setup'!A80&lt;&gt;"",IF('Memory setup'!A80="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A80),IF('Memory setup'!E80=1,_xlfn.CONCAT("#define ",'Memory setup'!B80," ",'Memory setup'!C80," ",'Memory setup'!D80),""))</f>
-        <v xml:space="preserve">#define ADR_AXIS2_DEGREES 0x343 </v>
+        <v xml:space="preserve">#define ADR_AXIS2_POWER 0x342 </v>
       </c>
     </row>
     <row r="116" spans="1:1">
       <c r="A116" t="str">
         <f>IF('Memory setup'!A81&lt;&gt;"",IF('Memory setup'!A81="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A81),IF('Memory setup'!E81=1,_xlfn.CONCAT("#define ",'Memory setup'!B81," ",'Memory setup'!C81," ",'Memory setup'!D81),""))</f>
-        <v>#define ADR_AXIS2_MAX_SPEED 0x344 // Store the max speed</v>
+        <v xml:space="preserve">#define ADR_AXIS2_DEGREES 0x343 </v>
       </c>
     </row>
     <row r="117" spans="1:1">
       <c r="A117" t="str">
         <f>IF('Memory setup'!A82&lt;&gt;"",IF('Memory setup'!A82="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A82),IF('Memory setup'!E82=1,_xlfn.CONCAT("#define ",'Memory setup'!B82," ",'Memory setup'!C82," ",'Memory setup'!D82),""))</f>
-        <v>#define ADR_AXIS2_MAX_ACCEL 0x345 // Store the max accel</v>
+        <v>#define ADR_AXIS2_MAX_SPEED 0x344 // Store the max speed</v>
       </c>
     </row>
     <row r="118" spans="1:1">
       <c r="A118" t="str">
         <f>IF('Memory setup'!A83&lt;&gt;"",IF('Memory setup'!A83="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A83),IF('Memory setup'!E83=1,_xlfn.CONCAT("#define ",'Memory setup'!B83," ",'Memory setup'!C83," ",'Memory setup'!D83),""))</f>
-        <v>#define ADR_AXIS2_ENDSTOP 0x347 // 0-7 endstop margin, 8-15 endstop stiffness</v>
+        <v>#define ADR_AXIS2_MAX_ACCEL 0x345 // Store the max accel</v>
       </c>
     </row>
     <row r="119" spans="1:1">
       <c r="A119" t="str">
         <f>IF('Memory setup'!A84&lt;&gt;"",IF('Memory setup'!A84="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A84),IF('Memory setup'!E84=1,_xlfn.CONCAT("#define ",'Memory setup'!B84," ",'Memory setup'!C84," ",'Memory setup'!D84),""))</f>
-        <v>#define ADR_AXIS2_EFFECTS1 0x348 // 0-7 idlespring, 8-15 damper</v>
+        <v>#define ADR_AXIS2_ENDSTOP 0x347 // 0-7 endstop margin, 8-15 endstop stiffness</v>
       </c>
     </row>
     <row r="120" spans="1:1">
       <c r="A120" t="str">
         <f>IF('Memory setup'!A85&lt;&gt;"",IF('Memory setup'!A85="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A85),IF('Memory setup'!E85=1,_xlfn.CONCAT("#define ",'Memory setup'!B85," ",'Memory setup'!C85," ",'Memory setup'!D85),""))</f>
-        <v>#define ADR_AXIS2_SPEEDACCEL_FILTER 0x349 // Speed/Accel filter Lowpass profile</v>
+        <v>#define ADR_AXIS2_EFFECTS1 0x348 // 0-7 idlespring, 8-15 damper</v>
       </c>
     </row>
     <row r="121" spans="1:1">
       <c r="A121" t="str">
         <f>IF('Memory setup'!A86&lt;&gt;"",IF('Memory setup'!A86="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A86),IF('Memory setup'!E86=1,_xlfn.CONCAT("#define ",'Memory setup'!B86," ",'Memory setup'!C86," ",'Memory setup'!D86),""))</f>
-        <v>#define ADR_AXIS2_ENC_RATIO 0x34A // Store the encoder ratio for an axis</v>
+        <v>#define ADR_AXIS2_SPEEDACCEL_FILTER 0x349 // Speed/Accel filter Lowpass profile</v>
       </c>
     </row>
     <row r="122" spans="1:1">
       <c r="A122" t="str">
         <f>IF('Memory setup'!A87&lt;&gt;"",IF('Memory setup'!A87="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A87),IF('Memory setup'!E87=1,_xlfn.CONCAT("#define ",'Memory setup'!B87," ",'Memory setup'!C87," ",'Memory setup'!D87),""))</f>
-        <v>// TMC2</v>
+        <v>#define ADR_AXIS2_ENC_RATIO 0x34A // Store the encoder ratio for an axis</v>
       </c>
     </row>
     <row r="123" spans="1:1">
       <c r="A123" t="str">
         <f>IF('Memory setup'!A88&lt;&gt;"",IF('Memory setup'!A88="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A88),IF('Memory setup'!E88=1,_xlfn.CONCAT("#define ",'Memory setup'!B88," ",'Memory setup'!C88," ",'Memory setup'!D88),""))</f>
-        <v>#define ADR_TMC2_MOTCONF 0x360 // 0-2: MotType 3-5: PhiE source 6-15: Poles</v>
+        <v>// TMC2</v>
       </c>
     </row>
     <row r="124" spans="1:1">
       <c r="A124" t="str">
         <f>IF('Memory setup'!A89&lt;&gt;"",IF('Memory setup'!A89="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A89),IF('Memory setup'!E89=1,_xlfn.CONCAT("#define ",'Memory setup'!B89," ",'Memory setup'!C89," ",'Memory setup'!D89),""))</f>
-        <v xml:space="preserve">#define ADR_TMC2_CPR 0x361 </v>
+        <v>#define ADR_TMC2_MOTCONF 0x360 // 0-2: MotType 3-5: PhiE source 6-15: Poles</v>
       </c>
     </row>
     <row r="125" spans="1:1">
       <c r="A125" t="str">
         <f>IF('Memory setup'!A90&lt;&gt;"",IF('Memory setup'!A90="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A90),IF('Memory setup'!E90=1,_xlfn.CONCAT("#define ",'Memory setup'!B90," ",'Memory setup'!C90," ",'Memory setup'!D90),""))</f>
-        <v>#define ADR_TMC2_ENCA 0x362 // Misc</v>
+        <v xml:space="preserve">#define ADR_TMC2_CPR 0x361 </v>
       </c>
     </row>
     <row r="126" spans="1:1">
       <c r="A126" t="str">
         <f>IF('Memory setup'!A91&lt;&gt;"",IF('Memory setup'!A91="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A91),IF('Memory setup'!E91=1,_xlfn.CONCAT("#define ",'Memory setup'!B91," ",'Memory setup'!C91," ",'Memory setup'!D91),""))</f>
-        <v xml:space="preserve">#define ADR_TMC2_ADC_I0_OFS 0x363 </v>
+        <v>#define ADR_TMC2_ENCA 0x362 // Misc</v>
       </c>
     </row>
     <row r="127" spans="1:1">
       <c r="A127" t="str">
         <f>IF('Memory setup'!A92&lt;&gt;"",IF('Memory setup'!A92="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A92),IF('Memory setup'!E92=1,_xlfn.CONCAT("#define ",'Memory setup'!B92," ",'Memory setup'!C92," ",'Memory setup'!D92),""))</f>
-        <v xml:space="preserve">#define ADR_TMC2_ADC_I1_OFS 0x364 </v>
+        <v xml:space="preserve">#define ADR_TMC2_ADC_I0_OFS 0x363 </v>
       </c>
     </row>
     <row r="128" spans="1:1">
       <c r="A128" t="str">
         <f>IF('Memory setup'!A93&lt;&gt;"",IF('Memory setup'!A93="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A93),IF('Memory setup'!E93=1,_xlfn.CONCAT("#define ",'Memory setup'!B93," ",'Memory setup'!C93," ",'Memory setup'!D93),""))</f>
-        <v xml:space="preserve">#define ADR_TMC2_ENC_OFFSET 0x365 </v>
+        <v xml:space="preserve">#define ADR_TMC2_ADC_I1_OFS 0x364 </v>
       </c>
     </row>
     <row r="129" spans="1:1">
       <c r="A129" t="str">
         <f>IF('Memory setup'!A94&lt;&gt;"",IF('Memory setup'!A94="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A94),IF('Memory setup'!E94=1,_xlfn.CONCAT("#define ",'Memory setup'!B94," ",'Memory setup'!C94," ",'Memory setup'!D94),""))</f>
-        <v xml:space="preserve">#define ADR_TMC2_OFFSETFLUX 0x366 </v>
+        <v xml:space="preserve">#define ADR_TMC2_ENC_OFFSET 0x365 </v>
       </c>
     </row>
     <row r="130" spans="1:1">
       <c r="A130" t="str">
         <f>IF('Memory setup'!A95&lt;&gt;"",IF('Memory setup'!A95="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A95),IF('Memory setup'!E95=1,_xlfn.CONCAT("#define ",'Memory setup'!B95," ",'Memory setup'!C95," ",'Memory setup'!D95),""))</f>
-        <v xml:space="preserve">#define ADR_TMC2_TORQUE_P 0x367 </v>
+        <v xml:space="preserve">#define ADR_TMC2_OFFSETFLUX 0x366 </v>
       </c>
     </row>
     <row r="131" spans="1:1">
       <c r="A131" t="str">
         <f>IF('Memory setup'!A96&lt;&gt;"",IF('Memory setup'!A96="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A96),IF('Memory setup'!E96=1,_xlfn.CONCAT("#define ",'Memory setup'!B96," ",'Memory setup'!C96," ",'Memory setup'!D96),""))</f>
-        <v xml:space="preserve">#define ADR_TMC2_TORQUE_I 0x368 </v>
+        <v xml:space="preserve">#define ADR_TMC2_TORQUE_P 0x367 </v>
       </c>
     </row>
     <row r="132" spans="1:1">
       <c r="A132" t="str">
         <f>IF('Memory setup'!A97&lt;&gt;"",IF('Memory setup'!A97="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A97),IF('Memory setup'!E97=1,_xlfn.CONCAT("#define ",'Memory setup'!B97," ",'Memory setup'!C97," ",'Memory setup'!D97),""))</f>
-        <v xml:space="preserve">#define ADR_TMC2_FLUX_P 0x369 </v>
+        <v xml:space="preserve">#define ADR_TMC2_TORQUE_I 0x368 </v>
       </c>
     </row>
     <row r="133" spans="1:1">
       <c r="A133" t="str">
         <f>IF('Memory setup'!A98&lt;&gt;"",IF('Memory setup'!A98="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A98),IF('Memory setup'!E98=1,_xlfn.CONCAT("#define ",'Memory setup'!B98," ",'Memory setup'!C98," ",'Memory setup'!D98),""))</f>
-        <v xml:space="preserve">#define ADR_TMC2_FLUX_I 0x36A </v>
+        <v xml:space="preserve">#define ADR_TMC2_FLUX_P 0x369 </v>
       </c>
     </row>
     <row r="134" spans="1:1">
       <c r="A134" t="str">
         <f>IF('Memory setup'!A99&lt;&gt;"",IF('Memory setup'!A99="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A99),IF('Memory setup'!E99=1,_xlfn.CONCAT("#define ",'Memory setup'!B99," ",'Memory setup'!C99," ",'Memory setup'!D99),""))</f>
-        <v xml:space="preserve">#define ADR_TMC2_PHIE_OFS 0x36B </v>
+        <v xml:space="preserve">#define ADR_TMC2_FLUX_I 0x36A </v>
       </c>
     </row>
     <row r="135" spans="1:1">
       <c r="A135" t="str">
         <f>IF('Memory setup'!A100&lt;&gt;"",IF('Memory setup'!A100="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A100),IF('Memory setup'!E100=1,_xlfn.CONCAT("#define ",'Memory setup'!B100," ",'Memory setup'!C100," ",'Memory setup'!D100),""))</f>
-        <v>// AXIS3</v>
+        <v xml:space="preserve">#define ADR_TMC2_PHIE_OFS 0x36B </v>
       </c>
     </row>
     <row r="136" spans="1:1">
       <c r="A136" t="str">
         <f>IF('Memory setup'!A101&lt;&gt;"",IF('Memory setup'!A101="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A101),IF('Memory setup'!E101=1,_xlfn.CONCAT("#define ",'Memory setup'!B101," ",'Memory setup'!C101," ",'Memory setup'!D101),""))</f>
-        <v>#define ADR_AXIS3_CONFIG 0x381 // 0-2 ENC, 3-5 DRV</v>
+        <v xml:space="preserve">#define ADR_TMC2_TRQ_FILT 0x36C </v>
       </c>
     </row>
     <row r="137" spans="1:1">
       <c r="A137" t="str">
         <f>IF('Memory setup'!A102&lt;&gt;"",IF('Memory setup'!A102="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A102),IF('Memory setup'!E102=1,_xlfn.CONCAT("#define ",'Memory setup'!B102," ",'Memory setup'!C102," ",'Memory setup'!D102),""))</f>
-        <v xml:space="preserve">#define ADR_AXIS3_POWER 0x382 </v>
+        <v>// AXIS3</v>
       </c>
     </row>
     <row r="138" spans="1:1">
       <c r="A138" t="str">
         <f>IF('Memory setup'!A103&lt;&gt;"",IF('Memory setup'!A103="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A103),IF('Memory setup'!E103=1,_xlfn.CONCAT("#define ",'Memory setup'!B103," ",'Memory setup'!C103," ",'Memory setup'!D103),""))</f>
-        <v xml:space="preserve">#define ADR_AXIS3_DEGREES 0x383 </v>
+        <v>#define ADR_AXIS3_CONFIG 0x381 // 0-2 ENC, 3-5 DRV</v>
       </c>
     </row>
     <row r="139" spans="1:1">
       <c r="A139" t="str">
         <f>IF('Memory setup'!A104&lt;&gt;"",IF('Memory setup'!A104="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A104),IF('Memory setup'!E104=1,_xlfn.CONCAT("#define ",'Memory setup'!B104," ",'Memory setup'!C104," ",'Memory setup'!D104),""))</f>
-        <v>#define ADR_AXIS3_MAX_SPEED 0x384 // Store the max speed</v>
+        <v xml:space="preserve">#define ADR_AXIS3_POWER 0x382 </v>
       </c>
     </row>
     <row r="140" spans="1:1">
       <c r="A140" t="str">
         <f>IF('Memory setup'!A105&lt;&gt;"",IF('Memory setup'!A105="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A105),IF('Memory setup'!E105=1,_xlfn.CONCAT("#define ",'Memory setup'!B105," ",'Memory setup'!C105," ",'Memory setup'!D105),""))</f>
-        <v>#define ADR_AXIS3_MAX_ACCEL 0x385 // Store the max accel</v>
+        <v xml:space="preserve">#define ADR_AXIS3_DEGREES 0x383 </v>
       </c>
     </row>
     <row r="141" spans="1:1">
       <c r="A141" t="str">
         <f>IF('Memory setup'!A106&lt;&gt;"",IF('Memory setup'!A106="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A106),IF('Memory setup'!E106=1,_xlfn.CONCAT("#define ",'Memory setup'!B106," ",'Memory setup'!C106," ",'Memory setup'!D106),""))</f>
-        <v>#define ADR_AXIS3_ENDSTOP 0x387 // 0-7 endstop margin, 8-15 endstop stiffness</v>
+        <v>#define ADR_AXIS3_MAX_SPEED 0x384 // Store the max speed</v>
       </c>
     </row>
     <row r="142" spans="1:1">
       <c r="A142" t="str">
         <f>IF('Memory setup'!A107&lt;&gt;"",IF('Memory setup'!A107="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A107),IF('Memory setup'!E107=1,_xlfn.CONCAT("#define ",'Memory setup'!B107," ",'Memory setup'!C107," ",'Memory setup'!D107),""))</f>
-        <v>#define ADR_AXIS3_EFFECTS1 0x388 // 0-7 idlespring, 8-15 damper</v>
+        <v>#define ADR_AXIS3_MAX_ACCEL 0x385 // Store the max accel</v>
       </c>
     </row>
     <row r="143" spans="1:1">
       <c r="A143" t="str">
         <f>IF('Memory setup'!A108&lt;&gt;"",IF('Memory setup'!A108="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A108),IF('Memory setup'!E108=1,_xlfn.CONCAT("#define ",'Memory setup'!B108," ",'Memory setup'!C108," ",'Memory setup'!D108),""))</f>
-        <v>#define ADR_AXIS3_SPEEDACCEL_FILTER 0x389 // Speed/Accel filter Lowpass profile</v>
+        <v>#define ADR_AXIS3_ENDSTOP 0x387 // 0-7 endstop margin, 8-15 endstop stiffness</v>
       </c>
     </row>
     <row r="144" spans="1:1">
       <c r="A144" t="str">
         <f>IF('Memory setup'!A109&lt;&gt;"",IF('Memory setup'!A109="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A109),IF('Memory setup'!E109=1,_xlfn.CONCAT("#define ",'Memory setup'!B109," ",'Memory setup'!C109," ",'Memory setup'!D109),""))</f>
-        <v>#define ADR_AXIS3_ENC_RATIO 0x38A // Store the encoder ratio for an axis</v>
+        <v>#define ADR_AXIS3_EFFECTS1 0x388 // 0-7 idlespring, 8-15 damper</v>
       </c>
     </row>
     <row r="145" spans="1:1">
       <c r="A145" t="str">
         <f>IF('Memory setup'!A110&lt;&gt;"",IF('Memory setup'!A110="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A110),IF('Memory setup'!E110=1,_xlfn.CONCAT("#define ",'Memory setup'!B110," ",'Memory setup'!C110," ",'Memory setup'!D110),""))</f>
-        <v>// TMC3</v>
+        <v>#define ADR_AXIS3_SPEEDACCEL_FILTER 0x389 // Speed/Accel filter Lowpass profile</v>
       </c>
     </row>
     <row r="146" spans="1:1">
       <c r="A146" t="str">
         <f>IF('Memory setup'!A111&lt;&gt;"",IF('Memory setup'!A111="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A111),IF('Memory setup'!E111=1,_xlfn.CONCAT("#define ",'Memory setup'!B111," ",'Memory setup'!C111," ",'Memory setup'!D111),""))</f>
-        <v>#define ADR_TMC3_MOTCONF 0x3A0 // 0-2: MotType 3-5: PhiE source 6-15: Poles</v>
+        <v>#define ADR_AXIS3_ENC_RATIO 0x38A // Store the encoder ratio for an axis</v>
       </c>
     </row>
     <row r="147" spans="1:1">
       <c r="A147" t="str">
         <f>IF('Memory setup'!A112&lt;&gt;"",IF('Memory setup'!A112="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A112),IF('Memory setup'!E112=1,_xlfn.CONCAT("#define ",'Memory setup'!B112," ",'Memory setup'!C112," ",'Memory setup'!D112),""))</f>
-        <v xml:space="preserve">#define ADR_TMC3_CPR 0x3A1 </v>
+        <v>// TMC3</v>
       </c>
     </row>
     <row r="148" spans="1:1">
       <c r="A148" t="str">
         <f>IF('Memory setup'!A113&lt;&gt;"",IF('Memory setup'!A113="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A113),IF('Memory setup'!E113=1,_xlfn.CONCAT("#define ",'Memory setup'!B113," ",'Memory setup'!C113," ",'Memory setup'!D113),""))</f>
-        <v>#define ADR_TMC3_ENCA 0x3A2 // Misc</v>
+        <v>#define ADR_TMC3_MOTCONF 0x3A0 // 0-2: MotType 3-5: PhiE source 6-15: Poles</v>
       </c>
     </row>
     <row r="149" spans="1:1">
       <c r="A149" t="str">
         <f>IF('Memory setup'!A114&lt;&gt;"",IF('Memory setup'!A114="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A114),IF('Memory setup'!E114=1,_xlfn.CONCAT("#define ",'Memory setup'!B114," ",'Memory setup'!C114," ",'Memory setup'!D114),""))</f>
-        <v xml:space="preserve">#define ADR_TMC3_ADC_I0_OFS 0x3A3 </v>
+        <v xml:space="preserve">#define ADR_TMC3_CPR 0x3A1 </v>
       </c>
     </row>
     <row r="150" spans="1:1">
       <c r="A150" t="str">
         <f>IF('Memory setup'!A115&lt;&gt;"",IF('Memory setup'!A115="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A115),IF('Memory setup'!E115=1,_xlfn.CONCAT("#define ",'Memory setup'!B115," ",'Memory setup'!C115," ",'Memory setup'!D115),""))</f>
-        <v xml:space="preserve">#define ADR_TMC3_ADC_I1_OFS 0x3A4 </v>
+        <v>#define ADR_TMC3_ENCA 0x3A2 // Misc</v>
       </c>
     </row>
     <row r="151" spans="1:1">
       <c r="A151" t="str">
         <f>IF('Memory setup'!A116&lt;&gt;"",IF('Memory setup'!A116="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A116),IF('Memory setup'!E116=1,_xlfn.CONCAT("#define ",'Memory setup'!B116," ",'Memory setup'!C116," ",'Memory setup'!D116),""))</f>
-        <v xml:space="preserve">#define ADR_TMC3_ENC_OFFSET 0x3A5 </v>
+        <v xml:space="preserve">#define ADR_TMC3_ADC_I0_OFS 0x3A3 </v>
       </c>
     </row>
     <row r="152" spans="1:1">
       <c r="A152" t="str">
         <f>IF('Memory setup'!A117&lt;&gt;"",IF('Memory setup'!A117="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A117),IF('Memory setup'!E117=1,_xlfn.CONCAT("#define ",'Memory setup'!B117," ",'Memory setup'!C117," ",'Memory setup'!D117),""))</f>
-        <v xml:space="preserve">#define ADR_TMC3_OFFSETFLUX 0x3A6 </v>
+        <v xml:space="preserve">#define ADR_TMC3_ADC_I1_OFS 0x3A4 </v>
       </c>
     </row>
     <row r="153" spans="1:1">
       <c r="A153" t="str">
         <f>IF('Memory setup'!A118&lt;&gt;"",IF('Memory setup'!A118="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A118),IF('Memory setup'!E118=1,_xlfn.CONCAT("#define ",'Memory setup'!B118," ",'Memory setup'!C118," ",'Memory setup'!D118),""))</f>
-        <v xml:space="preserve">#define ADR_TMC3_TORQUE_P 0x3A7 </v>
+        <v xml:space="preserve">#define ADR_TMC3_ENC_OFFSET 0x3A5 </v>
       </c>
     </row>
     <row r="154" spans="1:1">
       <c r="A154" t="str">
         <f>IF('Memory setup'!A119&lt;&gt;"",IF('Memory setup'!A119="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A119),IF('Memory setup'!E119=1,_xlfn.CONCAT("#define ",'Memory setup'!B119," ",'Memory setup'!C119," ",'Memory setup'!D119),""))</f>
-        <v xml:space="preserve">#define ADR_TMC3_TORQUE_I 0x3A8 </v>
+        <v xml:space="preserve">#define ADR_TMC3_OFFSETFLUX 0x3A6 </v>
       </c>
     </row>
     <row r="155" spans="1:1">
       <c r="A155" t="str">
         <f>IF('Memory setup'!A120&lt;&gt;"",IF('Memory setup'!A120="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A120),IF('Memory setup'!E120=1,_xlfn.CONCAT("#define ",'Memory setup'!B120," ",'Memory setup'!C120," ",'Memory setup'!D120),""))</f>
-        <v xml:space="preserve">#define ADR_TMC3_FLUX_P 0x3A9 </v>
+        <v xml:space="preserve">#define ADR_TMC3_TORQUE_P 0x3A7 </v>
       </c>
     </row>
     <row r="156" spans="1:1">
       <c r="A156" t="str">
         <f>IF('Memory setup'!A121&lt;&gt;"",IF('Memory setup'!A121="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A121),IF('Memory setup'!E121=1,_xlfn.CONCAT("#define ",'Memory setup'!B121," ",'Memory setup'!C121," ",'Memory setup'!D121),""))</f>
-        <v xml:space="preserve">#define ADR_TMC3_FLUX_I 0x3AA </v>
+        <v xml:space="preserve">#define ADR_TMC3_TORQUE_I 0x3A8 </v>
       </c>
     </row>
     <row r="157" spans="1:1">
       <c r="A157" t="str">
         <f>IF('Memory setup'!A122&lt;&gt;"",IF('Memory setup'!A122="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A122),IF('Memory setup'!E122=1,_xlfn.CONCAT("#define ",'Memory setup'!B122," ",'Memory setup'!C122," ",'Memory setup'!D122),""))</f>
-        <v xml:space="preserve">#define ADR_TMC3_PHIE_OFS 0x3AB </v>
+        <v xml:space="preserve">#define ADR_TMC3_FLUX_P 0x3A9 </v>
       </c>
     </row>
     <row r="158" spans="1:1">
       <c r="A158" t="str">
         <f>IF('Memory setup'!A123&lt;&gt;"",IF('Memory setup'!A123="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A123),IF('Memory setup'!E123=1,_xlfn.CONCAT("#define ",'Memory setup'!B123," ",'Memory setup'!C123," ",'Memory setup'!D123),""))</f>
-        <v>// Odrive</v>
+        <v xml:space="preserve">#define ADR_TMC3_FLUX_I 0x3AA </v>
       </c>
     </row>
     <row r="159" spans="1:1">
       <c r="A159" t="str">
         <f>IF('Memory setup'!A124&lt;&gt;"",IF('Memory setup'!A124="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A124),IF('Memory setup'!E124=1,_xlfn.CONCAT("#define ",'Memory setup'!B124," ",'Memory setup'!C124," ",'Memory setup'!D124),""))</f>
-        <v>#define ADR_ODRIVE_CANID 0x3D0 //0-6 ID M0, 7-12 ID M1, 13-15 can speed</v>
+        <v xml:space="preserve">#define ADR_TMC3_PHIE_OFS 0x3AB </v>
       </c>
     </row>
     <row r="160" spans="1:1">
       <c r="A160" t="str">
         <f>IF('Memory setup'!A125&lt;&gt;"",IF('Memory setup'!A125="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A125),IF('Memory setup'!E125=1,_xlfn.CONCAT("#define ",'Memory setup'!B125," ",'Memory setup'!C125," ",'Memory setup'!D125),""))</f>
-        <v xml:space="preserve">#define ADR_ODRIVE_SETTING1_M0 0x3D1 </v>
+        <v xml:space="preserve">#define ADR_TMC3_TRQ_FILT 0x3AC </v>
       </c>
     </row>
     <row r="161" spans="1:1">
       <c r="A161" t="str">
         <f>IF('Memory setup'!A126&lt;&gt;"",IF('Memory setup'!A126="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A126),IF('Memory setup'!E126=1,_xlfn.CONCAT("#define ",'Memory setup'!B126," ",'Memory setup'!C126," ",'Memory setup'!D126),""))</f>
-        <v xml:space="preserve">#define ADR_ODRIVE_SETTING1_M1 0x3D2 </v>
+        <v>// Odrive</v>
       </c>
     </row>
     <row r="162" spans="1:1">
       <c r="A162" t="str">
         <f>IF('Memory setup'!A127&lt;&gt;"",IF('Memory setup'!A127="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A127),IF('Memory setup'!E127=1,_xlfn.CONCAT("#define ",'Memory setup'!B127," ",'Memory setup'!C127," ",'Memory setup'!D127),""))</f>
-        <v>// VESC Section</v>
+        <v>#define ADR_ODRIVE_CANID 0x3D0 //0-6 ID M0, 7-12 ID M1, 13-15 can speed</v>
       </c>
     </row>
     <row r="163" spans="1:1">
       <c r="A163" t="str">
         <f>IF('Memory setup'!A128&lt;&gt;"",IF('Memory setup'!A128="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A128),IF('Memory setup'!E128=1,_xlfn.CONCAT("#define ",'Memory setup'!B128," ",'Memory setup'!C128," ",'Memory setup'!D128),""))</f>
-        <v>#define ADR_VESC1_CANID 0x3E0 //0-7 AxisCanID, 8-16 VescCanId</v>
+        <v xml:space="preserve">#define ADR_ODRIVE_SETTING1_M0 0x3D1 </v>
       </c>
     </row>
     <row r="164" spans="1:1">
       <c r="A164" t="str">
         <f>IF('Memory setup'!A129&lt;&gt;"",IF('Memory setup'!A129="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A129),IF('Memory setup'!E129=1,_xlfn.CONCAT("#define ",'Memory setup'!B129," ",'Memory setup'!C129," ",'Memory setup'!D129),""))</f>
-        <v>#define ADR_VESC1_DATA 0x3E1 //0-2 can speed, 3 useVescEncoder</v>
+        <v xml:space="preserve">#define ADR_ODRIVE_SETTING1_M1 0x3D2 </v>
       </c>
     </row>
     <row r="165" spans="1:1">
       <c r="A165" t="str">
         <f>IF('Memory setup'!A130&lt;&gt;"",IF('Memory setup'!A130="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A130),IF('Memory setup'!E130=1,_xlfn.CONCAT("#define ",'Memory setup'!B130," ",'Memory setup'!C130," ",'Memory setup'!D130),""))</f>
-        <v>#define ADR_VESC1_OFFSET 0x3E2 //16b offset</v>
+        <v>// VESC Section</v>
       </c>
     </row>
     <row r="166" spans="1:1">
       <c r="A166" t="str">
         <f>IF('Memory setup'!A131&lt;&gt;"",IF('Memory setup'!A131="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A131),IF('Memory setup'!E131=1,_xlfn.CONCAT("#define ",'Memory setup'!B131," ",'Memory setup'!C131," ",'Memory setup'!D131),""))</f>
-        <v>#define ADR_VESC2_CANID 0x3E3 //0-8 AxisCanID, 8-16 VescCanId</v>
+        <v>#define ADR_VESC1_CANID 0x3E0 //0-7 AxisCanID, 8-16 VescCanId</v>
       </c>
     </row>
     <row r="167" spans="1:1">
       <c r="A167" t="str">
         <f>IF('Memory setup'!A132&lt;&gt;"",IF('Memory setup'!A132="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A132),IF('Memory setup'!E132=1,_xlfn.CONCAT("#define ",'Memory setup'!B132," ",'Memory setup'!C132," ",'Memory setup'!D132),""))</f>
-        <v>#define ADR_VESC2_DATA 0x3E4 //0-2 can speed, 3 useVescEncoder</v>
+        <v>#define ADR_VESC1_DATA 0x3E1 //0-2 can speed, 3 useVescEncoder</v>
       </c>
     </row>
     <row r="168" spans="1:1">
       <c r="A168" t="str">
         <f>IF('Memory setup'!A133&lt;&gt;"",IF('Memory setup'!A133="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A133),IF('Memory setup'!E133=1,_xlfn.CONCAT("#define ",'Memory setup'!B133," ",'Memory setup'!C133," ",'Memory setup'!D133),""))</f>
-        <v>#define ADR_VESC2_OFFSET 0x3E5 //16b offset</v>
+        <v>#define ADR_VESC1_OFFSET 0x3E2 //16b offset</v>
       </c>
     </row>
     <row r="169" spans="1:1">
       <c r="A169" t="str">
         <f>IF('Memory setup'!A134&lt;&gt;"",IF('Memory setup'!A134="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A134),IF('Memory setup'!E134=1,_xlfn.CONCAT("#define ",'Memory setup'!B134," ",'Memory setup'!C134," ",'Memory setup'!D134),""))</f>
-        <v>#define ADR_VESC3_CANID 0x3E6 //0-8 AxisCanID, 8-16 VescCanId</v>
+        <v>#define ADR_VESC2_CANID 0x3E3 //0-8 AxisCanID, 8-16 VescCanId</v>
       </c>
     </row>
     <row r="170" spans="1:1">
       <c r="A170" t="str">
         <f>IF('Memory setup'!A135&lt;&gt;"",IF('Memory setup'!A135="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A135),IF('Memory setup'!E135=1,_xlfn.CONCAT("#define ",'Memory setup'!B135," ",'Memory setup'!C135," ",'Memory setup'!D135),""))</f>
-        <v>#define ADR_VESC3_DATA 0x3E7 //0-2 can speed, 3 useVescEncoder</v>
+        <v>#define ADR_VESC2_DATA 0x3E4 //0-2 can speed, 3 useVescEncoder</v>
       </c>
     </row>
     <row r="171" spans="1:1">
       <c r="A171" t="str">
         <f>IF('Memory setup'!A136&lt;&gt;"",IF('Memory setup'!A136="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A136),IF('Memory setup'!E136=1,_xlfn.CONCAT("#define ",'Memory setup'!B136," ",'Memory setup'!C136," ",'Memory setup'!D136),""))</f>
-        <v>#define ADR_VESC3_OFFSET 0x3E8 //16b offset</v>
+        <v>#define ADR_VESC2_OFFSET 0x3E5 //16b offset</v>
       </c>
     </row>
     <row r="172" spans="1:1">
       <c r="A172" t="str">
         <f>IF('Memory setup'!A137&lt;&gt;"",IF('Memory setup'!A137="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A137),IF('Memory setup'!E137=1,_xlfn.CONCAT("#define ",'Memory setup'!B137," ",'Memory setup'!C137," ",'Memory setup'!D137),""))</f>
-        <v>//MT Encoder</v>
+        <v>#define ADR_VESC3_CANID 0x3E6 //0-8 AxisCanID, 8-16 VescCanId</v>
       </c>
     </row>
     <row r="173" spans="1:1">
       <c r="A173" t="str">
         <f>IF('Memory setup'!A138&lt;&gt;"",IF('Memory setup'!A138="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A138),IF('Memory setup'!E138=1,_xlfn.CONCAT("#define ",'Memory setup'!B138," ",'Memory setup'!C138," ",'Memory setup'!D138),""))</f>
-        <v xml:space="preserve">#define ADR_MTENC_OFS 0x400 </v>
+        <v>#define ADR_VESC3_DATA 0x3E7 //0-2 can speed, 3 useVescEncoder</v>
       </c>
     </row>
     <row r="174" spans="1:1">
       <c r="A174" t="str">
         <f>IF('Memory setup'!A139&lt;&gt;"",IF('Memory setup'!A139="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A139),IF('Memory setup'!E139=1,_xlfn.CONCAT("#define ",'Memory setup'!B139," ",'Memory setup'!C139," ",'Memory setup'!D139),""))</f>
-        <v xml:space="preserve">#define ADR_MTENC_CONF1 0x401 </v>
+        <v>#define ADR_VESC3_OFFSET 0x3E8 //16b offset</v>
       </c>
     </row>
     <row r="175" spans="1:1">
       <c r="A175" t="str">
         <f>IF('Memory setup'!A140&lt;&gt;"",IF('Memory setup'!A140="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A140),IF('Memory setup'!E140=1,_xlfn.CONCAT("#define ",'Memory setup'!B140," ",'Memory setup'!C140," ",'Memory setup'!D140),""))</f>
-        <v>// Biss-C</v>
+        <v>//MT Encoder</v>
       </c>
     </row>
     <row r="176" spans="1:1">
       <c r="A176" t="str">
         <f>IF('Memory setup'!A141&lt;&gt;"",IF('Memory setup'!A141="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A141),IF('Memory setup'!E141=1,_xlfn.CONCAT("#define ",'Memory setup'!B141," ",'Memory setup'!C141," ",'Memory setup'!D141),""))</f>
-        <v xml:space="preserve">#define ADR_BISSENC_CONF1 0x410 </v>
+        <v xml:space="preserve">#define ADR_MTENC_OFS 0x400 </v>
       </c>
     </row>
     <row r="177" spans="1:1">
       <c r="A177" t="str">
         <f>IF('Memory setup'!A142&lt;&gt;"",IF('Memory setup'!A142="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A142),IF('Memory setup'!E142=1,_xlfn.CONCAT("#define ",'Memory setup'!B142," ",'Memory setup'!C142," ",'Memory setup'!D142),""))</f>
-        <v xml:space="preserve">#define ADR_BISSENC_OFS 0x411 </v>
+        <v xml:space="preserve">#define ADR_MTENC_CONF1 0x401 </v>
       </c>
     </row>
     <row r="178" spans="1:1">
       <c r="A178" t="str">
         <f>IF('Memory setup'!A143&lt;&gt;"",IF('Memory setup'!A143="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A143),IF('Memory setup'!E143=1,_xlfn.CONCAT("#define ",'Memory setup'!B143," ",'Memory setup'!C143," ",'Memory setup'!D143),""))</f>
-        <v>// Analog min/max calibrations</v>
+        <v>// Biss-C</v>
       </c>
     </row>
     <row r="179" spans="1:1">
       <c r="A179" t="str">
         <f>IF('Memory setup'!A144&lt;&gt;"",IF('Memory setup'!A144="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A144),IF('Memory setup'!E144=1,_xlfn.CONCAT("#define ",'Memory setup'!B144," ",'Memory setup'!C144," ",'Memory setup'!D144),""))</f>
-        <v xml:space="preserve">#define ADR_LOCALANALOG_MIN_0 0x500 </v>
+        <v xml:space="preserve">#define ADR_BISSENC_CONF1 0x410 </v>
       </c>
     </row>
     <row r="180" spans="1:1">
       <c r="A180" t="str">
         <f>IF('Memory setup'!A145&lt;&gt;"",IF('Memory setup'!A145="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A145),IF('Memory setup'!E145=1,_xlfn.CONCAT("#define ",'Memory setup'!B145," ",'Memory setup'!C145," ",'Memory setup'!D145),""))</f>
-        <v xml:space="preserve">#define ADR_LOCALANALOG_MAX_0 0x501 </v>
+        <v xml:space="preserve">#define ADR_BISSENC_OFS 0x411 </v>
       </c>
     </row>
     <row r="181" spans="1:1">
       <c r="A181" t="str">
         <f>IF('Memory setup'!A146&lt;&gt;"",IF('Memory setup'!A146="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A146),IF('Memory setup'!E146=1,_xlfn.CONCAT("#define ",'Memory setup'!B146," ",'Memory setup'!C146," ",'Memory setup'!D146),""))</f>
-        <v xml:space="preserve">#define ADR_LOCALANALOG_MIN_1 0x502 </v>
+        <v>// Analog min/max calibrations</v>
       </c>
     </row>
     <row r="182" spans="1:1">
       <c r="A182" t="str">
         <f>IF('Memory setup'!A147&lt;&gt;"",IF('Memory setup'!A147="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A147),IF('Memory setup'!E147=1,_xlfn.CONCAT("#define ",'Memory setup'!B147," ",'Memory setup'!C147," ",'Memory setup'!D147),""))</f>
-        <v xml:space="preserve">#define ADR_LOCALANALOG_MAX_1 0x503 </v>
+        <v xml:space="preserve">#define ADR_LOCALANALOG_MIN_0 0x500 </v>
       </c>
     </row>
     <row r="183" spans="1:1">
       <c r="A183" t="str">
         <f>IF('Memory setup'!A148&lt;&gt;"",IF('Memory setup'!A148="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A148),IF('Memory setup'!E148=1,_xlfn.CONCAT("#define ",'Memory setup'!B148," ",'Memory setup'!C148," ",'Memory setup'!D148),""))</f>
-        <v xml:space="preserve">#define ADR_LOCALANALOG_MIN_2 0x504 </v>
+        <v xml:space="preserve">#define ADR_LOCALANALOG_MAX_0 0x501 </v>
       </c>
     </row>
     <row r="184" spans="1:1">
       <c r="A184" t="str">
         <f>IF('Memory setup'!A149&lt;&gt;"",IF('Memory setup'!A149="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A149),IF('Memory setup'!E149=1,_xlfn.CONCAT("#define ",'Memory setup'!B149," ",'Memory setup'!C149," ",'Memory setup'!D149),""))</f>
-        <v xml:space="preserve">#define ADR_LOCALANALOG_MAX_2 0x505 </v>
+        <v xml:space="preserve">#define ADR_LOCALANALOG_MIN_1 0x502 </v>
       </c>
     </row>
     <row r="185" spans="1:1">
       <c r="A185" t="str">
         <f>IF('Memory setup'!A150&lt;&gt;"",IF('Memory setup'!A150="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A150),IF('Memory setup'!E150=1,_xlfn.CONCAT("#define ",'Memory setup'!B150," ",'Memory setup'!C150," ",'Memory setup'!D150),""))</f>
-        <v xml:space="preserve">#define ADR_LOCALANALOG_MIN_3 0x506 </v>
+        <v xml:space="preserve">#define ADR_LOCALANALOG_MAX_1 0x503 </v>
       </c>
     </row>
     <row r="186" spans="1:1">
       <c r="A186" t="str">
         <f>IF('Memory setup'!A151&lt;&gt;"",IF('Memory setup'!A151="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A151),IF('Memory setup'!E151=1,_xlfn.CONCAT("#define ",'Memory setup'!B151," ",'Memory setup'!C151," ",'Memory setup'!D151),""))</f>
-        <v xml:space="preserve">#define ADR_LOCALANALOG_MAX_3 0x507 </v>
+        <v xml:space="preserve">#define ADR_LOCALANALOG_MIN_2 0x504 </v>
       </c>
     </row>
     <row r="187" spans="1:1">
       <c r="A187" t="str">
         <f>IF('Memory setup'!A152&lt;&gt;"",IF('Memory setup'!A152="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A152),IF('Memory setup'!E152=1,_xlfn.CONCAT("#define ",'Memory setup'!B152," ",'Memory setup'!C152," ",'Memory setup'!D152),""))</f>
-        <v xml:space="preserve">#define ADR_LOCALANALOG_MIN_4 0x508 </v>
+        <v xml:space="preserve">#define ADR_LOCALANALOG_MAX_2 0x505 </v>
       </c>
     </row>
     <row r="188" spans="1:1">
       <c r="A188" t="str">
         <f>IF('Memory setup'!A153&lt;&gt;"",IF('Memory setup'!A153="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A153),IF('Memory setup'!E153=1,_xlfn.CONCAT("#define ",'Memory setup'!B153," ",'Memory setup'!C153," ",'Memory setup'!D153),""))</f>
-        <v xml:space="preserve">#define ADR_LOCALANALOG_MAX_4 0x509 </v>
+        <v xml:space="preserve">#define ADR_LOCALANALOG_MIN_3 0x506 </v>
       </c>
     </row>
     <row r="189" spans="1:1">
       <c r="A189" t="str">
         <f>IF('Memory setup'!A154&lt;&gt;"",IF('Memory setup'!A154="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A154),IF('Memory setup'!E154=1,_xlfn.CONCAT("#define ",'Memory setup'!B154," ",'Memory setup'!C154," ",'Memory setup'!D154),""))</f>
-        <v xml:space="preserve">#define ADR_LOCALANALOG_MIN_5 0x50A </v>
+        <v xml:space="preserve">#define ADR_LOCALANALOG_MAX_3 0x507 </v>
       </c>
     </row>
     <row r="190" spans="1:1">
       <c r="A190" t="str">
         <f>IF('Memory setup'!A155&lt;&gt;"",IF('Memory setup'!A155="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A155),IF('Memory setup'!E155=1,_xlfn.CONCAT("#define ",'Memory setup'!B155," ",'Memory setup'!C155," ",'Memory setup'!D155),""))</f>
-        <v xml:space="preserve">#define ADR_LOCALANALOG_MAX_5 0x50B </v>
+        <v xml:space="preserve">#define ADR_LOCALANALOG_MIN_4 0x508 </v>
       </c>
     </row>
     <row r="191" spans="1:1">
       <c r="A191" t="str">
         <f>IF('Memory setup'!A156&lt;&gt;"",IF('Memory setup'!A156="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A156),IF('Memory setup'!E156=1,_xlfn.CONCAT("#define ",'Memory setup'!B156," ",'Memory setup'!C156," ",'Memory setup'!D156),""))</f>
-        <v xml:space="preserve">#define ADR_LOCALANALOG_MIN_6 0x50C </v>
+        <v xml:space="preserve">#define ADR_LOCALANALOG_MAX_4 0x509 </v>
       </c>
     </row>
     <row r="192" spans="1:1">
       <c r="A192" t="str">
         <f>IF('Memory setup'!A157&lt;&gt;"",IF('Memory setup'!A157="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A157),IF('Memory setup'!E157=1,_xlfn.CONCAT("#define ",'Memory setup'!B157," ",'Memory setup'!C157," ",'Memory setup'!D157),""))</f>
-        <v xml:space="preserve">#define ADR_LOCALANALOG_MAX_6 0x50D </v>
+        <v xml:space="preserve">#define ADR_LOCALANALOG_MIN_5 0x50A </v>
       </c>
     </row>
     <row r="193" spans="1:1">
       <c r="A193" t="str">
         <f>IF('Memory setup'!A158&lt;&gt;"",IF('Memory setup'!A158="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A158),IF('Memory setup'!E158=1,_xlfn.CONCAT("#define ",'Memory setup'!B158," ",'Memory setup'!C158," ",'Memory setup'!D158),""))</f>
-        <v xml:space="preserve">#define ADR_LOCALANALOG_MIN_7 0x50E </v>
+        <v xml:space="preserve">#define ADR_LOCALANALOG_MAX_5 0x50B </v>
       </c>
     </row>
     <row r="194" spans="1:1">
       <c r="A194" t="str">
         <f>IF('Memory setup'!A159&lt;&gt;"",IF('Memory setup'!A159="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A159),IF('Memory setup'!E159=1,_xlfn.CONCAT("#define ",'Memory setup'!B159," ",'Memory setup'!C159," ",'Memory setup'!D159),""))</f>
-        <v xml:space="preserve">#define ADR_LOCALANALOG_MAX_7 0x50F </v>
+        <v xml:space="preserve">#define ADR_LOCALANALOG_MIN_6 0x50C </v>
       </c>
     </row>
     <row r="195" spans="1:1">
       <c r="A195" t="str">
         <f>IF('Memory setup'!A160&lt;&gt;"",IF('Memory setup'!A160="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A160),IF('Memory setup'!E160=1,_xlfn.CONCAT("#define ",'Memory setup'!B160," ",'Memory setup'!C160," ",'Memory setup'!D160),""))</f>
-        <v xml:space="preserve">#define ADR_ADS111X_MIN_0 0x510 </v>
+        <v xml:space="preserve">#define ADR_LOCALANALOG_MAX_6 0x50D </v>
       </c>
     </row>
     <row r="196" spans="1:1">
       <c r="A196" t="str">
         <f>IF('Memory setup'!A161&lt;&gt;"",IF('Memory setup'!A161="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A161),IF('Memory setup'!E161=1,_xlfn.CONCAT("#define ",'Memory setup'!B161," ",'Memory setup'!C161," ",'Memory setup'!D161),""))</f>
-        <v xml:space="preserve">#define ADR_ADS111X_MAX_0 0x511 </v>
+        <v xml:space="preserve">#define ADR_LOCALANALOG_MIN_7 0x50E </v>
       </c>
     </row>
     <row r="197" spans="1:1">
       <c r="A197" t="str">
         <f>IF('Memory setup'!A162&lt;&gt;"",IF('Memory setup'!A162="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A162),IF('Memory setup'!E162=1,_xlfn.CONCAT("#define ",'Memory setup'!B162," ",'Memory setup'!C162," ",'Memory setup'!D162),""))</f>
-        <v xml:space="preserve">#define ADR_ADS111X_MIN_1 0x512 </v>
+        <v xml:space="preserve">#define ADR_LOCALANALOG_MAX_7 0x50F </v>
       </c>
     </row>
     <row r="198" spans="1:1">
       <c r="A198" t="str">
         <f>IF('Memory setup'!A163&lt;&gt;"",IF('Memory setup'!A163="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A163),IF('Memory setup'!E163=1,_xlfn.CONCAT("#define ",'Memory setup'!B163," ",'Memory setup'!C163," ",'Memory setup'!D163),""))</f>
-        <v xml:space="preserve">#define ADR_ADS111X_MAX_1 0x513 </v>
+        <v xml:space="preserve">#define ADR_ADS111X_MIN_0 0x510 </v>
       </c>
     </row>
     <row r="199" spans="1:1">
       <c r="A199" t="str">
         <f>IF('Memory setup'!A164&lt;&gt;"",IF('Memory setup'!A164="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A164),IF('Memory setup'!E164=1,_xlfn.CONCAT("#define ",'Memory setup'!B164," ",'Memory setup'!C164," ",'Memory setup'!D164),""))</f>
-        <v xml:space="preserve">#define ADR_ADS111X_MIN_2 0x514 </v>
+        <v xml:space="preserve">#define ADR_ADS111X_MAX_0 0x511 </v>
       </c>
     </row>
     <row r="200" spans="1:1">
       <c r="A200" t="str">
         <f>IF('Memory setup'!A165&lt;&gt;"",IF('Memory setup'!A165="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A165),IF('Memory setup'!E165=1,_xlfn.CONCAT("#define ",'Memory setup'!B165," ",'Memory setup'!C165," ",'Memory setup'!D165),""))</f>
-        <v xml:space="preserve">#define ADR_ADS111X_MAX_2 0x515 </v>
+        <v xml:space="preserve">#define ADR_ADS111X_MIN_1 0x512 </v>
       </c>
     </row>
     <row r="201" spans="1:1">
       <c r="A201" t="str">
         <f>IF('Memory setup'!A166&lt;&gt;"",IF('Memory setup'!A166="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A166),IF('Memory setup'!E166=1,_xlfn.CONCAT("#define ",'Memory setup'!B166," ",'Memory setup'!C166," ",'Memory setup'!D166),""))</f>
-        <v xml:space="preserve">#define ADR_ADS111X_MIN_3 0x516 </v>
+        <v xml:space="preserve">#define ADR_ADS111X_MAX_1 0x513 </v>
       </c>
     </row>
     <row r="202" spans="1:1">
       <c r="A202" t="str">
         <f>IF('Memory setup'!A167&lt;&gt;"",IF('Memory setup'!A167="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A167),IF('Memory setup'!E167=1,_xlfn.CONCAT("#define ",'Memory setup'!B167," ",'Memory setup'!C167," ",'Memory setup'!D167),""))</f>
-        <v xml:space="preserve">#define ADR_ADS111X_MAX_3 0x517 </v>
+        <v xml:space="preserve">#define ADR_ADS111X_MIN_2 0x514 </v>
       </c>
     </row>
     <row r="203" spans="1:1">
       <c r="A203" t="str">
         <f>IF('Memory setup'!A168&lt;&gt;"",IF('Memory setup'!A168="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A168),IF('Memory setup'!E168=1,_xlfn.CONCAT("#define ",'Memory setup'!B168," ",'Memory setup'!C168," ",'Memory setup'!D168),""))</f>
-        <v>#endif /* EEPROM_ADDRESSES_H_ */</v>
+        <v xml:space="preserve">#define ADR_ADS111X_MAX_2 0x515 </v>
       </c>
     </row>
     <row r="204" spans="1:1">
       <c r="A204" t="str">
         <f>IF('Memory setup'!A169&lt;&gt;"",IF('Memory setup'!A169="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A169),IF('Memory setup'!E169=1,_xlfn.CONCAT("#define ",'Memory setup'!B169," ",'Memory setup'!C169," ",'Memory setup'!D169),""))</f>
-        <v/>
+        <v xml:space="preserve">#define ADR_ADS111X_MIN_3 0x516 </v>
       </c>
     </row>
     <row r="205" spans="1:1">
       <c r="A205" t="str">
         <f>IF('Memory setup'!A170&lt;&gt;"",IF('Memory setup'!A170="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A170),IF('Memory setup'!E170=1,_xlfn.CONCAT("#define ",'Memory setup'!B170," ",'Memory setup'!C170," ",'Memory setup'!D170),""))</f>
-        <v/>
+        <v xml:space="preserve">#define ADR_ADS111X_MAX_3 0x517 </v>
       </c>
     </row>
     <row r="206" spans="1:1">
       <c r="A206" t="str">
         <f>IF('Memory setup'!A171&lt;&gt;"",IF('Memory setup'!A171="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A171),IF('Memory setup'!E171=1,_xlfn.CONCAT("#define ",'Memory setup'!B171," ",'Memory setup'!C171," ",'Memory setup'!D171),""))</f>
-        <v/>
+        <v>#endif /* EEPROM_ADDRESSES_H_ */</v>
       </c>
     </row>
     <row r="207" spans="1:1">
@@ -5611,37 +5671,37 @@
     </row>
     <row r="221" spans="1:1">
       <c r="A221" t="str">
-        <f>IF('Memory setup'!A177&lt;&gt;"",IF('Memory setup'!A177="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A177),IF('Memory setup'!E177=1,_xlfn.CONCAT("#define ",'Memory setup'!B177," ",'Memory setup'!C177," ",'Memory setup'!D177),""))</f>
+        <f>IF('Memory setup'!A186&lt;&gt;"",IF('Memory setup'!A186="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A186),IF('Memory setup'!E186=1,_xlfn.CONCAT("#define ",'Memory setup'!B186," ",'Memory setup'!C186," ",'Memory setup'!D186),""))</f>
         <v/>
       </c>
     </row>
     <row r="222" spans="1:1">
       <c r="A222" t="str">
-        <f>IF('Memory setup'!A178&lt;&gt;"",IF('Memory setup'!A178="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A178),IF('Memory setup'!E178=1,_xlfn.CONCAT("#define ",'Memory setup'!B178," ",'Memory setup'!C178," ",'Memory setup'!D178),""))</f>
+        <f>IF('Memory setup'!A187&lt;&gt;"",IF('Memory setup'!A187="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A187),IF('Memory setup'!E187=1,_xlfn.CONCAT("#define ",'Memory setup'!B187," ",'Memory setup'!C187," ",'Memory setup'!D187),""))</f>
         <v/>
       </c>
     </row>
     <row r="223" spans="1:1">
       <c r="A223" t="str">
-        <f>IF('Memory setup'!A179&lt;&gt;"",IF('Memory setup'!A179="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A179),IF('Memory setup'!E179=1,_xlfn.CONCAT("#define ",'Memory setup'!B179," ",'Memory setup'!C179," ",'Memory setup'!D179),""))</f>
+        <f>IF('Memory setup'!A188&lt;&gt;"",IF('Memory setup'!A188="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A188),IF('Memory setup'!E188=1,_xlfn.CONCAT("#define ",'Memory setup'!B188," ",'Memory setup'!C188," ",'Memory setup'!D188),""))</f>
         <v/>
       </c>
     </row>
     <row r="224" spans="1:1">
       <c r="A224" t="str">
-        <f>IF('Memory setup'!A180&lt;&gt;"",IF('Memory setup'!A180="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A180),IF('Memory setup'!E180=1,_xlfn.CONCAT("#define ",'Memory setup'!B180," ",'Memory setup'!C180," ",'Memory setup'!D180),""))</f>
+        <f>IF('Memory setup'!A189&lt;&gt;"",IF('Memory setup'!A189="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A189),IF('Memory setup'!E189=1,_xlfn.CONCAT("#define ",'Memory setup'!B189," ",'Memory setup'!C189," ",'Memory setup'!D189),""))</f>
         <v/>
       </c>
     </row>
     <row r="225" spans="1:1">
       <c r="A225" t="str">
-        <f>IF('Memory setup'!A181&lt;&gt;"",IF('Memory setup'!A181="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A181),IF('Memory setup'!E181=1,_xlfn.CONCAT("#define ",'Memory setup'!B181," ",'Memory setup'!C181," ",'Memory setup'!D181),""))</f>
+        <f>IF('Memory setup'!A190&lt;&gt;"",IF('Memory setup'!A190="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A190),IF('Memory setup'!E190=1,_xlfn.CONCAT("#define ",'Memory setup'!B190," ",'Memory setup'!C190," ",'Memory setup'!D190),""))</f>
         <v/>
       </c>
     </row>
     <row r="226" spans="1:1">
       <c r="A226" t="str">
-        <f>IF('Memory setup'!A187&lt;&gt;"",IF('Memory setup'!A187="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A187),IF('Memory setup'!E187=1,_xlfn.CONCAT("#define ",'Memory setup'!B187," ",'Memory setup'!C187," ",'Memory setup'!D187),""))</f>
+        <f>IF('Memory setup'!A191&lt;&gt;"",IF('Memory setup'!A191="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A191),IF('Memory setup'!E191=1,_xlfn.CONCAT("#define ",'Memory setup'!B191," ",'Memory setup'!C191," ",'Memory setup'!D191),""))</f>
         <v/>
       </c>
     </row>
@@ -6313,8 +6373,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A15747F3-05ED-504F-B11C-F6CFE07DDC85}">
   <dimension ref="A1:C193"/>
   <sheetViews>
-    <sheetView topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="I186" sqref="I186"/>
+    <sheetView topLeftCell="A163" workbookViewId="0">
+      <selection activeCell="A187" sqref="A187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -7455,29 +7515,29 @@
     <row r="94" spans="1:3">
       <c r="A94" t="str">
         <f>IF('Memory setup'!A77&lt;&gt;"",IF('Memory setup'!A77&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A77,"};"),"")</f>
-        <v>// AXIS2</v>
+        <v/>
       </c>
       <c r="B94" t="str">
         <f>IF('Memory setup'!E77=1,'Memory setup'!B77,IF('Memory setup'!B77&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B77),""))</f>
-        <v/>
+        <v>ADR_TMC1_TRQ_FILT</v>
       </c>
       <c r="C94" t="str">
         <f>IF(AND(B94&lt;&gt;"",'Memory setup'!A78&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v/>
+        <v>,</v>
       </c>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" t="str">
         <f>IF('Memory setup'!A78&lt;&gt;"",IF('Memory setup'!A78&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A78,"};"),"")</f>
-        <v/>
+        <v>// AXIS2</v>
       </c>
       <c r="B95" t="str">
         <f>IF('Memory setup'!E78=1,'Memory setup'!B78,IF('Memory setup'!B78&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B78),""))</f>
-        <v>ADR_AXIS2_CONFIG</v>
+        <v/>
       </c>
       <c r="C95" t="str">
         <f>IF(AND(B95&lt;&gt;"",'Memory setup'!A79&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v>,</v>
+        <v/>
       </c>
     </row>
     <row r="96" spans="1:3">
@@ -7487,7 +7547,7 @@
       </c>
       <c r="B96" t="str">
         <f>IF('Memory setup'!E79=1,'Memory setup'!B79,IF('Memory setup'!B79&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B79),""))</f>
-        <v>ADR_AXIS2_POWER</v>
+        <v>ADR_AXIS2_CONFIG</v>
       </c>
       <c r="C96" t="str">
         <f>IF(AND(B96&lt;&gt;"",'Memory setup'!A80&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -7501,7 +7561,7 @@
       </c>
       <c r="B97" t="str">
         <f>IF('Memory setup'!E80=1,'Memory setup'!B80,IF('Memory setup'!B80&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B80),""))</f>
-        <v>ADR_AXIS2_DEGREES</v>
+        <v>ADR_AXIS2_POWER</v>
       </c>
       <c r="C97" t="str">
         <f>IF(AND(B97&lt;&gt;"",'Memory setup'!A81&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -7515,7 +7575,7 @@
       </c>
       <c r="B98" t="str">
         <f>IF('Memory setup'!E81=1,'Memory setup'!B81,IF('Memory setup'!B81&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B81),""))</f>
-        <v>ADR_AXIS2_MAX_SPEED</v>
+        <v>ADR_AXIS2_DEGREES</v>
       </c>
       <c r="C98" t="str">
         <f>IF(AND(B98&lt;&gt;"",'Memory setup'!A82&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -7529,7 +7589,7 @@
       </c>
       <c r="B99" t="str">
         <f>IF('Memory setup'!E82=1,'Memory setup'!B82,IF('Memory setup'!B82&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B82),""))</f>
-        <v>ADR_AXIS2_MAX_ACCEL</v>
+        <v>ADR_AXIS2_MAX_SPEED</v>
       </c>
       <c r="C99" t="str">
         <f>IF(AND(B99&lt;&gt;"",'Memory setup'!A83&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -7543,7 +7603,7 @@
       </c>
       <c r="B100" t="str">
         <f>IF('Memory setup'!E83=1,'Memory setup'!B83,IF('Memory setup'!B83&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B83),""))</f>
-        <v>ADR_AXIS2_ENDSTOP</v>
+        <v>ADR_AXIS2_MAX_ACCEL</v>
       </c>
       <c r="C100" t="str">
         <f>IF(AND(B100&lt;&gt;"",'Memory setup'!A84&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -7557,7 +7617,7 @@
       </c>
       <c r="B101" t="str">
         <f>IF('Memory setup'!E84=1,'Memory setup'!B84,IF('Memory setup'!B84&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B84),""))</f>
-        <v>ADR_AXIS2_EFFECTS1</v>
+        <v>ADR_AXIS2_ENDSTOP</v>
       </c>
       <c r="C101" t="str">
         <f>IF(AND(B101&lt;&gt;"",'Memory setup'!A85&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -7571,7 +7631,7 @@
       </c>
       <c r="B102" t="str">
         <f>IF('Memory setup'!E85=1,'Memory setup'!B85,IF('Memory setup'!B85&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B85),""))</f>
-        <v>ADR_AXIS2_SPEEDACCEL_FILTER</v>
+        <v>ADR_AXIS2_EFFECTS1</v>
       </c>
       <c r="C102" t="str">
         <f>IF(AND(B102&lt;&gt;"",'Memory setup'!A86&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -7585,7 +7645,7 @@
       </c>
       <c r="B103" t="str">
         <f>IF('Memory setup'!E86=1,'Memory setup'!B86,IF('Memory setup'!B86&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B86),""))</f>
-        <v>ADR_AXIS2_ENC_RATIO</v>
+        <v>ADR_AXIS2_SPEEDACCEL_FILTER</v>
       </c>
       <c r="C103" t="str">
         <f>IF(AND(B103&lt;&gt;"",'Memory setup'!A87&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -7595,29 +7655,29 @@
     <row r="104" spans="1:3">
       <c r="A104" t="str">
         <f>IF('Memory setup'!A87&lt;&gt;"",IF('Memory setup'!A87&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A87,"};"),"")</f>
-        <v>// TMC2</v>
+        <v/>
       </c>
       <c r="B104" t="str">
         <f>IF('Memory setup'!E87=1,'Memory setup'!B87,IF('Memory setup'!B87&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B87),""))</f>
-        <v/>
+        <v>ADR_AXIS2_ENC_RATIO</v>
       </c>
       <c r="C104" t="str">
         <f>IF(AND(B104&lt;&gt;"",'Memory setup'!A88&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v/>
+        <v>,</v>
       </c>
     </row>
     <row r="105" spans="1:3">
       <c r="A105" t="str">
         <f>IF('Memory setup'!A88&lt;&gt;"",IF('Memory setup'!A88&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A88,"};"),"")</f>
-        <v/>
+        <v>// TMC2</v>
       </c>
       <c r="B105" t="str">
         <f>IF('Memory setup'!E88=1,'Memory setup'!B88,IF('Memory setup'!B88&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B88),""))</f>
-        <v>ADR_TMC2_MOTCONF</v>
+        <v/>
       </c>
       <c r="C105" t="str">
         <f>IF(AND(B105&lt;&gt;"",'Memory setup'!A89&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v>,</v>
+        <v/>
       </c>
     </row>
     <row r="106" spans="1:3">
@@ -7627,7 +7687,7 @@
       </c>
       <c r="B106" t="str">
         <f>IF('Memory setup'!E89=1,'Memory setup'!B89,IF('Memory setup'!B89&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B89),""))</f>
-        <v>ADR_TMC2_CPR</v>
+        <v>ADR_TMC2_MOTCONF</v>
       </c>
       <c r="C106" t="str">
         <f>IF(AND(B106&lt;&gt;"",'Memory setup'!A90&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -7641,7 +7701,7 @@
       </c>
       <c r="B107" t="str">
         <f>IF('Memory setup'!E90=1,'Memory setup'!B90,IF('Memory setup'!B90&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B90),""))</f>
-        <v>ADR_TMC2_ENCA</v>
+        <v>ADR_TMC2_CPR</v>
       </c>
       <c r="C107" t="str">
         <f>IF(AND(B107&lt;&gt;"",'Memory setup'!A91&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -7655,7 +7715,7 @@
       </c>
       <c r="B108" t="str">
         <f>IF('Memory setup'!E91=1,'Memory setup'!B91,IF('Memory setup'!B91&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B91),""))</f>
-        <v>ADR_TMC2_ADC_I0_OFS</v>
+        <v>ADR_TMC2_ENCA</v>
       </c>
       <c r="C108" t="str">
         <f>IF(AND(B108&lt;&gt;"",'Memory setup'!A92&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -7669,7 +7729,7 @@
       </c>
       <c r="B109" t="str">
         <f>IF('Memory setup'!E92=1,'Memory setup'!B92,IF('Memory setup'!B92&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B92),""))</f>
-        <v>ADR_TMC2_ADC_I1_OFS</v>
+        <v>ADR_TMC2_ADC_I0_OFS</v>
       </c>
       <c r="C109" t="str">
         <f>IF(AND(B109&lt;&gt;"",'Memory setup'!A93&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -7683,7 +7743,7 @@
       </c>
       <c r="B110" t="str">
         <f>IF('Memory setup'!E93=1,'Memory setup'!B93,IF('Memory setup'!B93&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B93),""))</f>
-        <v>ADR_TMC2_ENC_OFFSET</v>
+        <v>ADR_TMC2_ADC_I1_OFS</v>
       </c>
       <c r="C110" t="str">
         <f>IF(AND(B110&lt;&gt;"",'Memory setup'!A94&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -7697,7 +7757,7 @@
       </c>
       <c r="B111" t="str">
         <f>IF('Memory setup'!E94=1,'Memory setup'!B94,IF('Memory setup'!B94&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B94),""))</f>
-        <v>ADR_TMC2_OFFSETFLUX</v>
+        <v>ADR_TMC2_ENC_OFFSET</v>
       </c>
       <c r="C111" t="str">
         <f>IF(AND(B111&lt;&gt;"",'Memory setup'!A95&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -7711,7 +7771,7 @@
       </c>
       <c r="B112" t="str">
         <f>IF('Memory setup'!E95=1,'Memory setup'!B95,IF('Memory setup'!B95&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B95),""))</f>
-        <v>ADR_TMC2_TORQUE_P</v>
+        <v>ADR_TMC2_OFFSETFLUX</v>
       </c>
       <c r="C112" t="str">
         <f>IF(AND(B112&lt;&gt;"",'Memory setup'!A96&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -7725,7 +7785,7 @@
       </c>
       <c r="B113" t="str">
         <f>IF('Memory setup'!E96=1,'Memory setup'!B96,IF('Memory setup'!B96&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B96),""))</f>
-        <v>ADR_TMC2_TORQUE_I</v>
+        <v>ADR_TMC2_TORQUE_P</v>
       </c>
       <c r="C113" t="str">
         <f>IF(AND(B113&lt;&gt;"",'Memory setup'!A97&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -7739,7 +7799,7 @@
       </c>
       <c r="B114" t="str">
         <f>IF('Memory setup'!E97=1,'Memory setup'!B97,IF('Memory setup'!B97&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B97),""))</f>
-        <v>ADR_TMC2_FLUX_P</v>
+        <v>ADR_TMC2_TORQUE_I</v>
       </c>
       <c r="C114" t="str">
         <f>IF(AND(B114&lt;&gt;"",'Memory setup'!A98&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -7753,7 +7813,7 @@
       </c>
       <c r="B115" t="str">
         <f>IF('Memory setup'!E98=1,'Memory setup'!B98,IF('Memory setup'!B98&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B98),""))</f>
-        <v>ADR_TMC2_FLUX_I</v>
+        <v>ADR_TMC2_FLUX_P</v>
       </c>
       <c r="C115" t="str">
         <f>IF(AND(B115&lt;&gt;"",'Memory setup'!A99&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -7767,7 +7827,7 @@
       </c>
       <c r="B116" t="str">
         <f>IF('Memory setup'!E99=1,'Memory setup'!B99,IF('Memory setup'!B99&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B99),""))</f>
-        <v>ADR_TMC2_PHIE_OFS</v>
+        <v>ADR_TMC2_FLUX_I</v>
       </c>
       <c r="C116" t="str">
         <f>IF(AND(B116&lt;&gt;"",'Memory setup'!A100&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -7777,15 +7837,15 @@
     <row r="117" spans="1:3">
       <c r="A117" t="str">
         <f>IF('Memory setup'!A100&lt;&gt;"",IF('Memory setup'!A100&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A100,"};"),"")</f>
-        <v>// AXIS3</v>
+        <v/>
       </c>
       <c r="B117" t="str">
         <f>IF('Memory setup'!E100=1,'Memory setup'!B100,IF('Memory setup'!B100&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B100),""))</f>
-        <v/>
+        <v>ADR_TMC2_PHIE_OFS</v>
       </c>
       <c r="C117" t="str">
         <f>IF(AND(B117&lt;&gt;"",'Memory setup'!A101&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v/>
+        <v>,</v>
       </c>
     </row>
     <row r="118" spans="1:3">
@@ -7795,7 +7855,7 @@
       </c>
       <c r="B118" t="str">
         <f>IF('Memory setup'!E101=1,'Memory setup'!B101,IF('Memory setup'!B101&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B101),""))</f>
-        <v>ADR_AXIS3_CONFIG</v>
+        <v>ADR_TMC2_TRQ_FILT</v>
       </c>
       <c r="C118" t="str">
         <f>IF(AND(B118&lt;&gt;"",'Memory setup'!A102&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -7805,15 +7865,15 @@
     <row r="119" spans="1:3">
       <c r="A119" t="str">
         <f>IF('Memory setup'!A102&lt;&gt;"",IF('Memory setup'!A102&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A102,"};"),"")</f>
-        <v/>
+        <v>// AXIS3</v>
       </c>
       <c r="B119" t="str">
         <f>IF('Memory setup'!E102=1,'Memory setup'!B102,IF('Memory setup'!B102&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B102),""))</f>
-        <v>ADR_AXIS3_POWER</v>
+        <v/>
       </c>
       <c r="C119" t="str">
         <f>IF(AND(B119&lt;&gt;"",'Memory setup'!A103&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v>,</v>
+        <v/>
       </c>
     </row>
     <row r="120" spans="1:3">
@@ -7823,7 +7883,7 @@
       </c>
       <c r="B120" t="str">
         <f>IF('Memory setup'!E103=1,'Memory setup'!B103,IF('Memory setup'!B103&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B103),""))</f>
-        <v>ADR_AXIS3_DEGREES</v>
+        <v>ADR_AXIS3_CONFIG</v>
       </c>
       <c r="C120" t="str">
         <f>IF(AND(B120&lt;&gt;"",'Memory setup'!A104&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -7837,7 +7897,7 @@
       </c>
       <c r="B121" t="str">
         <f>IF('Memory setup'!E104=1,'Memory setup'!B104,IF('Memory setup'!B104&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B104),""))</f>
-        <v>ADR_AXIS3_MAX_SPEED</v>
+        <v>ADR_AXIS3_POWER</v>
       </c>
       <c r="C121" t="str">
         <f>IF(AND(B121&lt;&gt;"",'Memory setup'!A105&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -7851,7 +7911,7 @@
       </c>
       <c r="B122" t="str">
         <f>IF('Memory setup'!E105=1,'Memory setup'!B105,IF('Memory setup'!B105&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B105),""))</f>
-        <v>ADR_AXIS3_MAX_ACCEL</v>
+        <v>ADR_AXIS3_DEGREES</v>
       </c>
       <c r="C122" t="str">
         <f>IF(AND(B122&lt;&gt;"",'Memory setup'!A106&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -7865,7 +7925,7 @@
       </c>
       <c r="B123" t="str">
         <f>IF('Memory setup'!E106=1,'Memory setup'!B106,IF('Memory setup'!B106&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B106),""))</f>
-        <v>ADR_AXIS3_ENDSTOP</v>
+        <v>ADR_AXIS3_MAX_SPEED</v>
       </c>
       <c r="C123" t="str">
         <f>IF(AND(B123&lt;&gt;"",'Memory setup'!A107&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -7879,7 +7939,7 @@
       </c>
       <c r="B124" t="str">
         <f>IF('Memory setup'!E107=1,'Memory setup'!B107,IF('Memory setup'!B107&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B107),""))</f>
-        <v>ADR_AXIS3_EFFECTS1</v>
+        <v>ADR_AXIS3_MAX_ACCEL</v>
       </c>
       <c r="C124" t="str">
         <f>IF(AND(B124&lt;&gt;"",'Memory setup'!A108&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -7893,7 +7953,7 @@
       </c>
       <c r="B125" t="str">
         <f>IF('Memory setup'!E108=1,'Memory setup'!B108,IF('Memory setup'!B108&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B108),""))</f>
-        <v>ADR_AXIS3_SPEEDACCEL_FILTER</v>
+        <v>ADR_AXIS3_ENDSTOP</v>
       </c>
       <c r="C125" t="str">
         <f>IF(AND(B125&lt;&gt;"",'Memory setup'!A109&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -7907,7 +7967,7 @@
       </c>
       <c r="B126" t="str">
         <f>IF('Memory setup'!E109=1,'Memory setup'!B109,IF('Memory setup'!B109&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B109),""))</f>
-        <v>ADR_AXIS3_ENC_RATIO</v>
+        <v>ADR_AXIS3_EFFECTS1</v>
       </c>
       <c r="C126" t="str">
         <f>IF(AND(B126&lt;&gt;"",'Memory setup'!A110&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -7917,15 +7977,15 @@
     <row r="127" spans="1:3">
       <c r="A127" t="str">
         <f>IF('Memory setup'!A110&lt;&gt;"",IF('Memory setup'!A110&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A110,"};"),"")</f>
-        <v>// TMC3</v>
+        <v/>
       </c>
       <c r="B127" t="str">
         <f>IF('Memory setup'!E110=1,'Memory setup'!B110,IF('Memory setup'!B110&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B110),""))</f>
-        <v/>
+        <v>ADR_AXIS3_SPEEDACCEL_FILTER</v>
       </c>
       <c r="C127" t="str">
         <f>IF(AND(B127&lt;&gt;"",'Memory setup'!A111&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v/>
+        <v>,</v>
       </c>
     </row>
     <row r="128" spans="1:3">
@@ -7935,7 +7995,7 @@
       </c>
       <c r="B128" t="str">
         <f>IF('Memory setup'!E111=1,'Memory setup'!B111,IF('Memory setup'!B111&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B111),""))</f>
-        <v>ADR_TMC3_MOTCONF</v>
+        <v>ADR_AXIS3_ENC_RATIO</v>
       </c>
       <c r="C128" t="str">
         <f>IF(AND(B128&lt;&gt;"",'Memory setup'!A112&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -7945,15 +8005,15 @@
     <row r="129" spans="1:3">
       <c r="A129" t="str">
         <f>IF('Memory setup'!A112&lt;&gt;"",IF('Memory setup'!A112&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A112,"};"),"")</f>
-        <v/>
+        <v>// TMC3</v>
       </c>
       <c r="B129" t="str">
         <f>IF('Memory setup'!E112=1,'Memory setup'!B112,IF('Memory setup'!B112&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B112),""))</f>
-        <v>ADR_TMC3_CPR</v>
+        <v/>
       </c>
       <c r="C129" t="str">
         <f>IF(AND(B129&lt;&gt;"",'Memory setup'!A113&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v>,</v>
+        <v/>
       </c>
     </row>
     <row r="130" spans="1:3">
@@ -7963,7 +8023,7 @@
       </c>
       <c r="B130" t="str">
         <f>IF('Memory setup'!E113=1,'Memory setup'!B113,IF('Memory setup'!B113&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B113),""))</f>
-        <v>ADR_TMC3_ENCA</v>
+        <v>ADR_TMC3_MOTCONF</v>
       </c>
       <c r="C130" t="str">
         <f>IF(AND(B130&lt;&gt;"",'Memory setup'!A114&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -7977,7 +8037,7 @@
       </c>
       <c r="B131" t="str">
         <f>IF('Memory setup'!E114=1,'Memory setup'!B114,IF('Memory setup'!B114&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B114),""))</f>
-        <v>ADR_TMC3_ADC_I0_OFS</v>
+        <v>ADR_TMC3_CPR</v>
       </c>
       <c r="C131" t="str">
         <f>IF(AND(B131&lt;&gt;"",'Memory setup'!A115&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -7991,7 +8051,7 @@
       </c>
       <c r="B132" t="str">
         <f>IF('Memory setup'!E115=1,'Memory setup'!B115,IF('Memory setup'!B115&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B115),""))</f>
-        <v>ADR_TMC3_ADC_I1_OFS</v>
+        <v>ADR_TMC3_ENCA</v>
       </c>
       <c r="C132" t="str">
         <f>IF(AND(B132&lt;&gt;"",'Memory setup'!A116&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8005,7 +8065,7 @@
       </c>
       <c r="B133" t="str">
         <f>IF('Memory setup'!E116=1,'Memory setup'!B116,IF('Memory setup'!B116&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B116),""))</f>
-        <v>ADR_TMC3_ENC_OFFSET</v>
+        <v>ADR_TMC3_ADC_I0_OFS</v>
       </c>
       <c r="C133" t="str">
         <f>IF(AND(B133&lt;&gt;"",'Memory setup'!A117&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8019,7 +8079,7 @@
       </c>
       <c r="B134" t="str">
         <f>IF('Memory setup'!E117=1,'Memory setup'!B117,IF('Memory setup'!B117&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B117),""))</f>
-        <v>ADR_TMC3_OFFSETFLUX</v>
+        <v>ADR_TMC3_ADC_I1_OFS</v>
       </c>
       <c r="C134" t="str">
         <f>IF(AND(B134&lt;&gt;"",'Memory setup'!A118&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8033,7 +8093,7 @@
       </c>
       <c r="B135" t="str">
         <f>IF('Memory setup'!E118=1,'Memory setup'!B118,IF('Memory setup'!B118&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B118),""))</f>
-        <v>ADR_TMC3_TORQUE_P</v>
+        <v>ADR_TMC3_ENC_OFFSET</v>
       </c>
       <c r="C135" t="str">
         <f>IF(AND(B135&lt;&gt;"",'Memory setup'!A119&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8047,7 +8107,7 @@
       </c>
       <c r="B136" t="str">
         <f>IF('Memory setup'!E119=1,'Memory setup'!B119,IF('Memory setup'!B119&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B119),""))</f>
-        <v>ADR_TMC3_TORQUE_I</v>
+        <v>ADR_TMC3_OFFSETFLUX</v>
       </c>
       <c r="C136" t="str">
         <f>IF(AND(B136&lt;&gt;"",'Memory setup'!A120&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8061,7 +8121,7 @@
       </c>
       <c r="B137" t="str">
         <f>IF('Memory setup'!E120=1,'Memory setup'!B120,IF('Memory setup'!B120&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B120),""))</f>
-        <v>ADR_TMC3_FLUX_P</v>
+        <v>ADR_TMC3_TORQUE_P</v>
       </c>
       <c r="C137" t="str">
         <f>IF(AND(B137&lt;&gt;"",'Memory setup'!A121&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8075,7 +8135,7 @@
       </c>
       <c r="B138" t="str">
         <f>IF('Memory setup'!E121=1,'Memory setup'!B121,IF('Memory setup'!B121&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B121),""))</f>
-        <v>ADR_TMC3_FLUX_I</v>
+        <v>ADR_TMC3_TORQUE_I</v>
       </c>
       <c r="C138" t="str">
         <f>IF(AND(B138&lt;&gt;"",'Memory setup'!A122&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8089,7 +8149,7 @@
       </c>
       <c r="B139" t="str">
         <f>IF('Memory setup'!E122=1,'Memory setup'!B122,IF('Memory setup'!B122&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B122),""))</f>
-        <v>ADR_TMC3_PHIE_OFS</v>
+        <v>ADR_TMC3_FLUX_P</v>
       </c>
       <c r="C139" t="str">
         <f>IF(AND(B139&lt;&gt;"",'Memory setup'!A123&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8099,15 +8159,15 @@
     <row r="140" spans="1:3">
       <c r="A140" t="str">
         <f>IF('Memory setup'!A123&lt;&gt;"",IF('Memory setup'!A123&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A123,"};"),"")</f>
-        <v>// Odrive</v>
+        <v/>
       </c>
       <c r="B140" t="str">
         <f>IF('Memory setup'!E123=1,'Memory setup'!B123,IF('Memory setup'!B123&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B123),""))</f>
-        <v/>
+        <v>ADR_TMC3_FLUX_I</v>
       </c>
       <c r="C140" t="str">
         <f>IF(AND(B140&lt;&gt;"",'Memory setup'!A124&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v/>
+        <v>,</v>
       </c>
     </row>
     <row r="141" spans="1:3">
@@ -8117,7 +8177,7 @@
       </c>
       <c r="B141" t="str">
         <f>IF('Memory setup'!E124=1,'Memory setup'!B124,IF('Memory setup'!B124&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B124),""))</f>
-        <v>ADR_ODRIVE_CANID</v>
+        <v>ADR_TMC3_PHIE_OFS</v>
       </c>
       <c r="C141" t="str">
         <f>IF(AND(B141&lt;&gt;"",'Memory setup'!A125&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8131,7 +8191,7 @@
       </c>
       <c r="B142" t="str">
         <f>IF('Memory setup'!E125=1,'Memory setup'!B125,IF('Memory setup'!B125&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B125),""))</f>
-        <v>ADR_ODRIVE_SETTING1_M0</v>
+        <v>ADR_TMC3_TRQ_FILT</v>
       </c>
       <c r="C142" t="str">
         <f>IF(AND(B142&lt;&gt;"",'Memory setup'!A126&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8141,29 +8201,29 @@
     <row r="143" spans="1:3">
       <c r="A143" t="str">
         <f>IF('Memory setup'!A126&lt;&gt;"",IF('Memory setup'!A126&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A126,"};"),"")</f>
-        <v/>
+        <v>// Odrive</v>
       </c>
       <c r="B143" t="str">
         <f>IF('Memory setup'!E126=1,'Memory setup'!B126,IF('Memory setup'!B126&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B126),""))</f>
-        <v>ADR_ODRIVE_SETTING1_M1</v>
+        <v/>
       </c>
       <c r="C143" t="str">
         <f>IF(AND(B143&lt;&gt;"",'Memory setup'!A127&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v>,</v>
+        <v/>
       </c>
     </row>
     <row r="144" spans="1:3">
       <c r="A144" t="str">
         <f>IF('Memory setup'!A127&lt;&gt;"",IF('Memory setup'!A127&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A127,"};"),"")</f>
-        <v>// VESC Section</v>
+        <v/>
       </c>
       <c r="B144" t="str">
         <f>IF('Memory setup'!E127=1,'Memory setup'!B127,IF('Memory setup'!B127&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B127),""))</f>
-        <v/>
+        <v>ADR_ODRIVE_CANID</v>
       </c>
       <c r="C144" t="str">
         <f>IF(AND(B144&lt;&gt;"",'Memory setup'!A128&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v/>
+        <v>,</v>
       </c>
     </row>
     <row r="145" spans="1:3">
@@ -8173,7 +8233,7 @@
       </c>
       <c r="B145" t="str">
         <f>IF('Memory setup'!E128=1,'Memory setup'!B128,IF('Memory setup'!B128&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B128),""))</f>
-        <v>ADR_VESC1_CANID</v>
+        <v>ADR_ODRIVE_SETTING1_M0</v>
       </c>
       <c r="C145" t="str">
         <f>IF(AND(B145&lt;&gt;"",'Memory setup'!A129&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8187,7 +8247,7 @@
       </c>
       <c r="B146" t="str">
         <f>IF('Memory setup'!E129=1,'Memory setup'!B129,IF('Memory setup'!B129&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B129),""))</f>
-        <v>ADR_VESC1_DATA</v>
+        <v>ADR_ODRIVE_SETTING1_M1</v>
       </c>
       <c r="C146" t="str">
         <f>IF(AND(B146&lt;&gt;"",'Memory setup'!A130&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8197,15 +8257,15 @@
     <row r="147" spans="1:3">
       <c r="A147" t="str">
         <f>IF('Memory setup'!A130&lt;&gt;"",IF('Memory setup'!A130&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A130,"};"),"")</f>
-        <v/>
+        <v>// VESC Section</v>
       </c>
       <c r="B147" t="str">
         <f>IF('Memory setup'!E130=1,'Memory setup'!B130,IF('Memory setup'!B130&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B130),""))</f>
-        <v>ADR_VESC1_OFFSET</v>
+        <v/>
       </c>
       <c r="C147" t="str">
         <f>IF(AND(B147&lt;&gt;"",'Memory setup'!A131&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v>,</v>
+        <v/>
       </c>
     </row>
     <row r="148" spans="1:3">
@@ -8215,7 +8275,7 @@
       </c>
       <c r="B148" t="str">
         <f>IF('Memory setup'!E131=1,'Memory setup'!B131,IF('Memory setup'!B131&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B131),""))</f>
-        <v>ADR_VESC2_CANID</v>
+        <v>ADR_VESC1_CANID</v>
       </c>
       <c r="C148" t="str">
         <f>IF(AND(B148&lt;&gt;"",'Memory setup'!A132&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8229,7 +8289,7 @@
       </c>
       <c r="B149" t="str">
         <f>IF('Memory setup'!E132=1,'Memory setup'!B132,IF('Memory setup'!B132&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B132),""))</f>
-        <v>ADR_VESC2_DATA</v>
+        <v>ADR_VESC1_DATA</v>
       </c>
       <c r="C149" t="str">
         <f>IF(AND(B149&lt;&gt;"",'Memory setup'!A133&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8243,7 +8303,7 @@
       </c>
       <c r="B150" t="str">
         <f>IF('Memory setup'!E133=1,'Memory setup'!B133,IF('Memory setup'!B133&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B133),""))</f>
-        <v>ADR_VESC2_OFFSET</v>
+        <v>ADR_VESC1_OFFSET</v>
       </c>
       <c r="C150" t="str">
         <f>IF(AND(B150&lt;&gt;"",'Memory setup'!A134&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8257,7 +8317,7 @@
       </c>
       <c r="B151" t="str">
         <f>IF('Memory setup'!E134=1,'Memory setup'!B134,IF('Memory setup'!B134&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B134),""))</f>
-        <v>ADR_VESC3_CANID</v>
+        <v>ADR_VESC2_CANID</v>
       </c>
       <c r="C151" t="str">
         <f>IF(AND(B151&lt;&gt;"",'Memory setup'!A135&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8271,7 +8331,7 @@
       </c>
       <c r="B152" t="str">
         <f>IF('Memory setup'!E135=1,'Memory setup'!B135,IF('Memory setup'!B135&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B135),""))</f>
-        <v>ADR_VESC3_DATA</v>
+        <v>ADR_VESC2_DATA</v>
       </c>
       <c r="C152" t="str">
         <f>IF(AND(B152&lt;&gt;"",'Memory setup'!A136&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8285,7 +8345,7 @@
       </c>
       <c r="B153" t="str">
         <f>IF('Memory setup'!E136=1,'Memory setup'!B136,IF('Memory setup'!B136&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B136),""))</f>
-        <v>ADR_VESC3_OFFSET</v>
+        <v>ADR_VESC2_OFFSET</v>
       </c>
       <c r="C153" t="str">
         <f>IF(AND(B153&lt;&gt;"",'Memory setup'!A137&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8295,15 +8355,15 @@
     <row r="154" spans="1:3">
       <c r="A154" t="str">
         <f>IF('Memory setup'!A137&lt;&gt;"",IF('Memory setup'!A137&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A137,"};"),"")</f>
-        <v>//MT Encoder</v>
+        <v/>
       </c>
       <c r="B154" t="str">
         <f>IF('Memory setup'!E137=1,'Memory setup'!B137,IF('Memory setup'!B137&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B137),""))</f>
-        <v/>
+        <v>ADR_VESC3_CANID</v>
       </c>
       <c r="C154" t="str">
         <f>IF(AND(B154&lt;&gt;"",'Memory setup'!A138&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v/>
+        <v>,</v>
       </c>
     </row>
     <row r="155" spans="1:3">
@@ -8313,7 +8373,7 @@
       </c>
       <c r="B155" t="str">
         <f>IF('Memory setup'!E138=1,'Memory setup'!B138,IF('Memory setup'!B138&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B138),""))</f>
-        <v>ADR_MTENC_OFS</v>
+        <v>ADR_VESC3_DATA</v>
       </c>
       <c r="C155" t="str">
         <f>IF(AND(B155&lt;&gt;"",'Memory setup'!A139&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8327,7 +8387,7 @@
       </c>
       <c r="B156" t="str">
         <f>IF('Memory setup'!E139=1,'Memory setup'!B139,IF('Memory setup'!B139&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B139),""))</f>
-        <v>ADR_MTENC_CONF1</v>
+        <v>ADR_VESC3_OFFSET</v>
       </c>
       <c r="C156" t="str">
         <f>IF(AND(B156&lt;&gt;"",'Memory setup'!A140&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8337,7 +8397,7 @@
     <row r="157" spans="1:3">
       <c r="A157" t="str">
         <f>IF('Memory setup'!A140&lt;&gt;"",IF('Memory setup'!A140&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A140,"};"),"")</f>
-        <v>// Biss-C</v>
+        <v>//MT Encoder</v>
       </c>
       <c r="B157" t="str">
         <f>IF('Memory setup'!E140=1,'Memory setup'!B140,IF('Memory setup'!B140&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B140),""))</f>
@@ -8355,7 +8415,7 @@
       </c>
       <c r="B158" t="str">
         <f>IF('Memory setup'!E141=1,'Memory setup'!B141,IF('Memory setup'!B141&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B141),""))</f>
-        <v>ADR_BISSENC_CONF1</v>
+        <v>ADR_MTENC_OFS</v>
       </c>
       <c r="C158" t="str">
         <f>IF(AND(B158&lt;&gt;"",'Memory setup'!A142&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8369,7 +8429,7 @@
       </c>
       <c r="B159" t="str">
         <f>IF('Memory setup'!E142=1,'Memory setup'!B142,IF('Memory setup'!B142&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B142),""))</f>
-        <v>ADR_BISSENC_OFS</v>
+        <v>ADR_MTENC_CONF1</v>
       </c>
       <c r="C159" t="str">
         <f>IF(AND(B159&lt;&gt;"",'Memory setup'!A143&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8379,7 +8439,7 @@
     <row r="160" spans="1:3">
       <c r="A160" t="str">
         <f>IF('Memory setup'!A143&lt;&gt;"",IF('Memory setup'!A143&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A143,"};"),"")</f>
-        <v>// Analog min/max calibrations</v>
+        <v>// Biss-C</v>
       </c>
       <c r="B160" t="str">
         <f>IF('Memory setup'!E143=1,'Memory setup'!B143,IF('Memory setup'!B143&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B143),""))</f>
@@ -8397,7 +8457,7 @@
       </c>
       <c r="B161" t="str">
         <f>IF('Memory setup'!E144=1,'Memory setup'!B144,IF('Memory setup'!B144&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B144),""))</f>
-        <v>ADR_LOCALANALOG_MIN_0</v>
+        <v>ADR_BISSENC_CONF1</v>
       </c>
       <c r="C161" t="str">
         <f>IF(AND(B161&lt;&gt;"",'Memory setup'!A145&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8411,7 +8471,7 @@
       </c>
       <c r="B162" t="str">
         <f>IF('Memory setup'!E145=1,'Memory setup'!B145,IF('Memory setup'!B145&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B145),""))</f>
-        <v>ADR_LOCALANALOG_MAX_0</v>
+        <v>ADR_BISSENC_OFS</v>
       </c>
       <c r="C162" t="str">
         <f>IF(AND(B162&lt;&gt;"",'Memory setup'!A146&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8421,15 +8481,15 @@
     <row r="163" spans="1:3">
       <c r="A163" t="str">
         <f>IF('Memory setup'!A146&lt;&gt;"",IF('Memory setup'!A146&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A146,"};"),"")</f>
-        <v/>
+        <v>// Analog min/max calibrations</v>
       </c>
       <c r="B163" t="str">
         <f>IF('Memory setup'!E146=1,'Memory setup'!B146,IF('Memory setup'!B146&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B146),""))</f>
-        <v>ADR_LOCALANALOG_MIN_1</v>
+        <v/>
       </c>
       <c r="C163" t="str">
         <f>IF(AND(B163&lt;&gt;"",'Memory setup'!A147&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v>,</v>
+        <v/>
       </c>
     </row>
     <row r="164" spans="1:3">
@@ -8439,7 +8499,7 @@
       </c>
       <c r="B164" t="str">
         <f>IF('Memory setup'!E147=1,'Memory setup'!B147,IF('Memory setup'!B147&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B147),""))</f>
-        <v>ADR_LOCALANALOG_MAX_1</v>
+        <v>ADR_LOCALANALOG_MIN_0</v>
       </c>
       <c r="C164" t="str">
         <f>IF(AND(B164&lt;&gt;"",'Memory setup'!A148&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8453,7 +8513,7 @@
       </c>
       <c r="B165" t="str">
         <f>IF('Memory setup'!E148=1,'Memory setup'!B148,IF('Memory setup'!B148&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B148),""))</f>
-        <v>ADR_LOCALANALOG_MIN_2</v>
+        <v>ADR_LOCALANALOG_MAX_0</v>
       </c>
       <c r="C165" t="str">
         <f>IF(AND(B165&lt;&gt;"",'Memory setup'!A149&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8467,7 +8527,7 @@
       </c>
       <c r="B166" t="str">
         <f>IF('Memory setup'!E149=1,'Memory setup'!B149,IF('Memory setup'!B149&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B149),""))</f>
-        <v>ADR_LOCALANALOG_MAX_2</v>
+        <v>ADR_LOCALANALOG_MIN_1</v>
       </c>
       <c r="C166" t="str">
         <f>IF(AND(B166&lt;&gt;"",'Memory setup'!A150&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8481,7 +8541,7 @@
       </c>
       <c r="B167" t="str">
         <f>IF('Memory setup'!E150=1,'Memory setup'!B150,IF('Memory setup'!B150&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B150),""))</f>
-        <v>ADR_LOCALANALOG_MIN_3</v>
+        <v>ADR_LOCALANALOG_MAX_1</v>
       </c>
       <c r="C167" t="str">
         <f>IF(AND(B167&lt;&gt;"",'Memory setup'!A151&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8495,7 +8555,7 @@
       </c>
       <c r="B168" t="str">
         <f>IF('Memory setup'!E151=1,'Memory setup'!B151,IF('Memory setup'!B151&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B151),""))</f>
-        <v>ADR_LOCALANALOG_MAX_3</v>
+        <v>ADR_LOCALANALOG_MIN_2</v>
       </c>
       <c r="C168" t="str">
         <f>IF(AND(B168&lt;&gt;"",'Memory setup'!A152&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8509,7 +8569,7 @@
       </c>
       <c r="B169" t="str">
         <f>IF('Memory setup'!E152=1,'Memory setup'!B152,IF('Memory setup'!B152&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B152),""))</f>
-        <v>ADR_LOCALANALOG_MIN_4</v>
+        <v>ADR_LOCALANALOG_MAX_2</v>
       </c>
       <c r="C169" t="str">
         <f>IF(AND(B169&lt;&gt;"",'Memory setup'!A153&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8523,7 +8583,7 @@
       </c>
       <c r="B170" t="str">
         <f>IF('Memory setup'!E153=1,'Memory setup'!B153,IF('Memory setup'!B153&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B153),""))</f>
-        <v>ADR_LOCALANALOG_MAX_4</v>
+        <v>ADR_LOCALANALOG_MIN_3</v>
       </c>
       <c r="C170" t="str">
         <f>IF(AND(B170&lt;&gt;"",'Memory setup'!A154&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8537,7 +8597,7 @@
       </c>
       <c r="B171" t="str">
         <f>IF('Memory setup'!E154=1,'Memory setup'!B154,IF('Memory setup'!B154&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B154),""))</f>
-        <v>ADR_LOCALANALOG_MIN_5</v>
+        <v>ADR_LOCALANALOG_MAX_3</v>
       </c>
       <c r="C171" t="str">
         <f>IF(AND(B171&lt;&gt;"",'Memory setup'!A155&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8551,7 +8611,7 @@
       </c>
       <c r="B172" t="str">
         <f>IF('Memory setup'!E155=1,'Memory setup'!B155,IF('Memory setup'!B155&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B155),""))</f>
-        <v>ADR_LOCALANALOG_MAX_5</v>
+        <v>ADR_LOCALANALOG_MIN_4</v>
       </c>
       <c r="C172" t="str">
         <f>IF(AND(B172&lt;&gt;"",'Memory setup'!A156&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8565,7 +8625,7 @@
       </c>
       <c r="B173" t="str">
         <f>IF('Memory setup'!E156=1,'Memory setup'!B156,IF('Memory setup'!B156&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B156),""))</f>
-        <v>ADR_LOCALANALOG_MIN_6</v>
+        <v>ADR_LOCALANALOG_MAX_4</v>
       </c>
       <c r="C173" t="str">
         <f>IF(AND(B173&lt;&gt;"",'Memory setup'!A157&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8579,7 +8639,7 @@
       </c>
       <c r="B174" t="str">
         <f>IF('Memory setup'!E157=1,'Memory setup'!B157,IF('Memory setup'!B157&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B157),""))</f>
-        <v>ADR_LOCALANALOG_MAX_6</v>
+        <v>ADR_LOCALANALOG_MIN_5</v>
       </c>
       <c r="C174" t="str">
         <f>IF(AND(B174&lt;&gt;"",'Memory setup'!A158&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8593,7 +8653,7 @@
       </c>
       <c r="B175" t="str">
         <f>IF('Memory setup'!E158=1,'Memory setup'!B158,IF('Memory setup'!B158&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B158),""))</f>
-        <v>ADR_LOCALANALOG_MIN_7</v>
+        <v>ADR_LOCALANALOG_MAX_5</v>
       </c>
       <c r="C175" t="str">
         <f>IF(AND(B175&lt;&gt;"",'Memory setup'!A159&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8607,7 +8667,7 @@
       </c>
       <c r="B176" t="str">
         <f>IF('Memory setup'!E159=1,'Memory setup'!B159,IF('Memory setup'!B159&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B159),""))</f>
-        <v>ADR_LOCALANALOG_MAX_7</v>
+        <v>ADR_LOCALANALOG_MIN_6</v>
       </c>
       <c r="C176" t="str">
         <f>IF(AND(B176&lt;&gt;"",'Memory setup'!A160&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8621,7 +8681,7 @@
       </c>
       <c r="B177" t="str">
         <f>IF('Memory setup'!E160=1,'Memory setup'!B160,IF('Memory setup'!B160&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B160),""))</f>
-        <v>ADR_ADS111X_MIN_0</v>
+        <v>ADR_LOCALANALOG_MAX_6</v>
       </c>
       <c r="C177" t="str">
         <f>IF(AND(B177&lt;&gt;"",'Memory setup'!A161&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8635,7 +8695,7 @@
       </c>
       <c r="B178" t="str">
         <f>IF('Memory setup'!E161=1,'Memory setup'!B161,IF('Memory setup'!B161&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B161),""))</f>
-        <v>ADR_ADS111X_MAX_0</v>
+        <v>ADR_LOCALANALOG_MIN_7</v>
       </c>
       <c r="C178" t="str">
         <f>IF(AND(B178&lt;&gt;"",'Memory setup'!A162&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8649,7 +8709,7 @@
       </c>
       <c r="B179" t="str">
         <f>IF('Memory setup'!E162=1,'Memory setup'!B162,IF('Memory setup'!B162&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B162),""))</f>
-        <v>ADR_ADS111X_MIN_1</v>
+        <v>ADR_LOCALANALOG_MAX_7</v>
       </c>
       <c r="C179" t="str">
         <f>IF(AND(B179&lt;&gt;"",'Memory setup'!A163&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8663,7 +8723,7 @@
       </c>
       <c r="B180" t="str">
         <f>IF('Memory setup'!E163=1,'Memory setup'!B163,IF('Memory setup'!B163&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B163),""))</f>
-        <v>ADR_ADS111X_MAX_1</v>
+        <v>ADR_ADS111X_MIN_0</v>
       </c>
       <c r="C180" t="str">
         <f>IF(AND(B180&lt;&gt;"",'Memory setup'!A164&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8677,7 +8737,7 @@
       </c>
       <c r="B181" t="str">
         <f>IF('Memory setup'!E164=1,'Memory setup'!B164,IF('Memory setup'!B164&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B164),""))</f>
-        <v>ADR_ADS111X_MIN_2</v>
+        <v>ADR_ADS111X_MAX_0</v>
       </c>
       <c r="C181" t="str">
         <f>IF(AND(B181&lt;&gt;"",'Memory setup'!A165&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8691,7 +8751,7 @@
       </c>
       <c r="B182" t="str">
         <f>IF('Memory setup'!E165=1,'Memory setup'!B165,IF('Memory setup'!B165&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B165),""))</f>
-        <v>ADR_ADS111X_MAX_2</v>
+        <v>ADR_ADS111X_MIN_1</v>
       </c>
       <c r="C182" t="str">
         <f>IF(AND(B182&lt;&gt;"",'Memory setup'!A166&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8705,7 +8765,7 @@
       </c>
       <c r="B183" t="str">
         <f>IF('Memory setup'!E166=1,'Memory setup'!B166,IF('Memory setup'!B166&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B166),""))</f>
-        <v>ADR_ADS111X_MIN_3</v>
+        <v>ADR_ADS111X_MAX_1</v>
       </c>
       <c r="C183" t="str">
         <f>IF(AND(B183&lt;&gt;"",'Memory setup'!A167&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8719,25 +8779,25 @@
       </c>
       <c r="B184" t="str">
         <f>IF('Memory setup'!E167=1,'Memory setup'!B167,IF('Memory setup'!B167&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B167),""))</f>
-        <v>ADR_ADS111X_MAX_3</v>
+        <v>ADR_ADS111X_MIN_2</v>
       </c>
       <c r="C184" t="str">
         <f>IF(AND(B184&lt;&gt;"",'Memory setup'!A168&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v/>
+        <v>,</v>
       </c>
     </row>
     <row r="185" spans="1:3">
       <c r="A185" t="str">
         <f>IF('Memory setup'!A168&lt;&gt;"",IF('Memory setup'!A168&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A168,"};"),"")</f>
-        <v>};</v>
+        <v/>
       </c>
       <c r="B185" t="str">
         <f>IF('Memory setup'!E168=1,'Memory setup'!B168,IF('Memory setup'!B168&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B168),""))</f>
-        <v/>
+        <v>ADR_ADS111X_MAX_2</v>
       </c>
       <c r="C185" t="str">
         <f>IF(AND(B185&lt;&gt;"",'Memory setup'!A169&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v/>
+        <v>,</v>
       </c>
     </row>
     <row r="186" spans="1:3">
@@ -8747,11 +8807,11 @@
       </c>
       <c r="B186" t="str">
         <f>IF('Memory setup'!E169=1,'Memory setup'!B169,IF('Memory setup'!B169&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B169),""))</f>
-        <v/>
+        <v>ADR_ADS111X_MIN_3</v>
       </c>
       <c r="C186" t="str">
         <f>IF(AND(B186&lt;&gt;"",'Memory setup'!A170&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v/>
+        <v>,</v>
       </c>
     </row>
     <row r="187" spans="1:3">
@@ -8761,7 +8821,7 @@
       </c>
       <c r="B187" t="str">
         <f>IF('Memory setup'!E170=1,'Memory setup'!B170,IF('Memory setup'!B170&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B170),""))</f>
-        <v/>
+        <v>ADR_ADS111X_MAX_3</v>
       </c>
       <c r="C187" t="str">
         <f>IF(AND(B187&lt;&gt;"",'Memory setup'!A171&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8771,7 +8831,7 @@
     <row r="188" spans="1:3">
       <c r="A188" t="str">
         <f>IF('Memory setup'!A171&lt;&gt;"",IF('Memory setup'!A171&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A171,"};"),"")</f>
-        <v/>
+        <v>};</v>
       </c>
       <c r="B188" t="str">
         <f>IF('Memory setup'!E171=1,'Memory setup'!B171,IF('Memory setup'!B171&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B171),""))</f>
@@ -8850,10 +8910,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCCA2C71-4C90-094A-BE8E-41D3DABF8E95}">
-  <dimension ref="A1:C187"/>
+  <dimension ref="A1:C191"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="A171" sqref="A1:XFD171"/>
+    <sheetView topLeftCell="A143" workbookViewId="0">
+      <selection activeCell="A175" sqref="A175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -9940,29 +10000,29 @@
     <row r="81" spans="1:3">
       <c r="A81" t="str">
         <f>IF('Memory setup'!A77&lt;&gt;"",IF('Memory setup'!A77&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A77,"};"),"")</f>
-        <v>// AXIS2</v>
+        <v/>
       </c>
       <c r="B81" t="str">
         <f>IF('Memory setup'!F77=1,'Memory setup'!B77,IF('Memory setup'!B77&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B77),""))</f>
-        <v/>
+        <v>ADR_TMC1_TRQ_FILT</v>
       </c>
       <c r="C81" t="str">
         <f>IF(AND(B81&lt;&gt;"",'Memory setup'!A78&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v/>
+        <v>,</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" t="str">
         <f>IF('Memory setup'!A78&lt;&gt;"",IF('Memory setup'!A78&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A78,"};"),"")</f>
-        <v/>
+        <v>// AXIS2</v>
       </c>
       <c r="B82" t="str">
         <f>IF('Memory setup'!F78=1,'Memory setup'!B78,IF('Memory setup'!B78&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B78),""))</f>
-        <v>ADR_AXIS2_CONFIG</v>
+        <v/>
       </c>
       <c r="C82" t="str">
         <f>IF(AND(B82&lt;&gt;"",'Memory setup'!A79&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v>,</v>
+        <v/>
       </c>
     </row>
     <row r="83" spans="1:3">
@@ -9972,7 +10032,7 @@
       </c>
       <c r="B83" t="str">
         <f>IF('Memory setup'!F79=1,'Memory setup'!B79,IF('Memory setup'!B79&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B79),""))</f>
-        <v>ADR_AXIS2_POWER</v>
+        <v>ADR_AXIS2_CONFIG</v>
       </c>
       <c r="C83" t="str">
         <f>IF(AND(B83&lt;&gt;"",'Memory setup'!A80&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -9986,7 +10046,7 @@
       </c>
       <c r="B84" t="str">
         <f>IF('Memory setup'!F80=1,'Memory setup'!B80,IF('Memory setup'!B80&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B80),""))</f>
-        <v>ADR_AXIS2_DEGREES</v>
+        <v>ADR_AXIS2_POWER</v>
       </c>
       <c r="C84" t="str">
         <f>IF(AND(B84&lt;&gt;"",'Memory setup'!A81&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10000,7 +10060,7 @@
       </c>
       <c r="B85" t="str">
         <f>IF('Memory setup'!F81=1,'Memory setup'!B81,IF('Memory setup'!B81&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B81),""))</f>
-        <v>ADR_AXIS2_MAX_SPEED</v>
+        <v>ADR_AXIS2_DEGREES</v>
       </c>
       <c r="C85" t="str">
         <f>IF(AND(B85&lt;&gt;"",'Memory setup'!A82&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10014,7 +10074,7 @@
       </c>
       <c r="B86" t="str">
         <f>IF('Memory setup'!F82=1,'Memory setup'!B82,IF('Memory setup'!B82&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B82),""))</f>
-        <v>ADR_AXIS2_MAX_ACCEL</v>
+        <v>ADR_AXIS2_MAX_SPEED</v>
       </c>
       <c r="C86" t="str">
         <f>IF(AND(B86&lt;&gt;"",'Memory setup'!A83&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10028,7 +10088,7 @@
       </c>
       <c r="B87" t="str">
         <f>IF('Memory setup'!F83=1,'Memory setup'!B83,IF('Memory setup'!B83&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B83),""))</f>
-        <v>ADR_AXIS2_ENDSTOP</v>
+        <v>ADR_AXIS2_MAX_ACCEL</v>
       </c>
       <c r="C87" t="str">
         <f>IF(AND(B87&lt;&gt;"",'Memory setup'!A84&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10042,7 +10102,7 @@
       </c>
       <c r="B88" t="str">
         <f>IF('Memory setup'!F84=1,'Memory setup'!B84,IF('Memory setup'!B84&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B84),""))</f>
-        <v>ADR_AXIS2_EFFECTS1</v>
+        <v>ADR_AXIS2_ENDSTOP</v>
       </c>
       <c r="C88" t="str">
         <f>IF(AND(B88&lt;&gt;"",'Memory setup'!A85&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10056,7 +10116,7 @@
       </c>
       <c r="B89" t="str">
         <f>IF('Memory setup'!F85=1,'Memory setup'!B85,IF('Memory setup'!B85&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B85),""))</f>
-        <v>ADR_AXIS2_SPEEDACCEL_FILTER</v>
+        <v>ADR_AXIS2_EFFECTS1</v>
       </c>
       <c r="C89" t="str">
         <f>IF(AND(B89&lt;&gt;"",'Memory setup'!A86&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10070,7 +10130,7 @@
       </c>
       <c r="B90" t="str">
         <f>IF('Memory setup'!F86=1,'Memory setup'!B86,IF('Memory setup'!B86&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B86),""))</f>
-        <v>ADR_AXIS2_ENC_RATIO</v>
+        <v>ADR_AXIS2_SPEEDACCEL_FILTER</v>
       </c>
       <c r="C90" t="str">
         <f>IF(AND(B90&lt;&gt;"",'Memory setup'!A87&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10080,29 +10140,29 @@
     <row r="91" spans="1:3">
       <c r="A91" t="str">
         <f>IF('Memory setup'!A87&lt;&gt;"",IF('Memory setup'!A87&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A87,"};"),"")</f>
-        <v>// TMC2</v>
+        <v/>
       </c>
       <c r="B91" t="str">
         <f>IF('Memory setup'!F87=1,'Memory setup'!B87,IF('Memory setup'!B87&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B87),""))</f>
-        <v/>
+        <v>ADR_AXIS2_ENC_RATIO</v>
       </c>
       <c r="C91" t="str">
         <f>IF(AND(B91&lt;&gt;"",'Memory setup'!A88&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v/>
+        <v>,</v>
       </c>
     </row>
     <row r="92" spans="1:3">
       <c r="A92" t="str">
         <f>IF('Memory setup'!A88&lt;&gt;"",IF('Memory setup'!A88&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A88,"};"),"")</f>
-        <v/>
+        <v>// TMC2</v>
       </c>
       <c r="B92" t="str">
         <f>IF('Memory setup'!F88=1,'Memory setup'!B88,IF('Memory setup'!B88&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B88),""))</f>
-        <v>ADR_TMC2_MOTCONF</v>
+        <v/>
       </c>
       <c r="C92" t="str">
         <f>IF(AND(B92&lt;&gt;"",'Memory setup'!A89&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v>,</v>
+        <v/>
       </c>
     </row>
     <row r="93" spans="1:3">
@@ -10112,7 +10172,7 @@
       </c>
       <c r="B93" t="str">
         <f>IF('Memory setup'!F89=1,'Memory setup'!B89,IF('Memory setup'!B89&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B89),""))</f>
-        <v>ADR_TMC2_CPR</v>
+        <v>ADR_TMC2_MOTCONF</v>
       </c>
       <c r="C93" t="str">
         <f>IF(AND(B93&lt;&gt;"",'Memory setup'!A90&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10126,7 +10186,7 @@
       </c>
       <c r="B94" t="str">
         <f>IF('Memory setup'!F90=1,'Memory setup'!B90,IF('Memory setup'!B90&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B90),""))</f>
-        <v>ADR_TMC2_ENCA</v>
+        <v>ADR_TMC2_CPR</v>
       </c>
       <c r="C94" t="str">
         <f>IF(AND(B94&lt;&gt;"",'Memory setup'!A91&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10140,7 +10200,7 @@
       </c>
       <c r="B95" t="str">
         <f>IF('Memory setup'!F91=1,'Memory setup'!B91,IF('Memory setup'!B91&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B91),""))</f>
-        <v>//ADR_TMC2_ADC_I0_OFS</v>
+        <v>ADR_TMC2_ENCA</v>
       </c>
       <c r="C95" t="str">
         <f>IF(AND(B95&lt;&gt;"",'Memory setup'!A92&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10154,7 +10214,7 @@
       </c>
       <c r="B96" t="str">
         <f>IF('Memory setup'!F92=1,'Memory setup'!B92,IF('Memory setup'!B92&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B92),""))</f>
-        <v>//ADR_TMC2_ADC_I1_OFS</v>
+        <v>//ADR_TMC2_ADC_I0_OFS</v>
       </c>
       <c r="C96" t="str">
         <f>IF(AND(B96&lt;&gt;"",'Memory setup'!A93&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10168,7 +10228,7 @@
       </c>
       <c r="B97" t="str">
         <f>IF('Memory setup'!F93=1,'Memory setup'!B93,IF('Memory setup'!B93&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B93),""))</f>
-        <v>//ADR_TMC2_ENC_OFFSET</v>
+        <v>//ADR_TMC2_ADC_I1_OFS</v>
       </c>
       <c r="C97" t="str">
         <f>IF(AND(B97&lt;&gt;"",'Memory setup'!A94&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10182,7 +10242,7 @@
       </c>
       <c r="B98" t="str">
         <f>IF('Memory setup'!F94=1,'Memory setup'!B94,IF('Memory setup'!B94&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B94),""))</f>
-        <v>ADR_TMC2_OFFSETFLUX</v>
+        <v>//ADR_TMC2_ENC_OFFSET</v>
       </c>
       <c r="C98" t="str">
         <f>IF(AND(B98&lt;&gt;"",'Memory setup'!A95&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10196,7 +10256,7 @@
       </c>
       <c r="B99" t="str">
         <f>IF('Memory setup'!F95=1,'Memory setup'!B95,IF('Memory setup'!B95&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B95),""))</f>
-        <v>ADR_TMC2_TORQUE_P</v>
+        <v>ADR_TMC2_OFFSETFLUX</v>
       </c>
       <c r="C99" t="str">
         <f>IF(AND(B99&lt;&gt;"",'Memory setup'!A96&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10210,7 +10270,7 @@
       </c>
       <c r="B100" t="str">
         <f>IF('Memory setup'!F96=1,'Memory setup'!B96,IF('Memory setup'!B96&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B96),""))</f>
-        <v>ADR_TMC2_TORQUE_I</v>
+        <v>ADR_TMC2_TORQUE_P</v>
       </c>
       <c r="C100" t="str">
         <f>IF(AND(B100&lt;&gt;"",'Memory setup'!A97&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10224,7 +10284,7 @@
       </c>
       <c r="B101" t="str">
         <f>IF('Memory setup'!F97=1,'Memory setup'!B97,IF('Memory setup'!B97&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B97),""))</f>
-        <v>ADR_TMC2_FLUX_P</v>
+        <v>ADR_TMC2_TORQUE_I</v>
       </c>
       <c r="C101" t="str">
         <f>IF(AND(B101&lt;&gt;"",'Memory setup'!A98&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10238,7 +10298,7 @@
       </c>
       <c r="B102" t="str">
         <f>IF('Memory setup'!F98=1,'Memory setup'!B98,IF('Memory setup'!B98&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B98),""))</f>
-        <v>ADR_TMC2_FLUX_I</v>
+        <v>ADR_TMC2_FLUX_P</v>
       </c>
       <c r="C102" t="str">
         <f>IF(AND(B102&lt;&gt;"",'Memory setup'!A99&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10252,7 +10312,7 @@
       </c>
       <c r="B103" t="str">
         <f>IF('Memory setup'!F99=1,'Memory setup'!B99,IF('Memory setup'!B99&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B99),""))</f>
-        <v>//ADR_TMC2_PHIE_OFS</v>
+        <v>ADR_TMC2_FLUX_I</v>
       </c>
       <c r="C103" t="str">
         <f>IF(AND(B103&lt;&gt;"",'Memory setup'!A100&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10262,15 +10322,15 @@
     <row r="104" spans="1:3">
       <c r="A104" t="str">
         <f>IF('Memory setup'!A100&lt;&gt;"",IF('Memory setup'!A100&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A100,"};"),"")</f>
-        <v>// AXIS3</v>
+        <v/>
       </c>
       <c r="B104" t="str">
         <f>IF('Memory setup'!F100=1,'Memory setup'!B100,IF('Memory setup'!B100&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B100),""))</f>
-        <v/>
+        <v>//ADR_TMC2_PHIE_OFS</v>
       </c>
       <c r="C104" t="str">
         <f>IF(AND(B104&lt;&gt;"",'Memory setup'!A101&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v/>
+        <v>,</v>
       </c>
     </row>
     <row r="105" spans="1:3">
@@ -10280,7 +10340,7 @@
       </c>
       <c r="B105" t="str">
         <f>IF('Memory setup'!F101=1,'Memory setup'!B101,IF('Memory setup'!B101&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B101),""))</f>
-        <v>ADR_AXIS3_CONFIG</v>
+        <v>ADR_TMC2_TRQ_FILT</v>
       </c>
       <c r="C105" t="str">
         <f>IF(AND(B105&lt;&gt;"",'Memory setup'!A102&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10290,15 +10350,15 @@
     <row r="106" spans="1:3">
       <c r="A106" t="str">
         <f>IF('Memory setup'!A102&lt;&gt;"",IF('Memory setup'!A102&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A102,"};"),"")</f>
-        <v/>
+        <v>// AXIS3</v>
       </c>
       <c r="B106" t="str">
         <f>IF('Memory setup'!F102=1,'Memory setup'!B102,IF('Memory setup'!B102&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B102),""))</f>
-        <v>ADR_AXIS3_POWER</v>
+        <v/>
       </c>
       <c r="C106" t="str">
         <f>IF(AND(B106&lt;&gt;"",'Memory setup'!A103&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v>,</v>
+        <v/>
       </c>
     </row>
     <row r="107" spans="1:3">
@@ -10308,7 +10368,7 @@
       </c>
       <c r="B107" t="str">
         <f>IF('Memory setup'!F103=1,'Memory setup'!B103,IF('Memory setup'!B103&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B103),""))</f>
-        <v>ADR_AXIS3_DEGREES</v>
+        <v>ADR_AXIS3_CONFIG</v>
       </c>
       <c r="C107" t="str">
         <f>IF(AND(B107&lt;&gt;"",'Memory setup'!A104&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10322,7 +10382,7 @@
       </c>
       <c r="B108" t="str">
         <f>IF('Memory setup'!F104=1,'Memory setup'!B104,IF('Memory setup'!B104&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B104),""))</f>
-        <v>ADR_AXIS3_MAX_SPEED</v>
+        <v>ADR_AXIS3_POWER</v>
       </c>
       <c r="C108" t="str">
         <f>IF(AND(B108&lt;&gt;"",'Memory setup'!A105&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10336,7 +10396,7 @@
       </c>
       <c r="B109" t="str">
         <f>IF('Memory setup'!F105=1,'Memory setup'!B105,IF('Memory setup'!B105&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B105),""))</f>
-        <v>ADR_AXIS3_MAX_ACCEL</v>
+        <v>ADR_AXIS3_DEGREES</v>
       </c>
       <c r="C109" t="str">
         <f>IF(AND(B109&lt;&gt;"",'Memory setup'!A106&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10350,7 +10410,7 @@
       </c>
       <c r="B110" t="str">
         <f>IF('Memory setup'!F106=1,'Memory setup'!B106,IF('Memory setup'!B106&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B106),""))</f>
-        <v>ADR_AXIS3_ENDSTOP</v>
+        <v>ADR_AXIS3_MAX_SPEED</v>
       </c>
       <c r="C110" t="str">
         <f>IF(AND(B110&lt;&gt;"",'Memory setup'!A107&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10364,7 +10424,7 @@
       </c>
       <c r="B111" t="str">
         <f>IF('Memory setup'!F107=1,'Memory setup'!B107,IF('Memory setup'!B107&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B107),""))</f>
-        <v>ADR_AXIS3_EFFECTS1</v>
+        <v>ADR_AXIS3_MAX_ACCEL</v>
       </c>
       <c r="C111" t="str">
         <f>IF(AND(B111&lt;&gt;"",'Memory setup'!A108&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10378,7 +10438,7 @@
       </c>
       <c r="B112" t="str">
         <f>IF('Memory setup'!F108=1,'Memory setup'!B108,IF('Memory setup'!B108&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B108),""))</f>
-        <v>ADR_AXIS3_SPEEDACCEL_FILTER</v>
+        <v>ADR_AXIS3_ENDSTOP</v>
       </c>
       <c r="C112" t="str">
         <f>IF(AND(B112&lt;&gt;"",'Memory setup'!A109&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10392,7 +10452,7 @@
       </c>
       <c r="B113" t="str">
         <f>IF('Memory setup'!F109=1,'Memory setup'!B109,IF('Memory setup'!B109&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B109),""))</f>
-        <v>ADR_AXIS3_ENC_RATIO</v>
+        <v>ADR_AXIS3_EFFECTS1</v>
       </c>
       <c r="C113" t="str">
         <f>IF(AND(B113&lt;&gt;"",'Memory setup'!A110&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10402,15 +10462,15 @@
     <row r="114" spans="1:3">
       <c r="A114" t="str">
         <f>IF('Memory setup'!A110&lt;&gt;"",IF('Memory setup'!A110&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A110,"};"),"")</f>
-        <v>// TMC3</v>
+        <v/>
       </c>
       <c r="B114" t="str">
         <f>IF('Memory setup'!F110=1,'Memory setup'!B110,IF('Memory setup'!B110&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B110),""))</f>
-        <v/>
+        <v>ADR_AXIS3_SPEEDACCEL_FILTER</v>
       </c>
       <c r="C114" t="str">
         <f>IF(AND(B114&lt;&gt;"",'Memory setup'!A111&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v/>
+        <v>,</v>
       </c>
     </row>
     <row r="115" spans="1:3">
@@ -10420,7 +10480,7 @@
       </c>
       <c r="B115" t="str">
         <f>IF('Memory setup'!F111=1,'Memory setup'!B111,IF('Memory setup'!B111&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B111),""))</f>
-        <v>ADR_TMC3_MOTCONF</v>
+        <v>ADR_AXIS3_ENC_RATIO</v>
       </c>
       <c r="C115" t="str">
         <f>IF(AND(B115&lt;&gt;"",'Memory setup'!A112&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10430,15 +10490,15 @@
     <row r="116" spans="1:3">
       <c r="A116" t="str">
         <f>IF('Memory setup'!A112&lt;&gt;"",IF('Memory setup'!A112&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A112,"};"),"")</f>
-        <v/>
+        <v>// TMC3</v>
       </c>
       <c r="B116" t="str">
         <f>IF('Memory setup'!F112=1,'Memory setup'!B112,IF('Memory setup'!B112&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B112),""))</f>
-        <v>ADR_TMC3_CPR</v>
+        <v/>
       </c>
       <c r="C116" t="str">
         <f>IF(AND(B116&lt;&gt;"",'Memory setup'!A113&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v>,</v>
+        <v/>
       </c>
     </row>
     <row r="117" spans="1:3">
@@ -10448,7 +10508,7 @@
       </c>
       <c r="B117" t="str">
         <f>IF('Memory setup'!F113=1,'Memory setup'!B113,IF('Memory setup'!B113&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B113),""))</f>
-        <v>ADR_TMC3_ENCA</v>
+        <v>ADR_TMC3_MOTCONF</v>
       </c>
       <c r="C117" t="str">
         <f>IF(AND(B117&lt;&gt;"",'Memory setup'!A114&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10462,7 +10522,7 @@
       </c>
       <c r="B118" t="str">
         <f>IF('Memory setup'!F114=1,'Memory setup'!B114,IF('Memory setup'!B114&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B114),""))</f>
-        <v>//ADR_TMC3_ADC_I0_OFS</v>
+        <v>ADR_TMC3_CPR</v>
       </c>
       <c r="C118" t="str">
         <f>IF(AND(B118&lt;&gt;"",'Memory setup'!A115&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10476,7 +10536,7 @@
       </c>
       <c r="B119" t="str">
         <f>IF('Memory setup'!F115=1,'Memory setup'!B115,IF('Memory setup'!B115&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B115),""))</f>
-        <v>//ADR_TMC3_ADC_I1_OFS</v>
+        <v>ADR_TMC3_ENCA</v>
       </c>
       <c r="C119" t="str">
         <f>IF(AND(B119&lt;&gt;"",'Memory setup'!A116&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10490,7 +10550,7 @@
       </c>
       <c r="B120" t="str">
         <f>IF('Memory setup'!F116=1,'Memory setup'!B116,IF('Memory setup'!B116&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B116),""))</f>
-        <v>//ADR_TMC3_ENC_OFFSET</v>
+        <v>//ADR_TMC3_ADC_I0_OFS</v>
       </c>
       <c r="C120" t="str">
         <f>IF(AND(B120&lt;&gt;"",'Memory setup'!A117&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10504,7 +10564,7 @@
       </c>
       <c r="B121" t="str">
         <f>IF('Memory setup'!F117=1,'Memory setup'!B117,IF('Memory setup'!B117&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B117),""))</f>
-        <v>ADR_TMC3_OFFSETFLUX</v>
+        <v>//ADR_TMC3_ADC_I1_OFS</v>
       </c>
       <c r="C121" t="str">
         <f>IF(AND(B121&lt;&gt;"",'Memory setup'!A118&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10518,7 +10578,7 @@
       </c>
       <c r="B122" t="str">
         <f>IF('Memory setup'!F118=1,'Memory setup'!B118,IF('Memory setup'!B118&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B118),""))</f>
-        <v>ADR_TMC3_TORQUE_P</v>
+        <v>//ADR_TMC3_ENC_OFFSET</v>
       </c>
       <c r="C122" t="str">
         <f>IF(AND(B122&lt;&gt;"",'Memory setup'!A119&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10532,7 +10592,7 @@
       </c>
       <c r="B123" t="str">
         <f>IF('Memory setup'!F119=1,'Memory setup'!B119,IF('Memory setup'!B119&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B119),""))</f>
-        <v>ADR_TMC3_TORQUE_I</v>
+        <v>ADR_TMC3_OFFSETFLUX</v>
       </c>
       <c r="C123" t="str">
         <f>IF(AND(B123&lt;&gt;"",'Memory setup'!A120&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10546,7 +10606,7 @@
       </c>
       <c r="B124" t="str">
         <f>IF('Memory setup'!F120=1,'Memory setup'!B120,IF('Memory setup'!B120&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B120),""))</f>
-        <v>ADR_TMC3_FLUX_P</v>
+        <v>ADR_TMC3_TORQUE_P</v>
       </c>
       <c r="C124" t="str">
         <f>IF(AND(B124&lt;&gt;"",'Memory setup'!A121&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10560,7 +10620,7 @@
       </c>
       <c r="B125" t="str">
         <f>IF('Memory setup'!F121=1,'Memory setup'!B121,IF('Memory setup'!B121&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B121),""))</f>
-        <v>ADR_TMC3_FLUX_I</v>
+        <v>ADR_TMC3_TORQUE_I</v>
       </c>
       <c r="C125" t="str">
         <f>IF(AND(B125&lt;&gt;"",'Memory setup'!A122&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10574,7 +10634,7 @@
       </c>
       <c r="B126" t="str">
         <f>IF('Memory setup'!F122=1,'Memory setup'!B122,IF('Memory setup'!B122&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B122),""))</f>
-        <v>//ADR_TMC3_PHIE_OFS</v>
+        <v>ADR_TMC3_FLUX_P</v>
       </c>
       <c r="C126" t="str">
         <f>IF(AND(B126&lt;&gt;"",'Memory setup'!A123&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10584,15 +10644,15 @@
     <row r="127" spans="1:3">
       <c r="A127" t="str">
         <f>IF('Memory setup'!A123&lt;&gt;"",IF('Memory setup'!A123&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A123,"};"),"")</f>
-        <v>// Odrive</v>
+        <v/>
       </c>
       <c r="B127" t="str">
         <f>IF('Memory setup'!F123=1,'Memory setup'!B123,IF('Memory setup'!B123&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B123),""))</f>
-        <v/>
+        <v>ADR_TMC3_FLUX_I</v>
       </c>
       <c r="C127" t="str">
         <f>IF(AND(B127&lt;&gt;"",'Memory setup'!A124&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v/>
+        <v>,</v>
       </c>
     </row>
     <row r="128" spans="1:3">
@@ -10602,7 +10662,7 @@
       </c>
       <c r="B128" t="str">
         <f>IF('Memory setup'!F124=1,'Memory setup'!B124,IF('Memory setup'!B124&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B124),""))</f>
-        <v>ADR_ODRIVE_CANID</v>
+        <v>//ADR_TMC3_PHIE_OFS</v>
       </c>
       <c r="C128" t="str">
         <f>IF(AND(B128&lt;&gt;"",'Memory setup'!A125&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10616,7 +10676,7 @@
       </c>
       <c r="B129" t="str">
         <f>IF('Memory setup'!F125=1,'Memory setup'!B125,IF('Memory setup'!B125&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B125),""))</f>
-        <v>ADR_ODRIVE_SETTING1_M0</v>
+        <v>ADR_TMC3_TRQ_FILT</v>
       </c>
       <c r="C129" t="str">
         <f>IF(AND(B129&lt;&gt;"",'Memory setup'!A126&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10626,29 +10686,29 @@
     <row r="130" spans="1:3">
       <c r="A130" t="str">
         <f>IF('Memory setup'!A126&lt;&gt;"",IF('Memory setup'!A126&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A126,"};"),"")</f>
-        <v/>
+        <v>// Odrive</v>
       </c>
       <c r="B130" t="str">
         <f>IF('Memory setup'!F126=1,'Memory setup'!B126,IF('Memory setup'!B126&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B126),""))</f>
-        <v>ADR_ODRIVE_SETTING1_M1</v>
+        <v/>
       </c>
       <c r="C130" t="str">
         <f>IF(AND(B130&lt;&gt;"",'Memory setup'!A127&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v>,</v>
+        <v/>
       </c>
     </row>
     <row r="131" spans="1:3">
       <c r="A131" t="str">
         <f>IF('Memory setup'!A127&lt;&gt;"",IF('Memory setup'!A127&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A127,"};"),"")</f>
-        <v>// VESC Section</v>
+        <v/>
       </c>
       <c r="B131" t="str">
         <f>IF('Memory setup'!F127=1,'Memory setup'!B127,IF('Memory setup'!B127&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B127),""))</f>
-        <v/>
+        <v>ADR_ODRIVE_CANID</v>
       </c>
       <c r="C131" t="str">
         <f>IF(AND(B131&lt;&gt;"",'Memory setup'!A128&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v/>
+        <v>,</v>
       </c>
     </row>
     <row r="132" spans="1:3">
@@ -10658,7 +10718,7 @@
       </c>
       <c r="B132" t="str">
         <f>IF('Memory setup'!F128=1,'Memory setup'!B128,IF('Memory setup'!B128&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B128),""))</f>
-        <v>ADR_VESC1_CANID</v>
+        <v>ADR_ODRIVE_SETTING1_M0</v>
       </c>
       <c r="C132" t="str">
         <f>IF(AND(B132&lt;&gt;"",'Memory setup'!A129&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10672,7 +10732,7 @@
       </c>
       <c r="B133" t="str">
         <f>IF('Memory setup'!F129=1,'Memory setup'!B129,IF('Memory setup'!B129&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B129),""))</f>
-        <v>ADR_VESC1_DATA</v>
+        <v>ADR_ODRIVE_SETTING1_M1</v>
       </c>
       <c r="C133" t="str">
         <f>IF(AND(B133&lt;&gt;"",'Memory setup'!A130&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10682,15 +10742,15 @@
     <row r="134" spans="1:3">
       <c r="A134" t="str">
         <f>IF('Memory setup'!A130&lt;&gt;"",IF('Memory setup'!A130&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A130,"};"),"")</f>
-        <v/>
+        <v>// VESC Section</v>
       </c>
       <c r="B134" t="str">
         <f>IF('Memory setup'!F130=1,'Memory setup'!B130,IF('Memory setup'!B130&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B130),""))</f>
-        <v>ADR_VESC1_OFFSET</v>
+        <v/>
       </c>
       <c r="C134" t="str">
         <f>IF(AND(B134&lt;&gt;"",'Memory setup'!A131&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v>,</v>
+        <v/>
       </c>
     </row>
     <row r="135" spans="1:3">
@@ -10700,7 +10760,7 @@
       </c>
       <c r="B135" t="str">
         <f>IF('Memory setup'!F131=1,'Memory setup'!B131,IF('Memory setup'!B131&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B131),""))</f>
-        <v>ADR_VESC2_CANID</v>
+        <v>ADR_VESC1_CANID</v>
       </c>
       <c r="C135" t="str">
         <f>IF(AND(B135&lt;&gt;"",'Memory setup'!A132&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10714,7 +10774,7 @@
       </c>
       <c r="B136" t="str">
         <f>IF('Memory setup'!F132=1,'Memory setup'!B132,IF('Memory setup'!B132&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B132),""))</f>
-        <v>ADR_VESC2_DATA</v>
+        <v>ADR_VESC1_DATA</v>
       </c>
       <c r="C136" t="str">
         <f>IF(AND(B136&lt;&gt;"",'Memory setup'!A133&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10728,7 +10788,7 @@
       </c>
       <c r="B137" t="str">
         <f>IF('Memory setup'!F133=1,'Memory setup'!B133,IF('Memory setup'!B133&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B133),""))</f>
-        <v>ADR_VESC2_OFFSET</v>
+        <v>ADR_VESC1_OFFSET</v>
       </c>
       <c r="C137" t="str">
         <f>IF(AND(B137&lt;&gt;"",'Memory setup'!A134&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10742,7 +10802,7 @@
       </c>
       <c r="B138" t="str">
         <f>IF('Memory setup'!F134=1,'Memory setup'!B134,IF('Memory setup'!B134&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B134),""))</f>
-        <v>ADR_VESC3_CANID</v>
+        <v>ADR_VESC2_CANID</v>
       </c>
       <c r="C138" t="str">
         <f>IF(AND(B138&lt;&gt;"",'Memory setup'!A135&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10756,7 +10816,7 @@
       </c>
       <c r="B139" t="str">
         <f>IF('Memory setup'!F135=1,'Memory setup'!B135,IF('Memory setup'!B135&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B135),""))</f>
-        <v>ADR_VESC3_DATA</v>
+        <v>ADR_VESC2_DATA</v>
       </c>
       <c r="C139" t="str">
         <f>IF(AND(B139&lt;&gt;"",'Memory setup'!A136&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10770,7 +10830,7 @@
       </c>
       <c r="B140" t="str">
         <f>IF('Memory setup'!F136=1,'Memory setup'!B136,IF('Memory setup'!B136&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B136),""))</f>
-        <v>ADR_VESC3_OFFSET</v>
+        <v>ADR_VESC2_OFFSET</v>
       </c>
       <c r="C140" t="str">
         <f>IF(AND(B140&lt;&gt;"",'Memory setup'!A137&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10780,15 +10840,15 @@
     <row r="141" spans="1:3">
       <c r="A141" t="str">
         <f>IF('Memory setup'!A137&lt;&gt;"",IF('Memory setup'!A137&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A137,"};"),"")</f>
-        <v>//MT Encoder</v>
+        <v/>
       </c>
       <c r="B141" t="str">
         <f>IF('Memory setup'!F137=1,'Memory setup'!B137,IF('Memory setup'!B137&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B137),""))</f>
-        <v/>
+        <v>ADR_VESC3_CANID</v>
       </c>
       <c r="C141" t="str">
         <f>IF(AND(B141&lt;&gt;"",'Memory setup'!A138&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v/>
+        <v>,</v>
       </c>
     </row>
     <row r="142" spans="1:3">
@@ -10798,7 +10858,7 @@
       </c>
       <c r="B142" t="str">
         <f>IF('Memory setup'!F138=1,'Memory setup'!B138,IF('Memory setup'!B138&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B138),""))</f>
-        <v>ADR_MTENC_OFS</v>
+        <v>ADR_VESC3_DATA</v>
       </c>
       <c r="C142" t="str">
         <f>IF(AND(B142&lt;&gt;"",'Memory setup'!A139&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10812,7 +10872,7 @@
       </c>
       <c r="B143" t="str">
         <f>IF('Memory setup'!F139=1,'Memory setup'!B139,IF('Memory setup'!B139&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B139),""))</f>
-        <v>ADR_MTENC_CONF1</v>
+        <v>ADR_VESC3_OFFSET</v>
       </c>
       <c r="C143" t="str">
         <f>IF(AND(B143&lt;&gt;"",'Memory setup'!A140&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10822,7 +10882,7 @@
     <row r="144" spans="1:3">
       <c r="A144" t="str">
         <f>IF('Memory setup'!A140&lt;&gt;"",IF('Memory setup'!A140&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A140,"};"),"")</f>
-        <v>// Biss-C</v>
+        <v>//MT Encoder</v>
       </c>
       <c r="B144" t="str">
         <f>IF('Memory setup'!F140=1,'Memory setup'!B140,IF('Memory setup'!B140&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B140),""))</f>
@@ -10840,7 +10900,7 @@
       </c>
       <c r="B145" t="str">
         <f>IF('Memory setup'!F141=1,'Memory setup'!B141,IF('Memory setup'!B141&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B141),""))</f>
-        <v>ADR_BISSENC_CONF1</v>
+        <v>ADR_MTENC_OFS</v>
       </c>
       <c r="C145" t="str">
         <f>IF(AND(B145&lt;&gt;"",'Memory setup'!A142&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10854,7 +10914,7 @@
       </c>
       <c r="B146" t="str">
         <f>IF('Memory setup'!F142=1,'Memory setup'!B142,IF('Memory setup'!B142&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B142),""))</f>
-        <v>ADR_BISSENC_OFS</v>
+        <v>ADR_MTENC_CONF1</v>
       </c>
       <c r="C146" t="str">
         <f>IF(AND(B146&lt;&gt;"",'Memory setup'!A143&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10864,7 +10924,7 @@
     <row r="147" spans="1:3">
       <c r="A147" t="str">
         <f>IF('Memory setup'!A143&lt;&gt;"",IF('Memory setup'!A143&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A143,"};"),"")</f>
-        <v>// Analog min/max calibrations</v>
+        <v>// Biss-C</v>
       </c>
       <c r="B147" t="str">
         <f>IF('Memory setup'!F143=1,'Memory setup'!B143,IF('Memory setup'!B143&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B143),""))</f>
@@ -10882,7 +10942,7 @@
       </c>
       <c r="B148" t="str">
         <f>IF('Memory setup'!F144=1,'Memory setup'!B144,IF('Memory setup'!B144&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B144),""))</f>
-        <v>ADR_LOCALANALOG_MIN_0</v>
+        <v>ADR_BISSENC_CONF1</v>
       </c>
       <c r="C148" t="str">
         <f>IF(AND(B148&lt;&gt;"",'Memory setup'!A145&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10896,7 +10956,7 @@
       </c>
       <c r="B149" t="str">
         <f>IF('Memory setup'!F145=1,'Memory setup'!B145,IF('Memory setup'!B145&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B145),""))</f>
-        <v>ADR_LOCALANALOG_MAX_0</v>
+        <v>ADR_BISSENC_OFS</v>
       </c>
       <c r="C149" t="str">
         <f>IF(AND(B149&lt;&gt;"",'Memory setup'!A146&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10906,15 +10966,15 @@
     <row r="150" spans="1:3">
       <c r="A150" t="str">
         <f>IF('Memory setup'!A146&lt;&gt;"",IF('Memory setup'!A146&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A146,"};"),"")</f>
-        <v/>
+        <v>// Analog min/max calibrations</v>
       </c>
       <c r="B150" t="str">
         <f>IF('Memory setup'!F146=1,'Memory setup'!B146,IF('Memory setup'!B146&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B146),""))</f>
-        <v>ADR_LOCALANALOG_MIN_1</v>
+        <v/>
       </c>
       <c r="C150" t="str">
         <f>IF(AND(B150&lt;&gt;"",'Memory setup'!A147&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v>,</v>
+        <v/>
       </c>
     </row>
     <row r="151" spans="1:3">
@@ -10924,7 +10984,7 @@
       </c>
       <c r="B151" t="str">
         <f>IF('Memory setup'!F147=1,'Memory setup'!B147,IF('Memory setup'!B147&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B147),""))</f>
-        <v>ADR_LOCALANALOG_MAX_1</v>
+        <v>ADR_LOCALANALOG_MIN_0</v>
       </c>
       <c r="C151" t="str">
         <f>IF(AND(B151&lt;&gt;"",'Memory setup'!A148&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10938,7 +10998,7 @@
       </c>
       <c r="B152" t="str">
         <f>IF('Memory setup'!F148=1,'Memory setup'!B148,IF('Memory setup'!B148&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B148),""))</f>
-        <v>ADR_LOCALANALOG_MIN_2</v>
+        <v>ADR_LOCALANALOG_MAX_0</v>
       </c>
       <c r="C152" t="str">
         <f>IF(AND(B152&lt;&gt;"",'Memory setup'!A149&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10952,7 +11012,7 @@
       </c>
       <c r="B153" t="str">
         <f>IF('Memory setup'!F149=1,'Memory setup'!B149,IF('Memory setup'!B149&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B149),""))</f>
-        <v>ADR_LOCALANALOG_MAX_2</v>
+        <v>ADR_LOCALANALOG_MIN_1</v>
       </c>
       <c r="C153" t="str">
         <f>IF(AND(B153&lt;&gt;"",'Memory setup'!A150&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10966,7 +11026,7 @@
       </c>
       <c r="B154" t="str">
         <f>IF('Memory setup'!F150=1,'Memory setup'!B150,IF('Memory setup'!B150&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B150),""))</f>
-        <v>ADR_LOCALANALOG_MIN_3</v>
+        <v>ADR_LOCALANALOG_MAX_1</v>
       </c>
       <c r="C154" t="str">
         <f>IF(AND(B154&lt;&gt;"",'Memory setup'!A151&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10980,7 +11040,7 @@
       </c>
       <c r="B155" t="str">
         <f>IF('Memory setup'!F151=1,'Memory setup'!B151,IF('Memory setup'!B151&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B151),""))</f>
-        <v>ADR_LOCALANALOG_MAX_3</v>
+        <v>ADR_LOCALANALOG_MIN_2</v>
       </c>
       <c r="C155" t="str">
         <f>IF(AND(B155&lt;&gt;"",'Memory setup'!A152&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -10994,7 +11054,7 @@
       </c>
       <c r="B156" t="str">
         <f>IF('Memory setup'!F152=1,'Memory setup'!B152,IF('Memory setup'!B152&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B152),""))</f>
-        <v>ADR_LOCALANALOG_MIN_4</v>
+        <v>ADR_LOCALANALOG_MAX_2</v>
       </c>
       <c r="C156" t="str">
         <f>IF(AND(B156&lt;&gt;"",'Memory setup'!A153&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -11008,7 +11068,7 @@
       </c>
       <c r="B157" t="str">
         <f>IF('Memory setup'!F153=1,'Memory setup'!B153,IF('Memory setup'!B153&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B153),""))</f>
-        <v>ADR_LOCALANALOG_MAX_4</v>
+        <v>ADR_LOCALANALOG_MIN_3</v>
       </c>
       <c r="C157" t="str">
         <f>IF(AND(B157&lt;&gt;"",'Memory setup'!A154&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -11022,7 +11082,7 @@
       </c>
       <c r="B158" t="str">
         <f>IF('Memory setup'!F154=1,'Memory setup'!B154,IF('Memory setup'!B154&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B154),""))</f>
-        <v>ADR_LOCALANALOG_MIN_5</v>
+        <v>ADR_LOCALANALOG_MAX_3</v>
       </c>
       <c r="C158" t="str">
         <f>IF(AND(B158&lt;&gt;"",'Memory setup'!A155&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -11036,7 +11096,7 @@
       </c>
       <c r="B159" t="str">
         <f>IF('Memory setup'!F155=1,'Memory setup'!B155,IF('Memory setup'!B155&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B155),""))</f>
-        <v>ADR_LOCALANALOG_MAX_5</v>
+        <v>ADR_LOCALANALOG_MIN_4</v>
       </c>
       <c r="C159" t="str">
         <f>IF(AND(B159&lt;&gt;"",'Memory setup'!A156&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -11050,7 +11110,7 @@
       </c>
       <c r="B160" t="str">
         <f>IF('Memory setup'!F156=1,'Memory setup'!B156,IF('Memory setup'!B156&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B156),""))</f>
-        <v>ADR_LOCALANALOG_MIN_6</v>
+        <v>ADR_LOCALANALOG_MAX_4</v>
       </c>
       <c r="C160" t="str">
         <f>IF(AND(B160&lt;&gt;"",'Memory setup'!A157&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -11064,7 +11124,7 @@
       </c>
       <c r="B161" t="str">
         <f>IF('Memory setup'!F157=1,'Memory setup'!B157,IF('Memory setup'!B157&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B157),""))</f>
-        <v>ADR_LOCALANALOG_MAX_6</v>
+        <v>ADR_LOCALANALOG_MIN_5</v>
       </c>
       <c r="C161" t="str">
         <f>IF(AND(B161&lt;&gt;"",'Memory setup'!A158&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -11078,7 +11138,7 @@
       </c>
       <c r="B162" t="str">
         <f>IF('Memory setup'!F158=1,'Memory setup'!B158,IF('Memory setup'!B158&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B158),""))</f>
-        <v>ADR_LOCALANALOG_MIN_7</v>
+        <v>ADR_LOCALANALOG_MAX_5</v>
       </c>
       <c r="C162" t="str">
         <f>IF(AND(B162&lt;&gt;"",'Memory setup'!A159&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -11092,7 +11152,7 @@
       </c>
       <c r="B163" t="str">
         <f>IF('Memory setup'!F159=1,'Memory setup'!B159,IF('Memory setup'!B159&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B159),""))</f>
-        <v>ADR_LOCALANALOG_MAX_7</v>
+        <v>ADR_LOCALANALOG_MIN_6</v>
       </c>
       <c r="C163" t="str">
         <f>IF(AND(B163&lt;&gt;"",'Memory setup'!A160&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -11106,7 +11166,7 @@
       </c>
       <c r="B164" t="str">
         <f>IF('Memory setup'!F160=1,'Memory setup'!B160,IF('Memory setup'!B160&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B160),""))</f>
-        <v>ADR_ADS111X_MIN_0</v>
+        <v>ADR_LOCALANALOG_MAX_6</v>
       </c>
       <c r="C164" t="str">
         <f>IF(AND(B164&lt;&gt;"",'Memory setup'!A161&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -11120,7 +11180,7 @@
       </c>
       <c r="B165" t="str">
         <f>IF('Memory setup'!F161=1,'Memory setup'!B161,IF('Memory setup'!B161&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B161),""))</f>
-        <v>ADR_ADS111X_MAX_0</v>
+        <v>ADR_LOCALANALOG_MIN_7</v>
       </c>
       <c r="C165" t="str">
         <f>IF(AND(B165&lt;&gt;"",'Memory setup'!A162&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -11134,7 +11194,7 @@
       </c>
       <c r="B166" t="str">
         <f>IF('Memory setup'!F162=1,'Memory setup'!B162,IF('Memory setup'!B162&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B162),""))</f>
-        <v>ADR_ADS111X_MIN_1</v>
+        <v>ADR_LOCALANALOG_MAX_7</v>
       </c>
       <c r="C166" t="str">
         <f>IF(AND(B166&lt;&gt;"",'Memory setup'!A163&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -11148,7 +11208,7 @@
       </c>
       <c r="B167" t="str">
         <f>IF('Memory setup'!F163=1,'Memory setup'!B163,IF('Memory setup'!B163&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B163),""))</f>
-        <v>ADR_ADS111X_MAX_1</v>
+        <v>ADR_ADS111X_MIN_0</v>
       </c>
       <c r="C167" t="str">
         <f>IF(AND(B167&lt;&gt;"",'Memory setup'!A164&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -11162,7 +11222,7 @@
       </c>
       <c r="B168" t="str">
         <f>IF('Memory setup'!F164=1,'Memory setup'!B164,IF('Memory setup'!B164&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B164),""))</f>
-        <v>ADR_ADS111X_MIN_2</v>
+        <v>ADR_ADS111X_MAX_0</v>
       </c>
       <c r="C168" t="str">
         <f>IF(AND(B168&lt;&gt;"",'Memory setup'!A165&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -11176,7 +11236,7 @@
       </c>
       <c r="B169" t="str">
         <f>IF('Memory setup'!F165=1,'Memory setup'!B165,IF('Memory setup'!B165&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B165),""))</f>
-        <v>ADR_ADS111X_MAX_2</v>
+        <v>ADR_ADS111X_MIN_1</v>
       </c>
       <c r="C169" t="str">
         <f>IF(AND(B169&lt;&gt;"",'Memory setup'!A166&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -11190,7 +11250,7 @@
       </c>
       <c r="B170" t="str">
         <f>IF('Memory setup'!F166=1,'Memory setup'!B166,IF('Memory setup'!B166&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B166),""))</f>
-        <v>ADR_ADS111X_MIN_3</v>
+        <v>ADR_ADS111X_MAX_1</v>
       </c>
       <c r="C170" t="str">
         <f>IF(AND(B170&lt;&gt;"",'Memory setup'!A167&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -11204,25 +11264,25 @@
       </c>
       <c r="B171" t="str">
         <f>IF('Memory setup'!F167=1,'Memory setup'!B167,IF('Memory setup'!B167&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B167),""))</f>
-        <v>ADR_ADS111X_MAX_3</v>
+        <v>ADR_ADS111X_MIN_2</v>
       </c>
       <c r="C171" t="str">
         <f>IF(AND(B171&lt;&gt;"",'Memory setup'!A168&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v/>
+        <v>,</v>
       </c>
     </row>
     <row r="172" spans="1:3">
       <c r="A172" t="str">
         <f>IF('Memory setup'!A168&lt;&gt;"",IF('Memory setup'!A168&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A168,"};"),"")</f>
-        <v>};</v>
+        <v/>
       </c>
       <c r="B172" t="str">
         <f>IF('Memory setup'!F168=1,'Memory setup'!B168,IF('Memory setup'!B168&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B168),""))</f>
-        <v/>
+        <v>ADR_ADS111X_MAX_2</v>
       </c>
       <c r="C172" t="str">
         <f>IF(AND(B172&lt;&gt;"",'Memory setup'!A169&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v/>
+        <v>,</v>
       </c>
     </row>
     <row r="173" spans="1:3">
@@ -11232,11 +11292,11 @@
       </c>
       <c r="B173" t="str">
         <f>IF('Memory setup'!F169=1,'Memory setup'!B169,IF('Memory setup'!B169&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B169),""))</f>
-        <v/>
+        <v>ADR_ADS111X_MIN_3</v>
       </c>
       <c r="C173" t="str">
         <f>IF(AND(B173&lt;&gt;"",'Memory setup'!A170&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v/>
+        <v>,</v>
       </c>
     </row>
     <row r="174" spans="1:3">
@@ -11246,7 +11306,7 @@
       </c>
       <c r="B174" t="str">
         <f>IF('Memory setup'!F170=1,'Memory setup'!B170,IF('Memory setup'!B170&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B170),""))</f>
-        <v/>
+        <v>ADR_ADS111X_MAX_3</v>
       </c>
       <c r="C174" t="str">
         <f>IF(AND(B174&lt;&gt;"",'Memory setup'!A171&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -11256,7 +11316,7 @@
     <row r="175" spans="1:3">
       <c r="A175" t="str">
         <f>IF('Memory setup'!A171&lt;&gt;"",IF('Memory setup'!A171&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A171,"};"),"")</f>
-        <v/>
+        <v>};</v>
       </c>
       <c r="B175" t="str">
         <f>IF('Memory setup'!F171=1,'Memory setup'!B171,IF('Memory setup'!B171&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B171),""))</f>
@@ -11367,71 +11427,127 @@
     </row>
     <row r="183" spans="1:3">
       <c r="A183" t="str">
-        <f>IF('Memory setup'!A175&lt;&gt;"",IF('Memory setup'!A175&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A175,"};"),"")</f>
+        <f>IF('Memory setup'!A179&lt;&gt;"",IF('Memory setup'!A179&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A179,"};"),"")</f>
         <v/>
       </c>
       <c r="B183" t="str">
-        <f>IF('Memory setup'!F175=1,'Memory setup'!B175,IF('Memory setup'!B175&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B175),""))</f>
+        <f>IF('Memory setup'!F179=1,'Memory setup'!B179,IF('Memory setup'!B179&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B179),""))</f>
         <v/>
       </c>
       <c r="C183" t="str">
-        <f>IF(AND(B183&lt;&gt;"",'Memory setup'!A176&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
+        <f>IF(AND(B183&lt;&gt;"",'Memory setup'!A180&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
         <v/>
       </c>
     </row>
     <row r="184" spans="1:3">
       <c r="A184" t="str">
-        <f>IF('Memory setup'!A176&lt;&gt;"",IF('Memory setup'!A176&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A176,"};"),"")</f>
+        <f>IF('Memory setup'!A180&lt;&gt;"",IF('Memory setup'!A180&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A180,"};"),"")</f>
         <v/>
       </c>
       <c r="B184" t="str">
-        <f>IF('Memory setup'!F176=1,'Memory setup'!B176,IF('Memory setup'!B176&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B176),""))</f>
+        <f>IF('Memory setup'!F180=1,'Memory setup'!B180,IF('Memory setup'!B180&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B180),""))</f>
         <v/>
       </c>
       <c r="C184" t="str">
-        <f>IF(AND(B184&lt;&gt;"",'Memory setup'!A177&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
+        <f>IF(AND(B184&lt;&gt;"",'Memory setup'!A181&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
         <v/>
       </c>
     </row>
     <row r="185" spans="1:3">
       <c r="A185" t="str">
-        <f>IF('Memory setup'!A177&lt;&gt;"",IF('Memory setup'!A177&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A177,"};"),"")</f>
+        <f>IF('Memory setup'!A181&lt;&gt;"",IF('Memory setup'!A181&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A181,"};"),"")</f>
         <v/>
       </c>
       <c r="B185" t="str">
-        <f>IF('Memory setup'!F177=1,'Memory setup'!B177,IF('Memory setup'!B177&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B177),""))</f>
+        <f>IF('Memory setup'!F181=1,'Memory setup'!B181,IF('Memory setup'!B181&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B181),""))</f>
         <v/>
       </c>
       <c r="C185" t="str">
-        <f>IF(AND(B185&lt;&gt;"",'Memory setup'!A178&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
+        <f>IF(AND(B185&lt;&gt;"",'Memory setup'!A182&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
         <v/>
       </c>
     </row>
     <row r="186" spans="1:3">
       <c r="A186" t="str">
-        <f>IF('Memory setup'!A178&lt;&gt;"",IF('Memory setup'!A178&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A178,"};"),"")</f>
+        <f>IF('Memory setup'!A182&lt;&gt;"",IF('Memory setup'!A182&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A182,"};"),"")</f>
         <v/>
       </c>
       <c r="B186" t="str">
-        <f>IF('Memory setup'!F178=1,'Memory setup'!B178,IF('Memory setup'!B178&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B178),""))</f>
+        <f>IF('Memory setup'!F182=1,'Memory setup'!B182,IF('Memory setup'!B182&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B182),""))</f>
         <v/>
       </c>
       <c r="C186" t="str">
-        <f>IF(AND(B186&lt;&gt;"",'Memory setup'!A179&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
+        <f>IF(AND(B186&lt;&gt;"",'Memory setup'!A183&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
         <v/>
       </c>
     </row>
     <row r="187" spans="1:3">
       <c r="A187" t="str">
-        <f>IF('Memory setup'!A179&lt;&gt;"",IF('Memory setup'!A179&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A179,"};"),"")</f>
+        <f>IF('Memory setup'!A183&lt;&gt;"",IF('Memory setup'!A183&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A183,"};"),"")</f>
         <v/>
       </c>
       <c r="B187" t="str">
-        <f>IF('Memory setup'!F179=1,'Memory setup'!B179,IF('Memory setup'!B179&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B179),""))</f>
+        <f>IF('Memory setup'!F183=1,'Memory setup'!B183,IF('Memory setup'!B183&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B183),""))</f>
         <v/>
       </c>
       <c r="C187" t="str">
-        <f>IF(AND(B187&lt;&gt;"",'Memory setup'!A180&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
+        <f>IF(AND(B187&lt;&gt;"",'Memory setup'!A184&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="188" spans="1:3">
+      <c r="A188" t="str">
+        <f>IF('Memory setup'!A184&lt;&gt;"",IF('Memory setup'!A184&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A184,"};"),"")</f>
+        <v/>
+      </c>
+      <c r="B188" t="str">
+        <f>IF('Memory setup'!F184=1,'Memory setup'!B184,IF('Memory setup'!B184&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B184),""))</f>
+        <v/>
+      </c>
+      <c r="C188" t="str">
+        <f>IF(AND(B188&lt;&gt;"",'Memory setup'!A185&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="189" spans="1:3">
+      <c r="A189" t="str">
+        <f>IF('Memory setup'!A185&lt;&gt;"",IF('Memory setup'!A185&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A185,"};"),"")</f>
+        <v/>
+      </c>
+      <c r="B189" t="str">
+        <f>IF('Memory setup'!F185=1,'Memory setup'!B185,IF('Memory setup'!B185&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B185),""))</f>
+        <v/>
+      </c>
+      <c r="C189" t="str">
+        <f>IF(AND(B189&lt;&gt;"",'Memory setup'!A186&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="190" spans="1:3">
+      <c r="A190" t="str">
+        <f>IF('Memory setup'!A186&lt;&gt;"",IF('Memory setup'!A186&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A186,"};"),"")</f>
+        <v/>
+      </c>
+      <c r="B190" t="str">
+        <f>IF('Memory setup'!F186=1,'Memory setup'!B186,IF('Memory setup'!B186&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B186),""))</f>
+        <v/>
+      </c>
+      <c r="C190" t="str">
+        <f>IF(AND(B190&lt;&gt;"",'Memory setup'!A187&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="191" spans="1:3">
+      <c r="A191" t="str">
+        <f>IF('Memory setup'!A187&lt;&gt;"",IF('Memory setup'!A187&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A187,"};"),"")</f>
+        <v/>
+      </c>
+      <c r="B191" t="str">
+        <f>IF('Memory setup'!F187=1,'Memory setup'!B187,IF('Memory setup'!B187&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B187),""))</f>
+        <v/>
+      </c>
+      <c r="C191" t="str">
+        <f>IF(AND(B191&lt;&gt;"",'Memory setup'!A188&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
Added SSI encoder class (AMT232B support)
</commit_message>
<xml_diff>
--- a/Firmware/memory_map.xlsx
+++ b/Firmware/memory_map.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ST\OpenFFBoard\Firmware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6458CF88-A14D-4A81-A589-8ED4EC072739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D3027C5-AE33-4262-ADA6-3F1C504D9995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="28800" windowHeight="15435" activeTab="3" xr2:uid="{4859EFD2-ECA4-5640-B170-200D9DB85F48}"/>
+    <workbookView xWindow="9525" yWindow="2190" windowWidth="28800" windowHeight="15435" activeTab="1" xr2:uid="{4859EFD2-ECA4-5640-B170-200D9DB85F48}"/>
   </bookViews>
   <sheets>
     <sheet name="Memory setup" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="376">
   <si>
     <t>// Ports</t>
   </si>
@@ -1627,6 +1627,21 @@
   </si>
   <si>
     <t>0x211</t>
+  </si>
+  <si>
+    <t>// SSI</t>
+  </si>
+  <si>
+    <t>0x413</t>
+  </si>
+  <si>
+    <t>0x414</t>
+  </si>
+  <si>
+    <t>ADR_SSI_CONF1</t>
+  </si>
+  <si>
+    <t>ADR_SSI_OFS</t>
   </si>
 </sst>
 </file>
@@ -1765,7 +1780,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1776,17 +1791,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1800,8 +1809,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1815,7 +1822,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2137,20 +2144,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C5323F2-8FDE-7443-A989-42E1FE5B01C7}">
-  <dimension ref="A1:G172"/>
+  <dimension ref="A1:G175"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView topLeftCell="A130" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B150" sqref="B150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="25.5" customWidth="1"/>
-    <col min="2" max="2" width="33.375" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.375" style="8" customWidth="1"/>
-    <col min="4" max="4" width="48.875" style="8" customWidth="1"/>
-    <col min="5" max="5" width="19.875" style="23" customWidth="1"/>
-    <col min="6" max="6" width="29.625" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.375" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.375" customWidth="1"/>
+    <col min="4" max="4" width="48.875" customWidth="1"/>
+    <col min="5" max="5" width="19.875" style="17" customWidth="1"/>
+    <col min="6" max="6" width="29.625" style="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -2160,16 +2167,16 @@
       <c r="B1" s="5" t="s">
         <v>282</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="4" t="s">
         <v>281</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="9" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2177,56 +2184,56 @@
       <c r="A2" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="E2" s="22"/>
-      <c r="F2" s="14"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="10"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="10">
-        <v>1</v>
-      </c>
-      <c r="E3" s="15">
+      <c r="C3" s="8">
+        <v>1</v>
+      </c>
+      <c r="E3" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="8">
         <v>2</v>
       </c>
-      <c r="E4" s="15">
+      <c r="E4" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="7" t="s">
         <v>362</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="8">
         <v>4</v>
       </c>
-      <c r="E5" s="15">
-        <v>1</v>
-      </c>
-      <c r="F5" s="15">
+      <c r="E5" s="11">
+        <v>1</v>
+      </c>
+      <c r="F5" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="8">
         <v>10</v>
       </c>
-      <c r="E6" s="15">
-        <v>1</v>
-      </c>
-      <c r="F6" s="15">
+      <c r="E6" s="11">
+        <v>1</v>
+      </c>
+      <c r="F6" s="11">
         <v>1</v>
       </c>
     </row>
@@ -2236,30 +2243,30 @@
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="15">
-        <v>1</v>
-      </c>
-      <c r="F8" s="15">
+      <c r="E8" s="11">
+        <v>1</v>
+      </c>
+      <c r="F8" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="15">
-        <v>1</v>
-      </c>
-      <c r="F9" s="15">
+      <c r="E9" s="11">
+        <v>1</v>
+      </c>
+      <c r="F9" s="11">
         <v>1</v>
       </c>
     </row>
@@ -2269,44 +2276,44 @@
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="15">
-        <v>1</v>
-      </c>
-      <c r="F11" s="15">
+      <c r="E11" s="11">
+        <v>1</v>
+      </c>
+      <c r="F11" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E12" s="15">
-        <v>1</v>
-      </c>
-      <c r="F12" s="15">
+      <c r="E12" s="11">
+        <v>1</v>
+      </c>
+      <c r="F12" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E13" s="15">
-        <v>1</v>
-      </c>
-      <c r="F13" s="15">
+      <c r="E13" s="11">
+        <v>1</v>
+      </c>
+      <c r="F13" s="11">
         <v>1</v>
       </c>
     </row>
@@ -2316,100 +2323,100 @@
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E15" s="15">
-        <v>1</v>
-      </c>
-      <c r="F15" s="15">
+      <c r="E15" s="11">
+        <v>1</v>
+      </c>
+      <c r="F15" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E16" s="15">
-        <v>1</v>
-      </c>
-      <c r="F16" s="15">
+      <c r="E16" s="11">
+        <v>1</v>
+      </c>
+      <c r="F16" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:6">
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E17" s="15">
-        <v>1</v>
-      </c>
-      <c r="F17" s="15">
+      <c r="E17" s="11">
+        <v>1</v>
+      </c>
+      <c r="F17" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:6">
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E18" s="15">
-        <v>1</v>
-      </c>
-      <c r="F18" s="15">
+      <c r="E18" s="11">
+        <v>1</v>
+      </c>
+      <c r="F18" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C19" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E19" s="15">
-        <v>1</v>
-      </c>
-      <c r="F19" s="15">
+      <c r="E19" s="11">
+        <v>1</v>
+      </c>
+      <c r="F19" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="7" t="s">
         <v>279</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E20" s="15">
-        <v>1</v>
-      </c>
-      <c r="F20" s="15">
+      <c r="E20" s="11">
+        <v>1</v>
+      </c>
+      <c r="F20" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:6">
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="7" t="s">
         <v>280</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E21" s="15">
-        <v>1</v>
-      </c>
-      <c r="F21" s="15">
+      <c r="E21" s="11">
+        <v>1</v>
+      </c>
+      <c r="F21" s="11">
         <v>1</v>
       </c>
     </row>
@@ -2419,30 +2426,30 @@
       </c>
     </row>
     <row r="23" spans="1:6">
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E23" s="15">
-        <v>1</v>
-      </c>
-      <c r="F23" s="15">
+      <c r="E23" s="11">
+        <v>1</v>
+      </c>
+      <c r="F23" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:6">
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="7" t="s">
         <v>369</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C24" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="E24" s="23">
-        <v>1</v>
-      </c>
-      <c r="F24" s="15">
+      <c r="E24" s="17">
+        <v>1</v>
+      </c>
+      <c r="F24" s="11">
         <v>1</v>
       </c>
     </row>
@@ -2452,16 +2459,16 @@
       </c>
     </row>
     <row r="26" spans="1:6">
-      <c r="B26" s="9" t="s">
+      <c r="B26" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="C26" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E26" s="15">
-        <v>1</v>
-      </c>
-      <c r="F26" s="15">
+      <c r="E26" s="11">
+        <v>1</v>
+      </c>
+      <c r="F26" s="11">
         <v>1</v>
       </c>
     </row>
@@ -2471,16 +2478,16 @@
       </c>
     </row>
     <row r="28" spans="1:6">
-      <c r="B28" s="9" t="s">
+      <c r="B28" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="C28" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E28" s="15">
-        <v>1</v>
-      </c>
-      <c r="F28" s="15">
+      <c r="E28" s="11">
+        <v>1</v>
+      </c>
+      <c r="F28" s="11">
         <v>1</v>
       </c>
     </row>
@@ -2490,86 +2497,86 @@
       </c>
     </row>
     <row r="30" spans="1:6">
-      <c r="B30" s="9" t="s">
+      <c r="B30" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="C30" s="11" t="s">
+      <c r="C30" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E30" s="15">
-        <v>1</v>
-      </c>
-      <c r="F30" s="15">
+      <c r="E30" s="11">
+        <v>1</v>
+      </c>
+      <c r="F30" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:6">
-      <c r="B31" s="9" t="s">
+      <c r="B31" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C31" s="11" t="s">
+      <c r="C31" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E31" s="15">
-        <v>1</v>
-      </c>
-      <c r="F31" s="15">
+      <c r="E31" s="11">
+        <v>1</v>
+      </c>
+      <c r="F31" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:6">
-      <c r="B32" s="9" t="s">
+      <c r="B32" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C32" s="11" t="s">
+      <c r="C32" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E32" s="15">
-        <v>1</v>
-      </c>
-      <c r="F32" s="15">
+      <c r="E32" s="11">
+        <v>1</v>
+      </c>
+      <c r="F32" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:6">
-      <c r="B33" s="9" t="s">
+      <c r="B33" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C33" s="11" t="s">
+      <c r="C33" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E33" s="15">
-        <v>1</v>
-      </c>
-      <c r="F33" s="15">
+      <c r="E33" s="11">
+        <v>1</v>
+      </c>
+      <c r="F33" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:6">
-      <c r="B34" s="9" t="s">
+      <c r="B34" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C34" s="11" t="s">
+      <c r="C34" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E34" s="15">
-        <v>1</v>
-      </c>
-      <c r="F34" s="15">
+      <c r="E34" s="11">
+        <v>1</v>
+      </c>
+      <c r="F34" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:6">
-      <c r="B35" s="9" t="s">
+      <c r="B35" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="C35" s="11" t="s">
+      <c r="C35" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="E35" s="15">
-        <v>1</v>
-      </c>
-      <c r="F35" s="15">
+      <c r="E35" s="11">
+        <v>1</v>
+      </c>
+      <c r="F35" s="11">
         <v>1</v>
       </c>
     </row>
@@ -2579,16 +2586,16 @@
       </c>
     </row>
     <row r="37" spans="1:6">
-      <c r="B37" s="9" t="s">
+      <c r="B37" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="C37" s="11" t="s">
+      <c r="C37" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E37" s="15">
-        <v>1</v>
-      </c>
-      <c r="F37" s="15">
+      <c r="E37" s="11">
+        <v>1</v>
+      </c>
+      <c r="F37" s="11">
         <v>1</v>
       </c>
     </row>
@@ -2598,33 +2605,33 @@
       </c>
     </row>
     <row r="39" spans="1:6">
-      <c r="B39" s="9" t="s">
+      <c r="B39" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C39" s="11" t="s">
+      <c r="C39" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E39" s="15">
-        <v>1</v>
-      </c>
-      <c r="F39" s="15">
+      <c r="E39" s="11">
+        <v>1</v>
+      </c>
+      <c r="F39" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:6">
-      <c r="B40" s="9" t="s">
+      <c r="B40" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="C40" s="11" t="s">
+      <c r="C40" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D40" s="12" t="s">
+      <c r="D40" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="E40" s="15">
-        <v>1</v>
-      </c>
-      <c r="F40" s="15">
+      <c r="E40" s="11">
+        <v>1</v>
+      </c>
+      <c r="F40" s="11">
         <v>1</v>
       </c>
     </row>
@@ -2634,13 +2641,13 @@
       </c>
     </row>
     <row r="42" spans="1:6">
-      <c r="B42" s="9" t="s">
+      <c r="B42" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C42" s="11" t="s">
+      <c r="C42" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E42" s="15">
+      <c r="E42" s="11">
         <v>1</v>
       </c>
     </row>
@@ -2650,121 +2657,121 @@
       </c>
     </row>
     <row r="44" spans="1:6">
-      <c r="B44" s="9" t="s">
+      <c r="B44" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C44" s="11" t="s">
+      <c r="C44" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D44" s="12" t="s">
+      <c r="D44" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="E44" s="15">
-        <v>1</v>
-      </c>
-      <c r="F44" s="15">
+      <c r="E44" s="11">
+        <v>1</v>
+      </c>
+      <c r="F44" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:6">
-      <c r="B45" s="9" t="s">
+      <c r="B45" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="C45" s="11" t="s">
+      <c r="C45" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D45" s="12" t="s">
+      <c r="D45" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="E45" s="15">
-        <v>1</v>
-      </c>
-      <c r="F45" s="15">
+      <c r="E45" s="11">
+        <v>1</v>
+      </c>
+      <c r="F45" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:6">
-      <c r="B46" s="9" t="s">
+      <c r="B46" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C46" s="11" t="s">
+      <c r="C46" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D46" s="12" t="s">
+      <c r="D46" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="E46" s="15">
-        <v>1</v>
-      </c>
-      <c r="F46" s="15">
+      <c r="E46" s="11">
+        <v>1</v>
+      </c>
+      <c r="F46" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:6">
-      <c r="B47" s="9" t="s">
+      <c r="B47" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="C47" s="11" t="s">
+      <c r="C47" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D47" s="12" t="s">
+      <c r="D47" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="E47" s="15">
-        <v>1</v>
-      </c>
-      <c r="F47" s="15">
+      <c r="E47" s="11">
+        <v>1</v>
+      </c>
+      <c r="F47" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:6">
-      <c r="B48" s="9" t="s">
+      <c r="B48" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="C48" s="11" t="s">
+      <c r="C48" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D48" s="12" t="s">
+      <c r="D48" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E48" s="15">
-        <v>1</v>
-      </c>
-      <c r="F48" s="15">
+      <c r="E48" s="11">
+        <v>1</v>
+      </c>
+      <c r="F48" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:7">
-      <c r="B49" s="9" t="s">
+      <c r="B49" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="C49" s="11" t="s">
+      <c r="C49" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D49" s="12" t="s">
+      <c r="D49" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="E49" s="15">
-        <v>1</v>
-      </c>
-      <c r="F49" s="15">
+      <c r="E49" s="11">
+        <v>1</v>
+      </c>
+      <c r="F49" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:7">
-      <c r="B50" s="9" t="s">
+      <c r="B50" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="C50" s="11" t="s">
+      <c r="C50" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D50" s="12" t="s">
+      <c r="D50" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="E50" s="15">
-        <v>1</v>
-      </c>
-      <c r="F50" s="15">
+      <c r="E50" s="11">
+        <v>1</v>
+      </c>
+      <c r="F50" s="11">
         <v>1</v>
       </c>
     </row>
@@ -2772,26 +2779,26 @@
       <c r="A51" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B51" s="9"/>
-      <c r="C51" s="11"/>
-      <c r="D51" s="12"/>
-      <c r="E51" s="15"/>
+      <c r="B51" s="7"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="11"/>
     </row>
     <row r="52" spans="1:7">
-      <c r="B52" s="9" t="s">
+      <c r="B52" s="7" t="s">
         <v>302</v>
       </c>
-      <c r="C52" s="11" t="s">
+      <c r="C52" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="D52" s="12"/>
-      <c r="E52" s="15">
-        <v>1</v>
-      </c>
-      <c r="F52" s="15">
-        <v>1</v>
-      </c>
-      <c r="G52" s="21"/>
+      <c r="D52" s="1"/>
+      <c r="E52" s="11">
+        <v>1</v>
+      </c>
+      <c r="F52" s="11">
+        <v>1</v>
+      </c>
+      <c r="G52" s="15"/>
     </row>
     <row r="53" spans="1:7">
       <c r="A53" s="1" t="s">
@@ -2799,16 +2806,16 @@
       </c>
     </row>
     <row r="54" spans="1:7">
-      <c r="B54" s="9" t="s">
+      <c r="B54" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="C54" s="11" t="s">
+      <c r="C54" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="E54" s="15">
-        <v>1</v>
-      </c>
-      <c r="F54" s="15">
+      <c r="E54" s="11">
+        <v>1</v>
+      </c>
+      <c r="F54" s="11">
         <v>1</v>
       </c>
     </row>
@@ -2818,149 +2825,149 @@
       </c>
     </row>
     <row r="56" spans="1:7">
-      <c r="B56" s="9" t="s">
+      <c r="B56" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="C56" s="11" t="s">
+      <c r="C56" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D56" s="12" t="s">
+      <c r="D56" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="E56" s="15">
-        <v>1</v>
-      </c>
-      <c r="F56" s="15">
+      <c r="E56" s="11">
+        <v>1</v>
+      </c>
+      <c r="F56" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:7">
-      <c r="B57" s="9" t="s">
+      <c r="B57" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="C57" s="11" t="s">
+      <c r="C57" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="E57" s="15">
-        <v>1</v>
-      </c>
-      <c r="F57" s="15">
+      <c r="E57" s="11">
+        <v>1</v>
+      </c>
+      <c r="F57" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:7">
-      <c r="B58" s="9" t="s">
+      <c r="B58" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="C58" s="11" t="s">
+      <c r="C58" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="E58" s="15">
-        <v>1</v>
-      </c>
-      <c r="F58" s="15">
+      <c r="E58" s="11">
+        <v>1</v>
+      </c>
+      <c r="F58" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:7">
-      <c r="B59" s="9" t="s">
+      <c r="B59" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="C59" s="11" t="s">
+      <c r="C59" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D59" s="12" t="s">
+      <c r="D59" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="E59" s="15">
-        <v>1</v>
-      </c>
-      <c r="F59" s="15">
+      <c r="E59" s="11">
+        <v>1</v>
+      </c>
+      <c r="F59" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:7">
-      <c r="B60" s="9" t="s">
+      <c r="B60" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C60" s="11" t="s">
+      <c r="C60" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="D60" s="12" t="s">
+      <c r="D60" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="E60" s="15">
-        <v>1</v>
-      </c>
-      <c r="F60" s="15">
+      <c r="E60" s="11">
+        <v>1</v>
+      </c>
+      <c r="F60" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:7">
-      <c r="B61" s="9" t="s">
+      <c r="B61" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="C61" s="11" t="s">
+      <c r="C61" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D61" s="12" t="s">
+      <c r="D61" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="E61" s="15">
-        <v>1</v>
-      </c>
-      <c r="F61" s="15">
+      <c r="E61" s="11">
+        <v>1</v>
+      </c>
+      <c r="F61" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:7">
-      <c r="B62" s="9" t="s">
+      <c r="B62" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="C62" s="11" t="s">
+      <c r="C62" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="D62" s="12" t="s">
+      <c r="D62" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="E62" s="15">
-        <v>1</v>
-      </c>
-      <c r="F62" s="15">
+      <c r="E62" s="11">
+        <v>1</v>
+      </c>
+      <c r="F62" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:7">
-      <c r="B63" s="9" t="s">
+      <c r="B63" s="7" t="s">
         <v>308</v>
       </c>
-      <c r="C63" s="11" t="s">
+      <c r="C63" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D63" s="24" t="s">
+      <c r="D63" s="18" t="s">
         <v>309</v>
       </c>
-      <c r="E63" s="15">
-        <v>1</v>
-      </c>
-      <c r="F63" s="15">
+      <c r="E63" s="11">
+        <v>1</v>
+      </c>
+      <c r="F63" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:7">
-      <c r="B64" s="9" t="s">
+      <c r="B64" s="7" t="s">
         <v>304</v>
       </c>
-      <c r="C64" s="11" t="s">
+      <c r="C64" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D64" s="12" t="s">
+      <c r="D64" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="E64" s="15">
-        <v>1</v>
-      </c>
-      <c r="F64" s="15">
+      <c r="E64" s="11">
+        <v>1</v>
+      </c>
+      <c r="F64" s="11">
         <v>1</v>
       </c>
     </row>
@@ -2970,178 +2977,178 @@
       </c>
     </row>
     <row r="66" spans="1:6">
-      <c r="B66" s="9" t="s">
+      <c r="B66" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="C66" s="11" t="s">
+      <c r="C66" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="D66" s="12" t="s">
+      <c r="D66" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="E66" s="15">
-        <v>1</v>
-      </c>
-      <c r="F66" s="15">
+      <c r="E66" s="11">
+        <v>1</v>
+      </c>
+      <c r="F66" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:6">
-      <c r="B67" s="9" t="s">
+      <c r="B67" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="C67" s="11" t="s">
+      <c r="C67" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="E67" s="15">
-        <v>1</v>
-      </c>
-      <c r="F67" s="15">
+      <c r="E67" s="11">
+        <v>1</v>
+      </c>
+      <c r="F67" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:6">
-      <c r="B68" s="9" t="s">
+      <c r="B68" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="C68" s="11" t="s">
+      <c r="C68" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="D68" s="12" t="s">
+      <c r="D68" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="E68" s="15">
-        <v>1</v>
-      </c>
-      <c r="F68" s="15">
+      <c r="E68" s="11">
+        <v>1</v>
+      </c>
+      <c r="F68" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:6">
-      <c r="B69" s="9" t="s">
+      <c r="B69" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="C69" s="11" t="s">
+      <c r="C69" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="E69" s="15">
+      <c r="E69" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:6">
-      <c r="B70" s="9" t="s">
+      <c r="B70" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="C70" s="11" t="s">
+      <c r="C70" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="E70" s="15">
+      <c r="E70" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:6">
-      <c r="B71" s="9" t="s">
+      <c r="B71" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="C71" s="11" t="s">
+      <c r="C71" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="E71" s="15">
+      <c r="E71" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:6">
-      <c r="B72" s="9" t="s">
+      <c r="B72" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="C72" s="11" t="s">
+      <c r="C72" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="E72" s="15">
-        <v>1</v>
-      </c>
-      <c r="F72" s="15">
+      <c r="E72" s="11">
+        <v>1</v>
+      </c>
+      <c r="F72" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:6">
-      <c r="B73" s="9" t="s">
+      <c r="B73" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="C73" s="11" t="s">
+      <c r="C73" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="E73" s="15">
-        <v>1</v>
-      </c>
-      <c r="F73" s="15">
+      <c r="E73" s="11">
+        <v>1</v>
+      </c>
+      <c r="F73" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:6">
-      <c r="B74" s="9" t="s">
+      <c r="B74" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="C74" s="11" t="s">
+      <c r="C74" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="E74" s="15">
-        <v>1</v>
-      </c>
-      <c r="F74" s="15">
+      <c r="E74" s="11">
+        <v>1</v>
+      </c>
+      <c r="F74" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:6">
-      <c r="B75" s="9" t="s">
+      <c r="B75" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="C75" s="11" t="s">
+      <c r="C75" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="E75" s="15">
-        <v>1</v>
-      </c>
-      <c r="F75" s="15">
+      <c r="E75" s="11">
+        <v>1</v>
+      </c>
+      <c r="F75" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:6">
-      <c r="B76" s="9" t="s">
+      <c r="B76" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="C76" s="11" t="s">
+      <c r="C76" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="E76" s="15">
-        <v>1</v>
-      </c>
-      <c r="F76" s="15">
+      <c r="E76" s="11">
+        <v>1</v>
+      </c>
+      <c r="F76" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:6">
-      <c r="B77" s="9" t="s">
+      <c r="B77" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="C77" s="11" t="s">
+      <c r="C77" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="E77" s="15">
+      <c r="E77" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:6">
-      <c r="B78" s="9" t="s">
+      <c r="B78" s="7" t="s">
         <v>363</v>
       </c>
-      <c r="C78" s="11" t="s">
+      <c r="C78" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="E78" s="23">
-        <v>1</v>
-      </c>
-      <c r="F78" s="15">
+      <c r="E78" s="17">
+        <v>1</v>
+      </c>
+      <c r="F78" s="11">
         <v>1</v>
       </c>
     </row>
@@ -3151,149 +3158,149 @@
       </c>
     </row>
     <row r="80" spans="1:6">
-      <c r="B80" s="9" t="s">
+      <c r="B80" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="C80" s="11" t="s">
+      <c r="C80" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="D80" s="12" t="s">
+      <c r="D80" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="E80" s="15">
-        <v>1</v>
-      </c>
-      <c r="F80" s="15">
+      <c r="E80" s="11">
+        <v>1</v>
+      </c>
+      <c r="F80" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:6">
-      <c r="B81" s="9" t="s">
+      <c r="B81" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="C81" s="11" t="s">
+      <c r="C81" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="E81" s="15">
-        <v>1</v>
-      </c>
-      <c r="F81" s="15">
+      <c r="E81" s="11">
+        <v>1</v>
+      </c>
+      <c r="F81" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="82" spans="1:6">
-      <c r="B82" s="9" t="s">
+      <c r="B82" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="C82" s="11" t="s">
+      <c r="C82" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="E82" s="15">
-        <v>1</v>
-      </c>
-      <c r="F82" s="15">
+      <c r="E82" s="11">
+        <v>1</v>
+      </c>
+      <c r="F82" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:6">
-      <c r="B83" s="9" t="s">
+      <c r="B83" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="C83" s="11" t="s">
+      <c r="C83" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="D83" s="12" t="s">
+      <c r="D83" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="E83" s="15">
-        <v>1</v>
-      </c>
-      <c r="F83" s="15">
+      <c r="E83" s="11">
+        <v>1</v>
+      </c>
+      <c r="F83" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="84" spans="1:6">
-      <c r="B84" s="9" t="s">
+      <c r="B84" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="C84" s="11" t="s">
+      <c r="C84" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="D84" s="12" t="s">
+      <c r="D84" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="E84" s="15">
-        <v>1</v>
-      </c>
-      <c r="F84" s="15">
+      <c r="E84" s="11">
+        <v>1</v>
+      </c>
+      <c r="F84" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="85" spans="1:6">
-      <c r="B85" s="9" t="s">
+      <c r="B85" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="C85" s="11" t="s">
+      <c r="C85" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="D85" s="12" t="s">
+      <c r="D85" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="E85" s="15">
-        <v>1</v>
-      </c>
-      <c r="F85" s="15">
+      <c r="E85" s="11">
+        <v>1</v>
+      </c>
+      <c r="F85" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="86" spans="1:6">
-      <c r="B86" s="9" t="s">
+      <c r="B86" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="C86" s="11" t="s">
+      <c r="C86" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="D86" s="12" t="s">
+      <c r="D86" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="E86" s="15">
-        <v>1</v>
-      </c>
-      <c r="F86" s="15">
+      <c r="E86" s="11">
+        <v>1</v>
+      </c>
+      <c r="F86" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="87" spans="1:6">
-      <c r="B87" s="9" t="s">
+      <c r="B87" s="7" t="s">
         <v>310</v>
       </c>
-      <c r="C87" s="11" t="s">
+      <c r="C87" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="D87" s="24" t="s">
+      <c r="D87" s="18" t="s">
         <v>309</v>
       </c>
-      <c r="E87" s="15">
-        <v>1</v>
-      </c>
-      <c r="F87" s="15">
+      <c r="E87" s="11">
+        <v>1</v>
+      </c>
+      <c r="F87" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:6">
-      <c r="B88" s="9" t="s">
+      <c r="B88" s="7" t="s">
         <v>306</v>
       </c>
-      <c r="C88" s="11" t="s">
+      <c r="C88" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="D88" s="12" t="s">
+      <c r="D88" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="E88" s="15">
-        <v>1</v>
-      </c>
-      <c r="F88" s="15">
+      <c r="E88" s="11">
+        <v>1</v>
+      </c>
+      <c r="F88" s="11">
         <v>1</v>
       </c>
     </row>
@@ -3303,178 +3310,178 @@
       </c>
     </row>
     <row r="90" spans="1:6">
-      <c r="B90" s="9" t="s">
+      <c r="B90" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="C90" s="11" t="s">
+      <c r="C90" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="D90" s="12" t="s">
+      <c r="D90" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="E90" s="15">
-        <v>1</v>
-      </c>
-      <c r="F90" s="15">
+      <c r="E90" s="11">
+        <v>1</v>
+      </c>
+      <c r="F90" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="91" spans="1:6">
-      <c r="B91" s="9" t="s">
+      <c r="B91" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="C91" s="11" t="s">
+      <c r="C91" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="E91" s="15">
-        <v>1</v>
-      </c>
-      <c r="F91" s="15">
+      <c r="E91" s="11">
+        <v>1</v>
+      </c>
+      <c r="F91" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="92" spans="1:6">
-      <c r="B92" s="9" t="s">
+      <c r="B92" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="C92" s="11" t="s">
+      <c r="C92" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="D92" s="12" t="s">
+      <c r="D92" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="E92" s="15">
-        <v>1</v>
-      </c>
-      <c r="F92" s="15">
+      <c r="E92" s="11">
+        <v>1</v>
+      </c>
+      <c r="F92" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="93" spans="1:6">
-      <c r="B93" s="9" t="s">
+      <c r="B93" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="C93" s="11" t="s">
+      <c r="C93" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="E93" s="15">
+      <c r="E93" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="94" spans="1:6">
-      <c r="B94" s="9" t="s">
+      <c r="B94" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="C94" s="11" t="s">
+      <c r="C94" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="E94" s="15">
+      <c r="E94" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="95" spans="1:6">
-      <c r="B95" s="9" t="s">
+      <c r="B95" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="C95" s="11" t="s">
+      <c r="C95" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="E95" s="15">
+      <c r="E95" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="96" spans="1:6">
-      <c r="B96" s="9" t="s">
+      <c r="B96" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="C96" s="11" t="s">
+      <c r="C96" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="E96" s="15">
-        <v>1</v>
-      </c>
-      <c r="F96" s="15">
+      <c r="E96" s="11">
+        <v>1</v>
+      </c>
+      <c r="F96" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="97" spans="1:6">
-      <c r="B97" s="9" t="s">
+      <c r="B97" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="C97" s="11" t="s">
+      <c r="C97" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="E97" s="15">
-        <v>1</v>
-      </c>
-      <c r="F97" s="15">
+      <c r="E97" s="11">
+        <v>1</v>
+      </c>
+      <c r="F97" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="98" spans="1:6">
-      <c r="B98" s="9" t="s">
+      <c r="B98" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="C98" s="11" t="s">
+      <c r="C98" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="E98" s="15">
-        <v>1</v>
-      </c>
-      <c r="F98" s="15">
+      <c r="E98" s="11">
+        <v>1</v>
+      </c>
+      <c r="F98" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="99" spans="1:6">
-      <c r="B99" s="9" t="s">
+      <c r="B99" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="C99" s="11" t="s">
+      <c r="C99" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="E99" s="15">
-        <v>1</v>
-      </c>
-      <c r="F99" s="15">
+      <c r="E99" s="11">
+        <v>1</v>
+      </c>
+      <c r="F99" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="100" spans="1:6">
-      <c r="B100" s="9" t="s">
+      <c r="B100" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="C100" s="11" t="s">
+      <c r="C100" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="E100" s="15">
-        <v>1</v>
-      </c>
-      <c r="F100" s="15">
+      <c r="E100" s="11">
+        <v>1</v>
+      </c>
+      <c r="F100" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="101" spans="1:6">
-      <c r="B101" s="9" t="s">
+      <c r="B101" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="C101" s="11" t="s">
+      <c r="C101" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="E101" s="15">
+      <c r="E101" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="102" spans="1:6">
-      <c r="B102" s="9" t="s">
+      <c r="B102" s="7" t="s">
         <v>365</v>
       </c>
-      <c r="C102" s="11" t="s">
+      <c r="C102" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="E102" s="23">
-        <v>1</v>
-      </c>
-      <c r="F102" s="15">
+      <c r="E102" s="17">
+        <v>1</v>
+      </c>
+      <c r="F102" s="11">
         <v>1</v>
       </c>
     </row>
@@ -3484,149 +3491,149 @@
       </c>
     </row>
     <row r="104" spans="1:6">
-      <c r="B104" s="9" t="s">
+      <c r="B104" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="C104" s="11" t="s">
+      <c r="C104" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="D104" s="12" t="s">
+      <c r="D104" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="E104" s="15">
-        <v>1</v>
-      </c>
-      <c r="F104" s="15">
+      <c r="E104" s="11">
+        <v>1</v>
+      </c>
+      <c r="F104" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="105" spans="1:6">
-      <c r="B105" s="9" t="s">
+      <c r="B105" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="C105" s="11" t="s">
+      <c r="C105" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="E105" s="15">
-        <v>1</v>
-      </c>
-      <c r="F105" s="15">
+      <c r="E105" s="11">
+        <v>1</v>
+      </c>
+      <c r="F105" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="106" spans="1:6">
-      <c r="B106" s="9" t="s">
+      <c r="B106" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="C106" s="11" t="s">
+      <c r="C106" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="E106" s="15">
-        <v>1</v>
-      </c>
-      <c r="F106" s="15">
+      <c r="E106" s="11">
+        <v>1</v>
+      </c>
+      <c r="F106" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="107" spans="1:6">
-      <c r="B107" s="9" t="s">
+      <c r="B107" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="C107" s="11" t="s">
+      <c r="C107" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="D107" s="12" t="s">
+      <c r="D107" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="E107" s="15">
-        <v>1</v>
-      </c>
-      <c r="F107" s="15">
+      <c r="E107" s="11">
+        <v>1</v>
+      </c>
+      <c r="F107" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="108" spans="1:6">
-      <c r="B108" s="9" t="s">
+      <c r="B108" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="C108" s="11" t="s">
+      <c r="C108" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="D108" s="12" t="s">
+      <c r="D108" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="E108" s="15">
-        <v>1</v>
-      </c>
-      <c r="F108" s="15">
+      <c r="E108" s="11">
+        <v>1</v>
+      </c>
+      <c r="F108" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="109" spans="1:6">
-      <c r="B109" s="9" t="s">
+      <c r="B109" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="C109" s="11" t="s">
+      <c r="C109" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="D109" s="12" t="s">
+      <c r="D109" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="E109" s="15">
-        <v>1</v>
-      </c>
-      <c r="F109" s="15">
+      <c r="E109" s="11">
+        <v>1</v>
+      </c>
+      <c r="F109" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="110" spans="1:6">
-      <c r="B110" s="9" t="s">
+      <c r="B110" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="C110" s="11" t="s">
+      <c r="C110" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="D110" s="12" t="s">
+      <c r="D110" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="E110" s="15">
-        <v>1</v>
-      </c>
-      <c r="F110" s="15">
+      <c r="E110" s="11">
+        <v>1</v>
+      </c>
+      <c r="F110" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="111" spans="1:6">
-      <c r="B111" s="9" t="s">
+      <c r="B111" s="7" t="s">
         <v>311</v>
       </c>
-      <c r="C111" s="11" t="s">
+      <c r="C111" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="D111" s="24" t="s">
+      <c r="D111" s="18" t="s">
         <v>309</v>
       </c>
-      <c r="E111" s="15">
-        <v>1</v>
-      </c>
-      <c r="F111" s="15">
+      <c r="E111" s="11">
+        <v>1</v>
+      </c>
+      <c r="F111" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="112" spans="1:6">
-      <c r="B112" s="9" t="s">
+      <c r="B112" s="7" t="s">
         <v>307</v>
       </c>
-      <c r="C112" s="11" t="s">
+      <c r="C112" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="D112" s="12" t="s">
+      <c r="D112" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="E112" s="15">
-        <v>1</v>
-      </c>
-      <c r="F112" s="15">
+      <c r="E112" s="11">
+        <v>1</v>
+      </c>
+      <c r="F112" s="11">
         <v>1</v>
       </c>
     </row>
@@ -3636,178 +3643,178 @@
       </c>
     </row>
     <row r="114" spans="1:6">
-      <c r="B114" s="9" t="s">
+      <c r="B114" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="C114" s="11" t="s">
+      <c r="C114" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="D114" s="12" t="s">
+      <c r="D114" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="E114" s="15">
-        <v>1</v>
-      </c>
-      <c r="F114" s="15">
+      <c r="E114" s="11">
+        <v>1</v>
+      </c>
+      <c r="F114" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="115" spans="1:6">
-      <c r="B115" s="9" t="s">
+      <c r="B115" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="C115" s="11" t="s">
+      <c r="C115" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="E115" s="15">
-        <v>1</v>
-      </c>
-      <c r="F115" s="15">
+      <c r="E115" s="11">
+        <v>1</v>
+      </c>
+      <c r="F115" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="116" spans="1:6">
-      <c r="B116" s="9" t="s">
+      <c r="B116" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="C116" s="11" t="s">
+      <c r="C116" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="D116" s="12" t="s">
+      <c r="D116" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="E116" s="15">
-        <v>1</v>
-      </c>
-      <c r="F116" s="15">
+      <c r="E116" s="11">
+        <v>1</v>
+      </c>
+      <c r="F116" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="117" spans="1:6">
-      <c r="B117" s="9" t="s">
+      <c r="B117" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="C117" s="11" t="s">
+      <c r="C117" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="E117" s="15">
+      <c r="E117" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="118" spans="1:6">
-      <c r="B118" s="9" t="s">
+      <c r="B118" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="C118" s="11" t="s">
+      <c r="C118" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="E118" s="15">
+      <c r="E118" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="119" spans="1:6">
-      <c r="B119" s="9" t="s">
+      <c r="B119" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="C119" s="11" t="s">
+      <c r="C119" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="E119" s="15">
+      <c r="E119" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="120" spans="1:6">
-      <c r="B120" s="9" t="s">
+      <c r="B120" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="C120" s="11" t="s">
+      <c r="C120" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="E120" s="15">
-        <v>1</v>
-      </c>
-      <c r="F120" s="15">
+      <c r="E120" s="11">
+        <v>1</v>
+      </c>
+      <c r="F120" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="121" spans="1:6">
-      <c r="B121" s="9" t="s">
+      <c r="B121" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="C121" s="11" t="s">
+      <c r="C121" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="E121" s="15">
-        <v>1</v>
-      </c>
-      <c r="F121" s="15">
+      <c r="E121" s="11">
+        <v>1</v>
+      </c>
+      <c r="F121" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="122" spans="1:6">
-      <c r="B122" s="9" t="s">
+      <c r="B122" s="7" t="s">
         <v>199</v>
       </c>
-      <c r="C122" s="11" t="s">
+      <c r="C122" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="E122" s="15">
-        <v>1</v>
-      </c>
-      <c r="F122" s="15">
+      <c r="E122" s="11">
+        <v>1</v>
+      </c>
+      <c r="F122" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="123" spans="1:6">
-      <c r="B123" s="9" t="s">
+      <c r="B123" s="7" t="s">
         <v>201</v>
       </c>
-      <c r="C123" s="11" t="s">
+      <c r="C123" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="E123" s="15">
-        <v>1</v>
-      </c>
-      <c r="F123" s="15">
+      <c r="E123" s="11">
+        <v>1</v>
+      </c>
+      <c r="F123" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="124" spans="1:6">
-      <c r="B124" s="9" t="s">
+      <c r="B124" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="C124" s="11" t="s">
+      <c r="C124" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="E124" s="15">
-        <v>1</v>
-      </c>
-      <c r="F124" s="15">
+      <c r="E124" s="11">
+        <v>1</v>
+      </c>
+      <c r="F124" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="125" spans="1:6">
-      <c r="B125" s="9" t="s">
+      <c r="B125" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="C125" s="11" t="s">
+      <c r="C125" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="E125" s="15">
+      <c r="E125" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="126" spans="1:6">
-      <c r="B126" s="9" t="s">
+      <c r="B126" s="7" t="s">
         <v>368</v>
       </c>
-      <c r="C126" s="11" t="s">
+      <c r="C126" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="E126" s="23">
-        <v>1</v>
-      </c>
-      <c r="F126" s="15">
+      <c r="E126" s="17">
+        <v>1</v>
+      </c>
+      <c r="F126" s="11">
         <v>1</v>
       </c>
     </row>
@@ -3817,47 +3824,47 @@
       </c>
     </row>
     <row r="128" spans="1:6">
-      <c r="B128" s="9" t="s">
+      <c r="B128" s="7" t="s">
         <v>207</v>
       </c>
-      <c r="C128" s="11" t="s">
+      <c r="C128" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="D128" s="12" t="s">
+      <c r="D128" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="E128" s="15">
-        <v>1</v>
-      </c>
-      <c r="F128" s="15">
+      <c r="E128" s="11">
+        <v>1</v>
+      </c>
+      <c r="F128" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="129" spans="1:6">
-      <c r="B129" s="9" t="s">
+      <c r="B129" s="7" t="s">
         <v>209</v>
       </c>
-      <c r="C129" s="11" t="s">
+      <c r="C129" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="E129" s="15">
-        <v>1</v>
-      </c>
-      <c r="F129" s="15">
+      <c r="E129" s="11">
+        <v>1</v>
+      </c>
+      <c r="F129" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="130" spans="1:6">
-      <c r="B130" s="9" t="s">
+      <c r="B130" s="7" t="s">
         <v>211</v>
       </c>
-      <c r="C130" s="11" t="s">
+      <c r="C130" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="E130" s="15">
-        <v>1</v>
-      </c>
-      <c r="F130" s="15">
+      <c r="E130" s="11">
+        <v>1</v>
+      </c>
+      <c r="F130" s="11">
         <v>1</v>
       </c>
     </row>
@@ -3867,155 +3874,155 @@
       </c>
     </row>
     <row r="132" spans="1:6">
-      <c r="B132" s="9" t="s">
+      <c r="B132" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="C132" s="11" t="s">
+      <c r="C132" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="D132" s="12" t="s">
+      <c r="D132" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="E132" s="15">
-        <v>1</v>
-      </c>
-      <c r="F132" s="15">
+      <c r="E132" s="11">
+        <v>1</v>
+      </c>
+      <c r="F132" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="133" spans="1:6">
-      <c r="B133" s="9" t="s">
+      <c r="B133" s="7" t="s">
         <v>215</v>
       </c>
-      <c r="C133" s="11" t="s">
+      <c r="C133" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="D133" s="12" t="s">
+      <c r="D133" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="E133" s="15">
-        <v>1</v>
-      </c>
-      <c r="F133" s="15">
+      <c r="E133" s="11">
+        <v>1</v>
+      </c>
+      <c r="F133" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="134" spans="1:6">
-      <c r="B134" s="9" t="s">
+      <c r="B134" s="7" t="s">
         <v>217</v>
       </c>
-      <c r="C134" s="11" t="s">
+      <c r="C134" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="D134" s="12" t="s">
+      <c r="D134" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="E134" s="15">
-        <v>1</v>
-      </c>
-      <c r="F134" s="15">
+      <c r="E134" s="11">
+        <v>1</v>
+      </c>
+      <c r="F134" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="135" spans="1:6">
-      <c r="B135" s="9" t="s">
+      <c r="B135" s="7" t="s">
         <v>219</v>
       </c>
-      <c r="C135" s="11" t="s">
+      <c r="C135" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="D135" s="12" t="s">
+      <c r="D135" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="E135" s="15">
-        <v>1</v>
-      </c>
-      <c r="F135" s="15">
+      <c r="E135" s="11">
+        <v>1</v>
+      </c>
+      <c r="F135" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="136" spans="1:6">
-      <c r="B136" s="9" t="s">
+      <c r="B136" s="7" t="s">
         <v>221</v>
       </c>
-      <c r="C136" s="11" t="s">
+      <c r="C136" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="D136" s="12" t="s">
+      <c r="D136" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="E136" s="15">
-        <v>1</v>
-      </c>
-      <c r="F136" s="15">
+      <c r="E136" s="11">
+        <v>1</v>
+      </c>
+      <c r="F136" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="137" spans="1:6">
-      <c r="B137" s="9" t="s">
+      <c r="B137" s="7" t="s">
         <v>223</v>
       </c>
-      <c r="C137" s="11" t="s">
+      <c r="C137" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="D137" s="12" t="s">
+      <c r="D137" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="E137" s="15">
-        <v>1</v>
-      </c>
-      <c r="F137" s="15">
+      <c r="E137" s="11">
+        <v>1</v>
+      </c>
+      <c r="F137" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="138" spans="1:6">
-      <c r="B138" s="9" t="s">
+      <c r="B138" s="7" t="s">
         <v>225</v>
       </c>
-      <c r="C138" s="11" t="s">
+      <c r="C138" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="D138" s="12" t="s">
+      <c r="D138" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="E138" s="15">
-        <v>1</v>
-      </c>
-      <c r="F138" s="15">
+      <c r="E138" s="11">
+        <v>1</v>
+      </c>
+      <c r="F138" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="139" spans="1:6">
-      <c r="B139" s="9" t="s">
+      <c r="B139" s="7" t="s">
         <v>227</v>
       </c>
-      <c r="C139" s="11" t="s">
+      <c r="C139" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="D139" s="12" t="s">
+      <c r="D139" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="E139" s="15">
-        <v>1</v>
-      </c>
-      <c r="F139" s="15">
+      <c r="E139" s="11">
+        <v>1</v>
+      </c>
+      <c r="F139" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="140" spans="1:6">
-      <c r="B140" s="9" t="s">
+      <c r="B140" s="7" t="s">
         <v>229</v>
       </c>
-      <c r="C140" s="11" t="s">
+      <c r="C140" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="D140" s="12" t="s">
+      <c r="D140" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="E140" s="15">
-        <v>1</v>
-      </c>
-      <c r="F140" s="15">
+      <c r="E140" s="11">
+        <v>1</v>
+      </c>
+      <c r="F140" s="11">
         <v>1</v>
       </c>
     </row>
@@ -4025,412 +4032,445 @@
       </c>
     </row>
     <row r="142" spans="1:6">
-      <c r="B142" s="9" t="s">
+      <c r="B142" s="7" t="s">
         <v>300</v>
       </c>
-      <c r="C142" s="11" t="s">
+      <c r="C142" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="E142" s="15">
-        <v>1</v>
-      </c>
-      <c r="F142" s="15">
+      <c r="E142" s="11">
+        <v>1</v>
+      </c>
+      <c r="F142" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="143" spans="1:6">
-      <c r="A143" s="20"/>
-      <c r="B143" s="9" t="s">
+      <c r="A143" s="14"/>
+      <c r="B143" s="7" t="s">
         <v>231</v>
       </c>
-      <c r="C143" s="11" t="s">
+      <c r="C143" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="E143" s="23">
-        <v>1</v>
-      </c>
-      <c r="F143" s="15">
+      <c r="E143" s="17">
+        <v>1</v>
+      </c>
+      <c r="F143" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="144" spans="1:6">
-      <c r="A144" s="20" t="s">
+      <c r="A144" s="14" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="145" spans="1:6">
-      <c r="B145" s="9" t="s">
+      <c r="B145" s="7" t="s">
         <v>296</v>
       </c>
-      <c r="C145" s="11" t="s">
+      <c r="C145" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="E145" s="23">
-        <v>1</v>
-      </c>
-      <c r="F145" s="15">
+      <c r="E145" s="17">
+        <v>1</v>
+      </c>
+      <c r="F145" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="146" spans="1:6">
-      <c r="B146" s="9" t="s">
+      <c r="B146" s="7" t="s">
         <v>297</v>
       </c>
-      <c r="C146" s="11" t="s">
+      <c r="C146" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="E146" s="23">
-        <v>1</v>
-      </c>
-      <c r="F146" s="15">
+      <c r="E146" s="17">
+        <v>1</v>
+      </c>
+      <c r="F146" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="147" spans="1:6">
       <c r="A147" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6">
+      <c r="B148" s="7" t="s">
+        <v>374</v>
+      </c>
+      <c r="C148" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="E148" s="17">
+        <v>1</v>
+      </c>
+      <c r="F148" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6">
+      <c r="B149" s="7" t="s">
+        <v>375</v>
+      </c>
+      <c r="C149" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="E149" s="17">
+        <v>1</v>
+      </c>
+      <c r="F149" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6">
+      <c r="A150" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="148" spans="1:6">
-      <c r="B148" s="25" t="s">
+    <row r="151" spans="1:6">
+      <c r="B151" s="19" t="s">
         <v>313</v>
       </c>
-      <c r="C148" s="26" t="s">
+      <c r="C151" s="20" t="s">
         <v>314</v>
       </c>
-      <c r="E148" s="23">
-        <v>1</v>
-      </c>
-      <c r="F148" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="149" spans="1:6">
-      <c r="B149" s="25" t="s">
+      <c r="E151" s="17">
+        <v>1</v>
+      </c>
+      <c r="F151" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6">
+      <c r="B152" s="19" t="s">
         <v>330</v>
       </c>
-      <c r="C149" s="26" t="s">
+      <c r="C152" s="20" t="s">
         <v>315</v>
       </c>
-      <c r="E149" s="23">
-        <v>1</v>
-      </c>
-      <c r="F149" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="150" spans="1:6">
-      <c r="B150" s="25" t="s">
+      <c r="E152" s="17">
+        <v>1</v>
+      </c>
+      <c r="F152" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6">
+      <c r="B153" s="19" t="s">
         <v>331</v>
       </c>
-      <c r="C150" s="26" t="s">
+      <c r="C153" s="20" t="s">
         <v>316</v>
       </c>
-      <c r="E150" s="23">
-        <v>1</v>
-      </c>
-      <c r="F150" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="151" spans="1:6">
-      <c r="A151" s="21"/>
-      <c r="B151" s="25" t="s">
+      <c r="E153" s="17">
+        <v>1</v>
+      </c>
+      <c r="F153" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6">
+      <c r="A154" s="15"/>
+      <c r="B154" s="19" t="s">
         <v>333</v>
       </c>
-      <c r="C151" s="26" t="s">
+      <c r="C154" s="20" t="s">
         <v>317</v>
       </c>
-      <c r="E151" s="23">
-        <v>1</v>
-      </c>
-      <c r="F151" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="152" spans="1:6">
-      <c r="A152" s="21"/>
-      <c r="B152" s="25" t="s">
+      <c r="E154" s="17">
+        <v>1</v>
+      </c>
+      <c r="F154" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6">
+      <c r="A155" s="15"/>
+      <c r="B155" s="19" t="s">
         <v>332</v>
       </c>
-      <c r="C152" s="26" t="s">
+      <c r="C155" s="20" t="s">
         <v>318</v>
       </c>
-      <c r="E152" s="23">
-        <v>1</v>
-      </c>
-      <c r="F152" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="153" spans="1:6">
-      <c r="B153" s="25" t="s">
+      <c r="E155" s="17">
+        <v>1</v>
+      </c>
+      <c r="F155" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6">
+      <c r="B156" s="19" t="s">
         <v>334</v>
       </c>
-      <c r="C153" s="26" t="s">
+      <c r="C156" s="20" t="s">
         <v>319</v>
       </c>
-      <c r="E153" s="23">
-        <v>1</v>
-      </c>
-      <c r="F153" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="154" spans="1:6">
-      <c r="B154" s="25" t="s">
+      <c r="E156" s="17">
+        <v>1</v>
+      </c>
+      <c r="F156" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6">
+      <c r="B157" s="19" t="s">
         <v>335</v>
       </c>
-      <c r="C154" s="26" t="s">
+      <c r="C157" s="20" t="s">
         <v>320</v>
       </c>
-      <c r="E154" s="23">
-        <v>1</v>
-      </c>
-      <c r="F154" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="155" spans="1:6">
-      <c r="B155" s="25" t="s">
+      <c r="E157" s="17">
+        <v>1</v>
+      </c>
+      <c r="F157" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6">
+      <c r="B158" s="19" t="s">
         <v>336</v>
       </c>
-      <c r="C155" s="26" t="s">
+      <c r="C158" s="20" t="s">
         <v>321</v>
       </c>
-      <c r="E155" s="23">
-        <v>1</v>
-      </c>
-      <c r="F155" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="156" spans="1:6">
-      <c r="B156" s="25" t="s">
+      <c r="E158" s="17">
+        <v>1</v>
+      </c>
+      <c r="F158" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6">
+      <c r="B159" s="19" t="s">
         <v>343</v>
       </c>
-      <c r="C156" s="26" t="s">
+      <c r="C159" s="20" t="s">
         <v>322</v>
       </c>
-      <c r="E156" s="23">
-        <v>1</v>
-      </c>
-      <c r="F156" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="157" spans="1:6">
-      <c r="B157" s="25" t="s">
+      <c r="E159" s="17">
+        <v>1</v>
+      </c>
+      <c r="F159" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6">
+      <c r="B160" s="19" t="s">
         <v>344</v>
       </c>
-      <c r="C157" s="26" t="s">
+      <c r="C160" s="20" t="s">
         <v>323</v>
       </c>
-      <c r="E157" s="23">
-        <v>1</v>
-      </c>
-      <c r="F157" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="158" spans="1:6">
-      <c r="B158" s="25" t="s">
+      <c r="E160" s="17">
+        <v>1</v>
+      </c>
+      <c r="F160" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6">
+      <c r="B161" s="19" t="s">
         <v>337</v>
       </c>
-      <c r="C158" s="26" t="s">
+      <c r="C161" s="20" t="s">
         <v>324</v>
       </c>
-      <c r="E158" s="23">
-        <v>1</v>
-      </c>
-      <c r="F158" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="159" spans="1:6">
-      <c r="B159" s="25" t="s">
+      <c r="E161" s="17">
+        <v>1</v>
+      </c>
+      <c r="F161" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6">
+      <c r="B162" s="19" t="s">
         <v>338</v>
       </c>
-      <c r="C159" s="26" t="s">
+      <c r="C162" s="20" t="s">
         <v>325</v>
       </c>
-      <c r="E159" s="23">
-        <v>1</v>
-      </c>
-      <c r="F159" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="160" spans="1:6">
-      <c r="B160" s="25" t="s">
+      <c r="E162" s="17">
+        <v>1</v>
+      </c>
+      <c r="F162" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6">
+      <c r="B163" s="19" t="s">
         <v>339</v>
       </c>
-      <c r="C160" s="26" t="s">
+      <c r="C163" s="20" t="s">
         <v>326</v>
       </c>
-      <c r="E160" s="23">
-        <v>1</v>
-      </c>
-      <c r="F160" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="161" spans="1:6">
-      <c r="B161" s="25" t="s">
+      <c r="E163" s="17">
+        <v>1</v>
+      </c>
+      <c r="F163" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6">
+      <c r="B164" s="19" t="s">
         <v>340</v>
       </c>
-      <c r="C161" s="26" t="s">
+      <c r="C164" s="20" t="s">
         <v>327</v>
       </c>
-      <c r="E161" s="23">
-        <v>1</v>
-      </c>
-      <c r="F161" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="162" spans="1:6">
-      <c r="B162" s="25" t="s">
+      <c r="E164" s="17">
+        <v>1</v>
+      </c>
+      <c r="F164" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6">
+      <c r="B165" s="19" t="s">
         <v>341</v>
       </c>
-      <c r="C162" s="26" t="s">
+      <c r="C165" s="20" t="s">
         <v>328</v>
       </c>
-      <c r="E162" s="23">
-        <v>1</v>
-      </c>
-      <c r="F162" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="163" spans="1:6">
-      <c r="B163" s="25" t="s">
+      <c r="E165" s="17">
+        <v>1</v>
+      </c>
+      <c r="F165" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6">
+      <c r="B166" s="19" t="s">
         <v>342</v>
       </c>
-      <c r="C163" s="26" t="s">
+      <c r="C166" s="20" t="s">
         <v>329</v>
       </c>
-      <c r="E163" s="23">
-        <v>1</v>
-      </c>
-      <c r="F163" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="164" spans="1:6">
-      <c r="B164" s="25" t="s">
+      <c r="E166" s="17">
+        <v>1</v>
+      </c>
+      <c r="F166" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6">
+      <c r="B167" s="19" t="s">
         <v>353</v>
       </c>
-      <c r="C164" s="27" t="s">
+      <c r="C167" s="21" t="s">
         <v>345</v>
       </c>
-      <c r="E164" s="23">
-        <v>1</v>
-      </c>
-      <c r="F164" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="165" spans="1:6">
-      <c r="B165" s="25" t="s">
+      <c r="E167" s="17">
+        <v>1</v>
+      </c>
+      <c r="F167" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6">
+      <c r="B168" s="19" t="s">
         <v>354</v>
       </c>
-      <c r="C165" s="27" t="s">
+      <c r="C168" s="21" t="s">
         <v>346</v>
       </c>
-      <c r="E165" s="23">
-        <v>1</v>
-      </c>
-      <c r="F165" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="166" spans="1:6">
-      <c r="B166" s="25" t="s">
+      <c r="E168" s="17">
+        <v>1</v>
+      </c>
+      <c r="F168" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6">
+      <c r="B169" s="19" t="s">
         <v>355</v>
       </c>
-      <c r="C166" s="27" t="s">
+      <c r="C169" s="21" t="s">
         <v>347</v>
       </c>
-      <c r="E166" s="23">
-        <v>1</v>
-      </c>
-      <c r="F166" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="167" spans="1:6">
-      <c r="B167" s="25" t="s">
+      <c r="E169" s="17">
+        <v>1</v>
+      </c>
+      <c r="F169" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6">
+      <c r="B170" s="19" t="s">
         <v>356</v>
       </c>
-      <c r="C167" s="27" t="s">
+      <c r="C170" s="21" t="s">
         <v>348</v>
       </c>
-      <c r="E167" s="23">
-        <v>1</v>
-      </c>
-      <c r="F167" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="168" spans="1:6">
-      <c r="B168" s="25" t="s">
+      <c r="E170" s="17">
+        <v>1</v>
+      </c>
+      <c r="F170" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6">
+      <c r="B171" s="19" t="s">
         <v>357</v>
       </c>
-      <c r="C168" s="27" t="s">
+      <c r="C171" s="21" t="s">
         <v>349</v>
       </c>
-      <c r="E168" s="23">
-        <v>1</v>
-      </c>
-      <c r="F168" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="169" spans="1:6">
-      <c r="B169" s="25" t="s">
+      <c r="E171" s="17">
+        <v>1</v>
+      </c>
+      <c r="F171" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6">
+      <c r="B172" s="19" t="s">
         <v>358</v>
       </c>
-      <c r="C169" s="27" t="s">
+      <c r="C172" s="21" t="s">
         <v>350</v>
       </c>
-      <c r="E169" s="23">
-        <v>1</v>
-      </c>
-      <c r="F169" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="170" spans="1:6">
-      <c r="B170" s="25" t="s">
+      <c r="E172" s="17">
+        <v>1</v>
+      </c>
+      <c r="F172" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6">
+      <c r="B173" s="19" t="s">
         <v>359</v>
       </c>
-      <c r="C170" s="27" t="s">
+      <c r="C173" s="21" t="s">
         <v>351</v>
       </c>
-      <c r="E170" s="23">
-        <v>1</v>
-      </c>
-      <c r="F170" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="171" spans="1:6">
-      <c r="B171" s="25" t="s">
+      <c r="E173" s="17">
+        <v>1</v>
+      </c>
+      <c r="F173" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6">
+      <c r="B174" s="19" t="s">
         <v>360</v>
       </c>
-      <c r="C171" s="27" t="s">
+      <c r="C174" s="21" t="s">
         <v>352</v>
       </c>
-      <c r="E171" s="23">
-        <v>1</v>
-      </c>
-      <c r="F171" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="172" spans="1:6">
-      <c r="A172" t="s">
+      <c r="E174" s="17">
+        <v>1</v>
+      </c>
+      <c r="F174" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6">
+      <c r="A175" t="s">
         <v>290</v>
       </c>
     </row>
@@ -4444,8 +4484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A28F574A-1A18-F84B-837D-BB0502A7BBD8}">
   <dimension ref="A1:C336"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="A211" sqref="A211"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -4516,7 +4556,7 @@
     <row r="15" spans="1:2">
       <c r="A15" s="2" t="str">
         <f>_xlfn.CONCAT("#define NB_OF_VAR ",FIXED(SUM('Memory setup'!E:E),0))</f>
-        <v>#define NB_OF_VAR 145</v>
+        <v>#define NB_OF_VAR 147</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -4532,7 +4572,7 @@
     <row r="19" spans="1:1">
       <c r="A19" s="2" t="str">
         <f>_xlfn.CONCAT("#define NB_EXPORTABLE_ADR ",FIXED(SUM('Memory setup'!F:F),0))</f>
-        <v>#define NB_EXPORTABLE_ADR 130</v>
+        <v>#define NB_EXPORTABLE_ADR 132</v>
       </c>
     </row>
     <row r="20" spans="1:1">
@@ -5458,175 +5498,175 @@
     <row r="182" spans="1:1">
       <c r="A182" t="str">
         <f>IF('Memory setup'!A147&lt;&gt;"",IF('Memory setup'!A147="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A147),IF('Memory setup'!E147=1,_xlfn.CONCAT("#define ",'Memory setup'!B147," ",'Memory setup'!C147," ",'Memory setup'!D147),""))</f>
-        <v>// Analog min/max calibrations</v>
+        <v>// SSI</v>
       </c>
     </row>
     <row r="183" spans="1:1">
       <c r="A183" t="str">
         <f>IF('Memory setup'!A148&lt;&gt;"",IF('Memory setup'!A148="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A148),IF('Memory setup'!E148=1,_xlfn.CONCAT("#define ",'Memory setup'!B148," ",'Memory setup'!C148," ",'Memory setup'!D148),""))</f>
-        <v xml:space="preserve">#define ADR_LOCALANALOG_MIN_0 0x500 </v>
+        <v xml:space="preserve">#define ADR_SSI_CONF1 0x413 </v>
       </c>
     </row>
     <row r="184" spans="1:1">
       <c r="A184" t="str">
         <f>IF('Memory setup'!A149&lt;&gt;"",IF('Memory setup'!A149="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A149),IF('Memory setup'!E149=1,_xlfn.CONCAT("#define ",'Memory setup'!B149," ",'Memory setup'!C149," ",'Memory setup'!D149),""))</f>
-        <v xml:space="preserve">#define ADR_LOCALANALOG_MAX_0 0x501 </v>
+        <v xml:space="preserve">#define ADR_SSI_OFS 0x414 </v>
       </c>
     </row>
     <row r="185" spans="1:1">
       <c r="A185" t="str">
         <f>IF('Memory setup'!A150&lt;&gt;"",IF('Memory setup'!A150="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A150),IF('Memory setup'!E150=1,_xlfn.CONCAT("#define ",'Memory setup'!B150," ",'Memory setup'!C150," ",'Memory setup'!D150),""))</f>
-        <v xml:space="preserve">#define ADR_LOCALANALOG_MIN_1 0x502 </v>
+        <v>// Analog min/max calibrations</v>
       </c>
     </row>
     <row r="186" spans="1:1">
       <c r="A186" t="str">
         <f>IF('Memory setup'!A151&lt;&gt;"",IF('Memory setup'!A151="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A151),IF('Memory setup'!E151=1,_xlfn.CONCAT("#define ",'Memory setup'!B151," ",'Memory setup'!C151," ",'Memory setup'!D151),""))</f>
-        <v xml:space="preserve">#define ADR_LOCALANALOG_MAX_1 0x503 </v>
+        <v xml:space="preserve">#define ADR_LOCALANALOG_MIN_0 0x500 </v>
       </c>
     </row>
     <row r="187" spans="1:1">
       <c r="A187" t="str">
         <f>IF('Memory setup'!A152&lt;&gt;"",IF('Memory setup'!A152="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A152),IF('Memory setup'!E152=1,_xlfn.CONCAT("#define ",'Memory setup'!B152," ",'Memory setup'!C152," ",'Memory setup'!D152),""))</f>
-        <v xml:space="preserve">#define ADR_LOCALANALOG_MIN_2 0x504 </v>
+        <v xml:space="preserve">#define ADR_LOCALANALOG_MAX_0 0x501 </v>
       </c>
     </row>
     <row r="188" spans="1:1">
       <c r="A188" t="str">
         <f>IF('Memory setup'!A153&lt;&gt;"",IF('Memory setup'!A153="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A153),IF('Memory setup'!E153=1,_xlfn.CONCAT("#define ",'Memory setup'!B153," ",'Memory setup'!C153," ",'Memory setup'!D153),""))</f>
-        <v xml:space="preserve">#define ADR_LOCALANALOG_MAX_2 0x505 </v>
+        <v xml:space="preserve">#define ADR_LOCALANALOG_MIN_1 0x502 </v>
       </c>
     </row>
     <row r="189" spans="1:1">
       <c r="A189" t="str">
         <f>IF('Memory setup'!A154&lt;&gt;"",IF('Memory setup'!A154="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A154),IF('Memory setup'!E154=1,_xlfn.CONCAT("#define ",'Memory setup'!B154," ",'Memory setup'!C154," ",'Memory setup'!D154),""))</f>
-        <v xml:space="preserve">#define ADR_LOCALANALOG_MIN_3 0x506 </v>
+        <v xml:space="preserve">#define ADR_LOCALANALOG_MAX_1 0x503 </v>
       </c>
     </row>
     <row r="190" spans="1:1">
       <c r="A190" t="str">
         <f>IF('Memory setup'!A155&lt;&gt;"",IF('Memory setup'!A155="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A155),IF('Memory setup'!E155=1,_xlfn.CONCAT("#define ",'Memory setup'!B155," ",'Memory setup'!C155," ",'Memory setup'!D155),""))</f>
-        <v xml:space="preserve">#define ADR_LOCALANALOG_MAX_3 0x507 </v>
+        <v xml:space="preserve">#define ADR_LOCALANALOG_MIN_2 0x504 </v>
       </c>
     </row>
     <row r="191" spans="1:1">
       <c r="A191" t="str">
         <f>IF('Memory setup'!A156&lt;&gt;"",IF('Memory setup'!A156="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A156),IF('Memory setup'!E156=1,_xlfn.CONCAT("#define ",'Memory setup'!B156," ",'Memory setup'!C156," ",'Memory setup'!D156),""))</f>
-        <v xml:space="preserve">#define ADR_LOCALANALOG_MIN_4 0x508 </v>
+        <v xml:space="preserve">#define ADR_LOCALANALOG_MAX_2 0x505 </v>
       </c>
     </row>
     <row r="192" spans="1:1">
       <c r="A192" t="str">
         <f>IF('Memory setup'!A157&lt;&gt;"",IF('Memory setup'!A157="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A157),IF('Memory setup'!E157=1,_xlfn.CONCAT("#define ",'Memory setup'!B157," ",'Memory setup'!C157," ",'Memory setup'!D157),""))</f>
-        <v xml:space="preserve">#define ADR_LOCALANALOG_MAX_4 0x509 </v>
+        <v xml:space="preserve">#define ADR_LOCALANALOG_MIN_3 0x506 </v>
       </c>
     </row>
     <row r="193" spans="1:1">
       <c r="A193" t="str">
         <f>IF('Memory setup'!A158&lt;&gt;"",IF('Memory setup'!A158="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A158),IF('Memory setup'!E158=1,_xlfn.CONCAT("#define ",'Memory setup'!B158," ",'Memory setup'!C158," ",'Memory setup'!D158),""))</f>
-        <v xml:space="preserve">#define ADR_LOCALANALOG_MIN_5 0x50A </v>
+        <v xml:space="preserve">#define ADR_LOCALANALOG_MAX_3 0x507 </v>
       </c>
     </row>
     <row r="194" spans="1:1">
       <c r="A194" t="str">
         <f>IF('Memory setup'!A159&lt;&gt;"",IF('Memory setup'!A159="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A159),IF('Memory setup'!E159=1,_xlfn.CONCAT("#define ",'Memory setup'!B159," ",'Memory setup'!C159," ",'Memory setup'!D159),""))</f>
-        <v xml:space="preserve">#define ADR_LOCALANALOG_MAX_5 0x50B </v>
+        <v xml:space="preserve">#define ADR_LOCALANALOG_MIN_4 0x508 </v>
       </c>
     </row>
     <row r="195" spans="1:1">
       <c r="A195" t="str">
         <f>IF('Memory setup'!A160&lt;&gt;"",IF('Memory setup'!A160="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A160),IF('Memory setup'!E160=1,_xlfn.CONCAT("#define ",'Memory setup'!B160," ",'Memory setup'!C160," ",'Memory setup'!D160),""))</f>
-        <v xml:space="preserve">#define ADR_LOCALANALOG_MIN_6 0x50C </v>
+        <v xml:space="preserve">#define ADR_LOCALANALOG_MAX_4 0x509 </v>
       </c>
     </row>
     <row r="196" spans="1:1">
       <c r="A196" t="str">
         <f>IF('Memory setup'!A161&lt;&gt;"",IF('Memory setup'!A161="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A161),IF('Memory setup'!E161=1,_xlfn.CONCAT("#define ",'Memory setup'!B161," ",'Memory setup'!C161," ",'Memory setup'!D161),""))</f>
-        <v xml:space="preserve">#define ADR_LOCALANALOG_MAX_6 0x50D </v>
+        <v xml:space="preserve">#define ADR_LOCALANALOG_MIN_5 0x50A </v>
       </c>
     </row>
     <row r="197" spans="1:1">
       <c r="A197" t="str">
         <f>IF('Memory setup'!A162&lt;&gt;"",IF('Memory setup'!A162="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A162),IF('Memory setup'!E162=1,_xlfn.CONCAT("#define ",'Memory setup'!B162," ",'Memory setup'!C162," ",'Memory setup'!D162),""))</f>
-        <v xml:space="preserve">#define ADR_LOCALANALOG_MIN_7 0x50E </v>
+        <v xml:space="preserve">#define ADR_LOCALANALOG_MAX_5 0x50B </v>
       </c>
     </row>
     <row r="198" spans="1:1">
       <c r="A198" t="str">
         <f>IF('Memory setup'!A163&lt;&gt;"",IF('Memory setup'!A163="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A163),IF('Memory setup'!E163=1,_xlfn.CONCAT("#define ",'Memory setup'!B163," ",'Memory setup'!C163," ",'Memory setup'!D163),""))</f>
-        <v xml:space="preserve">#define ADR_LOCALANALOG_MAX_7 0x50F </v>
+        <v xml:space="preserve">#define ADR_LOCALANALOG_MIN_6 0x50C </v>
       </c>
     </row>
     <row r="199" spans="1:1">
       <c r="A199" t="str">
         <f>IF('Memory setup'!A164&lt;&gt;"",IF('Memory setup'!A164="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A164),IF('Memory setup'!E164=1,_xlfn.CONCAT("#define ",'Memory setup'!B164," ",'Memory setup'!C164," ",'Memory setup'!D164),""))</f>
-        <v xml:space="preserve">#define ADR_ADS111X_MIN_0 0x510 </v>
+        <v xml:space="preserve">#define ADR_LOCALANALOG_MAX_6 0x50D </v>
       </c>
     </row>
     <row r="200" spans="1:1">
       <c r="A200" t="str">
         <f>IF('Memory setup'!A165&lt;&gt;"",IF('Memory setup'!A165="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A165),IF('Memory setup'!E165=1,_xlfn.CONCAT("#define ",'Memory setup'!B165," ",'Memory setup'!C165," ",'Memory setup'!D165),""))</f>
-        <v xml:space="preserve">#define ADR_ADS111X_MAX_0 0x511 </v>
+        <v xml:space="preserve">#define ADR_LOCALANALOG_MIN_7 0x50E </v>
       </c>
     </row>
     <row r="201" spans="1:1">
       <c r="A201" t="str">
         <f>IF('Memory setup'!A166&lt;&gt;"",IF('Memory setup'!A166="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A166),IF('Memory setup'!E166=1,_xlfn.CONCAT("#define ",'Memory setup'!B166," ",'Memory setup'!C166," ",'Memory setup'!D166),""))</f>
-        <v xml:space="preserve">#define ADR_ADS111X_MIN_1 0x512 </v>
+        <v xml:space="preserve">#define ADR_LOCALANALOG_MAX_7 0x50F </v>
       </c>
     </row>
     <row r="202" spans="1:1">
       <c r="A202" t="str">
         <f>IF('Memory setup'!A167&lt;&gt;"",IF('Memory setup'!A167="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A167),IF('Memory setup'!E167=1,_xlfn.CONCAT("#define ",'Memory setup'!B167," ",'Memory setup'!C167," ",'Memory setup'!D167),""))</f>
-        <v xml:space="preserve">#define ADR_ADS111X_MAX_1 0x513 </v>
+        <v xml:space="preserve">#define ADR_ADS111X_MIN_0 0x510 </v>
       </c>
     </row>
     <row r="203" spans="1:1">
       <c r="A203" t="str">
         <f>IF('Memory setup'!A168&lt;&gt;"",IF('Memory setup'!A168="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A168),IF('Memory setup'!E168=1,_xlfn.CONCAT("#define ",'Memory setup'!B168," ",'Memory setup'!C168," ",'Memory setup'!D168),""))</f>
-        <v xml:space="preserve">#define ADR_ADS111X_MIN_2 0x514 </v>
+        <v xml:space="preserve">#define ADR_ADS111X_MAX_0 0x511 </v>
       </c>
     </row>
     <row r="204" spans="1:1">
       <c r="A204" t="str">
         <f>IF('Memory setup'!A169&lt;&gt;"",IF('Memory setup'!A169="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A169),IF('Memory setup'!E169=1,_xlfn.CONCAT("#define ",'Memory setup'!B169," ",'Memory setup'!C169," ",'Memory setup'!D169),""))</f>
-        <v xml:space="preserve">#define ADR_ADS111X_MAX_2 0x515 </v>
+        <v xml:space="preserve">#define ADR_ADS111X_MIN_1 0x512 </v>
       </c>
     </row>
     <row r="205" spans="1:1">
       <c r="A205" t="str">
         <f>IF('Memory setup'!A170&lt;&gt;"",IF('Memory setup'!A170="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A170),IF('Memory setup'!E170=1,_xlfn.CONCAT("#define ",'Memory setup'!B170," ",'Memory setup'!C170," ",'Memory setup'!D170),""))</f>
-        <v xml:space="preserve">#define ADR_ADS111X_MIN_3 0x516 </v>
+        <v xml:space="preserve">#define ADR_ADS111X_MAX_1 0x513 </v>
       </c>
     </row>
     <row r="206" spans="1:1">
       <c r="A206" t="str">
         <f>IF('Memory setup'!A171&lt;&gt;"",IF('Memory setup'!A171="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A171),IF('Memory setup'!E171=1,_xlfn.CONCAT("#define ",'Memory setup'!B171," ",'Memory setup'!C171," ",'Memory setup'!D171),""))</f>
-        <v xml:space="preserve">#define ADR_ADS111X_MAX_3 0x517 </v>
+        <v xml:space="preserve">#define ADR_ADS111X_MIN_2 0x514 </v>
       </c>
     </row>
     <row r="207" spans="1:1">
       <c r="A207" t="str">
         <f>IF('Memory setup'!A172&lt;&gt;"",IF('Memory setup'!A172="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A172),IF('Memory setup'!E172=1,_xlfn.CONCAT("#define ",'Memory setup'!B172," ",'Memory setup'!C172," ",'Memory setup'!D172),""))</f>
-        <v>#endif /* EEPROM_ADDRESSES_H_ */</v>
+        <v xml:space="preserve">#define ADR_ADS111X_MAX_2 0x515 </v>
       </c>
     </row>
     <row r="208" spans="1:1">
       <c r="A208" t="str">
         <f>IF('Memory setup'!A173&lt;&gt;"",IF('Memory setup'!A173="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A173),IF('Memory setup'!E173=1,_xlfn.CONCAT("#define ",'Memory setup'!B173," ",'Memory setup'!C173," ",'Memory setup'!D173),""))</f>
-        <v/>
+        <v xml:space="preserve">#define ADR_ADS111X_MIN_3 0x516 </v>
       </c>
     </row>
     <row r="209" spans="1:1">
       <c r="A209" t="str">
         <f>IF('Memory setup'!A174&lt;&gt;"",IF('Memory setup'!A174="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A174),IF('Memory setup'!E174=1,_xlfn.CONCAT("#define ",'Memory setup'!B174," ",'Memory setup'!C174," ",'Memory setup'!D174),""))</f>
-        <v/>
+        <v xml:space="preserve">#define ADR_ADS111X_MAX_3 0x517 </v>
       </c>
     </row>
     <row r="210" spans="1:1">
       <c r="A210" t="str">
         <f>IF('Memory setup'!A175&lt;&gt;"",IF('Memory setup'!A175="#ENDOFSTRUCT#","#endif /* EEPROM_ADDRESSES_H_ */",'Memory setup'!A175),IF('Memory setup'!E175=1,_xlfn.CONCAT("#define ",'Memory setup'!B175," ",'Memory setup'!C175," ",'Memory setup'!D175),""))</f>
-        <v/>
+        <v>#endif /* EEPROM_ADDRESSES_H_ */</v>
       </c>
     </row>
     <row r="211" spans="1:1">
@@ -6379,10 +6419,10 @@
         <v/>
       </c>
     </row>
-    <row r="336" spans="1:3" s="18" customFormat="1">
-      <c r="A336" s="19"/>
-      <c r="B336" s="19"/>
-      <c r="C336" s="19"/>
+    <row r="336" spans="1:3">
+      <c r="A336" s="13"/>
+      <c r="B336" s="13"/>
+      <c r="C336" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6393,8 +6433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A15747F3-05ED-504F-B11C-F6CFE07DDC85}">
   <dimension ref="A1:C193"/>
   <sheetViews>
-    <sheetView topLeftCell="A160" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:C192"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C192" sqref="A17:C192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -8515,7 +8555,7 @@
     <row r="164" spans="1:3">
       <c r="A164" t="str">
         <f>IF('Memory setup'!A147&lt;&gt;"",IF('Memory setup'!A147&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A147,"};"),"")</f>
-        <v>// Analog min/max calibrations</v>
+        <v>// SSI</v>
       </c>
       <c r="B164" t="str">
         <f>IF('Memory setup'!E147=1,'Memory setup'!B147,IF('Memory setup'!B147&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B147),""))</f>
@@ -8533,7 +8573,7 @@
       </c>
       <c r="B165" t="str">
         <f>IF('Memory setup'!E148=1,'Memory setup'!B148,IF('Memory setup'!B148&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B148),""))</f>
-        <v>ADR_LOCALANALOG_MIN_0</v>
+        <v>ADR_SSI_CONF1</v>
       </c>
       <c r="C165" t="str">
         <f>IF(AND(B165&lt;&gt;"",'Memory setup'!A149&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8547,7 +8587,7 @@
       </c>
       <c r="B166" t="str">
         <f>IF('Memory setup'!E149=1,'Memory setup'!B149,IF('Memory setup'!B149&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B149),""))</f>
-        <v>ADR_LOCALANALOG_MAX_0</v>
+        <v>ADR_SSI_OFS</v>
       </c>
       <c r="C166" t="str">
         <f>IF(AND(B166&lt;&gt;"",'Memory setup'!A150&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8557,15 +8597,15 @@
     <row r="167" spans="1:3">
       <c r="A167" t="str">
         <f>IF('Memory setup'!A150&lt;&gt;"",IF('Memory setup'!A150&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A150,"};"),"")</f>
-        <v/>
+        <v>// Analog min/max calibrations</v>
       </c>
       <c r="B167" t="str">
         <f>IF('Memory setup'!E150=1,'Memory setup'!B150,IF('Memory setup'!B150&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B150),""))</f>
-        <v>ADR_LOCALANALOG_MIN_1</v>
+        <v/>
       </c>
       <c r="C167" t="str">
         <f>IF(AND(B167&lt;&gt;"",'Memory setup'!A151&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v>,</v>
+        <v/>
       </c>
     </row>
     <row r="168" spans="1:3">
@@ -8575,7 +8615,7 @@
       </c>
       <c r="B168" t="str">
         <f>IF('Memory setup'!E151=1,'Memory setup'!B151,IF('Memory setup'!B151&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B151),""))</f>
-        <v>ADR_LOCALANALOG_MAX_1</v>
+        <v>ADR_LOCALANALOG_MIN_0</v>
       </c>
       <c r="C168" t="str">
         <f>IF(AND(B168&lt;&gt;"",'Memory setup'!A152&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8589,7 +8629,7 @@
       </c>
       <c r="B169" t="str">
         <f>IF('Memory setup'!E152=1,'Memory setup'!B152,IF('Memory setup'!B152&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B152),""))</f>
-        <v>ADR_LOCALANALOG_MIN_2</v>
+        <v>ADR_LOCALANALOG_MAX_0</v>
       </c>
       <c r="C169" t="str">
         <f>IF(AND(B169&lt;&gt;"",'Memory setup'!A153&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8603,7 +8643,7 @@
       </c>
       <c r="B170" t="str">
         <f>IF('Memory setup'!E153=1,'Memory setup'!B153,IF('Memory setup'!B153&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B153),""))</f>
-        <v>ADR_LOCALANALOG_MAX_2</v>
+        <v>ADR_LOCALANALOG_MIN_1</v>
       </c>
       <c r="C170" t="str">
         <f>IF(AND(B170&lt;&gt;"",'Memory setup'!A154&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8617,7 +8657,7 @@
       </c>
       <c r="B171" t="str">
         <f>IF('Memory setup'!E154=1,'Memory setup'!B154,IF('Memory setup'!B154&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B154),""))</f>
-        <v>ADR_LOCALANALOG_MIN_3</v>
+        <v>ADR_LOCALANALOG_MAX_1</v>
       </c>
       <c r="C171" t="str">
         <f>IF(AND(B171&lt;&gt;"",'Memory setup'!A155&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8631,7 +8671,7 @@
       </c>
       <c r="B172" t="str">
         <f>IF('Memory setup'!E155=1,'Memory setup'!B155,IF('Memory setup'!B155&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B155),""))</f>
-        <v>ADR_LOCALANALOG_MAX_3</v>
+        <v>ADR_LOCALANALOG_MIN_2</v>
       </c>
       <c r="C172" t="str">
         <f>IF(AND(B172&lt;&gt;"",'Memory setup'!A156&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8645,7 +8685,7 @@
       </c>
       <c r="B173" t="str">
         <f>IF('Memory setup'!E156=1,'Memory setup'!B156,IF('Memory setup'!B156&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B156),""))</f>
-        <v>ADR_LOCALANALOG_MIN_4</v>
+        <v>ADR_LOCALANALOG_MAX_2</v>
       </c>
       <c r="C173" t="str">
         <f>IF(AND(B173&lt;&gt;"",'Memory setup'!A157&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8659,7 +8699,7 @@
       </c>
       <c r="B174" t="str">
         <f>IF('Memory setup'!E157=1,'Memory setup'!B157,IF('Memory setup'!B157&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B157),""))</f>
-        <v>ADR_LOCALANALOG_MAX_4</v>
+        <v>ADR_LOCALANALOG_MIN_3</v>
       </c>
       <c r="C174" t="str">
         <f>IF(AND(B174&lt;&gt;"",'Memory setup'!A158&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8673,7 +8713,7 @@
       </c>
       <c r="B175" t="str">
         <f>IF('Memory setup'!E158=1,'Memory setup'!B158,IF('Memory setup'!B158&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B158),""))</f>
-        <v>ADR_LOCALANALOG_MIN_5</v>
+        <v>ADR_LOCALANALOG_MAX_3</v>
       </c>
       <c r="C175" t="str">
         <f>IF(AND(B175&lt;&gt;"",'Memory setup'!A159&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8687,7 +8727,7 @@
       </c>
       <c r="B176" t="str">
         <f>IF('Memory setup'!E159=1,'Memory setup'!B159,IF('Memory setup'!B159&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B159),""))</f>
-        <v>ADR_LOCALANALOG_MAX_5</v>
+        <v>ADR_LOCALANALOG_MIN_4</v>
       </c>
       <c r="C176" t="str">
         <f>IF(AND(B176&lt;&gt;"",'Memory setup'!A160&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8701,7 +8741,7 @@
       </c>
       <c r="B177" t="str">
         <f>IF('Memory setup'!E160=1,'Memory setup'!B160,IF('Memory setup'!B160&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B160),""))</f>
-        <v>ADR_LOCALANALOG_MIN_6</v>
+        <v>ADR_LOCALANALOG_MAX_4</v>
       </c>
       <c r="C177" t="str">
         <f>IF(AND(B177&lt;&gt;"",'Memory setup'!A161&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8715,7 +8755,7 @@
       </c>
       <c r="B178" t="str">
         <f>IF('Memory setup'!E161=1,'Memory setup'!B161,IF('Memory setup'!B161&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B161),""))</f>
-        <v>ADR_LOCALANALOG_MAX_6</v>
+        <v>ADR_LOCALANALOG_MIN_5</v>
       </c>
       <c r="C178" t="str">
         <f>IF(AND(B178&lt;&gt;"",'Memory setup'!A162&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8729,7 +8769,7 @@
       </c>
       <c r="B179" t="str">
         <f>IF('Memory setup'!E162=1,'Memory setup'!B162,IF('Memory setup'!B162&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B162),""))</f>
-        <v>ADR_LOCALANALOG_MIN_7</v>
+        <v>ADR_LOCALANALOG_MAX_5</v>
       </c>
       <c r="C179" t="str">
         <f>IF(AND(B179&lt;&gt;"",'Memory setup'!A163&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8743,7 +8783,7 @@
       </c>
       <c r="B180" t="str">
         <f>IF('Memory setup'!E163=1,'Memory setup'!B163,IF('Memory setup'!B163&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B163),""))</f>
-        <v>ADR_LOCALANALOG_MAX_7</v>
+        <v>ADR_LOCALANALOG_MIN_6</v>
       </c>
       <c r="C180" t="str">
         <f>IF(AND(B180&lt;&gt;"",'Memory setup'!A164&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8757,7 +8797,7 @@
       </c>
       <c r="B181" t="str">
         <f>IF('Memory setup'!E164=1,'Memory setup'!B164,IF('Memory setup'!B164&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B164),""))</f>
-        <v>ADR_ADS111X_MIN_0</v>
+        <v>ADR_LOCALANALOG_MAX_6</v>
       </c>
       <c r="C181" t="str">
         <f>IF(AND(B181&lt;&gt;"",'Memory setup'!A165&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8771,7 +8811,7 @@
       </c>
       <c r="B182" t="str">
         <f>IF('Memory setup'!E165=1,'Memory setup'!B165,IF('Memory setup'!B165&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B165),""))</f>
-        <v>ADR_ADS111X_MAX_0</v>
+        <v>ADR_LOCALANALOG_MIN_7</v>
       </c>
       <c r="C182" t="str">
         <f>IF(AND(B182&lt;&gt;"",'Memory setup'!A166&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8785,7 +8825,7 @@
       </c>
       <c r="B183" t="str">
         <f>IF('Memory setup'!E166=1,'Memory setup'!B166,IF('Memory setup'!B166&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B166),""))</f>
-        <v>ADR_ADS111X_MIN_1</v>
+        <v>ADR_LOCALANALOG_MAX_7</v>
       </c>
       <c r="C183" t="str">
         <f>IF(AND(B183&lt;&gt;"",'Memory setup'!A167&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8799,7 +8839,7 @@
       </c>
       <c r="B184" t="str">
         <f>IF('Memory setup'!E167=1,'Memory setup'!B167,IF('Memory setup'!B167&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B167),""))</f>
-        <v>ADR_ADS111X_MAX_1</v>
+        <v>ADR_ADS111X_MIN_0</v>
       </c>
       <c r="C184" t="str">
         <f>IF(AND(B184&lt;&gt;"",'Memory setup'!A168&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8813,7 +8853,7 @@
       </c>
       <c r="B185" t="str">
         <f>IF('Memory setup'!E168=1,'Memory setup'!B168,IF('Memory setup'!B168&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B168),""))</f>
-        <v>ADR_ADS111X_MIN_2</v>
+        <v>ADR_ADS111X_MAX_0</v>
       </c>
       <c r="C185" t="str">
         <f>IF(AND(B185&lt;&gt;"",'Memory setup'!A169&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8827,7 +8867,7 @@
       </c>
       <c r="B186" t="str">
         <f>IF('Memory setup'!E169=1,'Memory setup'!B169,IF('Memory setup'!B169&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B169),""))</f>
-        <v>ADR_ADS111X_MAX_2</v>
+        <v>ADR_ADS111X_MIN_1</v>
       </c>
       <c r="C186" t="str">
         <f>IF(AND(B186&lt;&gt;"",'Memory setup'!A170&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8841,7 +8881,7 @@
       </c>
       <c r="B187" t="str">
         <f>IF('Memory setup'!E170=1,'Memory setup'!B170,IF('Memory setup'!B170&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B170),""))</f>
-        <v>ADR_ADS111X_MIN_3</v>
+        <v>ADR_ADS111X_MAX_1</v>
       </c>
       <c r="C187" t="str">
         <f>IF(AND(B187&lt;&gt;"",'Memory setup'!A171&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8855,25 +8895,25 @@
       </c>
       <c r="B188" t="str">
         <f>IF('Memory setup'!E171=1,'Memory setup'!B171,IF('Memory setup'!B171&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B171),""))</f>
-        <v>ADR_ADS111X_MAX_3</v>
+        <v>ADR_ADS111X_MIN_2</v>
       </c>
       <c r="C188" t="str">
         <f>IF(AND(B188&lt;&gt;"",'Memory setup'!A172&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v/>
+        <v>,</v>
       </c>
     </row>
     <row r="189" spans="1:3">
       <c r="A189" t="str">
         <f>IF('Memory setup'!A172&lt;&gt;"",IF('Memory setup'!A172&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A172,"};"),"")</f>
-        <v>};</v>
+        <v/>
       </c>
       <c r="B189" t="str">
         <f>IF('Memory setup'!E172=1,'Memory setup'!B172,IF('Memory setup'!B172&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B172),""))</f>
-        <v/>
+        <v>ADR_ADS111X_MAX_2</v>
       </c>
       <c r="C189" t="str">
         <f>IF(AND(B189&lt;&gt;"",'Memory setup'!A173&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v/>
+        <v>,</v>
       </c>
     </row>
     <row r="190" spans="1:3">
@@ -8883,11 +8923,11 @@
       </c>
       <c r="B190" t="str">
         <f>IF('Memory setup'!E173=1,'Memory setup'!B173,IF('Memory setup'!B173&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B173),""))</f>
-        <v/>
+        <v>ADR_ADS111X_MIN_3</v>
       </c>
       <c r="C190" t="str">
         <f>IF(AND(B190&lt;&gt;"",'Memory setup'!A174&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v/>
+        <v>,</v>
       </c>
     </row>
     <row r="191" spans="1:3">
@@ -8897,7 +8937,7 @@
       </c>
       <c r="B191" t="str">
         <f>IF('Memory setup'!E174=1,'Memory setup'!B174,IF('Memory setup'!B174&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B174),""))</f>
-        <v/>
+        <v>ADR_ADS111X_MAX_3</v>
       </c>
       <c r="C191" t="str">
         <f>IF(AND(B191&lt;&gt;"",'Memory setup'!A175&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -8907,7 +8947,7 @@
     <row r="192" spans="1:3">
       <c r="A192" t="str">
         <f>IF('Memory setup'!A175&lt;&gt;"",IF('Memory setup'!A175&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A175,"};"),"")</f>
-        <v/>
+        <v>};</v>
       </c>
       <c r="B192" t="str">
         <f>IF('Memory setup'!E175=1,'Memory setup'!B175,IF('Memory setup'!B175&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B175),""))</f>
@@ -8919,9 +8959,9 @@
       </c>
     </row>
     <row r="193" spans="1:3">
-      <c r="A193" s="17"/>
-      <c r="B193" s="17"/>
-      <c r="C193" s="17"/>
+      <c r="A193" s="13"/>
+      <c r="B193" s="13"/>
+      <c r="C193" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8932,8 +8972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCCA2C71-4C90-094A-BE8E-41D3DABF8E95}">
   <dimension ref="A1:C191"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="A176" sqref="A176"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C179" sqref="A1:C179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -11000,7 +11040,7 @@
     <row r="151" spans="1:3">
       <c r="A151" t="str">
         <f>IF('Memory setup'!A147&lt;&gt;"",IF('Memory setup'!A147&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A147,"};"),"")</f>
-        <v>// Analog min/max calibrations</v>
+        <v>// SSI</v>
       </c>
       <c r="B151" t="str">
         <f>IF('Memory setup'!F147=1,'Memory setup'!B147,IF('Memory setup'!B147&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B147),""))</f>
@@ -11018,7 +11058,7 @@
       </c>
       <c r="B152" t="str">
         <f>IF('Memory setup'!F148=1,'Memory setup'!B148,IF('Memory setup'!B148&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B148),""))</f>
-        <v>ADR_LOCALANALOG_MIN_0</v>
+        <v>ADR_SSI_CONF1</v>
       </c>
       <c r="C152" t="str">
         <f>IF(AND(B152&lt;&gt;"",'Memory setup'!A149&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -11032,7 +11072,7 @@
       </c>
       <c r="B153" t="str">
         <f>IF('Memory setup'!F149=1,'Memory setup'!B149,IF('Memory setup'!B149&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B149),""))</f>
-        <v>ADR_LOCALANALOG_MAX_0</v>
+        <v>ADR_SSI_OFS</v>
       </c>
       <c r="C153" t="str">
         <f>IF(AND(B153&lt;&gt;"",'Memory setup'!A150&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -11042,15 +11082,15 @@
     <row r="154" spans="1:3">
       <c r="A154" t="str">
         <f>IF('Memory setup'!A150&lt;&gt;"",IF('Memory setup'!A150&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A150,"};"),"")</f>
-        <v/>
+        <v>// Analog min/max calibrations</v>
       </c>
       <c r="B154" t="str">
         <f>IF('Memory setup'!F150=1,'Memory setup'!B150,IF('Memory setup'!B150&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B150),""))</f>
-        <v>ADR_LOCALANALOG_MIN_1</v>
+        <v/>
       </c>
       <c r="C154" t="str">
         <f>IF(AND(B154&lt;&gt;"",'Memory setup'!A151&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v>,</v>
+        <v/>
       </c>
     </row>
     <row r="155" spans="1:3">
@@ -11060,7 +11100,7 @@
       </c>
       <c r="B155" t="str">
         <f>IF('Memory setup'!F151=1,'Memory setup'!B151,IF('Memory setup'!B151&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B151),""))</f>
-        <v>ADR_LOCALANALOG_MAX_1</v>
+        <v>ADR_LOCALANALOG_MIN_0</v>
       </c>
       <c r="C155" t="str">
         <f>IF(AND(B155&lt;&gt;"",'Memory setup'!A152&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -11074,7 +11114,7 @@
       </c>
       <c r="B156" t="str">
         <f>IF('Memory setup'!F152=1,'Memory setup'!B152,IF('Memory setup'!B152&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B152),""))</f>
-        <v>ADR_LOCALANALOG_MIN_2</v>
+        <v>ADR_LOCALANALOG_MAX_0</v>
       </c>
       <c r="C156" t="str">
         <f>IF(AND(B156&lt;&gt;"",'Memory setup'!A153&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -11088,7 +11128,7 @@
       </c>
       <c r="B157" t="str">
         <f>IF('Memory setup'!F153=1,'Memory setup'!B153,IF('Memory setup'!B153&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B153),""))</f>
-        <v>ADR_LOCALANALOG_MAX_2</v>
+        <v>ADR_LOCALANALOG_MIN_1</v>
       </c>
       <c r="C157" t="str">
         <f>IF(AND(B157&lt;&gt;"",'Memory setup'!A154&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -11102,7 +11142,7 @@
       </c>
       <c r="B158" t="str">
         <f>IF('Memory setup'!F154=1,'Memory setup'!B154,IF('Memory setup'!B154&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B154),""))</f>
-        <v>ADR_LOCALANALOG_MIN_3</v>
+        <v>ADR_LOCALANALOG_MAX_1</v>
       </c>
       <c r="C158" t="str">
         <f>IF(AND(B158&lt;&gt;"",'Memory setup'!A155&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -11116,7 +11156,7 @@
       </c>
       <c r="B159" t="str">
         <f>IF('Memory setup'!F155=1,'Memory setup'!B155,IF('Memory setup'!B155&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B155),""))</f>
-        <v>ADR_LOCALANALOG_MAX_3</v>
+        <v>ADR_LOCALANALOG_MIN_2</v>
       </c>
       <c r="C159" t="str">
         <f>IF(AND(B159&lt;&gt;"",'Memory setup'!A156&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -11130,7 +11170,7 @@
       </c>
       <c r="B160" t="str">
         <f>IF('Memory setup'!F156=1,'Memory setup'!B156,IF('Memory setup'!B156&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B156),""))</f>
-        <v>ADR_LOCALANALOG_MIN_4</v>
+        <v>ADR_LOCALANALOG_MAX_2</v>
       </c>
       <c r="C160" t="str">
         <f>IF(AND(B160&lt;&gt;"",'Memory setup'!A157&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -11144,7 +11184,7 @@
       </c>
       <c r="B161" t="str">
         <f>IF('Memory setup'!F157=1,'Memory setup'!B157,IF('Memory setup'!B157&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B157),""))</f>
-        <v>ADR_LOCALANALOG_MAX_4</v>
+        <v>ADR_LOCALANALOG_MIN_3</v>
       </c>
       <c r="C161" t="str">
         <f>IF(AND(B161&lt;&gt;"",'Memory setup'!A158&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -11158,7 +11198,7 @@
       </c>
       <c r="B162" t="str">
         <f>IF('Memory setup'!F158=1,'Memory setup'!B158,IF('Memory setup'!B158&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B158),""))</f>
-        <v>ADR_LOCALANALOG_MIN_5</v>
+        <v>ADR_LOCALANALOG_MAX_3</v>
       </c>
       <c r="C162" t="str">
         <f>IF(AND(B162&lt;&gt;"",'Memory setup'!A159&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -11172,7 +11212,7 @@
       </c>
       <c r="B163" t="str">
         <f>IF('Memory setup'!F159=1,'Memory setup'!B159,IF('Memory setup'!B159&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B159),""))</f>
-        <v>ADR_LOCALANALOG_MAX_5</v>
+        <v>ADR_LOCALANALOG_MIN_4</v>
       </c>
       <c r="C163" t="str">
         <f>IF(AND(B163&lt;&gt;"",'Memory setup'!A160&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -11186,7 +11226,7 @@
       </c>
       <c r="B164" t="str">
         <f>IF('Memory setup'!F160=1,'Memory setup'!B160,IF('Memory setup'!B160&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B160),""))</f>
-        <v>ADR_LOCALANALOG_MIN_6</v>
+        <v>ADR_LOCALANALOG_MAX_4</v>
       </c>
       <c r="C164" t="str">
         <f>IF(AND(B164&lt;&gt;"",'Memory setup'!A161&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -11200,7 +11240,7 @@
       </c>
       <c r="B165" t="str">
         <f>IF('Memory setup'!F161=1,'Memory setup'!B161,IF('Memory setup'!B161&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B161),""))</f>
-        <v>ADR_LOCALANALOG_MAX_6</v>
+        <v>ADR_LOCALANALOG_MIN_5</v>
       </c>
       <c r="C165" t="str">
         <f>IF(AND(B165&lt;&gt;"",'Memory setup'!A162&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -11214,7 +11254,7 @@
       </c>
       <c r="B166" t="str">
         <f>IF('Memory setup'!F162=1,'Memory setup'!B162,IF('Memory setup'!B162&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B162),""))</f>
-        <v>ADR_LOCALANALOG_MIN_7</v>
+        <v>ADR_LOCALANALOG_MAX_5</v>
       </c>
       <c r="C166" t="str">
         <f>IF(AND(B166&lt;&gt;"",'Memory setup'!A163&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -11228,7 +11268,7 @@
       </c>
       <c r="B167" t="str">
         <f>IF('Memory setup'!F163=1,'Memory setup'!B163,IF('Memory setup'!B163&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B163),""))</f>
-        <v>ADR_LOCALANALOG_MAX_7</v>
+        <v>ADR_LOCALANALOG_MIN_6</v>
       </c>
       <c r="C167" t="str">
         <f>IF(AND(B167&lt;&gt;"",'Memory setup'!A164&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -11242,7 +11282,7 @@
       </c>
       <c r="B168" t="str">
         <f>IF('Memory setup'!F164=1,'Memory setup'!B164,IF('Memory setup'!B164&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B164),""))</f>
-        <v>ADR_ADS111X_MIN_0</v>
+        <v>ADR_LOCALANALOG_MAX_6</v>
       </c>
       <c r="C168" t="str">
         <f>IF(AND(B168&lt;&gt;"",'Memory setup'!A165&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -11256,7 +11296,7 @@
       </c>
       <c r="B169" t="str">
         <f>IF('Memory setup'!F165=1,'Memory setup'!B165,IF('Memory setup'!B165&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B165),""))</f>
-        <v>ADR_ADS111X_MAX_0</v>
+        <v>ADR_LOCALANALOG_MIN_7</v>
       </c>
       <c r="C169" t="str">
         <f>IF(AND(B169&lt;&gt;"",'Memory setup'!A166&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -11270,7 +11310,7 @@
       </c>
       <c r="B170" t="str">
         <f>IF('Memory setup'!F166=1,'Memory setup'!B166,IF('Memory setup'!B166&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B166),""))</f>
-        <v>ADR_ADS111X_MIN_1</v>
+        <v>ADR_LOCALANALOG_MAX_7</v>
       </c>
       <c r="C170" t="str">
         <f>IF(AND(B170&lt;&gt;"",'Memory setup'!A167&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -11284,7 +11324,7 @@
       </c>
       <c r="B171" t="str">
         <f>IF('Memory setup'!F167=1,'Memory setup'!B167,IF('Memory setup'!B167&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B167),""))</f>
-        <v>ADR_ADS111X_MAX_1</v>
+        <v>ADR_ADS111X_MIN_0</v>
       </c>
       <c r="C171" t="str">
         <f>IF(AND(B171&lt;&gt;"",'Memory setup'!A168&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -11298,7 +11338,7 @@
       </c>
       <c r="B172" t="str">
         <f>IF('Memory setup'!F168=1,'Memory setup'!B168,IF('Memory setup'!B168&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B168),""))</f>
-        <v>ADR_ADS111X_MIN_2</v>
+        <v>ADR_ADS111X_MAX_0</v>
       </c>
       <c r="C172" t="str">
         <f>IF(AND(B172&lt;&gt;"",'Memory setup'!A169&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -11312,7 +11352,7 @@
       </c>
       <c r="B173" t="str">
         <f>IF('Memory setup'!F169=1,'Memory setup'!B169,IF('Memory setup'!B169&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B169),""))</f>
-        <v>ADR_ADS111X_MAX_2</v>
+        <v>ADR_ADS111X_MIN_1</v>
       </c>
       <c r="C173" t="str">
         <f>IF(AND(B173&lt;&gt;"",'Memory setup'!A170&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -11326,7 +11366,7 @@
       </c>
       <c r="B174" t="str">
         <f>IF('Memory setup'!F170=1,'Memory setup'!B170,IF('Memory setup'!B170&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B170),""))</f>
-        <v>ADR_ADS111X_MIN_3</v>
+        <v>ADR_ADS111X_MAX_1</v>
       </c>
       <c r="C174" t="str">
         <f>IF(AND(B174&lt;&gt;"",'Memory setup'!A171&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -11340,25 +11380,25 @@
       </c>
       <c r="B175" t="str">
         <f>IF('Memory setup'!F171=1,'Memory setup'!B171,IF('Memory setup'!B171&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B171),""))</f>
-        <v>ADR_ADS111X_MAX_3</v>
+        <v>ADR_ADS111X_MIN_2</v>
       </c>
       <c r="C175" t="str">
         <f>IF(AND(B175&lt;&gt;"",'Memory setup'!A172&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v/>
+        <v>,</v>
       </c>
     </row>
     <row r="176" spans="1:3">
       <c r="A176" t="str">
         <f>IF('Memory setup'!A172&lt;&gt;"",IF('Memory setup'!A172&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A172,"};"),"")</f>
-        <v>};</v>
+        <v/>
       </c>
       <c r="B176" t="str">
         <f>IF('Memory setup'!F172=1,'Memory setup'!B172,IF('Memory setup'!B172&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B172),""))</f>
-        <v/>
+        <v>ADR_ADS111X_MAX_2</v>
       </c>
       <c r="C176" t="str">
         <f>IF(AND(B176&lt;&gt;"",'Memory setup'!A173&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v/>
+        <v>,</v>
       </c>
     </row>
     <row r="177" spans="1:3">
@@ -11368,11 +11408,11 @@
       </c>
       <c r="B177" t="str">
         <f>IF('Memory setup'!F173=1,'Memory setup'!B173,IF('Memory setup'!B173&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B173),""))</f>
-        <v/>
+        <v>ADR_ADS111X_MIN_3</v>
       </c>
       <c r="C177" t="str">
         <f>IF(AND(B177&lt;&gt;"",'Memory setup'!A174&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
-        <v/>
+        <v>,</v>
       </c>
     </row>
     <row r="178" spans="1:3">
@@ -11382,7 +11422,7 @@
       </c>
       <c r="B178" t="str">
         <f>IF('Memory setup'!F174=1,'Memory setup'!B174,IF('Memory setup'!B174&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B174),""))</f>
-        <v/>
+        <v>ADR_ADS111X_MAX_3</v>
       </c>
       <c r="C178" t="str">
         <f>IF(AND(B178&lt;&gt;"",'Memory setup'!A175&lt;&gt;"#ENDOFSTRUCT#"),",","")</f>
@@ -11392,7 +11432,7 @@
     <row r="179" spans="1:3">
       <c r="A179" t="str">
         <f>IF('Memory setup'!A175&lt;&gt;"",IF('Memory setup'!A175&lt;&gt;"#ENDOFSTRUCT#",'Memory setup'!A175,"};"),"")</f>
-        <v/>
+        <v>};</v>
       </c>
       <c r="B179" t="str">
         <f>IF('Memory setup'!F175=1,'Memory setup'!B175,IF('Memory setup'!B175&lt;&gt;"",_xlfn.CONCAT("//",'Memory setup'!B175),""))</f>

</xml_diff>